<commit_message>
add scalar index with partition cases
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="441">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1188,142 +1188,390 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select age,id from $scalar001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>select id,name from $scalar003</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_010.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_011.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_012.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_013.csv</t>
+  </si>
+  <si>
+    <t>scalar_index_014</t>
+  </si>
+  <si>
+    <t>联合索引的全部字段为全部主键</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_common_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar010_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select test_date,test_type,op_count,thread_num from $scalar010 where thread_num=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_014.csv</t>
+  </si>
+  <si>
+    <t>scalar_index_015</t>
+  </si>
+  <si>
+    <t>scalar_index_016</t>
+  </si>
+  <si>
+    <t>scalar_index_017</t>
+  </si>
+  <si>
+    <t>scalar_index_018</t>
+  </si>
+  <si>
+    <t>scalar_index_019</t>
+  </si>
+  <si>
+    <t>创建表，主键和非主键联合索引 int + int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar011</t>
+  </si>
+  <si>
+    <t>scalar012</t>
+  </si>
+  <si>
+    <t>scalar013</t>
+  </si>
+  <si>
+    <t>scalar014</t>
+  </si>
+  <si>
+    <t>scalar015</t>
+  </si>
+  <si>
+    <t>select id,age from $scalar011 where age&gt;10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_015.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_016.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_017.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_018.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_019.csv</t>
+  </si>
+  <si>
+    <t>创建表，主键和非主键联合索引 bigint + varchar + date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建表，多个非主键联合索引,按字段顺序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建表，多个非主键联合索引,不按字段顺序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建表，多个非主键索引</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,name,birthday from $scalar012 where name='zhangsan'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select update_time,gmt,address from $scalar014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $scalar001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age,id from $scalar001 where id&gt;age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>select birthday,id from $scalar006</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select * from $scalar001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_010.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_011.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_012.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_013.csv</t>
-  </si>
-  <si>
-    <t>scalar_index_014</t>
-  </si>
-  <si>
-    <t>联合索引的全部字段为全部主键</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scalar010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scalar_common_value1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scalar010_value1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select test_date,test_type,op_count,thread_num from $scalar010 where thread_num=100</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_014.csv</t>
-  </si>
-  <si>
-    <t>scalar_index_015</t>
-  </si>
-  <si>
-    <t>scalar_index_016</t>
-  </si>
-  <si>
-    <t>scalar_index_017</t>
-  </si>
-  <si>
-    <t>scalar_index_018</t>
-  </si>
-  <si>
-    <t>scalar_index_019</t>
-  </si>
-  <si>
-    <t>创建表，主键和非主键联合索引 int + int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scalar011</t>
-  </si>
-  <si>
-    <t>scalar012</t>
-  </si>
-  <si>
-    <t>scalar013</t>
-  </si>
-  <si>
-    <t>scalar014</t>
-  </si>
-  <si>
-    <t>scalar015</t>
-  </si>
-  <si>
-    <t>select id,age from $scalar011 where age&gt;10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_015.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_016.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_017.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_018.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_019.csv</t>
-  </si>
-  <si>
-    <t>创建表，主键和非主键联合索引 bigint + varchar + date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建表，多个非主键联合索引,按字段顺序</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建表，多个非主键联合索引,不按字段顺序</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建表，多个非主键索引</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select id,name,birthday from $scalar012 where name='zhangsan'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select name,age,amount,birthday from $scalar013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select update_time,gmt,address from $scalar014</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select name,amount,create_time from $scalar015 where create_time&lt;'12:00:00'</t>
+    <t>select name,age,amount,birthday from $scalar013 where name='zhangsan' and age=18 and birthday='2015-09-10'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name,amount,create_time from $scalar015 where create_time&lt;'12:00:00' and amount&gt;10.0 and name='lisi'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_index_020</t>
+  </si>
+  <si>
+    <t>scalar_index_021</t>
+  </si>
+  <si>
+    <t>创建单字段索引表，对索引表按索引字段分区 - int索引字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建单字段索引表，对索引表按索引字段分区 - varchar索引字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar016</t>
+  </si>
+  <si>
+    <t>scalar017</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_020.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_021.csv</t>
+  </si>
+  <si>
+    <t>select age from $scalar016 where age&gt;20 order by age desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name from $scalar017 where name='op' or name&lt;'l3'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_index_022</t>
+  </si>
+  <si>
+    <t>创建主键和非主键联合索引表，对索引表仅按主键分区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar018</t>
+  </si>
+  <si>
+    <t>select * from $scalar018 where id&lt;15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_022.csv</t>
+  </si>
+  <si>
+    <t>scalar_index_023</t>
+  </si>
+  <si>
+    <t>创建主键和非主键联合索引表，对索引表仅按索引字段分区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar019</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_023.csv</t>
+  </si>
+  <si>
+    <t>select id,gmt from $scalar019 where gmt=2147483648 or gmt=-2147483648 or gmt=2147483647</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_index_024</t>
+  </si>
+  <si>
+    <t>创建主键和非主键联合索引表，对索引表按主键和索引字段分区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar020</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_024.csv</t>
+  </si>
+  <si>
+    <t>select id,address,birthday from $scalar020 where address='CHANGping' and birthday='2020-11-11' and id&lt;10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_index_025</t>
+  </si>
+  <si>
+    <t>scalar021</t>
+  </si>
+  <si>
+    <t>创建非主键联合索引表，对索引表仅按其中一个索引字段分区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_025.csv</t>
+  </si>
+  <si>
+    <t>select id,name,age,gmt,price,amount,address,birthday,create_time,update_time,zip_code,is_delete from $scalar021 where name='Z' and gmt=2147483647</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_index_026</t>
+  </si>
+  <si>
+    <t>创建非主键联合索引表，对索引表按所有索引字段分区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar022</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_026.csv</t>
+  </si>
+  <si>
+    <t>select * from $scalar022 where name='777' or gmt=0 or update_time='1953-10-21 16:10:28'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_index_027</t>
+  </si>
+  <si>
+    <t>创建多个非主键索引表，只一个索引分区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar023</t>
+  </si>
+  <si>
+    <t>select price,id from $scalar023 where price=-5.4389387E10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_027.csv</t>
+  </si>
+  <si>
+    <t>scalar_index_028</t>
+  </si>
+  <si>
+    <t>scalar_index_029</t>
+  </si>
+  <si>
+    <t>创建非主键索引表，单个索引字段，分区值为两个元素，默认第二个为主键 - 单个主键</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar024</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_028.csv</t>
+  </si>
+  <si>
+    <t>select name,amount,gmt from $scalar024 where name&gt;='Z' and id between 10 and 30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建非主键索引表，两个索引字段，分区值为四个元素，默认第三个和第四个为主键 - 两个主键</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_029.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_index_030</t>
+  </si>
+  <si>
+    <t>scalar_index_031</t>
+  </si>
+  <si>
+    <t>scalar_index_032</t>
+  </si>
+  <si>
+    <t>创建表主键索引带有覆盖索引字段同主键字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar026</t>
+  </si>
+  <si>
+    <t>select id,id from $scalar026 where id&gt;10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_030.csv</t>
+  </si>
+  <si>
+    <t>scalar027</t>
+  </si>
+  <si>
+    <t>select id,name from $scalar027 where name='Dingo'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_031.csv</t>
+  </si>
+  <si>
+    <t>创建表主键索引带有覆盖索引字段为单个非主键字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select birthday,id,gmt from $scalar025 where name between 'Z' and 'z' and amount=1.18111600657875E11 or gmt=98211</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar025</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar025_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建表主键索引带有覆盖索引字段为多个非主键字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar028</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_032.csv</t>
+  </si>
+  <si>
+    <t>select id,price,gmt from $scalar028 where (price=0 or gmt=0) and birthday&gt;'2020-01-01'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_index_033</t>
+  </si>
+  <si>
+    <t>创建表主键索引带有覆盖索引字段为全部非主键字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar029</t>
+  </si>
+  <si>
+    <t>scalar029_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar_index_033.csv</t>
+  </si>
+  <si>
+    <t>select distinct age,gmt,price,amount,address,birthday,create_time,zip_code,is_delete from $scalar029 where update_time&gt;'2020-12-31 23:59:59'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1697,10 +1945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3118,7 +3366,7 @@
         <v>287</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>311</v>
@@ -3150,7 +3398,7 @@
         <v>288</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>295</v>
@@ -3182,7 +3430,7 @@
         <v>319</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>294</v>
@@ -3214,7 +3462,7 @@
         <v>289</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>296</v>
@@ -3246,7 +3494,7 @@
         <v>290</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>297</v>
@@ -3278,7 +3526,7 @@
         <v>321</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>298</v>
@@ -3310,7 +3558,7 @@
         <v>291</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>299</v>
@@ -3342,7 +3590,7 @@
         <v>292</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>300</v>
@@ -3374,7 +3622,7 @@
         <v>293</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>301</v>
@@ -3409,10 +3657,10 @@
         <v>318</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>329</v>
+        <v>365</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>10</v>
@@ -3441,10 +3689,10 @@
         <v>324</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>10</v>
@@ -3473,10 +3721,10 @@
         <v>326</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>331</v>
+        <v>366</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>10</v>
@@ -3505,10 +3753,10 @@
         <v>318</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>332</v>
+        <v>364</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>10</v>
@@ -3516,13 +3764,13 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>15</v>
@@ -3531,16 +3779,16 @@
         <v>286</v>
       </c>
       <c r="F57" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="I57" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="G57" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>342</v>
-      </c>
       <c r="J57" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>10</v>
@@ -3548,13 +3796,13 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>15</v>
@@ -3563,16 +3811,16 @@
         <v>286</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>10</v>
@@ -3580,13 +3828,13 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>15</v>
@@ -3595,16 +3843,16 @@
         <v>286</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>10</v>
@@ -3612,13 +3860,13 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>15</v>
@@ -3627,16 +3875,16 @@
         <v>286</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>10</v>
@@ -3644,13 +3892,13 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>15</v>
@@ -3659,16 +3907,16 @@
         <v>286</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>10</v>
@@ -3676,13 +3924,13 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>15</v>
@@ -3691,18 +3939,466 @@
         <v>286</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>368</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="K62" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A63" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A64" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A65" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A66" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A67" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A68" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A69" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A70" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A71" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A73" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A74" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A75" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A76" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="K76" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some cases data update
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
@@ -1768,18 +1768,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select id,feature_id,feature_index$distance from vector($vector052, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select id,feature_id,feature_index$distance from vector($vector053, feature, array[0.28576499223709106, 0.08687837421894073, 0.14799416065216064, 0.058550164103507996, 0.19060933589935303, 0.08999139070510864, 0.1514379382133484, 0.08630754053592682, 0.147443950176239, 0.11865786463022232, 0.08603266626596451, 0.026738379150629044, 0.04464268684387207, 0.07328195124864578, 0.1070372611284256, 0.08322914689779282, 0.034094709903001785, 0.16017472743988037, 0.03294524550437927, 0.14785508811473846, 0.18853361904621124, 0.14193195104599, 0.1404295563697815, 0.1011366918683052, 0.11323778331279755, 0.06974314898252487, 0.019739823415875435, 0.0017852566670626402, 0.19590851664543152, 0.04378505051136017, 0.13438871502876282, 0.12536169588565826, 0.037846311926841736, 0.19261693954467773, 0.15421807765960693, 0.012271392159163952, 0.08373595774173737, 0.1423385590314865, 0.13366387784481049, 0.14510740339756012, 0.02415030263364315, 0.04452469199895859, 0.0991881713271141, 0.13216648995876312, 0.10771691799163818, 0.1334938257932663, 0.10556206107139587, 0.10942403227090836, 0.10575082153081894, 0.18991316854953766, 0.1172894611954689, 0.09650064259767532, 0.16381768882274628, 0.03527522832155228, 0.09627934545278549, 0.1411363035440445, 0.09879021346569061, 0.18661963939666748, 0.036094631999731064, 0.2045263648033142, 0.18818239867687225, 0.15758785605430603, 0.02735513634979725, 0.16133542358875275], 10)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select id,feature_id,feature_index$distance from vector($vector054, feature, array[1.2949047088623047, 0.8476371169090271, 0.41010794043540955, 0.9785786271095276, 0.6064758896827698, 0.5890575647354126, 0.4460025131702423, 0.43684643507003784], 10)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>创建向量索引表 - 副本数2</t>
   </si>
   <si>
@@ -3256,6 +3244,18 @@
   </si>
   <si>
     <t>select id,feature_id,feature_index$distance from vector($vector028, feature, array[1.3535224199295044, 0.31392207741737366, 0.6286861896514893, 0.5430471301078796, 0.327924519777298, 0.6388945579528809, 0.6662382483482361, 0.9540348649024963, 0.8470741510391235, 0.558837354183197, 0.9277071952819824, 0.18017378449440002, 0.20220935344696045, 0.23732851445674896, 0.8634951710700989, 0.013733146712183952, 0.6470873951911926, 0.8624395728111267, 0.0532325841486454, 0.9079377055168152, 0.32841241359710693, 0.6605964303016663, 0.10226576030254364, 0.03404153883457184, 0.34508422017097473, 0.42952463030815125, 0.42589616775512695, 0.7463461756706238, 0.13148018717765808, 0.20628729462623596, 0.6974230408668518, 0.7751299738883972, 0.42980441451072693, 0.8757259249687195, 0.8634995222091675, 0.4060722291469574, 0.11937657743692398, 0.01659681834280491, 0.9395890831947327, 0.589221179485321, 0.3559124171733856, 0.9011857509613037, 0.5132598876953125, 0.8931979537010193, 0.017754850909113884, 0.05205504968762398, 0.10376431047916412, 0.5387919545173645, 0.09737808257341385, 0.6455812454223633, 0.5163909792900085, 0.8110367059707642, 0.7585089206695557, 0.3072868287563324, 0.5092869997024536, 0.07276355475187302, 0.27697500586509705, 0.5430586934089661, 0.6564051508903503, 0.2702702283859253, 0.7595415711402893, 0.1976347416639328, 0.9247005581855774, 0.578951358795166, 0.7895205616950989, 0.8593189716339111, 0.8979884386062622, 0.7156239151954651, 0.7308275103569031, 0.06604301929473877, 0.02126903086900711, 0.912445604801178, 0.6840839982032776, 0.9050001502037048, 0.7471106052398682, 0.6554510593414307, 0.05558401718735695, 0.008919947780668736, 0.06737808883190155, 0.02276572771370411, 0.11755851656198502, 0.7885823845863342, 0.2896302342414856, 0.6111487746238708, 0.5452771782875061, 0.5070639252662659, 0.5575328469276428, 0.9821842908859253, 0.6032338738441467, 0.2464839220046997, 0.04556428641080856, 0.20409837365150452, 0.5856149792671204, 0.6793073415756226, 0.5138164162635803, 0.06337228417396545, 0.5200310349464417, 0.8398666381835938, 0.17414791882038116, 0.7912601828575134, 0.3804928958415985, 0.6220223903656006, 0.23092465102672577, 0.6921454668045044, 0.4472225308418274, 0.5277025699615479, 0.139532670378685, 0.6781741380691528, 0.8661579489707947, 0.803992748260498, 0.31101688742637634, 0.2642950415611267, 0.35684001445770264, 0.9845317006111145, 0.6832847595214844, 0.9003570079803467, 0.5688319802284241, 0.3989367187023163, 0.19944503903388977, 0.5208761096000671, 0.9899275898933411, 0.5411144495010376, 0.5617583990097046, 0.20418207347393036, 0.9012929797172546, 0.718074381351471, 0.25599873065948486, 0.8763864636421204, 0.17597444355487823, 0.7684363126754761, 0.28905537724494934, 0.7825420498847961, 0.49110525846481323, 0.46907898783683777, 0.4610026478767395, 0.7931860089302063, 0.6691699624061584, 0.8590985536575317, 0.36251100897789, 0.302160382270813, 0.6255984902381897, 0.6185368299484253, 0.3431003987789154, 0.5225530862808228, 0.17594394087791443, 0.319243848323822, 0.34648874402046204, 0.6134116053581238, 0.5962549448013306, 0.15202587842941284, 0.03358858451247215, 0.9800461530685425, 0.11197073757648468, 0.7386590242385864, 0.08929972350597382, 0.8608983755111694, 0.4285961985588074, 0.6677455306053162, 0.8629558086395264, 0.9458568692207336, 0.10144906491041183, 0.7221893668174744, 0.6134009957313538, 0.635726809501648, 0.7860614061355591, 0.04271707311272621, 0.3278331756591797, 0.2661527693271637, 0.820303738117218, 0.6541527509689331, 0.06946848332881927, 0.4497787356376648, 0.26181983947753906, 0.8207583427429199, 0.526282787322998, 0.6442065238952637, 0.4397187829017639, 0.42431023716926575, 0.863955020904541, 0.8194906711578369, 0.3692033886909485, 0.29273590445518494, 0.20331180095672607, 0.3265809416770935, 0.7198004126548767, 0.7821041941642761, 0.22568848729133606, 0.7535693049430847, 0.10962527245283127, 0.7746263146400452, 0.41499581933021545, 0.9231970906257629, 0.12129457294940948, 0.03865664079785347, 0.8412232398986816, 0.8968071937561035, 0.5044061541557312, 0.527552604675293, 0.214138463139534, 0.5709258317947388, 0.4863903224468231, 0.6553916931152344, 0.3209784924983978, 0.43311354517936707, 0.9132612943649292, 0.6129176020622253, 0.7732480764389038, 0.10157007724046707, 0.8077899813652039, 0.6300846338272095, 0.5447371006011963, 0.03293538838624954, 0.2593502700328827, 0.36692947149276733, 0.7294648289680481, 0.8853902816772461, 0.1492408663034439, 0.323038250207901, 0.8157459497451782, 0.6161888241767883, 0.2771996557712555, 0.15968436002731323, 0.7917547821998596, 0.5117677450180054, 0.9797217845916748, 0.4572522044181824, 0.633741557598114, 0.050042491406202316, 0.9816424250602722, 0.03735988214612007, 0.20834188163280487, 0.40889671444892883, 0.46471431851387024, 0.3546723425388336, 0.3371832072734833, 0.46723422408103943, 0.1978747546672821, 0.12306314706802368, 0.8566398620605469, 0.29816874861717224, 0.5706659555435181, 0.13568951189517975, 0.58491450548172, 0.058242522180080414, 0.8876081109046936, 0.4532458484172821, 0.34756678342819214, 0.019598646089434624, 0.5479026436805725, 0.5178790092468262, 0.8009217381477356, 0.05276933312416077, 0.15879449248313904, 0.5511860847473145, 0.4744284152984619, 0.31998518109321594, 0.4216269552707672, 0.772039532661438, 0.12998369336128235, 0.350511759519577, 0.26288649439811707, 0.8798844814300537, 0.16706740856170654, 0.30563458800315857, 0.4884311556816101, 0.2878722548484802, 0.24419446289539337, 0.2479081153869629, 0.8877922296524048, 0.8932329416275024, 0.6359367370605469, 0.6506319046020508, 0.38934606313705444, 0.7937962412834167, 0.14109300076961517, 0.8118140697479248, 0.9655399322509766, 0.6201736927032471, 0.5559843182563782, 0.8355616927146912, 0.8100405931472778, 0.40611961483955383, 0.8194018006324768, 0.9660396575927734, 0.7525915503501892, 0.03655319660902023, 0.8989080786705017, 0.28844553232192993, 0.709339439868927, 0.782699465751648, 0.9315032958984375, 0.6763602495193481, 0.29540425539016724, 0.8221983313560486, 0.07585986703634262, 0.8574230074882507, 0.04927975684404373, 0.27592507004737854, 0.15236325562000275, 0.17199739813804626, 0.2829899787902832, 0.06075937673449516, 0.4812662601470947, 0.20124997198581696, 0.05699349567294121, 0.21945475041866302, 0.4001869857311249, 0.8960256576538086, 0.6441617608070374, 0.1969970315694809, 0.8967918157577515, 0.20898251235485077, 0.8699110150337219, 0.8007341623306274, 0.016917230561375618, 0.6108096837997437, 0.10050247609615326, 0.36888644099235535, 0.08611364662647247, 0.45928022265434265, 0.17870646715164185, 0.40315693616867065, 0.12586042284965515, 0.06276871263980865, 0.4162765443325043, 0.5260014533996582, 0.047529708594083786, 0.26816439628601074, 0.5966269969940186, 0.6473529934883118, 0.871753990650177, 0.144949272274971, 0.822285532951355, 0.7476346492767334, 0.42069026827812195, 0.9143622517585754, 0.49050143361091614, 0.3161744177341461, 0.9122335910797119, 0.6420398354530334, 0.4559533894062042, 0.7698162794113159, 0.3468329906463623, 0.3441320061683655, 0.5831806659698486, 0.9870078563690186, 0.529897153377533, 0.8140012621879578, 0.37875986099243164, 0.2879214286804199, 0.7916374802589417, 0.034201908856630325, 0.7240689396858215, 0.309619665145874, 0.5948328375816345, 0.1482827365398407, 0.064975306391716, 0.3544246256351471, 0.24767665565013885, 0.5309166312217712, 0.8236681818962097, 0.16633279621601105, 0.6045527458190918, 0.840312659740448, 0.8818798661231995, 0.2836647629737854, 0.24866093695163727, 0.16592605412006378, 0.8696073889732361, 0.15388169884681702, 0.1234707236289978, 0.0893031656742096, 0.759905993938446, 0.14988519251346588, 0.3773735761642456, 0.305133581161499, 0.9575893878936768, 0.036850590258836746, 0.20642253756523132, 0.9915892481803894, 0.5863695740699768, 0.9472546577453613, 0.9799618721008301, 0.8103383779525757, 0.35064542293548584, 0.10905013233423233, 0.6158831119537354, 0.31979936361312866, 0.7686752676963806, 0.29659366607666016, 0.175935298204422, 0.30370092391967773, 0.07879403233528137, 0.9581267833709717, 0.5903143882751465, 0.8368186950683594, 0.4258797764778137, 0.2547442317008972, 0.3142375946044922, 0.9655606150627136, 0.9529805779457092, 0.5794531106948853, 0.8737883567810059, 0.14201901853084564, 0.5911117196083069, 0.596875011920929, 0.3460487425327301, 0.617759108543396, 0.46116796135902405, 0.7459498047828674, 0.4751615524291992, 0.07415878027677536, 0.5300676822662354, 0.20728667080402374, 0.9711235165596008, 0.9838496446609497, 0.9765100479125977, 0.5397936701774597, 0.3189065456390381, 0.1277550756931305, 0.14100432395935059, 0.9208326935768127, 0.24735726416110992, 0.0042854794301092625, 0.7794864773750305, 0.01714763231575489, 0.7499006390571594, 0.09633156657218933, 0.11551760137081146, 0.43344646692276, 0.8221164345741272, 0.916947066783905, 0.9624882936477661, 0.23329205811023712, 0.820077657699585, 0.9002286195755005, 0.18546347320079803, 0.29306188225746155, 0.4147912561893463, 0.8118062019348145, 0.9458348155021667, 0.24703262746334076, 0.48520025610923767, 0.6130959987640381, 0.9061111807823181, 0.693015456199646, 0.5204097032546997, 0.8096333146095276, 0.7873492240905762, 0.3455691635608673, 0.6505943536758423, 0.5464634299278259, 0.9939194917678833, 0.009671092964708805, 0.172136127948761, 0.8355600237846375, 0.5392587184906006, 0.3844122886657715, 0.27245110273361206, 0.08908169716596603, 0.7321572303771973, 0.3043614625930786, 0.516395628452301, 0.8712427616119385, 0.9070706963539124, 0.6003034114837646, 0.4587913155555725, 0.43092480301856995, 0.05208354815840721, 0.17264613509178162, 0.11335580796003342, 0.7337794899940491, 0.8280722498893738, 0.8515526652336121, 0.182905375957489, 0.20550097525119781, 0.5318430066108704, 0.7694017887115479, 0.3260716497898102, 0.9888104200363159, 0.3905967175960541, 0.7081881165504456, 0.08131667971611023, 0.9327805042266846, 0.09879519045352936, 0.3782595098018646, 0.1964826136827469, 0.065560482442379, 0.4647301435470581, 0.4068993330001831, 0.068758025765419, 0.37635934352874756, 0.12430961430072784, 0.15205417573451996, 0.3794234097003937, 0.7064068913459778, 0.6421923637390137, 0.1213885024189949, 0.4444319009780884, 0.787514328956604, 0.6183278560638428, 0.5016001462936401, 0.1109316274523735, 0.23703736066818237, 0.48945075273513794, 0.06614242494106293, 0.2886432707309723, 0.6472116112709045, 0.5528389811515808, 0.260344922542572, 0.45896947383880615, 0.7337946891784668, 0.9727996587753296, 0.8410258889198303, 0.16144442558288574, 0.45416712760925293, 0.40877798199653625, 0.16939617693424225, 0.6642683744430542, 0.6432697176933289, 0.3228059709072113, 0.7809991836547852, 0.4492257535457611, 0.12247347831726074, 0.8468798995018005, 0.2833680212497711, 0.754226565361023, 0.2617167532444, 0.22498548030853271, 0.6968601942062378, 0.01867150515317917, 0.45630860328674316, 0.8501220345497131, 0.8321512937545776, 0.13769303262233734, 0.8910747170448303, 0.4661495089530945, 0.6513407230377197, 0.8318792581558228, 0.28195613622665405, 0.36692488193511963, 0.7187744379043579, 0.6934444904327393, 0.1999175250530243, 0.07552443444728851, 0.44622501730918884, 0.6139288544654846, 0.2826865613460541, 0.9559957981109619, 0.24807852506637573, 0.8561092615127563, 0.9534884691238403, 0.8511945009231567, 0.9334288239479065, 0.7140789031982422, 0.388191282749176, 0.8813086152076721, 0.2990174889564514, 0.8551315665245056, 0.6261729598045349, 0.47120681405067444, 0.4749518036842346, 0.2978686988353729, 0.7673436999320984, 0.5300029516220093, 0.7782717943191528, 0.48984426259994507, 0.5372359156608582, 0.7814760208129883, 0.9203964471817017, 0.12072478979825974, 0.9859831929206848, 0.7018551826477051, 0.5309759378433228, 0.2384367287158966, 0.9594374895095825, 0.5416489839553833, 0.6988224387168884, 0.17703697085380554, 0.8895614743232727, 0.4391710162162781, 0.7611968517303467, 0.7971492409706116, 0.4065127968788147, 0.4121829569339752, 0.7725569605827332, 0.4139801859855652, 0.0163713488727808, 0.6492041349411011, 0.08953416347503662, 0.8054971694946289, 0.6981039047241211, 0.7944212555885315, 0.13323798775672913, 0.8237714171409607, 0.5783477425575256, 0.776218593120575, 0.2682107388973236, 0.3471018671989441, 0.22101500630378723, 0.0013618111843243241, 0.46306857466697693, 0.9206815958023071, 0.4903622269630432, 0.016083497554063797, 0.2783198654651642, 0.3251529037952423, 0.5013194680213928, 0.11445412039756775, 0.012079134583473206, 0.2560001611709595, 0.9028116464614868, 0.19274145364761353, 0.05333879962563515, 0.7343361377716064, 0.7589075565338135, 0.3284699320793152, 0.07905074208974838, 0.612633466720581, 0.050045695155858994, 0.4453601837158203, 0.6522535681724548, 0.7844055891036987, 0.05484423041343689, 0.5774549841880798, 0.6620239615440369, 0.33169230818748474, 0.8406599760055542, 0.5894076228141785, 0.19468770921230316, 0.4066234827041626, 0.2146763801574707, 0.8467811942100525, 0.9844373464584351, 0.4828815460205078, 0.515873908996582, 0.08487104624509811, 0.6903231739997864, 0.9226033091545105, 0.802691638469696, 0.6860600113868713, 0.4897204637527466, 0.44427889585494995, 0.9516621232032776, 0.24357430636882782, 0.2184334099292755, 0.1172204315662384, 0.30623695254325867, 0.7359335422515869, 0.35206976532936096, 0.6945627331733704, 0.14384330809116364, 0.5232542753219604, 0.858997106552124, 0.09767534583806992, 0.3239775598049164, 0.5455408692359924, 0.5925885438919067, 0.44869863986968994, 0.918238639831543, 0.8670168519020081, 0.6096367239952087, 0.5765714049339294, 0.20481634140014648, 0.013852575793862343, 0.7634700536727905, 0.5896143913269043, 0.8080111742019653, 0.7057751417160034, 0.5197216868400574, 0.7997134923934937, 0.52923983335495, 0.03232930973172188, 0.018497133627533913, 0.7039249539375305, 0.011687240563333035, 0.5172359347343445, 0.5772852301597595, 0.10513359308242798, 0.2089967429637909, 0.5673447847366333, 0.18025241792201996, 0.4207831621170044, 0.5921681523323059, 0.09777862578630447, 0.08759112656116486, 0.9734905362129211, 0.9592893123626709, 0.15649233758449554, 0.7245137691497803, 0.14614325761795044, 0.06277640908956528, 0.7213056683540344, 0.9397366046905518, 0.6714769005775452, 0.5868414640426636, 0.17096030712127686, 0.04715782031416893, 0.6168940663337708, 0.06490743905305862, 0.20420877635478973, 0.9348860383033752, 0.04705149680376053, 0.9873403310775757, 0.16766494512557983, 0.7204188108444214, 0.4140930473804474, 0.539613664150238, 0.7032927870750427, 0.7088668942451477, 0.20077580213546753, 0.5277281403541565, 0.6421862244606018, 0.8054519891738892, 0.5765840411186218, 0.3639857769012451, 0.9252842664718628, 0.5993244647979736, 0.6518167853355408, 0.8031960725784302, 0.9634014368057251, 0.8032671809196472, 0.9200478196144104, 0.6832403540611267, 0.5457735657691956, 0.8271417617797852, 0.48793771862983704, 0.4425477385520935, 0.3262253701686859, 0.913882315158844, 0.02942078560590744, 0.6699893474578857, 0.8075922131538391, 0.6672304272651672, 0.15863613784313202, 0.6991033554077148, 0.5136383175849915, 0.4518413841724396, 0.11432988196611404, 0.8337645530700684, 0.19997699558734894, 0.7787659764289856, 0.8858902454376221, 0.3331146836280823, 0.4625246226787567, 0.709303617477417, 0.8493442535400391, 0.5922209620475769, 0.05531374737620354, 0.8209349513053894, 0.41280829906463623, 0.5246221423149109, 0.2334795892238617, 0.7214219570159912, 0.1311296820640564, 0.44521600008010864, 0.6902942657470703, 0.31479501724243164, 0.4011533260345459, 0.2884719967842102, 0.6499318480491638, 0.07902435213327408, 0.587889552116394, 0.4206700623035431, 0.6996663212776184, 0.35319074988365173, 0.025650616735219955, 0.23918427526950836, 0.7409505248069763, 0.4450435936450958, 0.5256019234657288, 0.4717833697795868, 0.8258699178695679, 0.5224175453186035, 0.7758104801177979, 0.5949121117591858, 0.9227606058120728, 0.9540846347808838, 0.5391230583190918, 0.4323936998844147, 0.5126331448554993, 0.5201613306999207, 0.9423797726631165, 0.48105093836784363, 0.9516801238059998, 0.28912651538848877, 0.02632157877087593, 0.9608991146087646, 0.01087308768182993, 0.024711405858397484, 0.6115622520446777, 0.6259920001029968, 0.4615266025066376, 0.9528838992118835, 0.1402873545885086, 0.11240574717521667, 0.658463180065155, 0.31963804364204407, 0.5899862051010132, 0.9113656878471375, 0.399395614862442, 0.13844920694828033, 0.027269160374999046, 0.25427162647247314, 0.42216628789901733, 0.04987042769789696, 0.18019147217273712, 0.7941862344741821, 0.9338135719299316, 0.46885237097740173, 0.23517246544361115, 0.4200786352157593, 0.48608848452568054, 0.4442487955093384, 0.09712281078100204, 0.07257167994976044, 0.4982982277870178, 0.5579163432121277, 0.6890251636505127, 0.9634112119674683, 0.038591355085372925, 0.011482151225209236, 0.10637529194355011, 0.47698545455932617, 0.7801839709281921, 0.7333822846412659, 0.7921286821365356, 0.7396711707115173, 0.918930172920227, 0.8444852232933044, 0.35946616530418396, 0.13169533014297485, 0.8867505192756653, 0.9843819737434387, 0.45732593536376953, 0.39677712321281433, 0.7165563702583313, 0.5174497365951538, 0.28845199942588806, 0.699768602848053, 0.22804494202136993, 0.7759913206100464, 0.017792699858546257, 0.22908005118370056, 0.033014751970767975, 0.38638630509376526, 0.7582269906997681, 0.9918963313102722, 0.2277938425540924, 0.3404541611671448, 0.2818209230899811, 0.5840474963188171, 0.20378121733665466, 0.2285759150981903, 0.3664989173412323, 0.26250016689300537, 0.8654340505599976, 0.293350487947464, 0.4659748673439026, 0.8676082491874695, 0.722886323928833, 0.7667917013168335, 0.3939172327518463, 0.010212404653429985, 0.6736516356468201, 0.1699751615524292, 0.41582465171813965, 0.05516976863145828, 0.16567884385585785, 0.6887815594673157, 0.6800487041473389, 0.31047749519348145, 0.3765132427215576, 0.7969440817832947, 0.6438823342323303, 0.15393388271331787, 0.6197165846824646, 0.6464699506759644, 0.6883950233459473, 0.1250983476638794, 0.06625806540250778, 0.0498005673289299, 0.36104512214660645, 0.14150340855121613, 0.3790360689163208, 0.3583654761314392, 0.49927186965942383, 0.05921294167637825, 0.35575079917907715, 0.5574421286582947, 0.15135829150676727, 0.5173702836036682, 0.08944489806890488, 0.7415786981582642, 0.610964834690094, 0.12629124522209167, 0.6571646332740784, 0.8580804467201233, 0.8047488927841187, 0.8786532282829285, 0.45353013277053833, 0.5217942595481873, 0.059725672006607056, 0.9192184209823608, 0.7132784128189087, 0.5126069188117981, 0.22028516232967377, 0.32300373911857605, 0.8696557879447937, 0.20453821122646332, 0.15377956628799438, 0.0202034842222929, 0.4030291736125946, 0.4018510580062866, 0.7322199940681458, 0.13991300761699677, 0.4270966351032257, 0.8927143216133118, 0.06635436415672302, 0.025243913754820824, 0.6089762449264526, 0.164319708943367, 0.6504514813423157, 0.9660682082176208, 0.013212698511779308, 0.17079849541187286, 0.2274859994649887, 0.8873509764671326, 0.11539249867200851, 0.8897441029548645, 0.7119466066360474, 0.8219953775405884, 0.4518047273159027, 0.5526160597801208, 0.5156668424606323, 0.3798842430114746, 0.7591387629508972, 0.9025423526763916, 0.2689059376716614, 0.6515424847602844, 0.2789366543292999, 0.5568122267723083, 0.6634635925292969, 0.6262637376785278, 0.2085745930671692, 0.9376164078712463, 0.22791308164596558, 0.7418540120124817, 0.4057253897190094, 0.04983304813504219, 0.387042760848999, 0.45331305265426636, 0.390306293964386, 0.9865545630455017, 0.018806803971529007, 0.5152460932731628, 0.996749997138977, 0.9486609101295471, 0.39116954803466797, 0.9426976442337036, 0.8067740797996521, 0.889554500579834, 0.8979684114456177, 0.6170464754104614, 0.4870646297931671, 0.7093315720558167, 0.16865132749080658, 0.8192521929740906, 0.5919701457023621, 0.49244385957717896, 0.3616722524166107, 0.8071326017379761, 0.5368145108222961, 0.5495433807373047, 0.7324987649917603, 0.34005603194236755, 0.5569435358047485, 0.4839858114719391, 0.623735249042511, 0.3610200881958008, 0.07797244936227798, 0.1523757129907608, 0.5165678262710571, 0.28967800736427307, 0.9974238276481628, 0.6469708681106567, 0.14755597710609436, 0.10067712515592575, 0.23362165689468384, 0.16978217661380768, 0.7000492811203003, 0.334881991147995, 0.0713207945227623, 0.9313864707946777, 0.5797341465950012, 0.6120589375495911, 0.14535905420780182, 0.10906676203012466, 0.9480545520782471, 0.6738556027412415, 0.18509434163570404, 0.2789756953716278, 0.5380411744117737, 0.8931823372840881, 0.801687479019165, 0.20614159107208252, 0.8113815784454346, 0.26392629742622375, 0.7574407458305359, 0.7305825352668762, 0.37589940428733826, 0.6839823126792908, 0.5169562101364136, 0.1914183497428894, 0.10160491615533829, 0.0792914405465126, 0.5758206844329834, 0.658331573009491, 0.26919224858283997, 0.5582151412963867, 0.4865487515926361, 0.0918538048863411, 0.6479836702346802, 0.6070619225502014], 1, map[efSearch, 40])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector052, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 10) order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector053, feature, array[0.28576499223709106, 0.08687837421894073, 0.14799416065216064, 0.058550164103507996, 0.19060933589935303, 0.08999139070510864, 0.1514379382133484, 0.08630754053592682, 0.147443950176239, 0.11865786463022232, 0.08603266626596451, 0.026738379150629044, 0.04464268684387207, 0.07328195124864578, 0.1070372611284256, 0.08322914689779282, 0.034094709903001785, 0.16017472743988037, 0.03294524550437927, 0.14785508811473846, 0.18853361904621124, 0.14193195104599, 0.1404295563697815, 0.1011366918683052, 0.11323778331279755, 0.06974314898252487, 0.019739823415875435, 0.0017852566670626402, 0.19590851664543152, 0.04378505051136017, 0.13438871502876282, 0.12536169588565826, 0.037846311926841736, 0.19261693954467773, 0.15421807765960693, 0.012271392159163952, 0.08373595774173737, 0.1423385590314865, 0.13366387784481049, 0.14510740339756012, 0.02415030263364315, 0.04452469199895859, 0.0991881713271141, 0.13216648995876312, 0.10771691799163818, 0.1334938257932663, 0.10556206107139587, 0.10942403227090836, 0.10575082153081894, 0.18991316854953766, 0.1172894611954689, 0.09650064259767532, 0.16381768882274628, 0.03527522832155228, 0.09627934545278549, 0.1411363035440445, 0.09879021346569061, 0.18661963939666748, 0.036094631999731064, 0.2045263648033142, 0.18818239867687225, 0.15758785605430603, 0.02735513634979725, 0.16133542358875275], 10) order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector054, feature, array[1.2949047088623047, 0.8476371169090271, 0.41010794043540955, 0.9785786271095276, 0.6064758896827698, 0.5890575647354126, 0.4460025131702423, 0.43684643507003784], 10) order by feature_index$distance limit 10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3631,8 +3631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3712,7 +3712,7 @@
         <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>9</v>
@@ -3744,7 +3744,7 @@
         <v>32</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>9</v>
@@ -3776,7 +3776,7 @@
         <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>9</v>
@@ -3808,7 +3808,7 @@
         <v>34</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>9</v>
@@ -3840,7 +3840,7 @@
         <v>35</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>9</v>
@@ -3872,7 +3872,7 @@
         <v>460</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>9</v>
@@ -3904,7 +3904,7 @@
         <v>39</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>9</v>
@@ -3936,7 +3936,7 @@
         <v>436</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>9</v>
@@ -3968,7 +3968,7 @@
         <v>48</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>9</v>
@@ -4000,7 +4000,7 @@
         <v>53</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>9</v>
@@ -4032,7 +4032,7 @@
         <v>58</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>9</v>
@@ -4064,7 +4064,7 @@
         <v>63</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>9</v>
@@ -4096,7 +4096,7 @@
         <v>68</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>9</v>
@@ -4128,7 +4128,7 @@
         <v>73</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>9</v>
@@ -4160,7 +4160,7 @@
         <v>105</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>129</v>
@@ -4192,7 +4192,7 @@
         <v>106</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>129</v>
@@ -4224,7 +4224,7 @@
         <v>107</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>129</v>
@@ -4256,7 +4256,7 @@
         <v>104</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>129</v>
@@ -4288,7 +4288,7 @@
         <v>103</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>129</v>
@@ -4320,7 +4320,7 @@
         <v>102</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>129</v>
@@ -4328,7 +4328,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>8</v>
@@ -4352,7 +4352,7 @@
         <v>101</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>129</v>
@@ -4384,7 +4384,7 @@
         <v>461</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>134</v>
@@ -4416,7 +4416,7 @@
         <v>133</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>129</v>
@@ -4430,7 +4430,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>13</v>
@@ -4448,7 +4448,7 @@
         <v>135</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>129</v>
@@ -4462,7 +4462,7 @@
         <v>8</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>13</v>
@@ -4480,7 +4480,7 @@
         <v>136</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>129</v>
@@ -4494,7 +4494,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>13</v>
@@ -4512,7 +4512,7 @@
         <v>130</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>134</v>
@@ -4526,7 +4526,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>13</v>
@@ -4544,7 +4544,7 @@
         <v>131</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>129</v>
@@ -4558,7 +4558,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>13</v>
@@ -4576,7 +4576,7 @@
         <v>132</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>129</v>
@@ -4608,7 +4608,7 @@
         <v>169</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>129</v>
@@ -4640,7 +4640,7 @@
         <v>168</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>129</v>
@@ -4672,7 +4672,7 @@
         <v>167</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>129</v>
@@ -4704,7 +4704,7 @@
         <v>166</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>129</v>
@@ -4736,7 +4736,7 @@
         <v>164</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>129</v>
@@ -4768,7 +4768,7 @@
         <v>165</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>129</v>
@@ -4797,10 +4797,10 @@
         <v>163</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>129</v>
@@ -4832,7 +4832,7 @@
         <v>449</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>129</v>
@@ -4864,7 +4864,7 @@
         <v>199</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>129</v>
@@ -4896,7 +4896,7 @@
         <v>200</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>129</v>
@@ -4928,7 +4928,7 @@
         <v>201</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>129</v>
@@ -4960,7 +4960,7 @@
         <v>202</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>129</v>
@@ -4992,7 +4992,7 @@
         <v>203</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>129</v>
@@ -5024,7 +5024,7 @@
         <v>204</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>129</v>
@@ -5056,7 +5056,7 @@
         <v>237</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>9</v>
@@ -5088,7 +5088,7 @@
         <v>230</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>9</v>
@@ -5120,7 +5120,7 @@
         <v>229</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>9</v>
@@ -5152,7 +5152,7 @@
         <v>231</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>9</v>
@@ -5184,7 +5184,7 @@
         <v>232</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>9</v>
@@ -5216,7 +5216,7 @@
         <v>233</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>9</v>
@@ -5248,7 +5248,7 @@
         <v>234</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>9</v>
@@ -5280,7 +5280,7 @@
         <v>235</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>9</v>
@@ -5312,7 +5312,7 @@
         <v>236</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>9</v>
@@ -5344,7 +5344,7 @@
         <v>281</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>9</v>
@@ -5376,7 +5376,7 @@
         <v>255</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>9</v>
@@ -5408,7 +5408,7 @@
         <v>282</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>9</v>
@@ -5440,7 +5440,7 @@
         <v>280</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>9</v>
@@ -5472,7 +5472,7 @@
         <v>261</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>9</v>
@@ -5504,7 +5504,7 @@
         <v>273</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>9</v>
@@ -5536,7 +5536,7 @@
         <v>278</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>9</v>
@@ -5568,7 +5568,7 @@
         <v>283</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>9</v>
@@ -5600,7 +5600,7 @@
         <v>279</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>9</v>
@@ -5632,7 +5632,7 @@
         <v>284</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>9</v>
@@ -5664,7 +5664,7 @@
         <v>291</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>9</v>
@@ -5696,7 +5696,7 @@
         <v>292</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>9</v>
@@ -5728,7 +5728,7 @@
         <v>296</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>9</v>
@@ -5760,7 +5760,7 @@
         <v>300</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>9</v>
@@ -5792,7 +5792,7 @@
         <v>304</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>9</v>
@@ -5824,7 +5824,7 @@
         <v>308</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>9</v>
@@ -5856,7 +5856,7 @@
         <v>312</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>9</v>
@@ -5888,7 +5888,7 @@
         <v>316</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>9</v>
@@ -5920,7 +5920,7 @@
         <v>321</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>9</v>
@@ -5952,7 +5952,7 @@
         <v>332</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>9</v>
@@ -5984,7 +5984,7 @@
         <v>328</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>9</v>
@@ -6016,7 +6016,7 @@
         <v>330</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>9</v>
@@ -6048,7 +6048,7 @@
         <v>337</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>9</v>
@@ -6080,7 +6080,7 @@
         <v>342</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>898</v>
+        <v>895</v>
       </c>
       <c r="K76" s="1" t="s">
         <v>9</v>
@@ -6112,7 +6112,7 @@
         <v>346</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>9</v>
@@ -6144,7 +6144,7 @@
         <v>362</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="K78" s="1" t="s">
         <v>9</v>
@@ -6173,10 +6173,10 @@
         <v>259</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>9</v>
@@ -6208,7 +6208,7 @@
         <v>365</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="K80" s="1" t="s">
         <v>9</v>
@@ -6240,7 +6240,7 @@
         <v>367</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="K81" s="1" t="s">
         <v>9</v>
@@ -6272,7 +6272,7 @@
         <v>369</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>9</v>
@@ -6304,7 +6304,7 @@
         <v>374</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>9</v>
@@ -6336,7 +6336,7 @@
         <v>375</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>9</v>
@@ -6368,7 +6368,7 @@
         <v>376</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>9</v>
@@ -6400,7 +6400,7 @@
         <v>390</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="K86" s="1" t="s">
         <v>9</v>
@@ -6432,7 +6432,7 @@
         <v>391</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="K87" s="1" t="s">
         <v>9</v>
@@ -6464,7 +6464,7 @@
         <v>392</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="K88" s="1" t="s">
         <v>9</v>
@@ -6496,7 +6496,7 @@
         <v>393</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="K89" s="1" t="s">
         <v>9</v>
@@ -6528,7 +6528,7 @@
         <v>405</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>9</v>
@@ -6560,7 +6560,7 @@
         <v>406</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="K91" s="1" t="s">
         <v>416</v>
@@ -6592,7 +6592,7 @@
         <v>415</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="K92" s="1" t="s">
         <v>9</v>
@@ -6624,7 +6624,7 @@
         <v>418</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>9</v>
@@ -6656,7 +6656,7 @@
         <v>419</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>9</v>
@@ -6688,7 +6688,7 @@
         <v>420</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>9</v>
@@ -6720,7 +6720,7 @@
         <v>421</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="K96" s="1" t="s">
         <v>416</v>
@@ -6752,7 +6752,7 @@
         <v>426</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="K97" s="1" t="s">
         <v>9</v>
@@ -6781,10 +6781,10 @@
         <v>123</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="K98" s="1" t="s">
         <v>129</v>
@@ -6792,7 +6792,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A99" s="3" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>8</v>
@@ -6816,7 +6816,7 @@
         <v>454</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="K99" s="1" t="s">
         <v>453</v>
@@ -6845,10 +6845,10 @@
         <v>123</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="K100" s="1" t="s">
         <v>129</v>
@@ -6880,7 +6880,7 @@
         <v>464</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="K101" s="1" t="s">
         <v>129</v>
@@ -6912,7 +6912,7 @@
         <v>466</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="K102" s="1" t="s">
         <v>129</v>
@@ -6944,7 +6944,7 @@
         <v>468</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>129</v>
@@ -6973,10 +6973,10 @@
         <v>123</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="K104" s="1" t="s">
         <v>129</v>
@@ -7005,10 +7005,10 @@
         <v>123</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="K105" s="1" t="s">
         <v>129</v>
@@ -7037,10 +7037,10 @@
         <v>123</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="K106" s="1" t="s">
         <v>129</v>
@@ -7066,13 +7066,13 @@
         <v>483</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>488</v>
+        <v>923</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>129</v>
@@ -7101,10 +7101,10 @@
         <v>52</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>489</v>
+        <v>924</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="K108" s="1" t="s">
         <v>129</v>
@@ -7133,10 +7133,10 @@
         <v>81</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>490</v>
+        <v>925</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="K109" s="1" t="s">
         <v>129</v>
@@ -7150,7 +7150,7 @@
         <v>8</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>13</v>
@@ -7165,10 +7165,10 @@
         <v>123</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="K110" s="1" t="s">
         <v>129</v>
@@ -7182,7 +7182,7 @@
         <v>8</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>13</v>
@@ -7191,16 +7191,16 @@
         <v>438</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="G111" s="3" t="s">
         <v>123</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="K111" s="1" t="s">
         <v>129</v>
@@ -7214,7 +7214,7 @@
         <v>8</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>13</v>
@@ -7223,16 +7223,16 @@
         <v>438</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>123</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="K112" s="1" t="s">
         <v>129</v>
@@ -7240,13 +7240,13 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A113" s="3" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>13</v>
@@ -7255,16 +7255,16 @@
         <v>438</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="K113" s="1" t="s">
         <v>129</v>
@@ -7272,13 +7272,13 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A114" s="3" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>13</v>
@@ -7287,16 +7287,16 @@
         <v>438</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="K114" s="1" t="s">
         <v>129</v>
@@ -7304,13 +7304,13 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A115" s="3" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>13</v>
@@ -7322,13 +7322,13 @@
         <v>452</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="K115" s="1" t="s">
         <v>453</v>
@@ -7336,13 +7336,13 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A116" s="3" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>13</v>
@@ -7354,27 +7354,27 @@
         <v>452</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A117" s="3" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>13</v>
@@ -7386,13 +7386,13 @@
         <v>80</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="K117" s="1" t="s">
         <v>9</v>
@@ -7400,19 +7400,19 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A118" s="3" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F118" s="3" t="s">
         <v>121</v>
@@ -7422,10 +7422,10 @@
         <v>114</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="K118" s="1" t="s">
         <v>9</v>
@@ -7433,13 +7433,13 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A119" s="3" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>13</v>
@@ -7448,16 +7448,16 @@
         <v>487</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>129</v>
@@ -7465,63 +7465,63 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A120" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="G120" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="B120" s="3" t="s">
-        <v>712</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E120" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="F120" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="G120" s="3" t="s">
+      <c r="I120" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="I120" s="1" t="s">
-        <v>531</v>
-      </c>
       <c r="J120" s="1" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A121" s="3" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E121" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="G121" s="3" t="s">
         <v>606</v>
       </c>
-      <c r="F121" s="3" t="s">
+      <c r="I121" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="G121" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="I121" s="1" t="s">
-        <v>611</v>
-      </c>
       <c r="J121" s="1" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="K121" s="1" t="s">
         <v>9</v>
@@ -7529,31 +7529,31 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A122" s="3" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="K122" s="1" t="s">
         <v>9</v>
@@ -7561,31 +7561,31 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A123" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H123" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="I123" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="I123" s="1" t="s">
-        <v>613</v>
-      </c>
       <c r="J123" s="1" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="K123" s="1" t="s">
         <v>9</v>
@@ -7593,31 +7593,31 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A124" s="3" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="K124" s="1" t="s">
         <v>9</v>
@@ -7625,31 +7625,31 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A125" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="K125" s="1" t="s">
         <v>9</v>
@@ -7657,31 +7657,31 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A126" s="3" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="K126" s="1" t="s">
         <v>9</v>
@@ -7689,31 +7689,31 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A127" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="K127" s="1" t="s">
         <v>9</v>
@@ -7721,31 +7721,31 @@
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A128" s="3" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="K128" s="1" t="s">
         <v>9</v>
@@ -7753,31 +7753,31 @@
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A129" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
       <c r="K129" s="1" t="s">
         <v>9</v>
@@ -7785,31 +7785,31 @@
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A130" s="3" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C130" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="E130" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="F130" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="H130" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="E130" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="F130" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="H130" s="1" t="s">
-        <v>610</v>
-      </c>
       <c r="I130" s="1" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
       <c r="K130" s="1" t="s">
         <v>9</v>
@@ -7817,31 +7817,31 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A131" s="3" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C131" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="E131" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="F131" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="H131" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="E131" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="F131" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="H131" s="1" t="s">
-        <v>610</v>
-      </c>
       <c r="I131" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="J131" s="1" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="K131" s="1" t="s">
         <v>9</v>
@@ -7849,31 +7849,31 @@
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A132" s="3" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C132" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="F132" s="3" t="s">
         <v>605</v>
       </c>
-      <c r="D132" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="F132" s="3" t="s">
-        <v>608</v>
-      </c>
       <c r="H132" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="J132" s="1" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="K132" s="1" t="s">
         <v>9</v>
@@ -7881,13 +7881,13 @@
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A133" s="3" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>13</v>
@@ -7896,16 +7896,16 @@
         <v>438</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="K133" s="1" t="s">
         <v>129</v>
@@ -7913,13 +7913,13 @@
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A134" s="3" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>13</v>
@@ -7928,16 +7928,16 @@
         <v>438</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="K134" s="1" t="s">
         <v>129</v>
@@ -7945,13 +7945,13 @@
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A135" s="3" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>13</v>
@@ -7960,16 +7960,16 @@
         <v>438</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="K135" s="1" t="s">
         <v>129</v>
@@ -7977,13 +7977,13 @@
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A136" s="3" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>13</v>
@@ -7992,16 +7992,16 @@
         <v>438</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="K136" s="1" t="s">
         <v>129</v>
@@ -8009,13 +8009,13 @@
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A137" s="3" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>13</v>
@@ -8024,16 +8024,16 @@
         <v>438</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="K137" s="1" t="s">
         <v>129</v>
@@ -8041,13 +8041,13 @@
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A138" s="3" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>13</v>
@@ -8056,16 +8056,16 @@
         <v>438</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="K138" s="1" t="s">
         <v>129</v>
@@ -8073,13 +8073,13 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A139" s="3" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>13</v>
@@ -8088,16 +8088,16 @@
         <v>438</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="K139" s="1" t="s">
         <v>129</v>
@@ -8105,13 +8105,13 @@
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A140" s="3" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>13</v>
@@ -8120,16 +8120,16 @@
         <v>438</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="K140" s="1" t="s">
         <v>129</v>
@@ -8137,13 +8137,13 @@
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A141" s="3" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>13</v>
@@ -8152,16 +8152,16 @@
         <v>438</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="K141" s="1" t="s">
         <v>129</v>
@@ -8169,13 +8169,13 @@
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A142" s="3" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>13</v>
@@ -8184,16 +8184,16 @@
         <v>438</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="K142" s="1" t="s">
         <v>129</v>
@@ -8201,13 +8201,13 @@
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A143" s="3" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>13</v>
@@ -8216,16 +8216,16 @@
         <v>438</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="K143" s="1" t="s">
         <v>129</v>
@@ -8233,13 +8233,13 @@
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A144" s="3" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>13</v>
@@ -8248,16 +8248,16 @@
         <v>438</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="K144" s="1" t="s">
         <v>129</v>
@@ -8265,13 +8265,13 @@
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A145" s="3" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>13</v>
@@ -8280,16 +8280,16 @@
         <v>438</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="K145" s="1" t="s">
         <v>129</v>
@@ -8297,13 +8297,13 @@
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A146" s="3" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>13</v>
@@ -8312,16 +8312,16 @@
         <v>438</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="K146" s="1" t="s">
         <v>129</v>
@@ -8329,13 +8329,13 @@
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A147" s="3" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>13</v>
@@ -8344,16 +8344,16 @@
         <v>438</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="J147" s="1" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="K147" s="1" t="s">
         <v>129</v>
@@ -8361,13 +8361,13 @@
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A148" s="3" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>13</v>
@@ -8376,16 +8376,16 @@
         <v>438</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="J148" s="1" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="K148" s="1" t="s">
         <v>129</v>
@@ -8393,13 +8393,13 @@
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A149" s="3" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>13</v>
@@ -8408,16 +8408,16 @@
         <v>438</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="K149" s="1" t="s">
         <v>129</v>
@@ -8425,13 +8425,13 @@
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A150" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>13</v>
@@ -8440,16 +8440,16 @@
         <v>438</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="J150" s="1" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="K150" s="1" t="s">
         <v>129</v>
@@ -8457,13 +8457,13 @@
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A151" s="3" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>13</v>
@@ -8472,16 +8472,16 @@
         <v>438</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="K151" s="1" t="s">
         <v>129</v>
@@ -8489,13 +8489,13 @@
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A152" s="3" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>13</v>
@@ -8504,16 +8504,16 @@
         <v>438</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="K152" s="1" t="s">
         <v>129</v>
@@ -8521,13 +8521,13 @@
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A153" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>13</v>
@@ -8536,16 +8536,16 @@
         <v>438</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="J153" s="1" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="K153" s="1" t="s">
         <v>129</v>
@@ -8553,13 +8553,13 @@
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A154" s="3" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>13</v>
@@ -8568,16 +8568,16 @@
         <v>438</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="J154" s="1" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="K154" s="1" t="s">
         <v>129</v>
@@ -8585,13 +8585,13 @@
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A155" s="3" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>13</v>
@@ -8600,16 +8600,16 @@
         <v>438</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="J155" s="1" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="K155" s="1" t="s">
         <v>129</v>
@@ -8617,13 +8617,13 @@
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A156" s="3" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>13</v>
@@ -8632,16 +8632,16 @@
         <v>438</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="J156" s="1" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="K156" s="1" t="s">
         <v>129</v>
@@ -8649,13 +8649,13 @@
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A157" s="3" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>13</v>
@@ -8664,16 +8664,16 @@
         <v>438</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="J157" s="1" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="K157" s="1" t="s">
         <v>129</v>
@@ -8681,13 +8681,13 @@
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A158" s="3" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="D158" s="3" t="s">
         <v>13</v>
@@ -8696,16 +8696,16 @@
         <v>438</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="J158" s="1" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="K158" s="1" t="s">
         <v>129</v>
@@ -8713,13 +8713,13 @@
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A159" s="3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>13</v>
@@ -8728,16 +8728,16 @@
         <v>438</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="K159" s="1" t="s">
         <v>129</v>
@@ -8745,13 +8745,13 @@
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A160" s="3" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>13</v>
@@ -8760,16 +8760,16 @@
         <v>438</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="K160" s="1" t="s">
         <v>129</v>
@@ -8777,13 +8777,13 @@
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A161" s="3" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>13</v>
@@ -8792,16 +8792,16 @@
         <v>438</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H161" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I161" s="1" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="K161" s="1" t="s">
         <v>129</v>
@@ -8809,13 +8809,13 @@
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A162" s="3" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>13</v>
@@ -8824,16 +8824,16 @@
         <v>438</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H162" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="K162" s="1" t="s">
         <v>129</v>
@@ -8841,13 +8841,13 @@
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A163" s="3" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>13</v>
@@ -8856,16 +8856,16 @@
         <v>438</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="K163" s="1" t="s">
         <v>129</v>
@@ -8873,13 +8873,13 @@
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A164" s="3" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>13</v>
@@ -8888,16 +8888,16 @@
         <v>438</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="J164" s="1" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="K164" s="1" t="s">
         <v>129</v>
@@ -8905,13 +8905,13 @@
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A165" s="3" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>13</v>
@@ -8920,16 +8920,16 @@
         <v>438</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="J165" s="1" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="K165" s="1" t="s">
         <v>129</v>
@@ -8937,13 +8937,13 @@
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A166" s="3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>13</v>
@@ -8952,16 +8952,16 @@
         <v>438</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H166" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="J166" s="1" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="K166" s="1" t="s">
         <v>129</v>
@@ -8969,13 +8969,13 @@
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A167" s="3" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>13</v>
@@ -8984,16 +8984,16 @@
         <v>438</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H167" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="J167" s="1" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="K167" s="1" t="s">
         <v>129</v>
@@ -9001,13 +9001,13 @@
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A168" s="3" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="D168" s="3" t="s">
         <v>13</v>
@@ -9016,16 +9016,16 @@
         <v>438</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H168" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="J168" s="1" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="K168" s="1" t="s">
         <v>129</v>
@@ -9033,13 +9033,13 @@
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A169" s="3" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D169" s="3" t="s">
         <v>13</v>
@@ -9048,16 +9048,16 @@
         <v>438</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="J169" s="1" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="K169" s="1" t="s">
         <v>129</v>
@@ -9065,13 +9065,13 @@
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A170" s="3" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>13</v>
@@ -9080,16 +9080,16 @@
         <v>438</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="J170" s="1" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="K170" s="1" t="s">
         <v>129</v>
@@ -9097,13 +9097,13 @@
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A171" s="3" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="D171" s="3" t="s">
         <v>13</v>
@@ -9112,16 +9112,16 @@
         <v>438</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H171" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="J171" s="1" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="K171" s="1" t="s">
         <v>129</v>
@@ -9129,13 +9129,13 @@
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A172" s="3" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>13</v>
@@ -9144,16 +9144,16 @@
         <v>438</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H172" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="J172" s="1" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="K172" s="1" t="s">
         <v>129</v>
@@ -9161,13 +9161,13 @@
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A173" s="3" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>13</v>
@@ -9176,16 +9176,16 @@
         <v>438</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H173" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="J173" s="1" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="K173" s="1" t="s">
         <v>129</v>
@@ -9193,13 +9193,13 @@
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A174" s="3" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>13</v>
@@ -9208,16 +9208,16 @@
         <v>438</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I174" s="1" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="J174" s="1" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="K174" s="1" t="s">
         <v>129</v>
@@ -9225,31 +9225,31 @@
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A175" s="3" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="D175" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="H175" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="E175" s="3" t="s">
-        <v>716</v>
-      </c>
-      <c r="F175" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="H175" s="1" t="s">
-        <v>610</v>
-      </c>
       <c r="I175" s="1" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="J175" s="1" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="K175" s="1" t="s">
         <v>416</v>
@@ -9257,13 +9257,13 @@
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A176" s="3" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>13</v>
@@ -9272,16 +9272,16 @@
         <v>438</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H176" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I176" s="1" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="J176" s="1" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="K176" s="1" t="s">
         <v>129</v>
@@ -9289,13 +9289,13 @@
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A177" s="3" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>13</v>
@@ -9304,16 +9304,16 @@
         <v>438</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H177" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="J177" s="1" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="K177" s="1" t="s">
         <v>129</v>
@@ -9321,13 +9321,13 @@
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A178" s="3" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>13</v>
@@ -9336,16 +9336,16 @@
         <v>438</v>
       </c>
       <c r="F178" s="3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H178" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="I178" s="1" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="J178" s="1" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="K178" s="1" t="s">
         <v>129</v>
@@ -9353,13 +9353,13 @@
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A179" s="1" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>13</v>
@@ -9368,16 +9368,16 @@
         <v>221</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="G179" s="1" t="s">
         <v>259</v>
       </c>
       <c r="I179" s="1" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="J179" s="1" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="K179" s="1" t="s">
         <v>9</v>
@@ -9385,13 +9385,13 @@
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A180" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>13</v>
@@ -9400,16 +9400,16 @@
         <v>221</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="G180" s="1" t="s">
         <v>259</v>
       </c>
       <c r="I180" s="1" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="J180" s="1" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="K180" s="1" t="s">
         <v>9</v>
@@ -9417,13 +9417,13 @@
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A181" s="1" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>13</v>
@@ -9432,16 +9432,16 @@
         <v>221</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="G181" s="1" t="s">
         <v>259</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="J181" s="1" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="K181" s="1" t="s">
         <v>9</v>
@@ -9449,13 +9449,13 @@
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A182" s="1" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>13</v>
@@ -9464,16 +9464,16 @@
         <v>221</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="J182" s="1" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="K182" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
add case about empty table query and auto_increment table insert
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="950">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3254,6 +3254,94 @@
   <si>
     <t>select feature_index$distance from vector($vector061, feature, array[0.6535896062850952], 10)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar_index_059</t>
+  </si>
+  <si>
+    <t>标量索引表空表查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量索引表空表查询 - flat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量索引表空表查询 - hnsw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name from $scalar003 where name='zhangsan'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/scalar/scalar_index_059.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_124.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector_index_124</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector_index_125</t>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ id,gmt,feature_id,feature_index$distance from vector($vector062, feature, array[0.4277552366256714, 0.5453793406486511, 0.2379351705312729, 0.8717846870422363, 0.17673374712467194, 0.37063586711883545, 0.7595845460891724, 0.30618390440940857], 10, map[efSearch, 40]) where gmt=2341940151 order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_125.csv</t>
+  </si>
+  <si>
+    <t>vector_index_126</t>
+  </si>
+  <si>
+    <t>vector_index_127</t>
+  </si>
+  <si>
+    <t>向量索引表主键自增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量索引表向量id字段自增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector063</t>
+  </si>
+  <si>
+    <t>vector064</t>
+  </si>
+  <si>
+    <t>vector063_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector064_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $vector063</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $vector064</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_126.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_127.csv</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -3627,10 +3715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K182"/>
+  <dimension ref="A1:K187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="C183" sqref="C183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3689,7 +3777,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>427</v>
@@ -3721,7 +3809,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>428</v>
@@ -3753,7 +3841,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>429</v>
@@ -3785,7 +3873,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>430</v>
@@ -3817,7 +3905,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>431</v>
@@ -3849,7 +3937,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>432</v>
@@ -3881,7 +3969,7 @@
         <v>36</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>433</v>
@@ -3913,7 +4001,7 @@
         <v>40</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>41</v>
@@ -3945,7 +4033,7 @@
         <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>45</v>
@@ -3977,7 +4065,7 @@
         <v>49</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>50</v>
@@ -4009,7 +4097,7 @@
         <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>55</v>
@@ -4041,7 +4129,7 @@
         <v>59</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>60</v>
@@ -4073,7 +4161,7 @@
         <v>64</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>65</v>
@@ -4105,7 +4193,7 @@
         <v>69</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>70</v>
@@ -4137,7 +4225,7 @@
         <v>88</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>94</v>
@@ -4169,7 +4257,7 @@
         <v>89</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>95</v>
@@ -4201,7 +4289,7 @@
         <v>90</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>96</v>
@@ -4233,7 +4321,7 @@
         <v>91</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>97</v>
@@ -4265,7 +4353,7 @@
         <v>92</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>98</v>
@@ -4297,7 +4385,7 @@
         <v>93</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>99</v>
@@ -4329,7 +4417,7 @@
         <v>521</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>100</v>
@@ -4361,7 +4449,7 @@
         <v>108</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>434</v>
@@ -4393,7 +4481,7 @@
         <v>109</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>435</v>
@@ -4425,7 +4513,7 @@
         <v>110</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>726</v>
@@ -4457,7 +4545,7 @@
         <v>111</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>727</v>
@@ -4489,7 +4577,7 @@
         <v>112</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>728</v>
@@ -4521,7 +4609,7 @@
         <v>113</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>729</v>
@@ -4553,7 +4641,7 @@
         <v>114</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>730</v>
@@ -4585,7 +4673,7 @@
         <v>137</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>170</v>
@@ -4617,7 +4705,7 @@
         <v>138</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>144</v>
@@ -4649,7 +4737,7 @@
         <v>139</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>145</v>
@@ -4681,7 +4769,7 @@
         <v>140</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>146</v>
@@ -4713,7 +4801,7 @@
         <v>141</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>147</v>
@@ -4745,7 +4833,7 @@
         <v>142</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>148</v>
@@ -4777,7 +4865,7 @@
         <v>143</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>149</v>
@@ -4809,7 +4897,7 @@
         <v>171</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>178</v>
@@ -4841,7 +4929,7 @@
         <v>172</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>179</v>
@@ -4873,7 +4961,7 @@
         <v>173</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>180</v>
@@ -4905,7 +4993,7 @@
         <v>174</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>181</v>
@@ -4937,7 +5025,7 @@
         <v>175</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>182</v>
@@ -4969,7 +5057,7 @@
         <v>176</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>183</v>
@@ -5001,7 +5089,7 @@
         <v>177</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>184</v>
@@ -5033,7 +5121,7 @@
         <v>205</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>210</v>
@@ -5065,7 +5153,7 @@
         <v>206</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>211</v>
@@ -5097,7 +5185,7 @@
         <v>249</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>212</v>
@@ -5129,7 +5217,7 @@
         <v>207</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>213</v>
@@ -5161,7 +5249,7 @@
         <v>208</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>214</v>
@@ -5193,7 +5281,7 @@
         <v>251</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>215</v>
@@ -5225,7 +5313,7 @@
         <v>209</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>218</v>
@@ -5257,7 +5345,7 @@
         <v>216</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>219</v>
@@ -5289,7 +5377,7 @@
         <v>217</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>220</v>
@@ -5321,7 +5409,7 @@
         <v>238</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>240</v>
@@ -5353,7 +5441,7 @@
         <v>239</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>243</v>
@@ -5385,7 +5473,7 @@
         <v>241</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>242</v>
@@ -5417,7 +5505,7 @@
         <v>253</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>254</v>
@@ -5449,7 +5537,7 @@
         <v>256</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>257</v>
@@ -5481,7 +5569,7 @@
         <v>262</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>267</v>
@@ -5513,7 +5601,7 @@
         <v>263</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>274</v>
@@ -5545,7 +5633,7 @@
         <v>264</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>275</v>
@@ -5577,7 +5665,7 @@
         <v>265</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>276</v>
@@ -5609,7 +5697,7 @@
         <v>266</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>277</v>
@@ -5641,7 +5729,7 @@
         <v>285</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>287</v>
@@ -5673,7 +5761,7 @@
         <v>286</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>288</v>
@@ -5705,7 +5793,7 @@
         <v>293</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>294</v>
@@ -5737,7 +5825,7 @@
         <v>297</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>298</v>
@@ -5769,7 +5857,7 @@
         <v>301</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>302</v>
@@ -5801,7 +5889,7 @@
         <v>305</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>307</v>
@@ -5833,7 +5921,7 @@
         <v>309</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>310</v>
@@ -5865,7 +5953,7 @@
         <v>313</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>314</v>
@@ -5897,7 +5985,7 @@
         <v>317</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>319</v>
@@ -5929,7 +6017,7 @@
         <v>318</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>322</v>
@@ -5961,7 +6049,7 @@
         <v>323</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>326</v>
@@ -5993,7 +6081,7 @@
         <v>324</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>331</v>
@@ -6025,7 +6113,7 @@
         <v>325</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>335</v>
@@ -6057,7 +6145,7 @@
         <v>338</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>339</v>
@@ -6089,7 +6177,7 @@
         <v>343</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>344</v>
@@ -6121,7 +6209,7 @@
         <v>347</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>361</v>
@@ -6153,7 +6241,7 @@
         <v>348</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>364</v>
@@ -6185,7 +6273,7 @@
         <v>349</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>363</v>
@@ -6217,7 +6305,7 @@
         <v>350</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>366</v>
@@ -6249,7 +6337,7 @@
         <v>351</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>368</v>
@@ -6281,7 +6369,7 @@
         <v>352</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>370</v>
@@ -6313,7 +6401,7 @@
         <v>353</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>371</v>
@@ -6345,7 +6433,7 @@
         <v>377</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>372</v>
@@ -6377,7 +6465,7 @@
         <v>378</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>382</v>
@@ -6409,7 +6497,7 @@
         <v>379</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>387</v>
@@ -6441,7 +6529,7 @@
         <v>380</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>388</v>
@@ -6473,7 +6561,7 @@
         <v>381</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>389</v>
@@ -6505,7 +6593,7 @@
         <v>394</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>398</v>
@@ -6537,7 +6625,7 @@
         <v>395</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>399</v>
@@ -6569,7 +6657,7 @@
         <v>396</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>400</v>
@@ -6601,7 +6689,7 @@
         <v>397</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>417</v>
@@ -6633,7 +6721,7 @@
         <v>407</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>410</v>
@@ -6665,7 +6753,7 @@
         <v>408</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>411</v>
@@ -6697,7 +6785,7 @@
         <v>409</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>423</v>
@@ -6729,7 +6817,7 @@
         <v>422</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>424</v>
@@ -6761,7 +6849,7 @@
         <v>440</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>450</v>
@@ -6793,7 +6881,7 @@
         <v>503</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>455</v>
@@ -6825,7 +6913,7 @@
         <v>441</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>456</v>
@@ -6857,7 +6945,7 @@
         <v>442</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>462</v>
@@ -6889,7 +6977,7 @@
         <v>443</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>457</v>
@@ -6921,7 +7009,7 @@
         <v>444</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>458</v>
@@ -6953,7 +7041,7 @@
         <v>445</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>469</v>
@@ -6985,7 +7073,7 @@
         <v>446</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>472</v>
@@ -7017,7 +7105,7 @@
         <v>447</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>473</v>
@@ -7049,7 +7137,7 @@
         <v>448</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>474</v>
@@ -7081,7 +7169,7 @@
         <v>477</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>475</v>
@@ -7113,7 +7201,7 @@
         <v>478</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>476</v>
@@ -7145,7 +7233,7 @@
         <v>479</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>490</v>
@@ -7177,7 +7265,7 @@
         <v>480</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>488</v>
@@ -7209,7 +7297,7 @@
         <v>481</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>489</v>
@@ -7241,7 +7329,7 @@
         <v>495</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>501</v>
@@ -7273,7 +7361,7 @@
         <v>496</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>502</v>
@@ -7305,7 +7393,7 @@
         <v>497</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>508</v>
@@ -7337,7 +7425,7 @@
         <v>507</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>509</v>
@@ -7369,7 +7457,7 @@
         <v>514</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>520</v>
@@ -7401,7 +7489,7 @@
         <v>515</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>523</v>
@@ -7434,7 +7522,7 @@
         <v>516</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>526</v>
@@ -7466,7 +7554,7 @@
         <v>522</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>527</v>
@@ -7498,7 +7586,7 @@
         <v>606</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>590</v>
@@ -7530,7 +7618,7 @@
         <v>533</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>591</v>
@@ -7562,7 +7650,7 @@
         <v>534</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>592</v>
@@ -7594,7 +7682,7 @@
         <v>535</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>593</v>
@@ -7626,7 +7714,7 @@
         <v>536</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>594</v>
@@ -7658,7 +7746,7 @@
         <v>537</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>595</v>
@@ -7690,7 +7778,7 @@
         <v>538</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>596</v>
@@ -7722,7 +7810,7 @@
         <v>539</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>597</v>
@@ -7754,7 +7842,7 @@
         <v>540</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>598</v>
@@ -7786,7 +7874,7 @@
         <v>541</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>599</v>
@@ -7818,7 +7906,7 @@
         <v>542</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>600</v>
@@ -7850,7 +7938,7 @@
         <v>543</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>601</v>
@@ -7882,7 +7970,7 @@
         <v>544</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>618</v>
@@ -7914,7 +8002,7 @@
         <v>545</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>619</v>
@@ -7946,7 +8034,7 @@
         <v>546</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>620</v>
@@ -7978,7 +8066,7 @@
         <v>547</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>621</v>
@@ -8010,7 +8098,7 @@
         <v>548</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>653</v>
@@ -8042,7 +8130,7 @@
         <v>549</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>654</v>
@@ -8074,7 +8162,7 @@
         <v>550</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>622</v>
@@ -8106,7 +8194,7 @@
         <v>551</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>623</v>
@@ -8138,7 +8226,7 @@
         <v>552</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>624</v>
@@ -8170,7 +8258,7 @@
         <v>553</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>625</v>
@@ -8202,7 +8290,7 @@
         <v>554</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>655</v>
@@ -8234,7 +8322,7 @@
         <v>555</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>656</v>
@@ -8266,7 +8354,7 @@
         <v>556</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>626</v>
@@ -8298,7 +8386,7 @@
         <v>557</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>627</v>
@@ -8330,7 +8418,7 @@
         <v>558</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>628</v>
@@ -8362,7 +8450,7 @@
         <v>559</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>629</v>
@@ -8394,7 +8482,7 @@
         <v>560</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>630</v>
@@ -8426,7 +8514,7 @@
         <v>561</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>631</v>
@@ -8458,7 +8546,7 @@
         <v>562</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>657</v>
@@ -8490,7 +8578,7 @@
         <v>563</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>658</v>
@@ -8522,7 +8610,7 @@
         <v>564</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>632</v>
@@ -8554,7 +8642,7 @@
         <v>565</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>633</v>
@@ -8586,7 +8674,7 @@
         <v>566</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>634</v>
@@ -8618,7 +8706,7 @@
         <v>567</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>635</v>
@@ -8650,7 +8738,7 @@
         <v>568</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>636</v>
@@ -8682,7 +8770,7 @@
         <v>569</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>637</v>
@@ -8714,7 +8802,7 @@
         <v>570</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>638</v>
@@ -8746,7 +8834,7 @@
         <v>571</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>639</v>
@@ -8778,7 +8866,7 @@
         <v>572</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>679</v>
@@ -8810,7 +8898,7 @@
         <v>573</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>680</v>
@@ -8842,7 +8930,7 @@
         <v>574</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>681</v>
@@ -8874,7 +8962,7 @@
         <v>575</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>682</v>
@@ -8906,7 +8994,7 @@
         <v>576</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>640</v>
@@ -8938,7 +9026,7 @@
         <v>577</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>641</v>
@@ -8970,7 +9058,7 @@
         <v>578</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>642</v>
@@ -9002,7 +9090,7 @@
         <v>579</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>643</v>
@@ -9034,7 +9122,7 @@
         <v>580</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>644</v>
@@ -9066,7 +9154,7 @@
         <v>581</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>645</v>
@@ -9098,7 +9186,7 @@
         <v>582</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>683</v>
@@ -9130,7 +9218,7 @@
         <v>583</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>684</v>
@@ -9162,7 +9250,7 @@
         <v>584</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>646</v>
@@ -9194,7 +9282,7 @@
         <v>585</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>647</v>
@@ -9226,7 +9314,7 @@
         <v>586</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>676</v>
@@ -9258,7 +9346,7 @@
         <v>587</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>677</v>
@@ -9290,7 +9378,7 @@
         <v>588</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>685</v>
@@ -9322,7 +9410,7 @@
         <v>589</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>686</v>
@@ -9354,7 +9442,7 @@
         <v>711</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>715</v>
@@ -9386,7 +9474,7 @@
         <v>712</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>716</v>
@@ -9418,7 +9506,7 @@
         <v>713</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>717</v>
@@ -9450,7 +9538,7 @@
         <v>714</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>718</v>
@@ -9474,6 +9562,157 @@
         <v>917</v>
       </c>
       <c r="K182" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A183" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="I183" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="J183" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="K183" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A184" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="F184" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="I184" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="J184" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="K184" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A185" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="I185" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="J185" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="K185" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A186" s="3" t="s">
+        <v>937</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>941</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="I186" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="J186" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="K186" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A187" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="I187" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="J187" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="K187" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix some case data and add some table join cases
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
@@ -3714,8 +3714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B182"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
add cases about query top1 vector from empty table
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="969">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3259,14 +3259,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>向量索引表空表查询 - flat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>向量索引表空表查询 - hnsw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>scalar003</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3286,58 +3278,139 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_125.csv</t>
+  </si>
+  <si>
+    <t>vector_index_126</t>
+  </si>
+  <si>
+    <t>vector_index_127</t>
+  </si>
+  <si>
+    <t>向量索引表主键自增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量索引表向量id字段自增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector063</t>
+  </si>
+  <si>
+    <t>vector064</t>
+  </si>
+  <si>
+    <t>vector063_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector064_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $vector063</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $vector064</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_126.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_127.csv</t>
+  </si>
+  <si>
+    <t>select id,gmt from $scalar019 where gmt=2147483648 or gmt=-238948525329 or gmt=2147483647</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select /*+ vector_pre */ id,gmt,feature_id,feature_index$distance from vector($vector062, feature, array[0.4277552366256714, 0.5453793406486511, 0.2379351705312729, 0.8717846870422363, 0.17673374712467194, 0.37063586711883545, 0.7595845460891724, 0.30618390440940857], 10, map[efSearch, 40]) where gmt=2341940151 order by feature_index$distance limit 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量索引表空表查询top10 - flat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量索引表空表查询top10 - hnsw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector_index_128</t>
+  </si>
+  <si>
+    <t>vector_index_129</t>
+  </si>
+  <si>
+    <t>vector_index_130</t>
+  </si>
+  <si>
+    <t>vector_index_131</t>
+  </si>
+  <si>
+    <t>向量索引表空表查询top1 - flat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量索引表空表查询top1 - hnsw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量索引表空表查询top200 - flat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向量索引表空表查询top200 - hnsw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>vector_index_125</t>
-  </si>
-  <si>
-    <t>select /*+ vector_pre */ id,gmt,feature_id,feature_index$distance from vector($vector062, feature, array[0.4277552366256714, 0.5453793406486511, 0.2379351705312729, 0.8717846870422363, 0.17673374712467194, 0.37063586711883545, 0.7595845460891724, 0.30618390440940857], 10, map[efSearch, 40]) where gmt=2341940151 order by feature_index$distance limit 10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_125.csv</t>
-  </si>
-  <si>
-    <t>vector_index_126</t>
-  </si>
-  <si>
-    <t>vector_index_127</t>
-  </si>
-  <si>
-    <t>向量索引表主键自增</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>向量索引表向量id字段自增</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vector063</t>
-  </si>
-  <si>
-    <t>vector064</t>
-  </si>
-  <si>
-    <t>vector063_value1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vector064_value1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select * from $vector063</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select * from $vector064</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_126.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_127.csv</t>
-  </si>
-  <si>
-    <t>select id,gmt from $scalar019 where gmt=2147483648 or gmt=-238948525329 or gmt=2147483647</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector003, feature, array[1.3893274068832397, 0.4223838150501251, 0.7195155024528503, 0.28465819358825684, 0.9267012476921082, 0.4375186264514923, 0.7362583875656128, 0.41960853338241577, 0.7168405055999756, 0.5768887996673584, 0.4182721674442291, 0.129996195435524, 0.21704305708408356, 0.35628095269203186, 0.5203919410705566, 0.4046420454978943, 0.1657610833644867, 0.7787348031997681, 0.16017264127731323, 0.7188393473625183, 0.916609525680542, 0.6900423765182495, 0.6827380657196045, 0.49170464277267456, 0.5505375266075134, 0.33907604217529297, 0.09597073495388031, 0.008679530583322048, 0.9524646997451782, 0.2128734141588211, 0.6533687710762024, 0.6094813346862793, 0.18400055170059204, 0.9364618062973022, 0.7497748732566833, 0.05966084823012352, 0.40710607171058655, 0.6920192241668701, 0.649844765663147, 0.705480694770813, 0.11741353571414948, 0.2164693921804428, 0.48223137855529785, 0.6425648331642151, 0.5236963033676147, 0.6490180492401123, 0.5132198333740234, 0.5319958925247192, 0.5141375660896301, 0.9233165979385376, 0.5702359080314636, 0.46916520595550537, 0.7964460849761963, 0.17150050401687622, 0.4680892825126648, 0.6861740946769714, 0.4802965819835663, 0.9073042273521423, 0.17548426985740662, 0.9943628311157227, 0.9149019718170166, 0.7661579847335815, 0.13299474120140076, 0.7843778133392334], 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_128.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_129.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_130.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_131.csv</t>
+  </si>
+  <si>
+    <t>vector032</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector032, feature, array[0.07635648548603058, 0.15315186977386475, 0.07998066395521164, 0.030244847759604454, 0.03660374879837036, 0.07020597904920578, 0.07753317058086395, 0.06954050064086914, 0.015842216089367867, 0.09847000241279602, 0.14333799481391907, 0.08972030133008957, 0.14679503440856934, 0.053985677659511566, 0.002433809684589505, 0.0023769710678607225, 0.1445109248161316, 0.14641882479190826, 0.10128048807382584, 0.1252911388874054, 0.10591669380664825, 0.0680871307849884, 0.1314261555671692, 0.10261483490467072, 0.03380761668086052, 0.026138586923480034, 0.14016865193843842, 0.13751810789108276, 0.0629085972905159, 0.1505446434020996, 0.06228705868124962, 0.1229817271232605, 0.1103021427989006, 0.03345080465078354, 0.11508025974035263, 0.1158876121044159, 0.009820408187806606, 0.0917428508400917, 0.04003928229212761, 0.03954596072435379, 0.04483354836702347, 0.06192560866475105, 0.11376481503248215, 0.08256463706493378, 0.053461335599422455, 0.02103513292968273, 0.00565503491088748, 0.10908288508653641, 0.04112488031387329, 0.022799896076321602, 0.11819855123758316, 0.11487363278865814, 0.12618036568164825, 0.13946618139743805, 0.11951262503862381, 0.05174343287944794, 0.0636037141084671, 0.08812220394611359, 0.04158082604408264, 0.09588614106178284, 0.027776390314102173, 0.06508250534534454, 0.005918444134294987, 0.021368220448493958, 0.004391259513795376, 0.15330512821674347, 0.02889648638665676, 0.1508062481880188, 0.150262713432312, 0.10929194837808609, 0.11180958151817322, 0.012830037623643875, 0.11655847728252411, 0.13481442630290985, 0.010158943012356758, 0.11980089545249939, 0.15085941553115845, 0.09553232789039612, 0.0875730887055397, 0.05343187600374222, 0.06500837206840515, 0.111661896109581, 0.003067383775487542, 0.0360986590385437, 0.12402313947677612, 0.12736830115318298, 0.0426727756857872, 0.061350468546152115, 0.03204718604683876, 0.03390524536371231, 0.06006992980837822, 0.060586053878068924, 0.053700245916843414, 0.11538811773061752, 0.06678721308708191, 0.01872638240456581, 0.008201477117836475, 0.005164149217307568, 0.12405505776405334, 0.05883660539984703, 0.06236365810036659, 0.09206810593605042, 0.09996166080236435, 0.12544621527194977, 0.015171129256486893, 0.07829906791448593, 0.0564851388335228, 0.021202033385634422, 0.027655914425849915, 0.09527980536222458, 0.06116790696978569, 0.059106335043907166, 0.005855979863554239, 0.0013711017090827227, 0.15338891744613647, 0.1270914375782013, 0.0006535736611112952, 0.09347102791070938, 0.05424905940890312, 0.07519031316041946, 0.06069091707468033, 0.07380328327417374, 0.012128415517508984, 0.14862750470638275, 0.1329932063817978, 0.13582192361354828, 0.07143492996692657, 0.023565614596009254], 1, map[efSearch, 40])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select feature_id,feature_index$distance from vector($vector021, feature, array[0.9239124059677124, 0.4843500256538391, 0.8469328284263611, 0.3649107813835144, 0.12166310846805573, 0.4924268424510956, 0.22334574162960052, 0.3681839108467102, 0.629433274269104, 0.7594435214996338, 0.4972413182258606, 0.8343933820724487, 0.024635562673211098, 0.03285043686628342, 0.03953443095088005, 0.7866605520248413, 0.5277446508407593, 0.5880250930786133, 0.5665906071662903, 0.8202308416366577, 0.8357234001159668, 0.9898386001586914, 0.12343018501996994, 0.14783860743045807, 0.3024723529815674, 0.12918686866760254, 0.5089493989944458, 0.1878420114517212, 0.43235525488853455, 0.7073430418968201, 0.3231576979160309, 0.4336588978767395, 0.009747916832566261, 0.6327077746391296, 0.1939246952533722, 0.4884851574897766, 0.18558892607688904, 0.22880852222442627, 0.6001395583152771, 0.21099650859832764, 0.8470631241798401, 0.578583300113678, 0.9217984080314636, 0.9745617508888245, 0.39740318059921265, 0.38332560658454895, 0.16164763271808624, 0.5284485220909119, 0.5045936107635498, 0.9989950060844421, 0.9766484498977661, 0.7316726446151733, 0.27011770009994507, 0.4881993234157562, 0.40483176708221436, 0.44103214144706726, 0.05593995004892349, 0.3786134719848633, 0.9554991126060486, 0.7375790476799011, 0.5030877590179443, 0.8656612038612366, 0.762405276298523, 0.0036561775486916304, 0.9369459748268127, 0.43684494495391846, 0.060403723269701004, 0.4711165428161621, 0.25497934222221375, 0.868898868560791, 0.6802678108215332, 0.7941082119941711, 0.452462762594223, 0.3453672230243683, 0.20798680186271667, 0.7321949601173401, 0.8815983533859253, 0.968714714050293, 0.6105460524559021, 0.2149900197982788, 0.580249547958374, 0.5977041721343994, 0.967699408531189, 0.8144114017486572, 0.05922708287835121, 0.20375977456569672, 0.03194655105471611, 0.15820658206939697, 0.31330418586730957, 0.21847577393054962, 0.3981025516986847, 0.5010366439819336, 0.26931583881378174, 0.4735915958881378, 0.5724477767944336, 0.33687132596969604, 0.04377315193414688, 0.36767345666885376, 0.3042020797729492, 0.4231858253479004, 0.1292417049407959, 0.42681407928466797, 0.5958619117736816, 0.6741296648979187, 0.3152969777584076, 0.029671069234609604, 0.11972007155418396, 0.04692043736577034, 0.5610555410385132, 0.8710808753967285, 0.47341039776802063, 0.5212073922157288, 0.39335399866104126, 0.8455687165260315, 0.11431540548801422, 0.6011691093444824, 0.12908993661403656, 0.12356450408697128, 0.4945315718650818, 0.15044346451759338, 0.122397780418396, 0.5098639726638794, 0.6716281771659851, 0.5017514228820801, 0.0836697667837143, 0.47981905937194824, 0.9932494163513184, 0.32886266708374023, 0.25824710726737976, 0.8751729130744934, 0.009066426195204258, 0.9942600727081299, 0.4162600636482239, 0.22180116176605225, 0.0817895233631134, 0.09719996899366379, 0.41029420495033264, 0.7469924092292786, 0.5244626402854919, 0.5819556713104248, 0.6311984658241272, 0.9177411198616028, 0.2920183837413788, 0.4236264228820801, 0.20676787197589874, 0.2873593866825104, 0.8544968366622925, 0.7005806565284729, 0.8832012414932251, 0.2170013040304184, 0.9764801263809204, 0.11152216792106628, 0.7473317384719849, 0.5044044852256775, 0.5740600228309631, 0.7580671310424805, 0.2689347565174103, 0.6154418587684631, 0.6277509927749634, 0.8064326643943787, 0.9296490550041199, 0.9630101323127747, 0.6272547245025635, 0.6518057584762573, 0.013520768843591213, 0.047964777797460556, 0.6291251182556152, 0.7565540075302124, 0.46829867362976074, 0.9790219068527222, 0.47444063425064087, 0.09158720821142197, 0.8554185032844543, 0.48793578147888184, 0.49829328060150146, 0.2399786114692688, 0.9039421081542969, 0.42510557174682617, 0.871625542640686, 0.5266937017440796, 0.9372545480728149, 0.4056784212589264, 0.20858386158943176, 0.6417825222015381, 0.6760283708572388, 0.7661968469619751, 0.932290256023407, 0.7984945178031921, 0.4229621887207031, 0.2860976755619049, 0.766200065612793, 0.030616188421845436, 0.27581310272216797, 0.8004037737846375, 0.38476547598838806, 0.3662087321281433, 0.1665489226579666, 0.8844420909881592, 0.21739384531974792, 0.4800202548503876, 0.5613713264465332, 0.9035276770591736, 0.9988727569580078, 0.4723106324672699, 0.2091149240732193, 0.28218305110931396, 0.39127182960510254, 0.108350969851017, 0.8098669648170471, 0.438691645860672, 0.9227825403213501, 0.2665433883666992, 0.47852227091789246, 0.7385755777359009, 0.7825472950935364, 0.24820971488952637, 0.8984768986701965, 0.8860059976577759, 0.7511387467384338, 0.6482298970222473, 0.41447964310646057, 0.26772522926330566, 0.21873252093791962, 0.9747976660728455, 0.2802465260028839, 0.4381829798221588, 0.8083264231681824, 0.27536892890930176, 0.7050621509552002, 0.13408638536930084, 0.17319123446941376, 0.9446348547935486, 0.7178460359573364, 0.8887788653373718, 0.8309583067893982, 0.39261874556541443, 0.922595739364624, 0.9685015678405762, 0.07747195661067963, 0.8439147472381592, 0.6838429570198059, 0.8240256905555725, 0.8779502511024475, 0.2603004276752472, 0.32454612851142883, 0.19199953973293304, 0.3028557002544403, 0.0005280417390167713, 0.7640310525894165, 0.3347814977169037, 0.551266074180603, 0.6681751608848572, 0.8570151925086975, 0.12389184534549713, 0.06018004193902016, 0.6769797801971436, 0.9307451844215393, 0.5886029601097107, 0.3267931640148163, 0.735440194606781, 0.2571922242641449, 0.23621384799480438, 0.3440623879432678, 0.7495661377906799, 0.7535163760185242, 0.817280650138855, 0.5316166281700134, 0.3759754002094269, 0.5891391038894653, 0.7784118056297302, 0.7402175664901733, 0.9727427363395691, 0.37990519404411316, 0.22303621470928192, 0.9542710185050964, 0.6015431880950928, 0.06037019193172455, 0.3491678237915039, 0.6032770276069641, 0.8124412298202515, 0.04897555708885193, 0.2266976684331894, 0.6840716004371643, 0.15190571546554565, 0.10871954262256622, 0.7997511625289917, 0.7069057822227478, 0.8865413665771484, 0.5871621370315552, 0.5804872512817383, 0.4280828833580017, 0.8842650651931763, 0.7895702123641968, 0.8246167302131653, 0.14378789067268372, 0.6453055143356323, 0.5512241125106812, 0.2704751491546631, 0.3207348585128784, 0.5607932806015015, 0.5885487794876099, 0.14936292171478271, 0.9230074286460876, 0.8225005269050598, 0.0403902642428875, 0.689630925655365, 0.9553170204162598, 0.45728158950805664, 0.6490166187286377, 0.4340020418167114, 0.13416516780853271, 0.8385115265846252, 0.6513805985450745, 0.8857315182685852, 0.43779656291007996, 0.6068954467773438, 0.6362829804420471, 0.7668876051902771, 0.16584451496601105, 0.3420253098011017, 0.41403064131736755, 0.747107744216919, 0.5989379286766052, 0.2100415825843811, 0.5971049070358276, 0.45167139172554016, 0.6367031335830688, 0.12591707706451416, 0.6078851222991943, 0.2811676859855652, 0.6002131104469299, 0.8782482743263245, 0.023016931489109993, 0.29077428579330444, 0.40800291299819946, 0.437203973531723, 0.7611927390098572, 0.5102689862251282, 0.8853865265846252, 0.6378153562545776, 0.8267585635185242, 0.12517410516738892, 0.1118943989276886, 0.5993191599845886, 0.3651404082775116, 0.9492583870887756, 0.5929558277130127, 0.8422895669937134, 0.03034876473248005, 0.06894740462303162, 0.8353880643844604, 0.7847146391868591, 0.9795354008674622, 0.018211867660284042, 0.9162828326225281, 0.2558964192867279, 0.6304334402084351, 0.8971966505050659, 0.01650533638894558, 0.9147691130638123, 0.8372026681900024, 0.07811513543128967, 0.18765734136104584, 0.8493755459785461, 0.7690473198890686, 0.6815782785415649, 0.038570236414670944, 0.6997503638267517, 0.15465512871742249, 0.10862003266811371, 0.3841232657432556, 0.36616501212120056, 0.5340136289596558, 0.9628089666366577, 0.09302754700183868, 0.4262010455131531, 0.3221454322338104, 0.26824313402175903, 0.9275528788566589, 0.17862263321876526, 0.986758828163147, 0.6954213380813599, 0.9778974652290344, 0.9411178231239319, 0.6336787343025208, 0.02665160596370697, 0.022254791110754013, 0.16388261318206787, 0.5364391803741455, 0.7553685307502747, 0.8228940963745117, 0.7755976915359497, 0.6978816390037537, 0.6342451572418213, 0.19358883798122406, 0.010019454173743725, 0.30235618352890015, 0.37945419549942017, 0.7997922897338867, 0.2015790492296219, 0.08810613304376602, 0.545327365398407, 0.8676781058311462, 0.11978304386138916, 0.3356499969959259, 0.22294066846370697, 0.34720921516418457, 0.46339941024780273, 0.6694201827049255, 0.4898035228252411, 0.7547814846038818, 0.529211163520813, 0.5337550044059753, 0.9234888553619385, 0.6419934630393982, 0.05446995049715042, 0.8422916531562805, 0.7053759694099426, 0.9406060576438904, 0.32067304849624634, 0.0726916715502739, 0.6268541216850281, 0.9703216552734375, 0.6178982853889465, 0.32758021354675293, 0.2391270250082016, 0.4773683249950409, 0.4751492440700531, 0.728840172290802, 0.5304896831512451, 0.9039581418037415, 0.9366835951805115, 0.9652710556983948, 0.07714381814002991, 0.7655075788497925, 0.09492266178131104, 0.7500200271606445, 0.6590962409973145, 0.19639156758785248, 0.12858077883720398, 0.1315186470746994, 0.8341460824012756, 0.5491176247596741, 0.2220095992088318, 0.8350792527198792, 0.2740192413330078, 0.8359421491622925, 0.005694213323295116, 0.1044410765171051, 0.8541707992553711, 0.33968979120254517, 0.14025482535362244, 0.8172051310539246, 0.39639943838119507, 0.37975409626960754, 0.2562301754951477, 0.5173991322517395, 0.20979797840118408, 0.24902884662151337, 0.40574580430984497, 0.9546396732330322, 0.6625224947929382, 0.3844829797744751, 0.2947736382484436, 0.39435213804244995, 0.6935738325119019, 0.27325505018234253, 0.4490673542022705, 0.4290046989917755, 0.6258346438407898, 0.7245139479637146, 0.5210762619972229, 0.3103833496570587, 0.984284520149231, 0.7271832227706909, 0.054386455565690994, 0.9886484742164612, 0.5912991762161255, 0.8480425477027893, 0.2404581904411316, 0.761442244052887, 0.23551371693611145, 0.7017846703529358, 0.38449934124946594, 0.8790562748908997, 0.06591027230024338, 0.46864843368530273, 0.13216416537761688, 0.692452073097229, 0.04988833889365196, 0.5691991448402405, 0.42036789655685425, 0.8218620419502258, 0.748799204826355, 0.5949804186820984, 0.760817289352417, 0.8749229311943054, 0.8209290504455566, 0.21112455427646637, 0.5346830487251282, 0.6935092210769653, 0.5279433727264404, 0.5479289889335632, 0.4417686462402344, 0.38963329792022705, 0.6661739945411682, 0.9739553332328796, 0.04269544035196304, 0.8578197360038757, 0.8881459832191467, 0.053067587316036224, 0.7503750920295715, 0.026237372308969498, 0.8519961833953857, 0.555051863193512, 0.747510552406311, 0.03300659358501434, 0.48286378383636475, 0.8855323195457458, 0.9632793068885803, 0.9104558825492859, 0.48694849014282227, 0.399563729763031, 0.6363621950149536, 0.11851905286312103, 0.017224308103322983, 0.8240532875061035, 0.7225683331489563, 0.14129522442817688, 0.03214777261018753, 0.22644132375717163, 0.12453615665435791, 0.14669975638389587, 0.20129647850990295, 0.37571659684181213, 0.28608691692352295, 0.5647987723350525, 0.5401462912559509, 0.8368682861328125, 0.4405445456504822, 0.6099599599838257, 0.31859633326530457, 0.4392208158969879, 0.8659310936927795, 0.5211570262908936, 0.971695601940155, 0.4802115559577942, 0.9608403444290161, 0.11427588760852814, 0.5906932950019836, 0.5829917192459106, 0.7723814845085144, 0.2851836085319519, 0.7487574815750122, 0.40168407559394836, 0.1096145436167717, 0.38012459874153137, 0.9993427395820618, 0.6248184442520142, 0.5964413285255432, 0.8974211812019348, 0.021383538842201233, 0.7045061588287354, 0.10735698789358139, 0.034189656376838684, 0.4253982603549957, 0.5137093663215637, 0.3070155680179596, 0.26458463072776794, 0.500767171382904, 0.35795703530311584, 0.43192875385284424, 0.0011799664935097098, 0.8871830105781555, 0.3413742184638977, 0.23464272916316986, 0.2985425889492035, 0.43168431520462036, 0.8043161630630493, 0.8787585496902466, 0.3137490153312683, 0.8155429363250732, 0.5388948321342468, 0.8555070757865906, 0.2806842625141144, 0.8434351086616516, 0.01054427120834589, 0.5914859175682068, 0.7061315178871155, 0.17015855014324188, 0.7105374932289124, 0.756917417049408, 0.9772598147392273, 0.4745588004589081, 0.9372658729553223, 0.9028635025024414, 0.0553511306643486, 0.059380579739809036, 0.03670920804142952, 0.5552451014518738, 0.0863645151257515, 0.7970898151397705, 0.709926962852478, 0.7950313687324524, 0.31617963314056396, 0.7190312743186951, 0.30269700288772583, 0.5575765371322632, 0.6522773504257202, 0.8686654567718506, 0.06443669646978378, 0.23735427856445312, 0.7017615437507629, 0.11044484376907349, 0.6743099689483643, 0.7618545293807983, 0.9179471135139465, 0.9271143078804016, 0.3715285658836365, 0.3158683180809021, 0.5581682324409485, 0.425870805978775, 0.9559334516525269, 0.32485705614089966, 0.22024419903755188, 0.738275408744812, 0.35260477662086487, 0.03648458421230316, 0.5063309073448181, 0.5714408159255981, 0.42382925748825073, 0.1744859516620636, 0.012257871218025684, 0.6470044255256653, 0.6596391201019287, 0.4375765323638916, 0.8324525356292725, 0.148403599858284, 0.32366088032722473, 0.28859803080558777, 0.036741212010383606, 0.6912445425987244, 0.5623661875724792, 0.24150314927101135, 0.6668141484260559, 0.457194447517395, 0.37331423163414, 0.7039971947669983, 0.5442853569984436, 0.16904520988464355, 0.5473294854164124, 0.42225542664527893, 0.1632952094078064, 0.13430103659629822, 0.7011837959289551, 0.35530123114585876, 0.22957314550876617, 0.30041030049324036, 0.8040412068367004, 0.7258527278900146, 0.7313927412033081, 0.1588331162929535, 0.135481595993042, 0.8655409812927246, 0.05593014135956764, 0.13720092177391052, 0.4199233651161194, 0.5524675250053406, 0.6945871710777283, 0.5422185063362122, 0.9759254455566406, 0.5732696056365967, 0.36203110218048096, 0.341176837682724, 0.6339867115020752, 0.7928552627563477, 0.3829185366630554, 0.5065315365791321, 0.30392715334892273, 0.448226660490036, 0.5905334949493408, 0.743084728717804, 0.8534137010574341, 0.14105093479156494, 0.36877334117889404, 0.18374945223331451, 0.20742535591125488, 0.05424303933978081, 0.9064294099807739, 0.7810009717941284, 0.3920835852622986, 0.6733852028846741, 0.7985923886299133, 0.56886887550354, 0.8983238339424133, 0.06639385968446732, 0.7757044434547424, 0.4609031677246094, 0.2285572588443756, 0.9890051484107971, 0.31385186314582825, 0.23206709325313568, 0.7099732160568237, 0.8873257040977478, 0.20876754820346832, 0.4126618802547455, 0.364944189786911, 0.9184130430221558, 0.21294458210468292, 0.1087569072842598, 0.12313185632228851, 0.6087223887443542, 0.3020622134208679, 0.6708245277404785, 0.00968034565448761, 0.8843799233436584, 0.8471185564994812, 0.009053618647158146, 0.5472723841667175, 0.950732409954071, 0.2927361726760864, 0.22065046429634094, 0.17401093244552612, 0.6433684229850769, 0.3871839642524719, 0.9706835746765137, 0.26617759466171265, 0.5593381524085999, 0.3533758223056793, 0.6942663192749023, 0.963712751865387, 0.8432105183601379, 0.23894959688186646, 0.17237906157970428, 0.41669386625289917, 0.9002247452735901, 0.43070852756500244, 0.3645652234554291, 0.37970998883247375, 0.09329424798488617, 0.2716970145702362, 0.5067605376243591, 0.5323185324668884, 0.0941026508808136, 0.6156055927276611, 0.2279163897037506, 0.46269893646240234, 0.46550822257995605, 0.9443367123603821, 0.2790738344192505, 0.6077525019645691, 0.633952796459198, 0.5716169476509094, 0.1307380050420761, 0.8753399848937988, 0.40633732080459595, 0.06160659343004227, 0.021534273400902748, 0.9461350440979004, 0.7492088079452515, 0.11246911436319351, 0.4941251277923584, 0.9788018465042114, 0.27250680327415466, 0.3345406651496887, 0.19131797552108765, 0.14440374076366425, 0.2348489910364151, 0.31302410364151, 0.9079352617263794, 0.4020977020263672, 0.6660201549530029, 0.6413438320159912, 0.20272615551948547, 0.6990474462509155, 0.9029505848884583, 0.05377570912241936, 0.5987172722816467, 0.8348270654678345, 0.22269052267074585, 0.7413466572761536, 0.3676571547985077, 0.2186078280210495, 0.49187159538269043, 0.5381358861923218, 0.06617742031812668, 0.3657665550708771, 0.5592037439346313, 0.8133091330528259, 0.5245937705039978, 0.9237461090087891, 0.18355919420719147, 0.9537744522094727, 0.9397586584091187, 0.9005112648010254, 0.3715962767601013, 0.038503702729940414, 0.08550792187452316, 0.0829492136836052, 0.23305834829807281, 0.7761086225509644, 0.15855655074119568, 0.9690130352973938, 0.5020524263381958, 0.3725299835205078, 0.8542638421058655, 0.019558819010853767, 0.15747599303722382, 0.8419409990310669, 0.6331632137298584, 0.7364429235458374, 0.6126334071159363, 0.8729809522628784, 0.8290192484855652, 0.05802781879901886, 0.5132171511650085, 0.8647670745849609, 0.3186877965927124, 0.2963152229785919, 0.09293709695339203, 0.2839053273200989, 0.41266000270843506, 0.5926613211631775, 0.748725950717926, 0.6268962621688843, 0.8735111951828003, 0.6876919865608215, 0.5448590517044067, 0.9995477199554443, 0.5211653709411621, 0.9796311259269714, 0.10060117393732071, 0.7818820476531982, 0.12879221141338348, 0.4428848922252655, 0.6108387112617493, 0.009913390502333641, 0.6105896830558777, 0.7839468121528625, 0.16570189595222473, 0.9330465793609619, 0.20278356969356537, 0.05767875909805298, 0.6311724185943604, 0.9409513473510742, 0.8009441494941711, 0.28160372376441956, 0.8198218941688538, 0.4478168785572052, 0.6826450824737549, 0.22241489589214325, 0.8591458201408386, 0.9293228387832642, 0.40108972787857056, 0.8202097415924072, 0.8996019959449768, 0.14287227392196655, 0.38321569561958313, 0.27360138297080994, 0.8402204513549805, 0.9253615736961365, 0.6166125535964966, 0.4354666769504547, 0.796143651008606, 0.4072890877723694, 0.2206253558397293, 0.3822609484195709, 0.7882177233695984, 0.3175186514854431, 0.4173959493637085, 0.22347642481327057, 0.9197232723236084, 0.35839006304740906, 0.9049082398414612, 0.9309132099151611, 0.045181240886449814, 0.09384647011756897, 0.05347450450062752, 0.19579052925109863, 0.7908905148506165, 0.20613841712474823, 0.14672277867794037, 0.7862143516540527, 0.9796620607376099, 0.3739449083805084, 0.17460660636425018, 0.28613653779029846, 0.5251057147979736, 0.3894467353820801, 0.28357192873954773, 0.36872538924217224, 0.7701210379600525, 0.6139308214187622, 0.8185737133026123, 0.5817059874534607, 0.6525381803512573, 0.24731449782848358, 0.20497308671474457, 0.47354310750961304, 0.5834407806396484, 0.17583248019218445, 0.7986509799957275, 0.5127730369567871, 0.8926236033439636, 0.31678536534309387, 0.789405882358551, 0.19309519231319427, 0.46440237760543823, 0.9070742726325989, 0.5251756906509399, 0.5822200179100037, 0.9608134031295776, 0.8702162504196167, 0.6776354908943176, 0.5664172172546387, 0.3142203390598297, 0.4488910138607025, 0.12798769772052765, 0.011343738064169884, 0.02167833410203457, 0.6363694667816162, 0.6574286222457886, 0.6331721544265747, 0.1860949695110321, 0.034065719693899155, 0.18757067620754242, 0.9766800403594971, 0.9342480301856995, 0.7307646870613098, 0.2236720770597458, 0.44722676277160645, 0.7844812870025635, 0.6553750038146973, 0.02890823595225811, 0.5502535700798035, 0.49368926882743835, 0.666702389717102, 0.1015218049287796, 0.3175419270992279, 0.647401750087738, 0.1520446091890335, 0.41871029138565063, 0.22599367797374725, 0.208740696310997, 0.2565656006336212, 0.8748878836631775, 0.6164125800132751, 0.026515310630202293, 0.35274752974510193, 0.38343608379364014, 0.5636261701583862, 0.26844000816345215, 0.8335092663764954, 0.7071099877357483, 0.9418774247169495, 0.07427223771810532, 0.9127421379089355, 0.9862300157546997, 0.7681083679199219, 0.01751137711107731, 0.34160518646240234, 0.705668568611145, 0.7790502905845642, 0.4326382577419281, 0.7700020670890808, 0.7228742837905884, 0.020561855286359787, 0.7313647270202637, 0.05350518971681595, 0.9003791809082031, 0.6505491137504578, 0.4541366398334503, 0.8059714436531067, 0.5164853930473328, 0.18433037400245667, 0.5248328447341919, 0.7833437323570251, 0.8773091435432434, 0.04765724018216133, 0.07328523695468903, 0.0812780112028122, 0.5028670430183411, 0.16256916522979736, 0.5242683291435242, 0.9959482550621033, 0.6369618773460388, 0.11678291857242584, 0.66120845079422, 0.6951324343681335, 0.7239258289337158, 0.6037524938583374, 0.12224157899618149, 0.08236031979322433, 0.6220316886901855, 0.3785780966281891, 0.017284560948610306, 0.324351966381073, 0.8785102367401123, 0.10727077722549438, 0.8287323713302612, 0.6088231801986694, 0.5255677103996277, 0.5691452622413635, 0.43685823678970337, 0.1062149852514267, 0.7524598240852356, 0.6816270351409912, 0.8537653088569641, 0.5840227603912354, 0.8530658483505249, 0.5536980032920837, 0.12879525125026703, 0.835331380367279, 0.8097959160804749, 0.24524140357971191, 0.19832557439804077, 0.6036972403526306, 0.19901812076568604, 0.5515961647033691, 0.15916021168231964, 0.4663938581943512, 0.33608734607696533, 0.804487407207489, 0.8883902430534363], 200)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector042</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select feature_id,feature_index$distance from vector($vector042, feature, array[0.9239124059677124, 0.4843500256538391, 0.8469328284263611, 0.3649107813835144, 0.12166310846805573, 0.4924268424510956, 0.22334574162960052, 0.3681839108467102, 0.629433274269104, 0.7594435214996338, 0.4972413182258606, 0.8343933820724487, 0.024635562673211098, 0.03285043686628342, 0.03953443095088005, 0.7866605520248413, 0.5277446508407593, 0.5880250930786133, 0.5665906071662903, 0.8202308416366577, 0.8357234001159668, 0.9898386001586914, 0.12343018501996994, 0.14783860743045807, 0.3024723529815674, 0.12918686866760254, 0.5089493989944458, 0.1878420114517212, 0.43235525488853455, 0.7073430418968201, 0.3231576979160309, 0.4336588978767395, 0.009747916832566261, 0.6327077746391296, 0.1939246952533722, 0.4884851574897766, 0.18558892607688904, 0.22880852222442627, 0.6001395583152771, 0.21099650859832764, 0.8470631241798401, 0.578583300113678, 0.9217984080314636, 0.9745617508888245, 0.39740318059921265, 0.38332560658454895, 0.16164763271808624, 0.5284485220909119, 0.5045936107635498, 0.9989950060844421, 0.9766484498977661, 0.7316726446151733, 0.27011770009994507, 0.4881993234157562, 0.40483176708221436, 0.44103214144706726, 0.05593995004892349, 0.3786134719848633, 0.9554991126060486, 0.7375790476799011, 0.5030877590179443, 0.8656612038612366, 0.762405276298523, 0.0036561775486916304, 0.9369459748268127, 0.43684494495391846, 0.060403723269701004, 0.4711165428161621, 0.25497934222221375, 0.868898868560791, 0.6802678108215332, 0.7941082119941711, 0.452462762594223, 0.3453672230243683, 0.20798680186271667, 0.7321949601173401, 0.8815983533859253, 0.968714714050293, 0.6105460524559021, 0.2149900197982788, 0.580249547958374, 0.5977041721343994, 0.967699408531189, 0.8144114017486572, 0.05922708287835121, 0.20375977456569672, 0.03194655105471611, 0.15820658206939697, 0.31330418586730957, 0.21847577393054962, 0.3981025516986847, 0.5010366439819336, 0.26931583881378174, 0.4735915958881378, 0.5724477767944336, 0.33687132596969604, 0.04377315193414688, 0.36767345666885376, 0.3042020797729492, 0.4231858253479004, 0.1292417049407959, 0.42681407928466797, 0.5958619117736816, 0.6741296648979187, 0.3152969777584076, 0.029671069234609604, 0.11972007155418396, 0.04692043736577034, 0.5610555410385132, 0.8710808753967285, 0.47341039776802063, 0.5212073922157288, 0.39335399866104126, 0.8455687165260315, 0.11431540548801422, 0.6011691093444824, 0.12908993661403656, 0.12356450408697128, 0.4945315718650818, 0.15044346451759338, 0.122397780418396, 0.5098639726638794, 0.6716281771659851, 0.5017514228820801, 0.0836697667837143, 0.47981905937194824, 0.9932494163513184, 0.32886266708374023, 0.25824710726737976, 0.8751729130744934, 0.009066426195204258, 0.9942600727081299, 0.4162600636482239, 0.22180116176605225, 0.0817895233631134, 0.09719996899366379, 0.41029420495033264, 0.7469924092292786, 0.5244626402854919, 0.5819556713104248, 0.6311984658241272, 0.9177411198616028, 0.2920183837413788, 0.4236264228820801, 0.20676787197589874, 0.2873593866825104, 0.8544968366622925, 0.7005806565284729, 0.8832012414932251, 0.2170013040304184, 0.9764801263809204, 0.11152216792106628, 0.7473317384719849, 0.5044044852256775, 0.5740600228309631, 0.7580671310424805, 0.2689347565174103, 0.6154418587684631, 0.6277509927749634, 0.8064326643943787, 0.9296490550041199, 0.9630101323127747, 0.6272547245025635, 0.6518057584762573, 0.013520768843591213, 0.047964777797460556, 0.6291251182556152, 0.7565540075302124, 0.46829867362976074, 0.9790219068527222, 0.47444063425064087, 0.09158720821142197, 0.8554185032844543, 0.48793578147888184, 0.49829328060150146, 0.2399786114692688, 0.9039421081542969, 0.42510557174682617, 0.871625542640686, 0.5266937017440796, 0.9372545480728149, 0.4056784212589264, 0.20858386158943176, 0.6417825222015381, 0.6760283708572388, 0.7661968469619751, 0.932290256023407, 0.7984945178031921, 0.4229621887207031, 0.2860976755619049, 0.766200065612793, 0.030616188421845436, 0.27581310272216797, 0.8004037737846375, 0.38476547598838806, 0.3662087321281433, 0.1665489226579666, 0.8844420909881592, 0.21739384531974792, 0.4800202548503876, 0.5613713264465332, 0.9035276770591736, 0.9988727569580078, 0.4723106324672699, 0.2091149240732193, 0.28218305110931396, 0.39127182960510254, 0.108350969851017, 0.8098669648170471, 0.438691645860672, 0.9227825403213501, 0.2665433883666992, 0.47852227091789246, 0.7385755777359009, 0.7825472950935364, 0.24820971488952637, 0.8984768986701965, 0.8860059976577759, 0.7511387467384338, 0.6482298970222473, 0.41447964310646057, 0.26772522926330566, 0.21873252093791962, 0.9747976660728455, 0.2802465260028839, 0.4381829798221588, 0.8083264231681824, 0.27536892890930176, 0.7050621509552002, 0.13408638536930084, 0.17319123446941376, 0.9446348547935486, 0.7178460359573364, 0.8887788653373718, 0.8309583067893982, 0.39261874556541443, 0.922595739364624, 0.9685015678405762, 0.07747195661067963, 0.8439147472381592, 0.6838429570198059, 0.8240256905555725, 0.8779502511024475, 0.2603004276752472, 0.32454612851142883, 0.19199953973293304, 0.3028557002544403, 0.0005280417390167713, 0.7640310525894165, 0.3347814977169037, 0.551266074180603, 0.6681751608848572, 0.8570151925086975, 0.12389184534549713, 0.06018004193902016, 0.6769797801971436, 0.9307451844215393, 0.5886029601097107, 0.3267931640148163, 0.735440194606781, 0.2571922242641449, 0.23621384799480438, 0.3440623879432678, 0.7495661377906799, 0.7535163760185242, 0.817280650138855, 0.5316166281700134, 0.3759754002094269, 0.5891391038894653, 0.7784118056297302, 0.7402175664901733, 0.9727427363395691, 0.37990519404411316, 0.22303621470928192, 0.9542710185050964, 0.6015431880950928, 0.06037019193172455, 0.3491678237915039, 0.6032770276069641, 0.8124412298202515, 0.04897555708885193, 0.2266976684331894, 0.6840716004371643, 0.15190571546554565, 0.10871954262256622, 0.7997511625289917, 0.7069057822227478, 0.8865413665771484, 0.5871621370315552, 0.5804872512817383, 0.4280828833580017, 0.8842650651931763, 0.7895702123641968, 0.8246167302131653, 0.14378789067268372, 0.6453055143356323, 0.5512241125106812, 0.2704751491546631, 0.3207348585128784, 0.5607932806015015, 0.5885487794876099, 0.14936292171478271, 0.9230074286460876, 0.8225005269050598, 0.0403902642428875, 0.689630925655365, 0.9553170204162598, 0.45728158950805664, 0.6490166187286377, 0.4340020418167114, 0.13416516780853271, 0.8385115265846252, 0.6513805985450745, 0.8857315182685852, 0.43779656291007996, 0.6068954467773438, 0.6362829804420471, 0.7668876051902771, 0.16584451496601105, 0.3420253098011017, 0.41403064131736755, 0.747107744216919, 0.5989379286766052, 0.2100415825843811, 0.5971049070358276, 0.45167139172554016, 0.6367031335830688, 0.12591707706451416, 0.6078851222991943, 0.2811676859855652, 0.6002131104469299, 0.8782482743263245, 0.023016931489109993, 0.29077428579330444, 0.40800291299819946, 0.437203973531723, 0.7611927390098572, 0.5102689862251282, 0.8853865265846252, 0.6378153562545776, 0.8267585635185242, 0.12517410516738892, 0.1118943989276886, 0.5993191599845886, 0.3651404082775116, 0.9492583870887756, 0.5929558277130127, 0.8422895669937134, 0.03034876473248005, 0.06894740462303162, 0.8353880643844604, 0.7847146391868591, 0.9795354008674622, 0.018211867660284042, 0.9162828326225281, 0.2558964192867279, 0.6304334402084351, 0.8971966505050659, 0.01650533638894558, 0.9147691130638123, 0.8372026681900024, 0.07811513543128967, 0.18765734136104584, 0.8493755459785461, 0.7690473198890686, 0.6815782785415649, 0.038570236414670944, 0.6997503638267517, 0.15465512871742249, 0.10862003266811371, 0.3841232657432556, 0.36616501212120056, 0.5340136289596558, 0.9628089666366577, 0.09302754700183868, 0.4262010455131531, 0.3221454322338104, 0.26824313402175903, 0.9275528788566589, 0.17862263321876526, 0.986758828163147, 0.6954213380813599, 0.9778974652290344, 0.9411178231239319, 0.6336787343025208, 0.02665160596370697, 0.022254791110754013, 0.16388261318206787, 0.5364391803741455, 0.7553685307502747, 0.8228940963745117, 0.7755976915359497, 0.6978816390037537, 0.6342451572418213, 0.19358883798122406, 0.010019454173743725, 0.30235618352890015, 0.37945419549942017, 0.7997922897338867, 0.2015790492296219, 0.08810613304376602, 0.545327365398407, 0.8676781058311462, 0.11978304386138916, 0.3356499969959259, 0.22294066846370697, 0.34720921516418457, 0.46339941024780273, 0.6694201827049255, 0.4898035228252411, 0.7547814846038818, 0.529211163520813, 0.5337550044059753, 0.9234888553619385, 0.6419934630393982, 0.05446995049715042, 0.8422916531562805, 0.7053759694099426, 0.9406060576438904, 0.32067304849624634, 0.0726916715502739, 0.6268541216850281, 0.9703216552734375, 0.6178982853889465, 0.32758021354675293, 0.2391270250082016, 0.4773683249950409, 0.4751492440700531, 0.728840172290802, 0.5304896831512451, 0.9039581418037415, 0.9366835951805115, 0.9652710556983948, 0.07714381814002991, 0.7655075788497925, 0.09492266178131104, 0.7500200271606445, 0.6590962409973145, 0.19639156758785248, 0.12858077883720398, 0.1315186470746994, 0.8341460824012756, 0.5491176247596741, 0.2220095992088318, 0.8350792527198792, 0.2740192413330078, 0.8359421491622925, 0.005694213323295116, 0.1044410765171051, 0.8541707992553711, 0.33968979120254517, 0.14025482535362244, 0.8172051310539246, 0.39639943838119507, 0.37975409626960754, 0.2562301754951477, 0.5173991322517395, 0.20979797840118408, 0.24902884662151337, 0.40574580430984497, 0.9546396732330322, 0.6625224947929382, 0.3844829797744751, 0.2947736382484436, 0.39435213804244995, 0.6935738325119019, 0.27325505018234253, 0.4490673542022705, 0.4290046989917755, 0.6258346438407898, 0.7245139479637146, 0.5210762619972229, 0.3103833496570587, 0.984284520149231, 0.7271832227706909, 0.054386455565690994, 0.9886484742164612, 0.5912991762161255, 0.8480425477027893, 0.2404581904411316, 0.761442244052887, 0.23551371693611145, 0.7017846703529358, 0.38449934124946594, 0.8790562748908997, 0.06591027230024338, 0.46864843368530273, 0.13216416537761688, 0.692452073097229, 0.04988833889365196, 0.5691991448402405, 0.42036789655685425, 0.8218620419502258, 0.748799204826355, 0.5949804186820984, 0.760817289352417, 0.8749229311943054, 0.8209290504455566, 0.21112455427646637, 0.5346830487251282, 0.6935092210769653, 0.5279433727264404, 0.5479289889335632, 0.4417686462402344, 0.38963329792022705, 0.6661739945411682, 0.9739553332328796, 0.04269544035196304, 0.8578197360038757, 0.8881459832191467, 0.053067587316036224, 0.7503750920295715, 0.026237372308969498, 0.8519961833953857, 0.555051863193512, 0.747510552406311, 0.03300659358501434, 0.48286378383636475, 0.8855323195457458, 0.9632793068885803, 0.9104558825492859, 0.48694849014282227, 0.399563729763031, 0.6363621950149536, 0.11851905286312103, 0.017224308103322983, 0.8240532875061035, 0.7225683331489563, 0.14129522442817688, 0.03214777261018753, 0.22644132375717163, 0.12453615665435791, 0.14669975638389587, 0.20129647850990295, 0.37571659684181213, 0.28608691692352295, 0.5647987723350525, 0.5401462912559509, 0.8368682861328125, 0.4405445456504822, 0.6099599599838257, 0.31859633326530457, 0.4392208158969879, 0.8659310936927795, 0.5211570262908936, 0.971695601940155, 0.4802115559577942, 0.9608403444290161, 0.11427588760852814, 0.5906932950019836, 0.5829917192459106, 0.7723814845085144, 0.2851836085319519, 0.7487574815750122, 0.40168407559394836, 0.1096145436167717, 0.38012459874153137, 0.9993427395820618, 0.6248184442520142, 0.5964413285255432, 0.8974211812019348, 0.021383538842201233, 0.7045061588287354, 0.10735698789358139, 0.034189656376838684, 0.4253982603549957, 0.5137093663215637, 0.3070155680179596, 0.26458463072776794, 0.500767171382904, 0.35795703530311584, 0.43192875385284424, 0.0011799664935097098, 0.8871830105781555, 0.3413742184638977, 0.23464272916316986, 0.2985425889492035, 0.43168431520462036, 0.8043161630630493, 0.8787585496902466, 0.3137490153312683, 0.8155429363250732, 0.5388948321342468, 0.8555070757865906, 0.2806842625141144, 0.8434351086616516, 0.01054427120834589, 0.5914859175682068, 0.7061315178871155, 0.17015855014324188, 0.7105374932289124, 0.756917417049408, 0.9772598147392273, 0.4745588004589081, 0.9372658729553223, 0.9028635025024414, 0.0553511306643486, 0.059380579739809036, 0.03670920804142952, 0.5552451014518738, 0.0863645151257515, 0.7970898151397705, 0.709926962852478, 0.7950313687324524, 0.31617963314056396, 0.7190312743186951, 0.30269700288772583, 0.5575765371322632, 0.6522773504257202, 0.8686654567718506, 0.06443669646978378, 0.23735427856445312, 0.7017615437507629, 0.11044484376907349, 0.6743099689483643, 0.7618545293807983, 0.9179471135139465, 0.9271143078804016, 0.3715285658836365, 0.3158683180809021, 0.5581682324409485, 0.425870805978775, 0.9559334516525269, 0.32485705614089966, 0.22024419903755188, 0.738275408744812, 0.35260477662086487, 0.03648458421230316, 0.5063309073448181, 0.5714408159255981, 0.42382925748825073, 0.1744859516620636, 0.012257871218025684, 0.6470044255256653, 0.6596391201019287, 0.4375765323638916, 0.8324525356292725, 0.148403599858284, 0.32366088032722473, 0.28859803080558777, 0.036741212010383606, 0.6912445425987244, 0.5623661875724792, 0.24150314927101135, 0.6668141484260559, 0.457194447517395, 0.37331423163414, 0.7039971947669983, 0.5442853569984436, 0.16904520988464355, 0.5473294854164124, 0.42225542664527893, 0.1632952094078064, 0.13430103659629822, 0.7011837959289551, 0.35530123114585876, 0.22957314550876617, 0.30041030049324036, 0.8040412068367004, 0.7258527278900146, 0.7313927412033081, 0.1588331162929535, 0.135481595993042, 0.8655409812927246, 0.05593014135956764, 0.13720092177391052, 0.4199233651161194, 0.5524675250053406, 0.6945871710777283, 0.5422185063362122, 0.9759254455566406, 0.5732696056365967, 0.36203110218048096, 0.341176837682724, 0.6339867115020752, 0.7928552627563477, 0.3829185366630554, 0.5065315365791321, 0.30392715334892273, 0.448226660490036, 0.5905334949493408, 0.743084728717804, 0.8534137010574341, 0.14105093479156494, 0.36877334117889404, 0.18374945223331451, 0.20742535591125488, 0.05424303933978081, 0.9064294099807739, 0.7810009717941284, 0.3920835852622986, 0.6733852028846741, 0.7985923886299133, 0.56886887550354, 0.8983238339424133, 0.06639385968446732, 0.7757044434547424, 0.4609031677246094, 0.2285572588443756, 0.9890051484107971, 0.31385186314582825, 0.23206709325313568, 0.7099732160568237, 0.8873257040977478, 0.20876754820346832, 0.4126618802547455, 0.364944189786911, 0.9184130430221558, 0.21294458210468292, 0.1087569072842598, 0.12313185632228851, 0.6087223887443542, 0.3020622134208679, 0.6708245277404785, 0.00968034565448761, 0.8843799233436584, 0.8471185564994812, 0.009053618647158146, 0.5472723841667175, 0.950732409954071, 0.2927361726760864, 0.22065046429634094, 0.17401093244552612, 0.6433684229850769, 0.3871839642524719, 0.9706835746765137, 0.26617759466171265, 0.5593381524085999, 0.3533758223056793, 0.6942663192749023, 0.963712751865387, 0.8432105183601379, 0.23894959688186646, 0.17237906157970428, 0.41669386625289917, 0.9002247452735901, 0.43070852756500244, 0.3645652234554291, 0.37970998883247375, 0.09329424798488617, 0.2716970145702362, 0.5067605376243591, 0.5323185324668884, 0.0941026508808136, 0.6156055927276611, 0.2279163897037506, 0.46269893646240234, 0.46550822257995605, 0.9443367123603821, 0.2790738344192505, 0.6077525019645691, 0.633952796459198, 0.5716169476509094, 0.1307380050420761, 0.8753399848937988, 0.40633732080459595, 0.06160659343004227, 0.021534273400902748, 0.9461350440979004, 0.7492088079452515, 0.11246911436319351, 0.4941251277923584, 0.9788018465042114, 0.27250680327415466, 0.3345406651496887, 0.19131797552108765, 0.14440374076366425, 0.2348489910364151, 0.31302410364151, 0.9079352617263794, 0.4020977020263672, 0.6660201549530029, 0.6413438320159912, 0.20272615551948547, 0.6990474462509155, 0.9029505848884583, 0.05377570912241936, 0.5987172722816467, 0.8348270654678345, 0.22269052267074585, 0.7413466572761536, 0.3676571547985077, 0.2186078280210495, 0.49187159538269043, 0.5381358861923218, 0.06617742031812668, 0.3657665550708771, 0.5592037439346313, 0.8133091330528259, 0.5245937705039978, 0.9237461090087891, 0.18355919420719147, 0.9537744522094727, 0.9397586584091187, 0.9005112648010254, 0.3715962767601013, 0.038503702729940414, 0.08550792187452316, 0.0829492136836052, 0.23305834829807281, 0.7761086225509644, 0.15855655074119568, 0.9690130352973938, 0.5020524263381958, 0.3725299835205078, 0.8542638421058655, 0.019558819010853767, 0.15747599303722382, 0.8419409990310669, 0.6331632137298584, 0.7364429235458374, 0.6126334071159363, 0.8729809522628784, 0.8290192484855652, 0.05802781879901886, 0.5132171511650085, 0.8647670745849609, 0.3186877965927124, 0.2963152229785919, 0.09293709695339203, 0.2839053273200989, 0.41266000270843506, 0.5926613211631775, 0.748725950717926, 0.6268962621688843, 0.8735111951828003, 0.6876919865608215, 0.5448590517044067, 0.9995477199554443, 0.5211653709411621, 0.9796311259269714, 0.10060117393732071, 0.7818820476531982, 0.12879221141338348, 0.4428848922252655, 0.6108387112617493, 0.009913390502333641, 0.6105896830558777, 0.7839468121528625, 0.16570189595222473, 0.9330465793609619, 0.20278356969356537, 0.05767875909805298, 0.6311724185943604, 0.9409513473510742, 0.8009441494941711, 0.28160372376441956, 0.8198218941688538, 0.4478168785572052, 0.6826450824737549, 0.22241489589214325, 0.8591458201408386, 0.9293228387832642, 0.40108972787857056, 0.8202097415924072, 0.8996019959449768, 0.14287227392196655, 0.38321569561958313, 0.27360138297080994, 0.8402204513549805, 0.9253615736961365, 0.6166125535964966, 0.4354666769504547, 0.796143651008606, 0.4072890877723694, 0.2206253558397293, 0.3822609484195709, 0.7882177233695984, 0.3175186514854431, 0.4173959493637085, 0.22347642481327057, 0.9197232723236084, 0.35839006304740906, 0.9049082398414612, 0.9309132099151611, 0.045181240886449814, 0.09384647011756897, 0.05347450450062752, 0.19579052925109863, 0.7908905148506165, 0.20613841712474823, 0.14672277867794037, 0.7862143516540527, 0.9796620607376099, 0.3739449083805084, 0.17460660636425018, 0.28613653779029846, 0.5251057147979736, 0.3894467353820801, 0.28357192873954773, 0.36872538924217224, 0.7701210379600525, 0.6139308214187622, 0.8185737133026123, 0.5817059874534607, 0.6525381803512573, 0.24731449782848358, 0.20497308671474457, 0.47354310750961304, 0.5834407806396484, 0.17583248019218445, 0.7986509799957275, 0.5127730369567871, 0.8926236033439636, 0.31678536534309387, 0.789405882358551, 0.19309519231319427, 0.46440237760543823, 0.9070742726325989, 0.5251756906509399, 0.5822200179100037, 0.9608134031295776, 0.8702162504196167, 0.6776354908943176, 0.5664172172546387, 0.3142203390598297, 0.4488910138607025, 0.12798769772052765, 0.011343738064169884, 0.02167833410203457, 0.6363694667816162, 0.6574286222457886, 0.6331721544265747, 0.1860949695110321, 0.034065719693899155, 0.18757067620754242, 0.9766800403594971, 0.9342480301856995, 0.7307646870613098, 0.2236720770597458, 0.44722676277160645, 0.7844812870025635, 0.6553750038146973, 0.02890823595225811, 0.5502535700798035, 0.49368926882743835, 0.666702389717102, 0.1015218049287796, 0.3175419270992279, 0.647401750087738, 0.1520446091890335, 0.41871029138565063, 0.22599367797374725, 0.208740696310997, 0.2565656006336212, 0.8748878836631775, 0.6164125800132751, 0.026515310630202293, 0.35274752974510193, 0.38343608379364014, 0.5636261701583862, 0.26844000816345215, 0.8335092663764954, 0.7071099877357483, 0.9418774247169495, 0.07427223771810532, 0.9127421379089355, 0.9862300157546997, 0.7681083679199219, 0.01751137711107731, 0.34160518646240234, 0.705668568611145, 0.7790502905845642, 0.4326382577419281, 0.7700020670890808, 0.7228742837905884, 0.020561855286359787, 0.7313647270202637, 0.05350518971681595, 0.9003791809082031, 0.6505491137504578, 0.4541366398334503, 0.8059714436531067, 0.5164853930473328, 0.18433037400245667, 0.5248328447341919, 0.7833437323570251, 0.8773091435432434, 0.04765724018216133, 0.07328523695468903, 0.0812780112028122, 0.5028670430183411, 0.16256916522979736, 0.5242683291435242, 0.9959482550621033, 0.6369618773460388, 0.11678291857242584, 0.66120845079422, 0.6951324343681335, 0.7239258289337158, 0.6037524938583374, 0.12224157899618149, 0.08236031979322433, 0.6220316886901855, 0.3785780966281891, 0.017284560948610306, 0.324351966381073, 0.8785102367401123, 0.10727077722549438, 0.8287323713302612, 0.6088231801986694, 0.5255677103996277, 0.5691452622413635, 0.43685823678970337, 0.1062149852514267, 0.7524598240852356, 0.6816270351409912, 0.8537653088569641, 0.5840227603912354, 0.8530658483505249, 0.5536980032920837, 0.12879525125026703, 0.835331380367279, 0.8097959160804749, 0.24524140357971191, 0.19832557439804077, 0.6036972403526306, 0.19901812076568604, 0.5515961647033691, 0.15916021168231964, 0.4663938581943512, 0.33608734607696533, 0.804487407207489, 0.8883902430534363], 200, map[efSearch, 40])</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3712,10 +3785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K187"/>
+  <dimension ref="A1:K191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D61" workbookViewId="0">
-      <selection activeCell="J83" sqref="J83"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5840,7 +5913,7 @@
         <v>259</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>881</v>
@@ -9579,13 +9652,13 @@
         <v>221</v>
       </c>
       <c r="F183" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="I183" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="J183" s="1" t="s">
         <v>928</v>
-      </c>
-      <c r="I183" s="1" t="s">
-        <v>929</v>
-      </c>
-      <c r="J183" s="1" t="s">
-        <v>930</v>
       </c>
       <c r="K183" s="1" t="s">
         <v>415</v>
@@ -9593,13 +9666,13 @@
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A184" s="3" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>926</v>
+        <v>946</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>13</v>
@@ -9614,7 +9687,7 @@
         <v>919</v>
       </c>
       <c r="J184" s="1" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="K184" s="1" t="s">
         <v>415</v>
@@ -9622,13 +9695,13 @@
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A185" s="3" t="s">
-        <v>933</v>
+        <v>956</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>927</v>
+        <v>947</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>13</v>
@@ -9640,10 +9713,10 @@
         <v>603</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>934</v>
+        <v>945</v>
       </c>
       <c r="J185" s="1" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="K185" s="1" t="s">
         <v>415</v>
@@ -9651,13 +9724,13 @@
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A186" s="3" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>602</v>
@@ -9666,16 +9739,16 @@
         <v>601</v>
       </c>
       <c r="F186" s="3" t="s">
+        <v>936</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="I186" s="1" t="s">
         <v>940</v>
       </c>
-      <c r="G186" s="1" t="s">
+      <c r="J186" s="1" t="s">
         <v>942</v>
-      </c>
-      <c r="I186" s="1" t="s">
-        <v>944</v>
-      </c>
-      <c r="J186" s="1" t="s">
-        <v>946</v>
       </c>
       <c r="K186" s="1" t="s">
         <v>9</v>
@@ -9683,13 +9756,13 @@
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A187" s="3" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>602</v>
@@ -9698,19 +9771,135 @@
         <v>601</v>
       </c>
       <c r="F187" s="3" t="s">
+        <v>937</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="I187" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="G187" s="1" t="s">
+      <c r="J187" s="1" t="s">
         <v>943</v>
-      </c>
-      <c r="I187" s="1" t="s">
-        <v>945</v>
-      </c>
-      <c r="J187" s="1" t="s">
-        <v>947</v>
       </c>
       <c r="K187" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A188" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="F188" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="I188" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="J188" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="K188" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A189" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="F189" s="3" t="s">
+        <v>963</v>
+      </c>
+      <c r="I189" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="J189" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="K189" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A190" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="F190" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="I190" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="J190" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="K190" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A191" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="F191" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="I191" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="J191" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="K191" s="1" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add high-ascii character insert and query, change index table delete logic
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$2</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2030" uniqueCount="972">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3411,6 +3411,16 @@
   </si>
   <si>
     <t>select feature_id,feature_index$distance from vector($vector042, feature, array[0.9239124059677124, 0.4843500256538391, 0.8469328284263611, 0.3649107813835144, 0.12166310846805573, 0.4924268424510956, 0.22334574162960052, 0.3681839108467102, 0.629433274269104, 0.7594435214996338, 0.4972413182258606, 0.8343933820724487, 0.024635562673211098, 0.03285043686628342, 0.03953443095088005, 0.7866605520248413, 0.5277446508407593, 0.5880250930786133, 0.5665906071662903, 0.8202308416366577, 0.8357234001159668, 0.9898386001586914, 0.12343018501996994, 0.14783860743045807, 0.3024723529815674, 0.12918686866760254, 0.5089493989944458, 0.1878420114517212, 0.43235525488853455, 0.7073430418968201, 0.3231576979160309, 0.4336588978767395, 0.009747916832566261, 0.6327077746391296, 0.1939246952533722, 0.4884851574897766, 0.18558892607688904, 0.22880852222442627, 0.6001395583152771, 0.21099650859832764, 0.8470631241798401, 0.578583300113678, 0.9217984080314636, 0.9745617508888245, 0.39740318059921265, 0.38332560658454895, 0.16164763271808624, 0.5284485220909119, 0.5045936107635498, 0.9989950060844421, 0.9766484498977661, 0.7316726446151733, 0.27011770009994507, 0.4881993234157562, 0.40483176708221436, 0.44103214144706726, 0.05593995004892349, 0.3786134719848633, 0.9554991126060486, 0.7375790476799011, 0.5030877590179443, 0.8656612038612366, 0.762405276298523, 0.0036561775486916304, 0.9369459748268127, 0.43684494495391846, 0.060403723269701004, 0.4711165428161621, 0.25497934222221375, 0.868898868560791, 0.6802678108215332, 0.7941082119941711, 0.452462762594223, 0.3453672230243683, 0.20798680186271667, 0.7321949601173401, 0.8815983533859253, 0.968714714050293, 0.6105460524559021, 0.2149900197982788, 0.580249547958374, 0.5977041721343994, 0.967699408531189, 0.8144114017486572, 0.05922708287835121, 0.20375977456569672, 0.03194655105471611, 0.15820658206939697, 0.31330418586730957, 0.21847577393054962, 0.3981025516986847, 0.5010366439819336, 0.26931583881378174, 0.4735915958881378, 0.5724477767944336, 0.33687132596969604, 0.04377315193414688, 0.36767345666885376, 0.3042020797729492, 0.4231858253479004, 0.1292417049407959, 0.42681407928466797, 0.5958619117736816, 0.6741296648979187, 0.3152969777584076, 0.029671069234609604, 0.11972007155418396, 0.04692043736577034, 0.5610555410385132, 0.8710808753967285, 0.47341039776802063, 0.5212073922157288, 0.39335399866104126, 0.8455687165260315, 0.11431540548801422, 0.6011691093444824, 0.12908993661403656, 0.12356450408697128, 0.4945315718650818, 0.15044346451759338, 0.122397780418396, 0.5098639726638794, 0.6716281771659851, 0.5017514228820801, 0.0836697667837143, 0.47981905937194824, 0.9932494163513184, 0.32886266708374023, 0.25824710726737976, 0.8751729130744934, 0.009066426195204258, 0.9942600727081299, 0.4162600636482239, 0.22180116176605225, 0.0817895233631134, 0.09719996899366379, 0.41029420495033264, 0.7469924092292786, 0.5244626402854919, 0.5819556713104248, 0.6311984658241272, 0.9177411198616028, 0.2920183837413788, 0.4236264228820801, 0.20676787197589874, 0.2873593866825104, 0.8544968366622925, 0.7005806565284729, 0.8832012414932251, 0.2170013040304184, 0.9764801263809204, 0.11152216792106628, 0.7473317384719849, 0.5044044852256775, 0.5740600228309631, 0.7580671310424805, 0.2689347565174103, 0.6154418587684631, 0.6277509927749634, 0.8064326643943787, 0.9296490550041199, 0.9630101323127747, 0.6272547245025635, 0.6518057584762573, 0.013520768843591213, 0.047964777797460556, 0.6291251182556152, 0.7565540075302124, 0.46829867362976074, 0.9790219068527222, 0.47444063425064087, 0.09158720821142197, 0.8554185032844543, 0.48793578147888184, 0.49829328060150146, 0.2399786114692688, 0.9039421081542969, 0.42510557174682617, 0.871625542640686, 0.5266937017440796, 0.9372545480728149, 0.4056784212589264, 0.20858386158943176, 0.6417825222015381, 0.6760283708572388, 0.7661968469619751, 0.932290256023407, 0.7984945178031921, 0.4229621887207031, 0.2860976755619049, 0.766200065612793, 0.030616188421845436, 0.27581310272216797, 0.8004037737846375, 0.38476547598838806, 0.3662087321281433, 0.1665489226579666, 0.8844420909881592, 0.21739384531974792, 0.4800202548503876, 0.5613713264465332, 0.9035276770591736, 0.9988727569580078, 0.4723106324672699, 0.2091149240732193, 0.28218305110931396, 0.39127182960510254, 0.108350969851017, 0.8098669648170471, 0.438691645860672, 0.9227825403213501, 0.2665433883666992, 0.47852227091789246, 0.7385755777359009, 0.7825472950935364, 0.24820971488952637, 0.8984768986701965, 0.8860059976577759, 0.7511387467384338, 0.6482298970222473, 0.41447964310646057, 0.26772522926330566, 0.21873252093791962, 0.9747976660728455, 0.2802465260028839, 0.4381829798221588, 0.8083264231681824, 0.27536892890930176, 0.7050621509552002, 0.13408638536930084, 0.17319123446941376, 0.9446348547935486, 0.7178460359573364, 0.8887788653373718, 0.8309583067893982, 0.39261874556541443, 0.922595739364624, 0.9685015678405762, 0.07747195661067963, 0.8439147472381592, 0.6838429570198059, 0.8240256905555725, 0.8779502511024475, 0.2603004276752472, 0.32454612851142883, 0.19199953973293304, 0.3028557002544403, 0.0005280417390167713, 0.7640310525894165, 0.3347814977169037, 0.551266074180603, 0.6681751608848572, 0.8570151925086975, 0.12389184534549713, 0.06018004193902016, 0.6769797801971436, 0.9307451844215393, 0.5886029601097107, 0.3267931640148163, 0.735440194606781, 0.2571922242641449, 0.23621384799480438, 0.3440623879432678, 0.7495661377906799, 0.7535163760185242, 0.817280650138855, 0.5316166281700134, 0.3759754002094269, 0.5891391038894653, 0.7784118056297302, 0.7402175664901733, 0.9727427363395691, 0.37990519404411316, 0.22303621470928192, 0.9542710185050964, 0.6015431880950928, 0.06037019193172455, 0.3491678237915039, 0.6032770276069641, 0.8124412298202515, 0.04897555708885193, 0.2266976684331894, 0.6840716004371643, 0.15190571546554565, 0.10871954262256622, 0.7997511625289917, 0.7069057822227478, 0.8865413665771484, 0.5871621370315552, 0.5804872512817383, 0.4280828833580017, 0.8842650651931763, 0.7895702123641968, 0.8246167302131653, 0.14378789067268372, 0.6453055143356323, 0.5512241125106812, 0.2704751491546631, 0.3207348585128784, 0.5607932806015015, 0.5885487794876099, 0.14936292171478271, 0.9230074286460876, 0.8225005269050598, 0.0403902642428875, 0.689630925655365, 0.9553170204162598, 0.45728158950805664, 0.6490166187286377, 0.4340020418167114, 0.13416516780853271, 0.8385115265846252, 0.6513805985450745, 0.8857315182685852, 0.43779656291007996, 0.6068954467773438, 0.6362829804420471, 0.7668876051902771, 0.16584451496601105, 0.3420253098011017, 0.41403064131736755, 0.747107744216919, 0.5989379286766052, 0.2100415825843811, 0.5971049070358276, 0.45167139172554016, 0.6367031335830688, 0.12591707706451416, 0.6078851222991943, 0.2811676859855652, 0.6002131104469299, 0.8782482743263245, 0.023016931489109993, 0.29077428579330444, 0.40800291299819946, 0.437203973531723, 0.7611927390098572, 0.5102689862251282, 0.8853865265846252, 0.6378153562545776, 0.8267585635185242, 0.12517410516738892, 0.1118943989276886, 0.5993191599845886, 0.3651404082775116, 0.9492583870887756, 0.5929558277130127, 0.8422895669937134, 0.03034876473248005, 0.06894740462303162, 0.8353880643844604, 0.7847146391868591, 0.9795354008674622, 0.018211867660284042, 0.9162828326225281, 0.2558964192867279, 0.6304334402084351, 0.8971966505050659, 0.01650533638894558, 0.9147691130638123, 0.8372026681900024, 0.07811513543128967, 0.18765734136104584, 0.8493755459785461, 0.7690473198890686, 0.6815782785415649, 0.038570236414670944, 0.6997503638267517, 0.15465512871742249, 0.10862003266811371, 0.3841232657432556, 0.36616501212120056, 0.5340136289596558, 0.9628089666366577, 0.09302754700183868, 0.4262010455131531, 0.3221454322338104, 0.26824313402175903, 0.9275528788566589, 0.17862263321876526, 0.986758828163147, 0.6954213380813599, 0.9778974652290344, 0.9411178231239319, 0.6336787343025208, 0.02665160596370697, 0.022254791110754013, 0.16388261318206787, 0.5364391803741455, 0.7553685307502747, 0.8228940963745117, 0.7755976915359497, 0.6978816390037537, 0.6342451572418213, 0.19358883798122406, 0.010019454173743725, 0.30235618352890015, 0.37945419549942017, 0.7997922897338867, 0.2015790492296219, 0.08810613304376602, 0.545327365398407, 0.8676781058311462, 0.11978304386138916, 0.3356499969959259, 0.22294066846370697, 0.34720921516418457, 0.46339941024780273, 0.6694201827049255, 0.4898035228252411, 0.7547814846038818, 0.529211163520813, 0.5337550044059753, 0.9234888553619385, 0.6419934630393982, 0.05446995049715042, 0.8422916531562805, 0.7053759694099426, 0.9406060576438904, 0.32067304849624634, 0.0726916715502739, 0.6268541216850281, 0.9703216552734375, 0.6178982853889465, 0.32758021354675293, 0.2391270250082016, 0.4773683249950409, 0.4751492440700531, 0.728840172290802, 0.5304896831512451, 0.9039581418037415, 0.9366835951805115, 0.9652710556983948, 0.07714381814002991, 0.7655075788497925, 0.09492266178131104, 0.7500200271606445, 0.6590962409973145, 0.19639156758785248, 0.12858077883720398, 0.1315186470746994, 0.8341460824012756, 0.5491176247596741, 0.2220095992088318, 0.8350792527198792, 0.2740192413330078, 0.8359421491622925, 0.005694213323295116, 0.1044410765171051, 0.8541707992553711, 0.33968979120254517, 0.14025482535362244, 0.8172051310539246, 0.39639943838119507, 0.37975409626960754, 0.2562301754951477, 0.5173991322517395, 0.20979797840118408, 0.24902884662151337, 0.40574580430984497, 0.9546396732330322, 0.6625224947929382, 0.3844829797744751, 0.2947736382484436, 0.39435213804244995, 0.6935738325119019, 0.27325505018234253, 0.4490673542022705, 0.4290046989917755, 0.6258346438407898, 0.7245139479637146, 0.5210762619972229, 0.3103833496570587, 0.984284520149231, 0.7271832227706909, 0.054386455565690994, 0.9886484742164612, 0.5912991762161255, 0.8480425477027893, 0.2404581904411316, 0.761442244052887, 0.23551371693611145, 0.7017846703529358, 0.38449934124946594, 0.8790562748908997, 0.06591027230024338, 0.46864843368530273, 0.13216416537761688, 0.692452073097229, 0.04988833889365196, 0.5691991448402405, 0.42036789655685425, 0.8218620419502258, 0.748799204826355, 0.5949804186820984, 0.760817289352417, 0.8749229311943054, 0.8209290504455566, 0.21112455427646637, 0.5346830487251282, 0.6935092210769653, 0.5279433727264404, 0.5479289889335632, 0.4417686462402344, 0.38963329792022705, 0.6661739945411682, 0.9739553332328796, 0.04269544035196304, 0.8578197360038757, 0.8881459832191467, 0.053067587316036224, 0.7503750920295715, 0.026237372308969498, 0.8519961833953857, 0.555051863193512, 0.747510552406311, 0.03300659358501434, 0.48286378383636475, 0.8855323195457458, 0.9632793068885803, 0.9104558825492859, 0.48694849014282227, 0.399563729763031, 0.6363621950149536, 0.11851905286312103, 0.017224308103322983, 0.8240532875061035, 0.7225683331489563, 0.14129522442817688, 0.03214777261018753, 0.22644132375717163, 0.12453615665435791, 0.14669975638389587, 0.20129647850990295, 0.37571659684181213, 0.28608691692352295, 0.5647987723350525, 0.5401462912559509, 0.8368682861328125, 0.4405445456504822, 0.6099599599838257, 0.31859633326530457, 0.4392208158969879, 0.8659310936927795, 0.5211570262908936, 0.971695601940155, 0.4802115559577942, 0.9608403444290161, 0.11427588760852814, 0.5906932950019836, 0.5829917192459106, 0.7723814845085144, 0.2851836085319519, 0.7487574815750122, 0.40168407559394836, 0.1096145436167717, 0.38012459874153137, 0.9993427395820618, 0.6248184442520142, 0.5964413285255432, 0.8974211812019348, 0.021383538842201233, 0.7045061588287354, 0.10735698789358139, 0.034189656376838684, 0.4253982603549957, 0.5137093663215637, 0.3070155680179596, 0.26458463072776794, 0.500767171382904, 0.35795703530311584, 0.43192875385284424, 0.0011799664935097098, 0.8871830105781555, 0.3413742184638977, 0.23464272916316986, 0.2985425889492035, 0.43168431520462036, 0.8043161630630493, 0.8787585496902466, 0.3137490153312683, 0.8155429363250732, 0.5388948321342468, 0.8555070757865906, 0.2806842625141144, 0.8434351086616516, 0.01054427120834589, 0.5914859175682068, 0.7061315178871155, 0.17015855014324188, 0.7105374932289124, 0.756917417049408, 0.9772598147392273, 0.4745588004589081, 0.9372658729553223, 0.9028635025024414, 0.0553511306643486, 0.059380579739809036, 0.03670920804142952, 0.5552451014518738, 0.0863645151257515, 0.7970898151397705, 0.709926962852478, 0.7950313687324524, 0.31617963314056396, 0.7190312743186951, 0.30269700288772583, 0.5575765371322632, 0.6522773504257202, 0.8686654567718506, 0.06443669646978378, 0.23735427856445312, 0.7017615437507629, 0.11044484376907349, 0.6743099689483643, 0.7618545293807983, 0.9179471135139465, 0.9271143078804016, 0.3715285658836365, 0.3158683180809021, 0.5581682324409485, 0.425870805978775, 0.9559334516525269, 0.32485705614089966, 0.22024419903755188, 0.738275408744812, 0.35260477662086487, 0.03648458421230316, 0.5063309073448181, 0.5714408159255981, 0.42382925748825073, 0.1744859516620636, 0.012257871218025684, 0.6470044255256653, 0.6596391201019287, 0.4375765323638916, 0.8324525356292725, 0.148403599858284, 0.32366088032722473, 0.28859803080558777, 0.036741212010383606, 0.6912445425987244, 0.5623661875724792, 0.24150314927101135, 0.6668141484260559, 0.457194447517395, 0.37331423163414, 0.7039971947669983, 0.5442853569984436, 0.16904520988464355, 0.5473294854164124, 0.42225542664527893, 0.1632952094078064, 0.13430103659629822, 0.7011837959289551, 0.35530123114585876, 0.22957314550876617, 0.30041030049324036, 0.8040412068367004, 0.7258527278900146, 0.7313927412033081, 0.1588331162929535, 0.135481595993042, 0.8655409812927246, 0.05593014135956764, 0.13720092177391052, 0.4199233651161194, 0.5524675250053406, 0.6945871710777283, 0.5422185063362122, 0.9759254455566406, 0.5732696056365967, 0.36203110218048096, 0.341176837682724, 0.6339867115020752, 0.7928552627563477, 0.3829185366630554, 0.5065315365791321, 0.30392715334892273, 0.448226660490036, 0.5905334949493408, 0.743084728717804, 0.8534137010574341, 0.14105093479156494, 0.36877334117889404, 0.18374945223331451, 0.20742535591125488, 0.05424303933978081, 0.9064294099807739, 0.7810009717941284, 0.3920835852622986, 0.6733852028846741, 0.7985923886299133, 0.56886887550354, 0.8983238339424133, 0.06639385968446732, 0.7757044434547424, 0.4609031677246094, 0.2285572588443756, 0.9890051484107971, 0.31385186314582825, 0.23206709325313568, 0.7099732160568237, 0.8873257040977478, 0.20876754820346832, 0.4126618802547455, 0.364944189786911, 0.9184130430221558, 0.21294458210468292, 0.1087569072842598, 0.12313185632228851, 0.6087223887443542, 0.3020622134208679, 0.6708245277404785, 0.00968034565448761, 0.8843799233436584, 0.8471185564994812, 0.009053618647158146, 0.5472723841667175, 0.950732409954071, 0.2927361726760864, 0.22065046429634094, 0.17401093244552612, 0.6433684229850769, 0.3871839642524719, 0.9706835746765137, 0.26617759466171265, 0.5593381524085999, 0.3533758223056793, 0.6942663192749023, 0.963712751865387, 0.8432105183601379, 0.23894959688186646, 0.17237906157970428, 0.41669386625289917, 0.9002247452735901, 0.43070852756500244, 0.3645652234554291, 0.37970998883247375, 0.09329424798488617, 0.2716970145702362, 0.5067605376243591, 0.5323185324668884, 0.0941026508808136, 0.6156055927276611, 0.2279163897037506, 0.46269893646240234, 0.46550822257995605, 0.9443367123603821, 0.2790738344192505, 0.6077525019645691, 0.633952796459198, 0.5716169476509094, 0.1307380050420761, 0.8753399848937988, 0.40633732080459595, 0.06160659343004227, 0.021534273400902748, 0.9461350440979004, 0.7492088079452515, 0.11246911436319351, 0.4941251277923584, 0.9788018465042114, 0.27250680327415466, 0.3345406651496887, 0.19131797552108765, 0.14440374076366425, 0.2348489910364151, 0.31302410364151, 0.9079352617263794, 0.4020977020263672, 0.6660201549530029, 0.6413438320159912, 0.20272615551948547, 0.6990474462509155, 0.9029505848884583, 0.05377570912241936, 0.5987172722816467, 0.8348270654678345, 0.22269052267074585, 0.7413466572761536, 0.3676571547985077, 0.2186078280210495, 0.49187159538269043, 0.5381358861923218, 0.06617742031812668, 0.3657665550708771, 0.5592037439346313, 0.8133091330528259, 0.5245937705039978, 0.9237461090087891, 0.18355919420719147, 0.9537744522094727, 0.9397586584091187, 0.9005112648010254, 0.3715962767601013, 0.038503702729940414, 0.08550792187452316, 0.0829492136836052, 0.23305834829807281, 0.7761086225509644, 0.15855655074119568, 0.9690130352973938, 0.5020524263381958, 0.3725299835205078, 0.8542638421058655, 0.019558819010853767, 0.15747599303722382, 0.8419409990310669, 0.6331632137298584, 0.7364429235458374, 0.6126334071159363, 0.8729809522628784, 0.8290192484855652, 0.05802781879901886, 0.5132171511650085, 0.8647670745849609, 0.3186877965927124, 0.2963152229785919, 0.09293709695339203, 0.2839053273200989, 0.41266000270843506, 0.5926613211631775, 0.748725950717926, 0.6268962621688843, 0.8735111951828003, 0.6876919865608215, 0.5448590517044067, 0.9995477199554443, 0.5211653709411621, 0.9796311259269714, 0.10060117393732071, 0.7818820476531982, 0.12879221141338348, 0.4428848922252655, 0.6108387112617493, 0.009913390502333641, 0.6105896830558777, 0.7839468121528625, 0.16570189595222473, 0.9330465793609619, 0.20278356969356537, 0.05767875909805298, 0.6311724185943604, 0.9409513473510742, 0.8009441494941711, 0.28160372376441956, 0.8198218941688538, 0.4478168785572052, 0.6826450824737549, 0.22241489589214325, 0.8591458201408386, 0.9293228387832642, 0.40108972787857056, 0.8202097415924072, 0.8996019959449768, 0.14287227392196655, 0.38321569561958313, 0.27360138297080994, 0.8402204513549805, 0.9253615736961365, 0.6166125535964966, 0.4354666769504547, 0.796143651008606, 0.4072890877723694, 0.2206253558397293, 0.3822609484195709, 0.7882177233695984, 0.3175186514854431, 0.4173959493637085, 0.22347642481327057, 0.9197232723236084, 0.35839006304740906, 0.9049082398414612, 0.9309132099151611, 0.045181240886449814, 0.09384647011756897, 0.05347450450062752, 0.19579052925109863, 0.7908905148506165, 0.20613841712474823, 0.14672277867794037, 0.7862143516540527, 0.9796620607376099, 0.3739449083805084, 0.17460660636425018, 0.28613653779029846, 0.5251057147979736, 0.3894467353820801, 0.28357192873954773, 0.36872538924217224, 0.7701210379600525, 0.6139308214187622, 0.8185737133026123, 0.5817059874534607, 0.6525381803512573, 0.24731449782848358, 0.20497308671474457, 0.47354310750961304, 0.5834407806396484, 0.17583248019218445, 0.7986509799957275, 0.5127730369567871, 0.8926236033439636, 0.31678536534309387, 0.789405882358551, 0.19309519231319427, 0.46440237760543823, 0.9070742726325989, 0.5251756906509399, 0.5822200179100037, 0.9608134031295776, 0.8702162504196167, 0.6776354908943176, 0.5664172172546387, 0.3142203390598297, 0.4488910138607025, 0.12798769772052765, 0.011343738064169884, 0.02167833410203457, 0.6363694667816162, 0.6574286222457886, 0.6331721544265747, 0.1860949695110321, 0.034065719693899155, 0.18757067620754242, 0.9766800403594971, 0.9342480301856995, 0.7307646870613098, 0.2236720770597458, 0.44722676277160645, 0.7844812870025635, 0.6553750038146973, 0.02890823595225811, 0.5502535700798035, 0.49368926882743835, 0.666702389717102, 0.1015218049287796, 0.3175419270992279, 0.647401750087738, 0.1520446091890335, 0.41871029138565063, 0.22599367797374725, 0.208740696310997, 0.2565656006336212, 0.8748878836631775, 0.6164125800132751, 0.026515310630202293, 0.35274752974510193, 0.38343608379364014, 0.5636261701583862, 0.26844000816345215, 0.8335092663764954, 0.7071099877357483, 0.9418774247169495, 0.07427223771810532, 0.9127421379089355, 0.9862300157546997, 0.7681083679199219, 0.01751137711107731, 0.34160518646240234, 0.705668568611145, 0.7790502905845642, 0.4326382577419281, 0.7700020670890808, 0.7228742837905884, 0.020561855286359787, 0.7313647270202637, 0.05350518971681595, 0.9003791809082031, 0.6505491137504578, 0.4541366398334503, 0.8059714436531067, 0.5164853930473328, 0.18433037400245667, 0.5248328447341919, 0.7833437323570251, 0.8773091435432434, 0.04765724018216133, 0.07328523695468903, 0.0812780112028122, 0.5028670430183411, 0.16256916522979736, 0.5242683291435242, 0.9959482550621033, 0.6369618773460388, 0.11678291857242584, 0.66120845079422, 0.6951324343681335, 0.7239258289337158, 0.6037524938583374, 0.12224157899618149, 0.08236031979322433, 0.6220316886901855, 0.3785780966281891, 0.017284560948610306, 0.324351966381073, 0.8785102367401123, 0.10727077722549438, 0.8287323713302612, 0.6088231801986694, 0.5255677103996277, 0.5691452622413635, 0.43685823678970337, 0.1062149852514267, 0.7524598240852356, 0.6816270351409912, 0.8537653088569641, 0.5840227603912354, 0.8530658483505249, 0.5536980032920837, 0.12879525125026703, 0.835331380367279, 0.8097959160804749, 0.24524140357971191, 0.19832557439804077, 0.6036972403526306, 0.19901812076568604, 0.5515961647033691, 0.15916021168231964, 0.4663938581943512, 0.33608734607696533, 0.804487407207489, 0.8883902430534363], 200, map[efSearch, 40])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Table_deletable</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3785,10 +3795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K191"/>
+  <dimension ref="A1:L191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="C200" sqref="C200"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="H181" sqref="H181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3800,14 +3810,14 @@
     <col min="5" max="5" width="17.75" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.25" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="72.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="111.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="8" max="9" width="18.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="72.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="111.75" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3833,16 +3843,19 @@
         <v>10</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -3864,17 +3877,20 @@
       <c r="G2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -3896,17 +3912,20 @@
       <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -3928,17 +3947,20 @@
       <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -3960,17 +3982,20 @@
       <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -3992,17 +4017,20 @@
       <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -4024,17 +4052,20 @@
       <c r="G7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
@@ -4056,17 +4087,20 @@
       <c r="G8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
@@ -4088,17 +4122,20 @@
       <c r="G9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>44</v>
       </c>
@@ -4120,17 +4157,20 @@
       <c r="G10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
@@ -4152,17 +4192,20 @@
       <c r="G11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="L11" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>54</v>
       </c>
@@ -4184,17 +4227,20 @@
       <c r="G12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="L12" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>59</v>
       </c>
@@ -4216,17 +4262,20 @@
       <c r="G13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>747</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>64</v>
       </c>
@@ -4248,17 +4297,20 @@
       <c r="G14" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I14" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>69</v>
       </c>
@@ -4280,17 +4332,20 @@
       <c r="G15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I15" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>88</v>
       </c>
@@ -4312,17 +4367,20 @@
       <c r="G16" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>89</v>
       </c>
@@ -4344,17 +4402,20 @@
       <c r="G17" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>90</v>
       </c>
@@ -4376,17 +4437,20 @@
       <c r="G18" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>91</v>
       </c>
@@ -4408,17 +4472,20 @@
       <c r="G19" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>753</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="L19" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>92</v>
       </c>
@@ -4440,17 +4507,20 @@
       <c r="G20" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>93</v>
       </c>
@@ -4472,17 +4542,20 @@
       <c r="G21" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="L21" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22" s="3" t="s">
         <v>520</v>
       </c>
@@ -4504,17 +4577,20 @@
       <c r="G22" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I22" s="3" t="s">
+        <v>970</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="L22" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
         <v>108</v>
       </c>
@@ -4536,17 +4612,20 @@
       <c r="G23" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I23" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
         <v>109</v>
       </c>
@@ -4568,17 +4647,20 @@
       <c r="G24" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="I24" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>110</v>
       </c>
@@ -4600,17 +4682,20 @@
       <c r="G25" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="I25" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A26" s="3" t="s">
         <v>111</v>
       </c>
@@ -4632,17 +4717,20 @@
       <c r="G26" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
         <v>112</v>
       </c>
@@ -4664,17 +4752,20 @@
       <c r="G27" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="I27" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A28" s="3" t="s">
         <v>113</v>
       </c>
@@ -4696,17 +4787,20 @@
       <c r="G28" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I28" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>762</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A29" s="3" t="s">
         <v>114</v>
       </c>
@@ -4728,17 +4822,20 @@
       <c r="G29" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I29" s="3" t="s">
+        <v>970</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A30" s="5" t="s">
         <v>137</v>
       </c>
@@ -4760,17 +4857,20 @@
       <c r="G30" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="I30" s="1" t="s">
+      <c r="I30" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
         <v>138</v>
       </c>
@@ -4792,17 +4892,20 @@
       <c r="G31" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="I31" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
         <v>139</v>
       </c>
@@ -4824,17 +4927,20 @@
       <c r="G32" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I32" s="1" t="s">
+      <c r="I32" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
         <v>140</v>
       </c>
@@ -4856,17 +4962,20 @@
       <c r="G33" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="I33" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>767</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>141</v>
       </c>
@@ -4888,17 +4997,20 @@
       <c r="G34" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="I34" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>142</v>
       </c>
@@ -4920,17 +5032,20 @@
       <c r="G35" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="I35" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
         <v>143</v>
       </c>
@@ -4952,17 +5067,20 @@
       <c r="G36" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="I36" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
         <v>171</v>
       </c>
@@ -4984,17 +5102,20 @@
       <c r="G37" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="I37" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>771</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A38" s="3" t="s">
         <v>172</v>
       </c>
@@ -5016,17 +5137,20 @@
       <c r="G38" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I38" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J38" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
         <v>173</v>
       </c>
@@ -5048,17 +5172,20 @@
       <c r="G39" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="I39" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J39" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
         <v>174</v>
       </c>
@@ -5080,17 +5207,20 @@
       <c r="G40" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="I40" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
         <v>175</v>
       </c>
@@ -5112,17 +5242,20 @@
       <c r="G41" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I41" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J41" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>775</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A42" s="3" t="s">
         <v>176</v>
       </c>
@@ -5144,17 +5277,20 @@
       <c r="G42" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I42" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J42" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="L42" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A43" s="3" t="s">
         <v>177</v>
       </c>
@@ -5176,17 +5312,20 @@
       <c r="G43" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="I43" s="3" t="s">
+        <v>969</v>
+      </c>
+      <c r="J43" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="L43" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>205</v>
       </c>
@@ -5209,16 +5348,19 @@
         <v>259</v>
       </c>
       <c r="I44" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="J44" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>859</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="L44" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>206</v>
       </c>
@@ -5241,16 +5383,19 @@
         <v>259</v>
       </c>
       <c r="I45" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J45" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="K45" s="1" t="s">
         <v>860</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="L45" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>249</v>
       </c>
@@ -5273,16 +5418,19 @@
         <v>259</v>
       </c>
       <c r="I46" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="J46" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="K46" s="1" t="s">
         <v>861</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="L46" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>207</v>
       </c>
@@ -5305,16 +5453,19 @@
         <v>259</v>
       </c>
       <c r="I47" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J47" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>862</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>208</v>
       </c>
@@ -5337,16 +5488,19 @@
         <v>259</v>
       </c>
       <c r="I48" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J48" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="K48" s="1" t="s">
         <v>863</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="L48" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>251</v>
       </c>
@@ -5369,16 +5523,19 @@
         <v>259</v>
       </c>
       <c r="I49" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="J49" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="L49" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>209</v>
       </c>
@@ -5401,16 +5558,19 @@
         <v>259</v>
       </c>
       <c r="I50" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J50" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="K50" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="K50" s="1" t="s">
+      <c r="L50" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>216</v>
       </c>
@@ -5433,16 +5593,19 @@
         <v>259</v>
       </c>
       <c r="I51" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J51" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="J51" s="1" t="s">
+      <c r="K51" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="K51" s="1" t="s">
+      <c r="L51" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>217</v>
       </c>
@@ -5465,16 +5628,19 @@
         <v>259</v>
       </c>
       <c r="I52" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J52" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="K52" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="L52" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>238</v>
       </c>
@@ -5496,17 +5662,17 @@
       <c r="H53" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="I53" s="1" t="s">
+      <c r="J53" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="K53" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="L53" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>239</v>
       </c>
@@ -5528,17 +5694,17 @@
       <c r="H54" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="I54" s="1" t="s">
+      <c r="J54" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="J54" s="1" t="s">
+      <c r="K54" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="L54" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>241</v>
       </c>
@@ -5560,17 +5726,17 @@
       <c r="H55" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="I55" s="1" t="s">
+      <c r="J55" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="J55" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="L55" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>253</v>
       </c>
@@ -5592,17 +5758,17 @@
       <c r="H56" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="I56" s="1" t="s">
+      <c r="J56" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="J56" s="1" t="s">
+      <c r="K56" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="L56" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>256</v>
       </c>
@@ -5625,16 +5791,19 @@
         <v>260</v>
       </c>
       <c r="I57" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J57" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="J57" s="1" t="s">
+      <c r="K57" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="K57" s="1" t="s">
+      <c r="L57" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>262</v>
       </c>
@@ -5657,16 +5826,19 @@
         <v>259</v>
       </c>
       <c r="I58" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J58" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="J58" s="1" t="s">
+      <c r="K58" s="1" t="s">
         <v>873</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="L58" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>263</v>
       </c>
@@ -5689,16 +5861,19 @@
         <v>259</v>
       </c>
       <c r="I59" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J59" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="J59" s="1" t="s">
+      <c r="K59" s="1" t="s">
         <v>874</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="L59" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>264</v>
       </c>
@@ -5721,16 +5896,19 @@
         <v>259</v>
       </c>
       <c r="I60" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="J60" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>875</v>
       </c>
-      <c r="K60" s="1" t="s">
+      <c r="L60" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>265</v>
       </c>
@@ -5753,16 +5931,19 @@
         <v>259</v>
       </c>
       <c r="I61" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J61" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="J61" s="1" t="s">
+      <c r="K61" s="1" t="s">
         <v>876</v>
       </c>
-      <c r="K61" s="1" t="s">
+      <c r="L61" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>266</v>
       </c>
@@ -5785,16 +5966,19 @@
         <v>259</v>
       </c>
       <c r="I62" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J62" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="J62" s="1" t="s">
+      <c r="K62" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="K62" s="1" t="s">
+      <c r="L62" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>285</v>
       </c>
@@ -5817,16 +6001,19 @@
         <v>259</v>
       </c>
       <c r="I63" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J63" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="J63" s="1" t="s">
+      <c r="K63" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="K63" s="1" t="s">
+      <c r="L63" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>286</v>
       </c>
@@ -5849,16 +6036,19 @@
         <v>259</v>
       </c>
       <c r="I64" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J64" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="J64" s="1" t="s">
+      <c r="K64" s="1" t="s">
         <v>879</v>
       </c>
-      <c r="K64" s="1" t="s">
+      <c r="L64" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>293</v>
       </c>
@@ -5881,16 +6071,19 @@
         <v>259</v>
       </c>
       <c r="I65" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J65" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="J65" s="1" t="s">
+      <c r="K65" s="1" t="s">
         <v>880</v>
       </c>
-      <c r="K65" s="1" t="s">
+      <c r="L65" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>297</v>
       </c>
@@ -5913,16 +6106,19 @@
         <v>259</v>
       </c>
       <c r="I66" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J66" s="1" t="s">
         <v>944</v>
       </c>
-      <c r="J66" s="1" t="s">
+      <c r="K66" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="K66" s="1" t="s">
+      <c r="L66" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>300</v>
       </c>
@@ -5945,16 +6141,19 @@
         <v>259</v>
       </c>
       <c r="I67" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J67" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="J67" s="1" t="s">
+      <c r="K67" s="1" t="s">
         <v>882</v>
       </c>
-      <c r="K67" s="1" t="s">
+      <c r="L67" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>304</v>
       </c>
@@ -5977,16 +6176,19 @@
         <v>259</v>
       </c>
       <c r="I68" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J68" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="J68" s="1" t="s">
+      <c r="K68" s="1" t="s">
         <v>883</v>
       </c>
-      <c r="K68" s="1" t="s">
+      <c r="L68" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>308</v>
       </c>
@@ -6009,16 +6211,19 @@
         <v>259</v>
       </c>
       <c r="I69" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J69" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="J69" s="1" t="s">
+      <c r="K69" s="1" t="s">
         <v>884</v>
       </c>
-      <c r="K69" s="1" t="s">
+      <c r="L69" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>312</v>
       </c>
@@ -6041,16 +6246,19 @@
         <v>259</v>
       </c>
       <c r="I70" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J70" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="J70" s="1" t="s">
+      <c r="K70" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="K70" s="1" t="s">
+      <c r="L70" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>316</v>
       </c>
@@ -6073,16 +6281,19 @@
         <v>259</v>
       </c>
       <c r="I71" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J71" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="J71" s="1" t="s">
+      <c r="K71" s="1" t="s">
         <v>886</v>
       </c>
-      <c r="K71" s="1" t="s">
+      <c r="L71" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>317</v>
       </c>
@@ -6105,16 +6316,19 @@
         <v>333</v>
       </c>
       <c r="I72" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J72" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="J72" s="1" t="s">
+      <c r="K72" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="K72" s="1" t="s">
+      <c r="L72" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>322</v>
       </c>
@@ -6137,16 +6351,19 @@
         <v>259</v>
       </c>
       <c r="I73" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J73" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="J73" s="1" t="s">
+      <c r="K73" s="1" t="s">
         <v>888</v>
       </c>
-      <c r="K73" s="1" t="s">
+      <c r="L73" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
         <v>323</v>
       </c>
@@ -6169,16 +6386,19 @@
         <v>259</v>
       </c>
       <c r="I74" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J74" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="J74" s="1" t="s">
+      <c r="K74" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="K74" s="1" t="s">
+      <c r="L74" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>324</v>
       </c>
@@ -6201,16 +6421,19 @@
         <v>333</v>
       </c>
       <c r="I75" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J75" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="J75" s="1" t="s">
+      <c r="K75" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="K75" s="1" t="s">
+      <c r="L75" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>337</v>
       </c>
@@ -6233,16 +6456,19 @@
         <v>340</v>
       </c>
       <c r="I76" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J76" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="J76" s="1" t="s">
+      <c r="K76" s="1" t="s">
         <v>891</v>
       </c>
-      <c r="K76" s="1" t="s">
+      <c r="L76" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
         <v>342</v>
       </c>
@@ -6265,16 +6491,19 @@
         <v>259</v>
       </c>
       <c r="I77" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J77" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="J77" s="1" t="s">
+      <c r="K77" s="1" t="s">
         <v>892</v>
       </c>
-      <c r="K77" s="1" t="s">
+      <c r="L77" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
         <v>346</v>
       </c>
@@ -6297,16 +6526,19 @@
         <v>259</v>
       </c>
       <c r="I78" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J78" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="J78" s="1" t="s">
+      <c r="K78" s="1" t="s">
         <v>893</v>
       </c>
-      <c r="K78" s="1" t="s">
+      <c r="L78" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
         <v>347</v>
       </c>
@@ -6329,16 +6561,19 @@
         <v>259</v>
       </c>
       <c r="I79" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J79" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="J79" s="1" t="s">
+      <c r="K79" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="K79" s="1" t="s">
+      <c r="L79" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
         <v>348</v>
       </c>
@@ -6361,16 +6596,19 @@
         <v>259</v>
       </c>
       <c r="I80" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J80" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="J80" s="1" t="s">
+      <c r="K80" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="K80" s="1" t="s">
+      <c r="L80" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
         <v>349</v>
       </c>
@@ -6393,16 +6631,19 @@
         <v>259</v>
       </c>
       <c r="I81" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J81" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="J81" s="1" t="s">
+      <c r="K81" s="1" t="s">
         <v>896</v>
       </c>
-      <c r="K81" s="1" t="s">
+      <c r="L81" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
         <v>350</v>
       </c>
@@ -6425,16 +6666,19 @@
         <v>259</v>
       </c>
       <c r="I82" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J82" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="J82" s="1" t="s">
+      <c r="K82" s="1" t="s">
         <v>897</v>
       </c>
-      <c r="K82" s="1" t="s">
+      <c r="L82" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
         <v>351</v>
       </c>
@@ -6457,16 +6701,19 @@
         <v>259</v>
       </c>
       <c r="I83" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J83" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="J83" s="1" t="s">
+      <c r="K83" s="1" t="s">
         <v>898</v>
       </c>
-      <c r="K83" s="1" t="s">
+      <c r="L83" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
         <v>352</v>
       </c>
@@ -6489,16 +6736,19 @@
         <v>259</v>
       </c>
       <c r="I84" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J84" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="J84" s="1" t="s">
+      <c r="K84" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="K84" s="1" t="s">
+      <c r="L84" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
         <v>376</v>
       </c>
@@ -6521,16 +6771,19 @@
         <v>259</v>
       </c>
       <c r="I85" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J85" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="J85" s="1" t="s">
+      <c r="K85" s="1" t="s">
         <v>900</v>
       </c>
-      <c r="K85" s="1" t="s">
+      <c r="L85" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
         <v>377</v>
       </c>
@@ -6553,16 +6806,19 @@
         <v>259</v>
       </c>
       <c r="I86" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J86" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="J86" s="1" t="s">
+      <c r="K86" s="1" t="s">
         <v>901</v>
       </c>
-      <c r="K86" s="1" t="s">
+      <c r="L86" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
         <v>378</v>
       </c>
@@ -6585,16 +6841,19 @@
         <v>259</v>
       </c>
       <c r="I87" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J87" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="J87" s="1" t="s">
+      <c r="K87" s="1" t="s">
         <v>902</v>
       </c>
-      <c r="K87" s="1" t="s">
+      <c r="L87" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
         <v>379</v>
       </c>
@@ -6617,16 +6876,19 @@
         <v>259</v>
       </c>
       <c r="I88" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J88" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="J88" s="1" t="s">
+      <c r="K88" s="1" t="s">
         <v>903</v>
       </c>
-      <c r="K88" s="1" t="s">
+      <c r="L88" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
         <v>380</v>
       </c>
@@ -6649,16 +6911,19 @@
         <v>259</v>
       </c>
       <c r="I89" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J89" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="J89" s="1" t="s">
+      <c r="K89" s="1" t="s">
         <v>904</v>
       </c>
-      <c r="K89" s="1" t="s">
+      <c r="L89" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
         <v>393</v>
       </c>
@@ -6681,16 +6946,19 @@
         <v>340</v>
       </c>
       <c r="I90" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J90" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="J90" s="1" t="s">
+      <c r="K90" s="1" t="s">
         <v>905</v>
       </c>
-      <c r="K90" s="1" t="s">
+      <c r="L90" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
         <v>394</v>
       </c>
@@ -6713,16 +6981,19 @@
         <v>340</v>
       </c>
       <c r="I91" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J91" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="J91" s="1" t="s">
+      <c r="K91" s="1" t="s">
         <v>906</v>
       </c>
-      <c r="K91" s="1" t="s">
+      <c r="L91" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
         <v>395</v>
       </c>
@@ -6745,16 +7016,19 @@
         <v>340</v>
       </c>
       <c r="I92" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J92" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="J92" s="1" t="s">
+      <c r="K92" s="1" t="s">
         <v>907</v>
       </c>
-      <c r="K92" s="1" t="s">
+      <c r="L92" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
         <v>396</v>
       </c>
@@ -6777,16 +7051,19 @@
         <v>340</v>
       </c>
       <c r="I93" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J93" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="J93" s="1" t="s">
+      <c r="K93" s="1" t="s">
         <v>908</v>
       </c>
-      <c r="K93" s="1" t="s">
+      <c r="L93" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
         <v>406</v>
       </c>
@@ -6809,16 +7086,19 @@
         <v>259</v>
       </c>
       <c r="I94" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J94" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="J94" s="1" t="s">
+      <c r="K94" s="1" t="s">
         <v>909</v>
       </c>
-      <c r="K94" s="1" t="s">
+      <c r="L94" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
         <v>407</v>
       </c>
@@ -6841,16 +7121,19 @@
         <v>259</v>
       </c>
       <c r="I95" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J95" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="J95" s="1" t="s">
+      <c r="K95" s="1" t="s">
         <v>910</v>
       </c>
-      <c r="K95" s="1" t="s">
+      <c r="L95" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
         <v>408</v>
       </c>
@@ -6873,16 +7156,19 @@
         <v>340</v>
       </c>
       <c r="I96" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J96" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="J96" s="1" t="s">
+      <c r="K96" s="1" t="s">
         <v>911</v>
       </c>
-      <c r="K96" s="1" t="s">
+      <c r="L96" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
         <v>421</v>
       </c>
@@ -6905,16 +7191,19 @@
         <v>259</v>
       </c>
       <c r="I97" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J97" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="J97" s="1" t="s">
+      <c r="K97" s="1" t="s">
         <v>912</v>
       </c>
-      <c r="K97" s="1" t="s">
+      <c r="L97" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A98" s="3" t="s">
         <v>439</v>
       </c>
@@ -6937,16 +7226,19 @@
         <v>123</v>
       </c>
       <c r="I98" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J98" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="J98" s="1" t="s">
+      <c r="K98" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="K98" s="1" t="s">
+      <c r="L98" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A99" s="3" t="s">
         <v>502</v>
       </c>
@@ -6969,16 +7261,19 @@
         <v>123</v>
       </c>
       <c r="I99" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="J99" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="J99" s="1" t="s">
+      <c r="K99" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="K99" s="1" t="s">
+      <c r="L99" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A100" s="3" t="s">
         <v>440</v>
       </c>
@@ -7001,16 +7296,19 @@
         <v>123</v>
       </c>
       <c r="I100" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J100" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="J100" s="1" t="s">
+      <c r="K100" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="K100" s="1" t="s">
+      <c r="L100" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A101" s="3" t="s">
         <v>441</v>
       </c>
@@ -7033,16 +7331,19 @@
         <v>123</v>
       </c>
       <c r="I101" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J101" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="J101" s="1" t="s">
+      <c r="K101" s="1" t="s">
         <v>781</v>
       </c>
-      <c r="K101" s="1" t="s">
+      <c r="L101" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A102" s="3" t="s">
         <v>442</v>
       </c>
@@ -7065,16 +7366,19 @@
         <v>123</v>
       </c>
       <c r="I102" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J102" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="J102" s="1" t="s">
+      <c r="K102" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="K102" s="1" t="s">
+      <c r="L102" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A103" s="3" t="s">
         <v>443</v>
       </c>
@@ -7097,16 +7401,19 @@
         <v>122</v>
       </c>
       <c r="I103" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J103" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="J103" s="1" t="s">
+      <c r="K103" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="K103" s="1" t="s">
+      <c r="L103" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A104" s="3" t="s">
         <v>444</v>
       </c>
@@ -7129,16 +7436,19 @@
         <v>123</v>
       </c>
       <c r="I104" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J104" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="J104" s="1" t="s">
+      <c r="K104" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="K104" s="1" t="s">
+      <c r="L104" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A105" s="3" t="s">
         <v>445</v>
       </c>
@@ -7161,16 +7471,19 @@
         <v>123</v>
       </c>
       <c r="I105" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J105" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="J105" s="1" t="s">
+      <c r="K105" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="K105" s="1" t="s">
+      <c r="L105" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A106" s="3" t="s">
         <v>446</v>
       </c>
@@ -7193,16 +7506,19 @@
         <v>123</v>
       </c>
       <c r="I106" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J106" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="J106" s="1" t="s">
+      <c r="K106" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="K106" s="1" t="s">
+      <c r="L106" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A107" s="3" t="s">
         <v>447</v>
       </c>
@@ -7225,16 +7541,19 @@
         <v>512</v>
       </c>
       <c r="I107" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J107" s="1" t="s">
         <v>919</v>
       </c>
-      <c r="J107" s="1" t="s">
+      <c r="K107" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="K107" s="1" t="s">
+      <c r="L107" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A108" s="3" t="s">
         <v>476</v>
       </c>
@@ -7257,16 +7576,19 @@
         <v>52</v>
       </c>
       <c r="I108" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J108" s="1" t="s">
         <v>920</v>
       </c>
-      <c r="J108" s="1" t="s">
+      <c r="K108" s="1" t="s">
         <v>788</v>
       </c>
-      <c r="K108" s="1" t="s">
+      <c r="L108" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A109" s="3" t="s">
         <v>477</v>
       </c>
@@ -7289,16 +7611,19 @@
         <v>81</v>
       </c>
       <c r="I109" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J109" s="1" t="s">
         <v>921</v>
       </c>
-      <c r="J109" s="1" t="s">
+      <c r="K109" s="1" t="s">
         <v>789</v>
       </c>
-      <c r="K109" s="1" t="s">
+      <c r="L109" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A110" s="3" t="s">
         <v>478</v>
       </c>
@@ -7321,16 +7646,19 @@
         <v>123</v>
       </c>
       <c r="I110" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J110" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="J110" s="1" t="s">
+      <c r="K110" s="1" t="s">
         <v>790</v>
       </c>
-      <c r="K110" s="1" t="s">
+      <c r="L110" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A111" s="3" t="s">
         <v>479</v>
       </c>
@@ -7353,16 +7681,19 @@
         <v>123</v>
       </c>
       <c r="I111" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J111" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="J111" s="1" t="s">
+      <c r="K111" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="K111" s="1" t="s">
+      <c r="L111" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A112" s="3" t="s">
         <v>480</v>
       </c>
@@ -7385,16 +7716,19 @@
         <v>123</v>
       </c>
       <c r="I112" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J112" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="J112" s="1" t="s">
+      <c r="K112" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="K112" s="1" t="s">
+      <c r="L112" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A113" s="3" t="s">
         <v>494</v>
       </c>
@@ -7417,16 +7751,19 @@
         <v>499</v>
       </c>
       <c r="I113" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J113" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="J113" s="1" t="s">
+      <c r="K113" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="K113" s="1" t="s">
+      <c r="L113" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A114" s="3" t="s">
         <v>495</v>
       </c>
@@ -7449,16 +7786,19 @@
         <v>15</v>
       </c>
       <c r="I114" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J114" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="J114" s="1" t="s">
+      <c r="K114" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="K114" s="1" t="s">
+      <c r="L114" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A115" s="3" t="s">
         <v>496</v>
       </c>
@@ -7480,17 +7820,17 @@
       <c r="H115" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="I115" s="1" t="s">
+      <c r="J115" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="J115" s="1" t="s">
+      <c r="K115" s="1" t="s">
         <v>795</v>
       </c>
-      <c r="K115" s="1" t="s">
+      <c r="L115" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A116" s="3" t="s">
         <v>506</v>
       </c>
@@ -7512,17 +7852,17 @@
       <c r="H116" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="I116" s="1" t="s">
+      <c r="J116" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="J116" s="1" t="s">
+      <c r="K116" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="K116" s="1" t="s">
+      <c r="L116" s="1" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A117" s="3" t="s">
         <v>513</v>
       </c>
@@ -7544,17 +7884,17 @@
       <c r="H117" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="I117" s="1" t="s">
+      <c r="J117" s="1" t="s">
         <v>917</v>
       </c>
-      <c r="J117" s="1" t="s">
+      <c r="K117" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="K117" s="1" t="s">
+      <c r="L117" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A118" s="3" t="s">
         <v>514</v>
       </c>
@@ -7577,17 +7917,17 @@
       <c r="H118" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I118" s="1" t="s">
+      <c r="J118" s="1" t="s">
         <v>918</v>
       </c>
-      <c r="J118" s="1" t="s">
+      <c r="K118" s="1" t="s">
         <v>798</v>
       </c>
-      <c r="K118" s="1" t="s">
+      <c r="L118" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A119" s="4" t="s">
         <v>515</v>
       </c>
@@ -7610,16 +7950,19 @@
         <v>523</v>
       </c>
       <c r="I119" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J119" s="1" t="s">
         <v>922</v>
       </c>
-      <c r="J119" s="1" t="s">
+      <c r="K119" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="K119" s="1" t="s">
+      <c r="L119" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A120" s="4" t="s">
         <v>521</v>
       </c>
@@ -7642,16 +7985,19 @@
         <v>524</v>
       </c>
       <c r="I120" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J120" s="1" t="s">
         <v>923</v>
       </c>
-      <c r="J120" s="1" t="s">
+      <c r="K120" s="1" t="s">
         <v>800</v>
       </c>
-      <c r="K120" s="1" t="s">
+      <c r="L120" s="1" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A121" s="3" t="s">
         <v>605</v>
       </c>
@@ -7674,16 +8020,19 @@
         <v>604</v>
       </c>
       <c r="I121" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="J121" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="J121" s="1" t="s">
+      <c r="K121" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="K121" s="1" t="s">
+      <c r="L121" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A122" s="3" t="s">
         <v>532</v>
       </c>
@@ -7705,17 +8054,17 @@
       <c r="H122" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I122" s="1" t="s">
+      <c r="J122" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="J122" s="1" t="s">
+      <c r="K122" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="K122" s="1" t="s">
+      <c r="L122" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A123" s="3" t="s">
         <v>533</v>
       </c>
@@ -7737,17 +8086,17 @@
       <c r="H123" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I123" s="1" t="s">
+      <c r="J123" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="J123" s="1" t="s">
+      <c r="K123" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="K123" s="1" t="s">
+      <c r="L123" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A124" s="3" t="s">
         <v>534</v>
       </c>
@@ -7769,17 +8118,17 @@
       <c r="H124" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I124" s="1" t="s">
+      <c r="J124" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="J124" s="1" t="s">
+      <c r="K124" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="K124" s="1" t="s">
+      <c r="L124" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A125" s="3" t="s">
         <v>535</v>
       </c>
@@ -7801,17 +8150,17 @@
       <c r="H125" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I125" s="1" t="s">
+      <c r="J125" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="J125" s="1" t="s">
+      <c r="K125" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="K125" s="1" t="s">
+      <c r="L125" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A126" s="3" t="s">
         <v>536</v>
       </c>
@@ -7833,17 +8182,17 @@
       <c r="H126" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I126" s="1" t="s">
+      <c r="J126" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="J126" s="1" t="s">
+      <c r="K126" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="K126" s="1" t="s">
+      <c r="L126" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A127" s="3" t="s">
         <v>537</v>
       </c>
@@ -7865,17 +8214,17 @@
       <c r="H127" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I127" s="1" t="s">
+      <c r="J127" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="J127" s="1" t="s">
+      <c r="K127" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="K127" s="1" t="s">
+      <c r="L127" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A128" s="3" t="s">
         <v>538</v>
       </c>
@@ -7897,17 +8246,17 @@
       <c r="H128" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I128" s="1" t="s">
+      <c r="J128" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="J128" s="1" t="s">
+      <c r="K128" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="K128" s="1" t="s">
+      <c r="L128" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A129" s="3" t="s">
         <v>539</v>
       </c>
@@ -7929,17 +8278,17 @@
       <c r="H129" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I129" s="1" t="s">
+      <c r="J129" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="J129" s="1" t="s">
+      <c r="K129" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="K129" s="1" t="s">
+      <c r="L129" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A130" s="3" t="s">
         <v>540</v>
       </c>
@@ -7961,17 +8310,17 @@
       <c r="H130" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I130" s="1" t="s">
+      <c r="J130" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="J130" s="1" t="s">
+      <c r="K130" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="K130" s="1" t="s">
+      <c r="L130" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A131" s="3" t="s">
         <v>541</v>
       </c>
@@ -7993,17 +8342,17 @@
       <c r="H131" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I131" s="1" t="s">
+      <c r="J131" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="J131" s="1" t="s">
+      <c r="K131" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="K131" s="1" t="s">
+      <c r="L131" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A132" s="3" t="s">
         <v>542</v>
       </c>
@@ -8025,17 +8374,17 @@
       <c r="H132" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I132" s="1" t="s">
+      <c r="J132" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="J132" s="1" t="s">
+      <c r="K132" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="K132" s="1" t="s">
+      <c r="L132" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A133" s="3" t="s">
         <v>543</v>
       </c>
@@ -8057,17 +8406,17 @@
       <c r="H133" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I133" s="1" t="s">
+      <c r="J133" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="J133" s="1" t="s">
+      <c r="K133" s="1" t="s">
         <v>813</v>
       </c>
-      <c r="K133" s="1" t="s">
+      <c r="L133" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A134" s="3" t="s">
         <v>544</v>
       </c>
@@ -8089,17 +8438,17 @@
       <c r="H134" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I134" s="1" t="s">
+      <c r="J134" s="1" t="s">
         <v>649</v>
       </c>
-      <c r="J134" s="1" t="s">
+      <c r="K134" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="K134" s="1" t="s">
+      <c r="L134" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A135" s="3" t="s">
         <v>545</v>
       </c>
@@ -8121,17 +8470,17 @@
       <c r="H135" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I135" s="1" t="s">
+      <c r="J135" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="J135" s="1" t="s">
+      <c r="K135" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="K135" s="1" t="s">
+      <c r="L135" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A136" s="3" t="s">
         <v>546</v>
       </c>
@@ -8153,17 +8502,17 @@
       <c r="H136" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I136" s="1" t="s">
+      <c r="J136" s="1" t="s">
         <v>651</v>
       </c>
-      <c r="J136" s="1" t="s">
+      <c r="K136" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="K136" s="1" t="s">
+      <c r="L136" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A137" s="3" t="s">
         <v>547</v>
       </c>
@@ -8185,17 +8534,17 @@
       <c r="H137" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I137" s="1" t="s">
+      <c r="J137" s="1" t="s">
         <v>658</v>
       </c>
-      <c r="J137" s="1" t="s">
+      <c r="K137" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="K137" s="1" t="s">
+      <c r="L137" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A138" s="3" t="s">
         <v>548</v>
       </c>
@@ -8217,17 +8566,17 @@
       <c r="H138" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I138" s="1" t="s">
+      <c r="J138" s="1" t="s">
         <v>659</v>
       </c>
-      <c r="J138" s="1" t="s">
+      <c r="K138" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="K138" s="1" t="s">
+      <c r="L138" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A139" s="3" t="s">
         <v>549</v>
       </c>
@@ -8249,17 +8598,17 @@
       <c r="H139" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I139" s="1" t="s">
+      <c r="J139" s="1" t="s">
         <v>660</v>
       </c>
-      <c r="J139" s="1" t="s">
+      <c r="K139" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="K139" s="1" t="s">
+      <c r="L139" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A140" s="3" t="s">
         <v>550</v>
       </c>
@@ -8281,17 +8630,17 @@
       <c r="H140" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I140" s="1" t="s">
+      <c r="J140" s="1" t="s">
         <v>661</v>
       </c>
-      <c r="J140" s="1" t="s">
+      <c r="K140" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="K140" s="1" t="s">
+      <c r="L140" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A141" s="3" t="s">
         <v>551</v>
       </c>
@@ -8313,17 +8662,17 @@
       <c r="H141" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I141" s="1" t="s">
+      <c r="J141" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="J141" s="1" t="s">
+      <c r="K141" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="K141" s="1" t="s">
+      <c r="L141" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A142" s="3" t="s">
         <v>552</v>
       </c>
@@ -8345,17 +8694,17 @@
       <c r="H142" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I142" s="1" t="s">
+      <c r="J142" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="J142" s="1" t="s">
+      <c r="K142" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="K142" s="1" t="s">
+      <c r="L142" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A143" s="3" t="s">
         <v>553</v>
       </c>
@@ -8377,17 +8726,17 @@
       <c r="H143" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I143" s="1" t="s">
+      <c r="J143" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="J143" s="1" t="s">
+      <c r="K143" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="K143" s="1" t="s">
+      <c r="L143" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A144" s="3" t="s">
         <v>554</v>
       </c>
@@ -8409,17 +8758,17 @@
       <c r="H144" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I144" s="1" t="s">
+      <c r="J144" s="1" t="s">
         <v>707</v>
       </c>
-      <c r="J144" s="1" t="s">
+      <c r="K144" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="K144" s="1" t="s">
+      <c r="L144" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A145" s="3" t="s">
         <v>555</v>
       </c>
@@ -8441,17 +8790,17 @@
       <c r="H145" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I145" s="1" t="s">
+      <c r="J145" s="1" t="s">
         <v>665</v>
       </c>
-      <c r="J145" s="1" t="s">
+      <c r="K145" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="K145" s="1" t="s">
+      <c r="L145" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A146" s="3" t="s">
         <v>556</v>
       </c>
@@ -8473,17 +8822,17 @@
       <c r="H146" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I146" s="1" t="s">
+      <c r="J146" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="J146" s="1" t="s">
+      <c r="K146" s="1" t="s">
         <v>826</v>
       </c>
-      <c r="K146" s="1" t="s">
+      <c r="L146" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A147" s="3" t="s">
         <v>557</v>
       </c>
@@ -8505,17 +8854,17 @@
       <c r="H147" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I147" s="1" t="s">
+      <c r="J147" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="J147" s="1" t="s">
+      <c r="K147" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="K147" s="1" t="s">
+      <c r="L147" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A148" s="3" t="s">
         <v>558</v>
       </c>
@@ -8537,17 +8886,17 @@
       <c r="H148" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I148" s="1" t="s">
+      <c r="J148" s="1" t="s">
         <v>668</v>
       </c>
-      <c r="J148" s="1" t="s">
+      <c r="K148" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="K148" s="1" t="s">
+      <c r="L148" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A149" s="3" t="s">
         <v>559</v>
       </c>
@@ -8569,17 +8918,17 @@
       <c r="H149" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I149" s="1" t="s">
+      <c r="J149" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="J149" s="1" t="s">
+      <c r="K149" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="K149" s="1" t="s">
+      <c r="L149" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A150" s="3" t="s">
         <v>560</v>
       </c>
@@ -8601,17 +8950,17 @@
       <c r="H150" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I150" s="1" t="s">
+      <c r="J150" s="1" t="s">
         <v>670</v>
       </c>
-      <c r="J150" s="1" t="s">
+      <c r="K150" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="K150" s="1" t="s">
+      <c r="L150" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A151" s="3" t="s">
         <v>561</v>
       </c>
@@ -8633,17 +8982,17 @@
       <c r="H151" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I151" s="1" t="s">
+      <c r="J151" s="1" t="s">
         <v>671</v>
       </c>
-      <c r="J151" s="1" t="s">
+      <c r="K151" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="K151" s="1" t="s">
+      <c r="L151" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A152" s="3" t="s">
         <v>562</v>
       </c>
@@ -8665,17 +9014,17 @@
       <c r="H152" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I152" s="1" t="s">
+      <c r="J152" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="J152" s="1" t="s">
+      <c r="K152" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="K152" s="1" t="s">
+      <c r="L152" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A153" s="3" t="s">
         <v>563</v>
       </c>
@@ -8697,17 +9046,17 @@
       <c r="H153" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I153" s="1" t="s">
+      <c r="J153" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="J153" s="1" t="s">
+      <c r="K153" s="1" t="s">
         <v>833</v>
       </c>
-      <c r="K153" s="1" t="s">
+      <c r="L153" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A154" s="3" t="s">
         <v>564</v>
       </c>
@@ -8729,17 +9078,17 @@
       <c r="H154" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I154" s="1" t="s">
+      <c r="J154" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="J154" s="1" t="s">
+      <c r="K154" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="K154" s="1" t="s">
+      <c r="L154" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A155" s="3" t="s">
         <v>565</v>
       </c>
@@ -8761,17 +9110,17 @@
       <c r="H155" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I155" s="1" t="s">
+      <c r="J155" s="1" t="s">
         <v>677</v>
       </c>
-      <c r="J155" s="1" t="s">
+      <c r="K155" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="K155" s="1" t="s">
+      <c r="L155" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A156" s="3" t="s">
         <v>566</v>
       </c>
@@ -8793,17 +9142,17 @@
       <c r="H156" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I156" s="1" t="s">
+      <c r="J156" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="J156" s="1" t="s">
+      <c r="K156" s="1" t="s">
         <v>836</v>
       </c>
-      <c r="K156" s="1" t="s">
+      <c r="L156" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A157" s="3" t="s">
         <v>567</v>
       </c>
@@ -8825,17 +9174,17 @@
       <c r="H157" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I157" s="1" t="s">
+      <c r="J157" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="J157" s="1" t="s">
+      <c r="K157" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="K157" s="1" t="s">
+      <c r="L157" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A158" s="3" t="s">
         <v>568</v>
       </c>
@@ -8857,17 +9206,17 @@
       <c r="H158" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I158" s="1" t="s">
+      <c r="J158" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="J158" s="1" t="s">
+      <c r="K158" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="K158" s="1" t="s">
+      <c r="L158" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A159" s="3" t="s">
         <v>569</v>
       </c>
@@ -8889,17 +9238,17 @@
       <c r="H159" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I159" s="1" t="s">
+      <c r="J159" s="1" t="s">
         <v>689</v>
       </c>
-      <c r="J159" s="1" t="s">
+      <c r="K159" s="1" t="s">
         <v>839</v>
       </c>
-      <c r="K159" s="1" t="s">
+      <c r="L159" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A160" s="3" t="s">
         <v>570</v>
       </c>
@@ -8921,17 +9270,17 @@
       <c r="H160" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I160" s="1" t="s">
+      <c r="J160" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="J160" s="1" t="s">
+      <c r="K160" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="K160" s="1" t="s">
+      <c r="L160" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A161" s="3" t="s">
         <v>571</v>
       </c>
@@ -8953,17 +9302,17 @@
       <c r="H161" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I161" s="1" t="s">
+      <c r="J161" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="J161" s="1" t="s">
+      <c r="K161" s="1" t="s">
         <v>841</v>
       </c>
-      <c r="K161" s="1" t="s">
+      <c r="L161" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A162" s="3" t="s">
         <v>572</v>
       </c>
@@ -8985,17 +9334,17 @@
       <c r="H162" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I162" s="1" t="s">
+      <c r="J162" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="J162" s="1" t="s">
+      <c r="K162" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="K162" s="1" t="s">
+      <c r="L162" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A163" s="3" t="s">
         <v>573</v>
       </c>
@@ -9017,17 +9366,17 @@
       <c r="H163" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I163" s="1" t="s">
+      <c r="J163" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="J163" s="1" t="s">
+      <c r="K163" s="1" t="s">
         <v>843</v>
       </c>
-      <c r="K163" s="1" t="s">
+      <c r="L163" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A164" s="3" t="s">
         <v>574</v>
       </c>
@@ -9049,17 +9398,17 @@
       <c r="H164" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I164" s="1" t="s">
+      <c r="J164" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="J164" s="1" t="s">
+      <c r="K164" s="1" t="s">
         <v>844</v>
       </c>
-      <c r="K164" s="1" t="s">
+      <c r="L164" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A165" s="3" t="s">
         <v>575</v>
       </c>
@@ -9081,17 +9430,17 @@
       <c r="H165" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I165" s="1" t="s">
+      <c r="J165" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="J165" s="1" t="s">
+      <c r="K165" s="1" t="s">
         <v>845</v>
       </c>
-      <c r="K165" s="1" t="s">
+      <c r="L165" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A166" s="3" t="s">
         <v>576</v>
       </c>
@@ -9113,17 +9462,17 @@
       <c r="H166" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I166" s="1" t="s">
+      <c r="J166" s="1" t="s">
         <v>695</v>
       </c>
-      <c r="J166" s="1" t="s">
+      <c r="K166" s="1" t="s">
         <v>846</v>
       </c>
-      <c r="K166" s="1" t="s">
+      <c r="L166" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A167" s="3" t="s">
         <v>577</v>
       </c>
@@ -9145,17 +9494,17 @@
       <c r="H167" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I167" s="1" t="s">
+      <c r="J167" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="J167" s="1" t="s">
+      <c r="K167" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="K167" s="1" t="s">
+      <c r="L167" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A168" s="3" t="s">
         <v>578</v>
       </c>
@@ -9177,17 +9526,17 @@
       <c r="H168" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I168" s="1" t="s">
+      <c r="J168" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="J168" s="1" t="s">
+      <c r="K168" s="1" t="s">
         <v>848</v>
       </c>
-      <c r="K168" s="1" t="s">
+      <c r="L168" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A169" s="3" t="s">
         <v>579</v>
       </c>
@@ -9209,17 +9558,17 @@
       <c r="H169" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I169" s="1" t="s">
+      <c r="J169" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="J169" s="1" t="s">
+      <c r="K169" s="1" t="s">
         <v>849</v>
       </c>
-      <c r="K169" s="1" t="s">
+      <c r="L169" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A170" s="3" t="s">
         <v>580</v>
       </c>
@@ -9241,17 +9590,17 @@
       <c r="H170" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I170" s="1" t="s">
+      <c r="J170" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="J170" s="1" t="s">
+      <c r="K170" s="1" t="s">
         <v>850</v>
       </c>
-      <c r="K170" s="1" t="s">
+      <c r="L170" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A171" s="3" t="s">
         <v>581</v>
       </c>
@@ -9273,17 +9622,17 @@
       <c r="H171" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I171" s="1" t="s">
+      <c r="J171" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="J171" s="1" t="s">
+      <c r="K171" s="1" t="s">
         <v>851</v>
       </c>
-      <c r="K171" s="1" t="s">
+      <c r="L171" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A172" s="3" t="s">
         <v>582</v>
       </c>
@@ -9305,17 +9654,17 @@
       <c r="H172" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I172" s="1" t="s">
+      <c r="J172" s="1" t="s">
         <v>701</v>
       </c>
-      <c r="J172" s="1" t="s">
+      <c r="K172" s="1" t="s">
         <v>852</v>
       </c>
-      <c r="K172" s="1" t="s">
+      <c r="L172" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A173" s="3" t="s">
         <v>583</v>
       </c>
@@ -9337,17 +9686,17 @@
       <c r="H173" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I173" s="1" t="s">
+      <c r="J173" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="J173" s="1" t="s">
+      <c r="K173" s="1" t="s">
         <v>853</v>
       </c>
-      <c r="K173" s="1" t="s">
+      <c r="L173" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A174" s="3" t="s">
         <v>584</v>
       </c>
@@ -9369,17 +9718,17 @@
       <c r="H174" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I174" s="1" t="s">
+      <c r="J174" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="J174" s="1" t="s">
+      <c r="K174" s="1" t="s">
         <v>854</v>
       </c>
-      <c r="K174" s="1" t="s">
+      <c r="L174" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A175" s="3" t="s">
         <v>585</v>
       </c>
@@ -9401,17 +9750,17 @@
       <c r="H175" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I175" s="1" t="s">
+      <c r="J175" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="J175" s="1" t="s">
+      <c r="K175" s="1" t="s">
         <v>855</v>
       </c>
-      <c r="K175" s="1" t="s">
+      <c r="L175" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A176" s="3" t="s">
         <v>586</v>
       </c>
@@ -9433,17 +9782,17 @@
       <c r="H176" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I176" s="1" t="s">
+      <c r="J176" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="J176" s="1" t="s">
+      <c r="K176" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="K176" s="1" t="s">
+      <c r="L176" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A177" s="3" t="s">
         <v>587</v>
       </c>
@@ -9465,17 +9814,17 @@
       <c r="H177" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I177" s="1" t="s">
+      <c r="J177" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="J177" s="1" t="s">
+      <c r="K177" s="1" t="s">
         <v>857</v>
       </c>
-      <c r="K177" s="1" t="s">
+      <c r="L177" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A178" s="3" t="s">
         <v>588</v>
       </c>
@@ -9497,17 +9846,17 @@
       <c r="H178" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="I178" s="1" t="s">
+      <c r="J178" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="J178" s="1" t="s">
+      <c r="K178" s="1" t="s">
         <v>858</v>
       </c>
-      <c r="K178" s="1" t="s">
+      <c r="L178" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A179" s="1" t="s">
         <v>710</v>
       </c>
@@ -9530,16 +9879,19 @@
         <v>259</v>
       </c>
       <c r="I179" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J179" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="J179" s="1" t="s">
+      <c r="K179" s="1" t="s">
         <v>913</v>
       </c>
-      <c r="K179" s="1" t="s">
+      <c r="L179" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A180" s="1" t="s">
         <v>711</v>
       </c>
@@ -9562,16 +9914,19 @@
         <v>259</v>
       </c>
       <c r="I180" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J180" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="J180" s="1" t="s">
+      <c r="K180" s="1" t="s">
         <v>914</v>
       </c>
-      <c r="K180" s="1" t="s">
+      <c r="L180" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A181" s="1" t="s">
         <v>712</v>
       </c>
@@ -9594,16 +9949,19 @@
         <v>259</v>
       </c>
       <c r="I181" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J181" s="1" t="s">
         <v>735</v>
       </c>
-      <c r="J181" s="1" t="s">
+      <c r="K181" s="1" t="s">
         <v>915</v>
       </c>
-      <c r="K181" s="1" t="s">
+      <c r="L181" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A182" s="1" t="s">
         <v>713</v>
       </c>
@@ -9626,16 +9984,19 @@
         <v>733</v>
       </c>
       <c r="I182" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J182" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="J182" s="1" t="s">
+      <c r="K182" s="1" t="s">
         <v>916</v>
       </c>
-      <c r="K182" s="1" t="s">
+      <c r="L182" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A183" s="1" t="s">
         <v>924</v>
       </c>
@@ -9655,16 +10016,19 @@
         <v>926</v>
       </c>
       <c r="I183" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J183" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="J183" s="1" t="s">
+      <c r="K183" s="1" t="s">
         <v>928</v>
       </c>
-      <c r="K183" s="1" t="s">
+      <c r="L183" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A184" s="3" t="s">
         <v>930</v>
       </c>
@@ -9684,16 +10048,19 @@
         <v>482</v>
       </c>
       <c r="I184" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J184" s="1" t="s">
         <v>919</v>
       </c>
-      <c r="J184" s="1" t="s">
+      <c r="K184" s="1" t="s">
         <v>929</v>
       </c>
-      <c r="K184" s="1" t="s">
+      <c r="L184" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A185" s="3" t="s">
         <v>956</v>
       </c>
@@ -9713,16 +10080,19 @@
         <v>603</v>
       </c>
       <c r="I185" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J185" s="1" t="s">
         <v>945</v>
       </c>
-      <c r="J185" s="1" t="s">
+      <c r="K185" s="1" t="s">
         <v>931</v>
       </c>
-      <c r="K185" s="1" t="s">
+      <c r="L185" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A186" s="3" t="s">
         <v>932</v>
       </c>
@@ -9745,16 +10115,19 @@
         <v>938</v>
       </c>
       <c r="I186" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J186" s="1" t="s">
         <v>940</v>
       </c>
-      <c r="J186" s="1" t="s">
+      <c r="K186" s="1" t="s">
         <v>942</v>
       </c>
-      <c r="K186" s="1" t="s">
+      <c r="L186" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A187" s="3" t="s">
         <v>933</v>
       </c>
@@ -9777,16 +10150,19 @@
         <v>939</v>
       </c>
       <c r="I187" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J187" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="J187" s="1" t="s">
+      <c r="K187" s="1" t="s">
         <v>943</v>
       </c>
-      <c r="K187" s="1" t="s">
+      <c r="L187" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A188" s="3" t="s">
         <v>948</v>
       </c>
@@ -9806,16 +10182,19 @@
         <v>957</v>
       </c>
       <c r="I188" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J188" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="J188" s="1" t="s">
+      <c r="K188" s="1" t="s">
         <v>959</v>
       </c>
-      <c r="K188" s="1" t="s">
+      <c r="L188" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A189" s="3" t="s">
         <v>949</v>
       </c>
@@ -9835,16 +10214,19 @@
         <v>963</v>
       </c>
       <c r="I189" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J189" s="1" t="s">
         <v>964</v>
       </c>
-      <c r="J189" s="1" t="s">
+      <c r="K189" s="1" t="s">
         <v>960</v>
       </c>
-      <c r="K189" s="1" t="s">
+      <c r="L189" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A190" s="3" t="s">
         <v>950</v>
       </c>
@@ -9864,16 +10246,19 @@
         <v>965</v>
       </c>
       <c r="I190" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J190" s="1" t="s">
         <v>966</v>
       </c>
-      <c r="J190" s="1" t="s">
+      <c r="K190" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="K190" s="1" t="s">
+      <c r="L190" s="1" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A191" s="3" t="s">
         <v>951</v>
       </c>
@@ -9893,24 +10278,30 @@
         <v>967</v>
       </c>
       <c r="I191" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J191" s="1" t="s">
         <v>968</v>
       </c>
-      <c r="J191" s="1" t="s">
+      <c r="K191" s="1" t="s">
         <v>962</v>
       </c>
-      <c r="K191" s="1" t="s">
+      <c r="L191" s="1" t="s">
         <v>415</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K2"/>
+  <autoFilter ref="A1:L2"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>"y,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
       <formula1>"csv_equals,csv_containsAll,string_equals,double_equals,assertNull,justExec,similarity,similarityID,similarityDistance,SQLException"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
+      <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add chinese character data support cases and add some IVFPQ cases
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="1182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="1302">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4123,44 +4123,459 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>vector091</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector091_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_168.csv</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector091, feature, array[1.8621821403503418, 0.2708185911178589, 0.09189905226230621, 0.933274507522583, 0.7153090834617615, 0.7983555793762207, 0.750082790851593, 0.6883314847946167, 0.31263604760169983, 0.4566596448421478, 0.1965976357460022, 0.6520524621009827, 0.7225580811500549, 0.6169158816337585, 0.4757600426673889, 0.8930113315582275, 0.16275887191295624, 0.8677147626876831, 0.38705652952194214, 0.3529115915298462, 0.43060439825057983, 0.03425328806042671, 0.6368623375892639, 0.07757068425416946, 0.26419928669929504, 0.8277255296707153, 0.43137165904045105, 0.08842884749174118, 0.2713584899902344, 0.9682172536849976, 0.7530999183654785, 0.9315038323402405, 0.7047898173332214, 0.724409282207489, 0.6946336627006531, 0.7282527685165405, 0.6133454442024231, 0.16090521216392517, 0.9238371253013611, 0.6565712094306946, 0.8871753215789795, 0.14609310030937195, 0.7698654532432556, 0.7012138962745667, 0.5944278836250305, 0.09350641816854477, 0.5790979266166687, 0.4277772903442383, 0.7462419867515564, 0.9512709379196167, 0.7253237366676331, 0.45405250787734985, 0.5477305054664612, 0.691687285900116, 0.8943620920181274, 0.5033979415893555, 0.486189603805542, 0.7285860180854797, 0.17546194791793823, 0.05633839592337608, 0.2782122492790222, 0.6356047987937927, 0.21174538135528564, 0.4946894347667694], 32, map[nprobe, 2048])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector080_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector080, feature, array[0.010204729624092579, 0.033147819340229034, 0.02332344464957714, 0.04184626042842865, 0.04155944660305977, 0.014524550177156925, 0.014730843715369701, 0.04272615164518356, 0.051052533090114594, 0.046672314405441284, 0.019065575674176216, 0.026694519445300102, 0.036416951566934586, 0.037974897772073746, 0.019728070124983788, 0.02990221418440342, 0.026805777102708817, 0.0007336242124438286, 0.041178517043590546, 0.0470297671854496, 0.01944221742451191, 0.032790154218673706, 0.00401653815060854, 0.019652048125863075, 0.04972049966454506, 0.03470737859606743, 0.021164143458008766, 0.04202590510249138, 0.016881978139281273, 0.03026999905705452, 0.046309709548950195, 0.023240625858306885, 0.0427408292889595, 0.007660326547920704, 0.03752513229846954, 0.037542201578617096, 0.011657899245619774, 0.04927971586585045, 0.023558583110570908, 0.048451077193021774, 0.0031868144869804382, 0.00981936790049076, 0.0025232310872524977, 0.035959675908088684, 0.031683389097452164, 0.028416363522410393, 0.002308435970917344, 0.02991483546793461, 0.01756572164595127, 0.026799578219652176, 0.005962064489722252, 0.032353099435567856, 0.030155226588249207, 0.00036040949635207653, 0.032899145036935806, 0.04860064014792442, 0.04212149232625961, 0.05286107212305069, 0.05108783021569252, 0.042198218405246735, 0.01519902516156435, 0.03329743444919586, 0.025474268943071365, 0.01042615994811058, 0.02037101797759533, 0.002870551310479641, 0.024065179750323296, 0.05232415348291397, 0.006604038178920746, 0.006360971834510565, 0.0393507219851017, 0.031293295323848724, 0.02512999437749386, 0.005708037409931421, 0.012213451787829399, 0.047952838242053986, 0.02220587618649006, 0.028551781550049782, 0.0003308083687443286, 0.01601909101009369, 0.0232789758592844, 0.03261713311076164, 0.048924341797828674, 0.03334112465381622, 0.03761766478419304, 0.007983588613569736, 0.03975249454379082, 0.04427854344248772, 0.03376680612564087, 0.023354463279247284, 0.008129534311592579, 0.03028656728565693, 0.02814537286758423, 0.05069497600197792, 0.02559497579932213, 0.026777878403663635, 0.0286064762622118, 0.04364953935146332, 0.0030432920902967453, 0.03566879406571388, 0.04087426885962486, 0.03773050755262375, 0.04245946928858757, 0.029719168320298195, 0.05146266147494316, 0.007840960286557674, 0.0015796809457242489, 0.03164442256093025, 0.0060777622275054455, 0.05066199600696564, 0.01735466532409191, 0.010316583327949047, 0.02439357526600361, 0.049041807651519775, 0.04683943837881088, 0.013460123911499977, 0.018542950972914696, 0.009728874079883099, 0.04805039241909981, 0.037645936012268066, 0.03871854022145271, 0.047959376126527786, 0.04151618108153343, 0.031924761831760406, 0.015512024983763695, 0.008066792972385883, 0.01785910874605179, 0.035036325454711914, 0.003907910548150539, 0.0029309054370969534, 0.017220787703990936, 0.031462639570236206, 0.04549827426671982, 0.015295546501874924, 0.009221539832651615, 0.007141051348298788, 0.0529981330037117, 0.00956418365240097, 0.016919845715165138, 0.03028026968240738, 0.0004981200327165425, 0.04798925295472145, 0.05207035318017006, 0.02967301569879055, 0.004517004359513521, 0.017743369564414024, 0.03881286084651947, 0.00758938305079937, 0.029437201097607613, 0.014548561535775661, 0.05192401632666588, 0.03558168560266495, 0.013621972873806953, 0.0057711610570549965, 0.04135723412036896, 0.04169277101755142, 0.04058053717017174, 0.04872213676571846, 0.03509339690208435, 0.030284328386187553, 0.010750147514045238, 0.03720732033252716, 0.050735823810100555, 0.04741990938782692, 0.0529402419924736, 0.043622974306344986, 0.029045740142464638, 0.02404416911303997, 0.047451552003622055, 0.051858462393283844, 0.03161873295903206, 0.019505545496940613, 0.01721545308828354, 0.04643204063177109, 0.011489628814160824, 0.03916008025407791, 0.01948128081858158, 0.042711786925792694, 0.041706494987010956, 0.03737031668424606, 0.033183399587869644, 0.02630488947033882, 0.04478636756539345, 0.037942659109830856, 0.023652801290154457, 0.0016536302864551544, 0.019354501739144325, 0.038935042917728424, 0.025339610874652863, 0.018351567909121513, 0.03414802625775337, 0.0067245978862047195, 0.009136182256042957, 0.039274174720048904, 0.006768506485968828, 0.019696053117513657, 0.03220072388648987, 0.005493713542819023, 0.04275289922952652, 0.05038191005587578, 0.05216612294316292, 0.046954695135354996, 0.03344477340579033, 0.049579109996557236, 0.03861898183822632, 0.03818674385547638, 0.0021887891925871372, 0.023416904732584953, 0.015029522590339184, 0.01784958690404892, 0.004450568929314613, 0.04054031893610954, 0.027135562151670456, 0.03522258624434471, 0.033585041761398315, 0.019764091819524765, 0.023803653195500374, 0.022118208929896355, 0.025596538558602333, 0.05239442363381386, 0.019897133111953735, 0.0006610811105929315, 0.04912177100777626, 0.04653076454997063, 0.018742123618721962, 0.033575378358364105, 0.019066091626882553, 0.011339683085680008, 0.011899116449058056, 0.022355616092681885, 0.003884874749928713, 0.03467865660786629, 0.040265221148729324, 0.049665145576000214, 0.020055940374732018, 0.015821173787117004, 0.01981830596923828, 0.044102299958467484, 0.04801541566848755, 0.02276802621781826, 0.00011665943020489067, 0.002236034022644162, 0.00755485612899065, 0.031875867396593094, 0.005672535393387079, 0.015833521261811256, 0.0031113000586628914, 0.03310604766011238, 0.0012084837071597576, 0.045559875667095184, 0.016322564333677292, 0.040430255234241486, 0.030012983828783035, 0.002033502096310258, 0.03013242408633232, 0.03510675206780434, 0.009764980524778366, 0.0424884632229805, 0.03262877091765404, 0.029606876894831657, 0.03354119509458542, 0.03656172752380371, 0.012808301486074924, 0.04198315367102623, 0.045635681599378586, 0.03877915069460869, 0.03689022362232208, 0.025168271735310555, 0.045656755566596985, 0.035419512540102005, 0.01776326820254326, 0.027608344331383705, 0.021030189469456673, 0.001654415624216199, 0.03073575533926487, 0.045303959399461746, 0.0506981760263443, 0.036391157656908035, 0.004058168735355139, 0.021850179880857468, 0.002232631901279092, 0.00928119570016861, 0.030126312747597694, 0.009212159551680088, 0.03019070252776146, 0.02738768421113491, 0.04629604518413544, 0.038382258266210556, 0.04814605414867401, 0.01479215919971466, 0.013675902970135212, 0.03728228434920311, 0.048038288950920105, 0.052414074540138245, 0.03414975479245186, 0.017583781853318214, 0.03232547268271446, 0.04380713403224945, 0.0334598608314991, 0.006283293943852186, 0.015232418663799763, 0.05257684737443924, 0.023007642477750778, 0.030596930533647537, 0.028093036264181137, 0.010531546548008919, 0.008829441852867603, 0.026694271713495255, 0.05276103690266609, 0.0209930632263422, 0.0380447655916214, 0.009372706525027752, 0.0037669038865715265, 0.0083986297249794, 0.008608294650912285, 0.015113032422959805, 0.028597304597496986, 0.04120047390460968, 0.046907342970371246, 0.033962126821279526, 0.04542919993400574, 0.031860850751399994, 0.03697022795677185, 0.028622381389141083, 0.04738084226846695, 0.0027849117759615183, 0.0417303740978241, 0.007735266350209713, 0.00312762800604105, 0.0031434078700840473, 0.002769182901829481, 0.02749328315258026, 0.021579410880804062, 0.053264323621988297, 0.005784935317933559, 0.01744401641190052, 0.05316736549139023, 0.02137257717549801, 0.04706677421927452, 0.030325409024953842, 0.050791528075933456, 0.04717608541250229, 0.04152267053723335, 0.0016948288539424539, 0.051291197538375854, 0.027687732130289078, 0.011071727611124516, 0.04662783071398735, 0.011943462304770947, 0.007388184312731028, 0.038642920553684235, 0.05188639089465141, 0.028532078489661217, 0.0237001683562994, 0.0011781497159972787, 0.032288871705532074, 0.05140724778175354, 0.051556169986724854, 0.049554720520973206, 0.00984029471874237, 0.03319329023361206, 0.022003887221217155, 0.019344987347722054, 0.0019503142684698105, 0.046257562935352325, 0.03585030138492584, 0.004660749342292547, 0.04726020246744156, 0.04169205576181412, 0.01690692827105522, 0.04360220953822136, 0.027044054120779037, 0.001129242591559887, 0.02309933677315712, 0.02378089539706707, 0.012725044041872025, 0.044237978756427765, 0.0396832637488842, 0.031249357387423515, 0.026261474937200546, 0.025967780500650406, 0.014212743379175663, 0.03223680332303047, 0.040151067078113556, 0.014417537488043308, 0.027829883620142937, 0.0052392384968698025, 0.03802470117807388, 0.047104328870773315, 0.030214359983801842, 0.05298895761370659, 0.009523790329694748, 0.0006500571616925299, 0.024350246414542198, 0.0496465340256691, 0.04507872834801674, 0.025220433250069618, 0.04809083417057991, 0.012041718699038029, 0.016206221655011177, 0.038097016513347626, 0.038581762462854385, 0.0009951365645974874, 0.015228977426886559, 0.03093005158007145, 0.049595098942518234, 0.018062768504023552, 0.006398388650268316, 0.027508556842803955, 0.037255845963954926, 0.01591246947646141, 0.04590914025902748, 0.048264119774103165, 0.040952417999506, 0.013919203542172909, 0.05000372231006622, 0.05001368001103401, 0.03969820216298103, 0.048526693135499954, 0.012640043161809444, 0.02637334167957306, 0.043152742087841034, 0.05086212232708931, 0.03396701440215111, 0.04853280261158943, 0.03687911853194237, 0.0022881310433149338, 0.04441600665450096, 0.019711963832378387, 0.04990256205201149, 0.02573850378394127, 0.006678043399006128, 0.05138900503516197, 0.0009071872336789966, 0.03604971617460251, 0.007483062334358692, 0.008275534026324749, 0.034610383212566376, 0.05230547860264778, 0.037021420896053314, 0.0406002514064312, 0.02265641838312149, 0.007400658447295427, 0.0115190539509058, 0.04074552282691002, 0.0029095641802996397, 0.02611522190272808, 0.009627713821828365, 0.03361756354570389, 0.029371827840805054, 0.030215784907341003, 0.04360387101769447, 0.050032056868076324, 0.010278365574777126, 0.03798246383666992, 0.0371883250772953, 0.01376281026750803, 0.04879698529839516, 0.028365638107061386, 0.029730016365647316, 0.017198272049427032, 0.018043262884020805, 0.017706021666526794, 0.052154362201690674, 0.010827913880348206, 0.035541146993637085, 0.03062622807919979, 0.002769398968666792, 0.028924038633704185, 0.011080151423811913, 0.004853557795286179, 0.04634851589798927, 0.001458343816921115, 0.05161121487617493, 0.017450176179409027, 0.021860837936401367, 0.0072222016751766205, 0.006770473904907703, 0.022058306261897087, 0.03289925307035446, 0.007047576829791069, 0.05192327871918678, 0.009624779224395752, 0.040513720363378525, 0.025691024959087372, 0.04092554375529289, 0.016139335930347443, 0.0008085743174888194, 0.024689670652151108, 0.03747590631246567, 0.0035188565962016582, 0.03564693033695221, 0.01840815879404545, 0.031528692692518234, 0.012204653583467007, 0.014256843365728855, 0.04970381408929825, 0.04401948302984238, 0.0077496482990682125, 0.03447428718209267, 0.04709956794977188, 0.03950190916657448, 0.027478614822030067, 0.007206623442471027, 0.0021251202560961246, 0.04445516690611839, 0.006237193942070007, 0.027872459962964058, 0.04651917144656181, 0.0020624694880098104, 0.03689265623688698, 0.02537701092660427, 0.009018919430673122, 0.003365987678989768, 0.0017169961938634515, 0.012917441315948963, 0.006005357019603252, 0.021579081192612648, 0.0022417737636715174, 0.049370184540748596, 0.04983361065387726, 0.043181970715522766, 0.010035483166575432, 0.0312940739095211, 0.04814174771308899, 0.051542893052101135, 0.00359869166277349, 0.016921937465667725, 0.03713094815611839, 0.0341152586042881, 0.03370806574821472, 0.044158317148685455, 0.03799666091799736, 0.017875390127301216, 0.008935274556279182, 0.04074496403336525, 0.019145382568240166, 0.004689158406108618, 0.038873545825481415, 0.04694497957825661, 0.002198663307353854, 0.00931747816503048, 0.022384047508239746, 0.01814853772521019, 0.0023854218889027834, 0.006015187595039606, 0.02334016188979149, 0.0037869932129979134, 0.04349198192358017, 0.04614923521876335, 0.006986458320170641, 0.010295310989022255, 0.02331092394888401, 0.05173381045460701, 0.04123363271355629, 0.007021444849669933, 0.04940291866660118, 0.044107481837272644, 0.020925918594002724, 0.0074900249019265175, 0.0027779804076999426, 0.004940895829349756, 0.04726146534085274, 0.00895958673208952, 0.019335685297846794, 0.03486210107803345, 0.03222672641277313, 0.02104640193283558, 0.01996009610593319, 0.0033607061486691236, 0.022856222465634346, 0.038348883390426636, 0.04092298448085785, 0.01035651657730341, 0.04597633704543114, 0.0015303916297852993, 0.048068124800920486, 0.012603872455656528, 0.006851354613900185, 0.01693737506866455, 0.045224543660879135, 0.04434731602668762, 0.018417339771986008, 0.012786383740603924, 0.02854836732149124, 0.01446457114070654, 0.0018345799762755632, 0.03341299667954445, 0.02771783620119095, 0.0022355313412845135, 0.04036041721701622, 0.052662234753370285, 0.04270104318857193, 0.018328342586755753, 0.017870649695396423, 0.01873277686536312, 0.0236014723777771, 0.030877146869897842, 0.032905496656894684, 0.009437349624931812, 0.046088818460702896, 0.03784535080194473, 0.009091767482459545, 0.04556136205792427, 0.0010580202797427773, 0.034190833568573, 0.008649660274386406, 0.013723060488700867, 0.018255097791552544, 0.00032737827859818935, 0.02336731366813183, 0.04246889799833298, 0.036001451313495636, 0.029040461406111717, 0.030063703656196594, 0.0007451173732988536, 0.03244812414050102, 0.05267377942800522, 0.0119410939514637, 0.031288716942071915, 0.0444943904876709, 0.042226642370224, 0.01754225231707096, 0.01903282292187214, 0.051157694309949875, 0.0119244996458292, 0.011271309107542038, 0.008201060816645622, 0.026422815397381783, 0.013922568410634995, 0.02960863709449768, 0.0038851830177009106, 0.02016851119697094, 0.02456820383667946, 0.041482966393232346, 0.038387347012758255, 0.01231926679611206, 0.0013077986659482121, 0.013713174499571323, 0.02185221016407013, 0.00044752363464795053, 0.025125540792942047, 0.0454196035861969, 0.04918977990746498, 0.012331610545516014, 0.05280104652047157, 0.00031958590261638165, 0.01786315254867077, 0.042054034769535065, 0.005248988512903452, 0.023568786680698395, 0.020283201709389687, 0.04436333850026131, 0.03793547675013542, 0.018915507942438126, 0.0013126976555213332, 0.0369524210691452, 0.022443432360887527, 0.0457354299724102, 0.030641639605164528, 0.050089336931705475, 0.046902649104595184, 0.024411339312791824, 0.0009223322849720716, 0.0036581249441951513, 0.017082955688238144, 0.031559620052576065, 0.032505422830581665, 0.027303671464323997, 0.007713057100772858, 0.04671899229288101, 0.039335381239652634, 0.01989162713289261, 0.04415488988161087, 0.004808233119547367, 0.0034102832432836294, 0.026955703273415565, 0.04973577335476875, 0.00793713703751564, 0.030343536287546158, 0.003183587221428752, 0.009019634686410427, 0.0036780377849936485, 0.04827558994293213, 0.023839347064495087, 0.005668522324413061, 0.03544703498482704, 0.02676263079047203, 0.02180374227464199, 0.03878967463970184, 0.009169492870569229, 0.020485227927565575, 0.014226621016860008, 0.016422931104898453, 0.00944722443819046, 0.025712162256240845, 0.033553216606378555, 0.0031731794588267803, 0.010490743443369865, 0.014877060428261757, 0.03771480172872543, 0.017446402460336685, 0.022660940885543823, 0.0375521257519722, 0.008476108312606812, 0.023412754759192467, 0.03353258594870567, 0.04928986728191376, 0.01902138814330101, 0.04364588484168053, 0.0341087244451046, 0.03810013830661774, 0.03934536129236221, 0.051737766712903976, 0.013110239990055561, 0.0022688740864396095, 0.013203381560742855, 0.0023986210580915213, 0.03758910670876503, 0.044475678354501724, 0.049773555248975754, 0.02508527971804142, 0.027300048619508743, 0.014012387953698635, 0.005269512999802828, 0.04256492480635643, 0.007608959451317787, 0.04292828589677811, 0.04686378315091133, 0.02663724310696125, 0.04871407896280289, 0.021974576637148857, 0.010676505044102669, 0.03429139405488968, 0.021306011825799942, 0.03272809460759163, 0.02330126240849495, 0.031602345407009125, 0.05069557577371597, 0.02947191335260868, 0.048153724521398544, 0.007379948161542416, 8.225629426306114e-05, 0.032653648406267166, 0.028863554820418358, 0.04159433767199516, 0.0437716580927372, 0.05080052465200424, 0.032500285655260086, 0.01545642875134945, 0.04405480623245239, 0.020035305991768837, 0.03245877847075462, 0.03303660824894905, 0.023524440824985504, 0.01059116143733263, 0.023655179888010025, 0.049274373799562454, 0.035776033997535706, 0.004343794658780098, 0.03051299974322319, 0.006429243367165327, 0.053281061351299286, 0.05314341187477112, 0.03701634332537651, 0.01992143876850605, 0.02139369584619999, 0.04929206892848015, 0.013046812266111374, 0.03538058325648308, 0.025640882551670074, 0.0018618974136188626, 0.005908842198550701, 0.04770796000957489, 0.04753381758928299, 0.04876251891255379, 0.016379280015826225, 0.015900691971182823, 0.03512691333889961, 0.03171072155237198, 0.05245013162493706, 0.03280219808220863, 0.008243748918175697, 0.044303182512521744, 0.043462783098220825, 0.004904266446828842, 0.04730410501360893, 0.0008759222109802067, 0.04603278264403343, 0.04788919538259506, 0.04531008005142212, 0.03478683531284332, 0.01751706376671791, 0.02905944548547268, 0.01267789863049984, 0.046451300382614136, 0.009416903369128704, 0.019748589023947716, 0.04047293961048126, 0.016314394772052765, 0.03282974287867546, 0.011684490367770195, 0.04649067297577858, 0.03452018275856972, 0.02520301379263401, 0.012478360906243324, 0.04442852362990379, 0.005249244626611471, 0.0109244454652071, 0.012507148087024689, 0.03180855140089989, 0.033486634492874146, 0.05235859006643295, 0.00939468014985323, 0.04262519255280495, 0.008272930979728699, 0.019234731793403625, 0.0508892685174942, 0.006935227662324905, 0.014538083225488663, 0.043112222105264664, 0.05145309865474701, 0.0049245296977460384, 0.031086592003703117, 0.02160232700407505, 0.04791868478059769, 0.004517515655606985, 0.009651483036577702, 0.002699608216062188, 0.016053033992648125, 0.010133565403521061, 0.00045852080802433193, 0.006794801913201809, 0.006013770587742329, 0.038918670266866684, 0.012754619121551514, 0.04803835600614548, 0.01750420592725277, 0.04657161608338356, 0.012603000737726688, 0.02016519382596016, 0.02889486588537693, 0.027483047917485237, 0.022048616781830788, 0.020719977095723152, 0.018133845180273056, 0.021432265639305115, 0.024356184527277946, 0.02040690928697586, 0.03506499156355858, 0.046953730285167694, 0.030513711273670197, 0.022807275876402855, 0.013767150230705738, 0.04610414430499077, 0.009232786484062672, 0.030901623889803886, 0.038756851106882095, 0.03891802579164505, 0.02152610756456852, 0.006283528637140989, 0.040686607360839844, 0.028435060754418373, 0.03847217932343483, 0.0318436399102211, 0.02253156527876854, 0.04973893612623215, 0.05296175181865692, 0.02919049561023712, 0.03890908509492874, 0.001491086557507515, 0.046014729887247086, 0.05321003869175911, 0.017333481460809708, 0.045304443687200546, 0.032582130283117294, 0.023503826931118965, 0.028091037645936012, 0.04155117645859718, 0.013392691500484943, 0.024664288386702538, 0.045140642672777176, 0.03612712770700455, 0.019600804895162582, 0.007352148182690144, 0.02146289311349392, 0.049622297286987305, 0.03586812689900398, 0.022337820380926132, 0.030300261452794075, 0.0022224702406674623, 0.05305036902427673, 0.03298239782452583, 0.04153228923678398, 0.04962451010942459, 0.018202459439635277, 0.043228451162576675, 0.046500593423843384, 0.03548584505915642, 0.0313723087310791, 0.047600485384464264, 0.02390190027654171, 0.013021488673985004, 0.043381575495004654, 0.03714620694518089, 0.02182495780289173, 0.00030451681232079864, 0.05083274096250534, 0.03224967420101166, 0.00034880521707236767, 0.026561226695775986, 0.03189708665013313, 0.015992755070328712, 0.024603823199868202, 0.026407040655612946, 0.0312056727707386, 0.04633691534399986, 0.04434354230761528, 0.04148416966199875, 0.0292221587151289, 0.03268655762076378, 0.03912409022450447, 0.03017784282565117, 0.04130551964044571, 0.052566103637218475, 0.04205124080181122, 0.03273366019129753, 0.008433874696493149, 0.02538328990340233, 0.015113677829504013, 0.008195578120648861, 0.041412632912397385, 0.003141732420772314, 0.004215883556753397, 0.03539261221885681, 0.02788538858294487, 0.023785896599292755, 0.01634884439408779, 0.0009210030548274517, 0.01563998870551586, 0.014268863946199417, 0.0019568500574678183, 0.04284163936972618, 0.01778584159910679, 0.047522395849227905, 0.043178047984838486, 0.051370199769735336, 0.05102987587451935, 0.031499069184064865, 0.01659782975912094, 0.048936206847429276, 0.00269880797713995, 0.012028246186673641, 0.019326066598296165, 0.021966218948364258, 0.05033225193619728, 0.030871236696839333, 0.009951140731573105, 0.03178248926997185, 0.049753330647945404, 0.007147281430661678, 0.05233900994062424, 0.008198955096304417, 0.043730851262807846, 0.03610117360949516, 0.021531086415052414, 0.011577704921364784, 0.04121891036629677, 0.04516777768731117, 0.028223982080817223, 0.021824698895215988, 0.0009755022474564612, 0.007921029813587666, 0.04285738617181778, 0.02236703597009182, 0.018074527382850647, 0.015832820907235146, 0.0382564440369606, 0.05316615477204323, 0.02940700761973858, 0.0474163256585598, 0.008976494893431664, 0.04707895219326019, 0.03744599223136902, 0.0224912129342556, 0.046000003814697266, 0.012523806653916836, 0.030038325116038322, 0.0014152097282931209, 0.02025027945637703, 0.019279656931757927, 0.00486172828823328, 0.002411243738606572, 0.018246842548251152, 0.018937520682811737, 0.053061243146657944, 0.05031004548072815, 0.00698775053024292, 0.027619510889053345, 0.02542906254529953, 0.021372150629758835, 0.04958592355251312, 0.02745865285396576, 0.04313695430755615, 0.04698346555233002, 0.04063722491264343, 0.024745726957917213, 0.003938657697290182, 0.025069614872336388, 0.010687075555324554, 0.01111308578401804, 0.00945984199643135, 0.01887504570186138, 0.04858093708753586, 0.023099292069673538, 0.009500138461589813, 0.04007745906710625, 0.0026892228052020073, 0.004404826555401087, 0.002055841265246272, 0.02479143626987934, 0.032173801213502884, 0.00968628004193306, 0.027655456215143204], 1, map[nprobe, 16])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector080, feature, array[0.010204729624092579, 0.033147819340229034, 0.02332344464957714, 0.04184626042842865, 0.04155944660305977, 0.014524550177156925, 0.014730843715369701, 0.04272615164518356, 0.051052533090114594, 0.046672314405441284, 0.019065575674176216, 0.026694519445300102, 0.036416951566934586, 0.037974897772073746, 0.019728070124983788, 0.02990221418440342, 0.026805777102708817, 0.0007336242124438286, 0.041178517043590546, 0.0470297671854496, 0.01944221742451191, 0.032790154218673706, 0.00401653815060854, 0.019652048125863075, 0.04972049966454506, 0.03470737859606743, 0.021164143458008766, 0.04202590510249138, 0.016881978139281273, 0.03026999905705452, 0.046309709548950195, 0.023240625858306885, 0.0427408292889595, 0.007660326547920704, 0.03752513229846954, 0.037542201578617096, 0.011657899245619774, 0.04927971586585045, 0.023558583110570908, 0.048451077193021774, 0.0031868144869804382, 0.00981936790049076, 0.0025232310872524977, 0.035959675908088684, 0.031683389097452164, 0.028416363522410393, 0.002308435970917344, 0.02991483546793461, 0.01756572164595127, 0.026799578219652176, 0.005962064489722252, 0.032353099435567856, 0.030155226588249207, 0.00036040949635207653, 0.032899145036935806, 0.04860064014792442, 0.04212149232625961, 0.05286107212305069, 0.05108783021569252, 0.042198218405246735, 0.01519902516156435, 0.03329743444919586, 0.025474268943071365, 0.01042615994811058, 0.02037101797759533, 0.002870551310479641, 0.024065179750323296, 0.05232415348291397, 0.006604038178920746, 0.006360971834510565, 0.0393507219851017, 0.031293295323848724, 0.02512999437749386, 0.005708037409931421, 0.012213451787829399, 0.047952838242053986, 0.02220587618649006, 0.028551781550049782, 0.0003308083687443286, 0.01601909101009369, 0.0232789758592844, 0.03261713311076164, 0.048924341797828674, 0.03334112465381622, 0.03761766478419304, 0.007983588613569736, 0.03975249454379082, 0.04427854344248772, 0.03376680612564087, 0.023354463279247284, 0.008129534311592579, 0.03028656728565693, 0.02814537286758423, 0.05069497600197792, 0.02559497579932213, 0.026777878403663635, 0.0286064762622118, 0.04364953935146332, 0.0030432920902967453, 0.03566879406571388, 0.04087426885962486, 0.03773050755262375, 0.04245946928858757, 0.029719168320298195, 0.05146266147494316, 0.007840960286557674, 0.0015796809457242489, 0.03164442256093025, 0.0060777622275054455, 0.05066199600696564, 0.01735466532409191, 0.010316583327949047, 0.02439357526600361, 0.049041807651519775, 0.04683943837881088, 0.013460123911499977, 0.018542950972914696, 0.009728874079883099, 0.04805039241909981, 0.037645936012268066, 0.03871854022145271, 0.047959376126527786, 0.04151618108153343, 0.031924761831760406, 0.015512024983763695, 0.008066792972385883, 0.01785910874605179, 0.035036325454711914, 0.003907910548150539, 0.0029309054370969534, 0.017220787703990936, 0.031462639570236206, 0.04549827426671982, 0.015295546501874924, 0.009221539832651615, 0.007141051348298788, 0.0529981330037117, 0.00956418365240097, 0.016919845715165138, 0.03028026968240738, 0.0004981200327165425, 0.04798925295472145, 0.05207035318017006, 0.02967301569879055, 0.004517004359513521, 0.017743369564414024, 0.03881286084651947, 0.00758938305079937, 0.029437201097607613, 0.014548561535775661, 0.05192401632666588, 0.03558168560266495, 0.013621972873806953, 0.0057711610570549965, 0.04135723412036896, 0.04169277101755142, 0.04058053717017174, 0.04872213676571846, 0.03509339690208435, 0.030284328386187553, 0.010750147514045238, 0.03720732033252716, 0.050735823810100555, 0.04741990938782692, 0.0529402419924736, 0.043622974306344986, 0.029045740142464638, 0.02404416911303997, 0.047451552003622055, 0.051858462393283844, 0.03161873295903206, 0.019505545496940613, 0.01721545308828354, 0.04643204063177109, 0.011489628814160824, 0.03916008025407791, 0.01948128081858158, 0.042711786925792694, 0.041706494987010956, 0.03737031668424606, 0.033183399587869644, 0.02630488947033882, 0.04478636756539345, 0.037942659109830856, 0.023652801290154457, 0.0016536302864551544, 0.019354501739144325, 0.038935042917728424, 0.025339610874652863, 0.018351567909121513, 0.03414802625775337, 0.0067245978862047195, 0.009136182256042957, 0.039274174720048904, 0.006768506485968828, 0.019696053117513657, 0.03220072388648987, 0.005493713542819023, 0.04275289922952652, 0.05038191005587578, 0.05216612294316292, 0.046954695135354996, 0.03344477340579033, 0.049579109996557236, 0.03861898183822632, 0.03818674385547638, 0.0021887891925871372, 0.023416904732584953, 0.015029522590339184, 0.01784958690404892, 0.004450568929314613, 0.04054031893610954, 0.027135562151670456, 0.03522258624434471, 0.033585041761398315, 0.019764091819524765, 0.023803653195500374, 0.022118208929896355, 0.025596538558602333, 0.05239442363381386, 0.019897133111953735, 0.0006610811105929315, 0.04912177100777626, 0.04653076454997063, 0.018742123618721962, 0.033575378358364105, 0.019066091626882553, 0.011339683085680008, 0.011899116449058056, 0.022355616092681885, 0.003884874749928713, 0.03467865660786629, 0.040265221148729324, 0.049665145576000214, 0.020055940374732018, 0.015821173787117004, 0.01981830596923828, 0.044102299958467484, 0.04801541566848755, 0.02276802621781826, 0.00011665943020489067, 0.002236034022644162, 0.00755485612899065, 0.031875867396593094, 0.005672535393387079, 0.015833521261811256, 0.0031113000586628914, 0.03310604766011238, 0.0012084837071597576, 0.045559875667095184, 0.016322564333677292, 0.040430255234241486, 0.030012983828783035, 0.002033502096310258, 0.03013242408633232, 0.03510675206780434, 0.009764980524778366, 0.0424884632229805, 0.03262877091765404, 0.029606876894831657, 0.03354119509458542, 0.03656172752380371, 0.012808301486074924, 0.04198315367102623, 0.045635681599378586, 0.03877915069460869, 0.03689022362232208, 0.025168271735310555, 0.045656755566596985, 0.035419512540102005, 0.01776326820254326, 0.027608344331383705, 0.021030189469456673, 0.001654415624216199, 0.03073575533926487, 0.045303959399461746, 0.0506981760263443, 0.036391157656908035, 0.004058168735355139, 0.021850179880857468, 0.002232631901279092, 0.00928119570016861, 0.030126312747597694, 0.009212159551680088, 0.03019070252776146, 0.02738768421113491, 0.04629604518413544, 0.038382258266210556, 0.04814605414867401, 0.01479215919971466, 0.013675902970135212, 0.03728228434920311, 0.048038288950920105, 0.052414074540138245, 0.03414975479245186, 0.017583781853318214, 0.03232547268271446, 0.04380713403224945, 0.0334598608314991, 0.006283293943852186, 0.015232418663799763, 0.05257684737443924, 0.023007642477750778, 0.030596930533647537, 0.028093036264181137, 0.010531546548008919, 0.008829441852867603, 0.026694271713495255, 0.05276103690266609, 0.0209930632263422, 0.0380447655916214, 0.009372706525027752, 0.0037669038865715265, 0.0083986297249794, 0.008608294650912285, 0.015113032422959805, 0.028597304597496986, 0.04120047390460968, 0.046907342970371246, 0.033962126821279526, 0.04542919993400574, 0.031860850751399994, 0.03697022795677185, 0.028622381389141083, 0.04738084226846695, 0.0027849117759615183, 0.0417303740978241, 0.007735266350209713, 0.00312762800604105, 0.0031434078700840473, 0.002769182901829481, 0.02749328315258026, 0.021579410880804062, 0.053264323621988297, 0.005784935317933559, 0.01744401641190052, 0.05316736549139023, 0.02137257717549801, 0.04706677421927452, 0.030325409024953842, 0.050791528075933456, 0.04717608541250229, 0.04152267053723335, 0.0016948288539424539, 0.051291197538375854, 0.027687732130289078, 0.011071727611124516, 0.04662783071398735, 0.011943462304770947, 0.007388184312731028, 0.038642920553684235, 0.05188639089465141, 0.028532078489661217, 0.0237001683562994, 0.0011781497159972787, 0.032288871705532074, 0.05140724778175354, 0.051556169986724854, 0.049554720520973206, 0.00984029471874237, 0.03319329023361206, 0.022003887221217155, 0.019344987347722054, 0.0019503142684698105, 0.046257562935352325, 0.03585030138492584, 0.004660749342292547, 0.04726020246744156, 0.04169205576181412, 0.01690692827105522, 0.04360220953822136, 0.027044054120779037, 0.001129242591559887, 0.02309933677315712, 0.02378089539706707, 0.012725044041872025, 0.044237978756427765, 0.0396832637488842, 0.031249357387423515, 0.026261474937200546, 0.025967780500650406, 0.014212743379175663, 0.03223680332303047, 0.040151067078113556, 0.014417537488043308, 0.027829883620142937, 0.0052392384968698025, 0.03802470117807388, 0.047104328870773315, 0.030214359983801842, 0.05298895761370659, 0.009523790329694748, 0.0006500571616925299, 0.024350246414542198, 0.0496465340256691, 0.04507872834801674, 0.025220433250069618, 0.04809083417057991, 0.012041718699038029, 0.016206221655011177, 0.038097016513347626, 0.038581762462854385, 0.0009951365645974874, 0.015228977426886559, 0.03093005158007145, 0.049595098942518234, 0.018062768504023552, 0.006398388650268316, 0.027508556842803955, 0.037255845963954926, 0.01591246947646141, 0.04590914025902748, 0.048264119774103165, 0.040952417999506, 0.013919203542172909, 0.05000372231006622, 0.05001368001103401, 0.03969820216298103, 0.048526693135499954, 0.012640043161809444, 0.02637334167957306, 0.043152742087841034, 0.05086212232708931, 0.03396701440215111, 0.04853280261158943, 0.03687911853194237, 0.0022881310433149338, 0.04441600665450096, 0.019711963832378387, 0.04990256205201149, 0.02573850378394127, 0.006678043399006128, 0.05138900503516197, 0.0009071872336789966, 0.03604971617460251, 0.007483062334358692, 0.008275534026324749, 0.034610383212566376, 0.05230547860264778, 0.037021420896053314, 0.0406002514064312, 0.02265641838312149, 0.007400658447295427, 0.0115190539509058, 0.04074552282691002, 0.0029095641802996397, 0.02611522190272808, 0.009627713821828365, 0.03361756354570389, 0.029371827840805054, 0.030215784907341003, 0.04360387101769447, 0.050032056868076324, 0.010278365574777126, 0.03798246383666992, 0.0371883250772953, 0.01376281026750803, 0.04879698529839516, 0.028365638107061386, 0.029730016365647316, 0.017198272049427032, 0.018043262884020805, 0.017706021666526794, 0.052154362201690674, 0.010827913880348206, 0.035541146993637085, 0.03062622807919979, 0.002769398968666792, 0.028924038633704185, 0.011080151423811913, 0.004853557795286179, 0.04634851589798927, 0.001458343816921115, 0.05161121487617493, 0.017450176179409027, 0.021860837936401367, 0.0072222016751766205, 0.006770473904907703, 0.022058306261897087, 0.03289925307035446, 0.007047576829791069, 0.05192327871918678, 0.009624779224395752, 0.040513720363378525, 0.025691024959087372, 0.04092554375529289, 0.016139335930347443, 0.0008085743174888194, 0.024689670652151108, 0.03747590631246567, 0.0035188565962016582, 0.03564693033695221, 0.01840815879404545, 0.031528692692518234, 0.012204653583467007, 0.014256843365728855, 0.04970381408929825, 0.04401948302984238, 0.0077496482990682125, 0.03447428718209267, 0.04709956794977188, 0.03950190916657448, 0.027478614822030067, 0.007206623442471027, 0.0021251202560961246, 0.04445516690611839, 0.006237193942070007, 0.027872459962964058, 0.04651917144656181, 0.0020624694880098104, 0.03689265623688698, 0.02537701092660427, 0.009018919430673122, 0.003365987678989768, 0.0017169961938634515, 0.012917441315948963, 0.006005357019603252, 0.021579081192612648, 0.0022417737636715174, 0.049370184540748596, 0.04983361065387726, 0.043181970715522766, 0.010035483166575432, 0.0312940739095211, 0.04814174771308899, 0.051542893052101135, 0.00359869166277349, 0.016921937465667725, 0.03713094815611839, 0.0341152586042881, 0.03370806574821472, 0.044158317148685455, 0.03799666091799736, 0.017875390127301216, 0.008935274556279182, 0.04074496403336525, 0.019145382568240166, 0.004689158406108618, 0.038873545825481415, 0.04694497957825661, 0.002198663307353854, 0.00931747816503048, 0.022384047508239746, 0.01814853772521019, 0.0023854218889027834, 0.006015187595039606, 0.02334016188979149, 0.0037869932129979134, 0.04349198192358017, 0.04614923521876335, 0.006986458320170641, 0.010295310989022255, 0.02331092394888401, 0.05173381045460701, 0.04123363271355629, 0.007021444849669933, 0.04940291866660118, 0.044107481837272644, 0.020925918594002724, 0.0074900249019265175, 0.0027779804076999426, 0.004940895829349756, 0.04726146534085274, 0.00895958673208952, 0.019335685297846794, 0.03486210107803345, 0.03222672641277313, 0.02104640193283558, 0.01996009610593319, 0.0033607061486691236, 0.022856222465634346, 0.038348883390426636, 0.04092298448085785, 0.01035651657730341, 0.04597633704543114, 0.0015303916297852993, 0.048068124800920486, 0.012603872455656528, 0.006851354613900185, 0.01693737506866455, 0.045224543660879135, 0.04434731602668762, 0.018417339771986008, 0.012786383740603924, 0.02854836732149124, 0.01446457114070654, 0.0018345799762755632, 0.03341299667954445, 0.02771783620119095, 0.0022355313412845135, 0.04036041721701622, 0.052662234753370285, 0.04270104318857193, 0.018328342586755753, 0.017870649695396423, 0.01873277686536312, 0.0236014723777771, 0.030877146869897842, 0.032905496656894684, 0.009437349624931812, 0.046088818460702896, 0.03784535080194473, 0.009091767482459545, 0.04556136205792427, 0.0010580202797427773, 0.034190833568573, 0.008649660274386406, 0.013723060488700867, 0.018255097791552544, 0.00032737827859818935, 0.02336731366813183, 0.04246889799833298, 0.036001451313495636, 0.029040461406111717, 0.030063703656196594, 0.0007451173732988536, 0.03244812414050102, 0.05267377942800522, 0.0119410939514637, 0.031288716942071915, 0.0444943904876709, 0.042226642370224, 0.01754225231707096, 0.01903282292187214, 0.051157694309949875, 0.0119244996458292, 0.011271309107542038, 0.008201060816645622, 0.026422815397381783, 0.013922568410634995, 0.02960863709449768, 0.0038851830177009106, 0.02016851119697094, 0.02456820383667946, 0.041482966393232346, 0.038387347012758255, 0.01231926679611206, 0.0013077986659482121, 0.013713174499571323, 0.02185221016407013, 0.00044752363464795053, 0.025125540792942047, 0.0454196035861969, 0.04918977990746498, 0.012331610545516014, 0.05280104652047157, 0.00031958590261638165, 0.01786315254867077, 0.042054034769535065, 0.005248988512903452, 0.023568786680698395, 0.020283201709389687, 0.04436333850026131, 0.03793547675013542, 0.018915507942438126, 0.0013126976555213332, 0.0369524210691452, 0.022443432360887527, 0.0457354299724102, 0.030641639605164528, 0.050089336931705475, 0.046902649104595184, 0.024411339312791824, 0.0009223322849720716, 0.0036581249441951513, 0.017082955688238144, 0.031559620052576065, 0.032505422830581665, 0.027303671464323997, 0.007713057100772858, 0.04671899229288101, 0.039335381239652634, 0.01989162713289261, 0.04415488988161087, 0.004808233119547367, 0.0034102832432836294, 0.026955703273415565, 0.04973577335476875, 0.00793713703751564, 0.030343536287546158, 0.003183587221428752, 0.009019634686410427, 0.0036780377849936485, 0.04827558994293213, 0.023839347064495087, 0.005668522324413061, 0.03544703498482704, 0.02676263079047203, 0.02180374227464199, 0.03878967463970184, 0.009169492870569229, 0.020485227927565575, 0.014226621016860008, 0.016422931104898453, 0.00944722443819046, 0.025712162256240845, 0.033553216606378555, 0.0031731794588267803, 0.010490743443369865, 0.014877060428261757, 0.03771480172872543, 0.017446402460336685, 0.022660940885543823, 0.0375521257519722, 0.008476108312606812, 0.023412754759192467, 0.03353258594870567, 0.04928986728191376, 0.01902138814330101, 0.04364588484168053, 0.0341087244451046, 0.03810013830661774, 0.03934536129236221, 0.051737766712903976, 0.013110239990055561, 0.0022688740864396095, 0.013203381560742855, 0.0023986210580915213, 0.03758910670876503, 0.044475678354501724, 0.049773555248975754, 0.02508527971804142, 0.027300048619508743, 0.014012387953698635, 0.005269512999802828, 0.04256492480635643, 0.007608959451317787, 0.04292828589677811, 0.04686378315091133, 0.02663724310696125, 0.04871407896280289, 0.021974576637148857, 0.010676505044102669, 0.03429139405488968, 0.021306011825799942, 0.03272809460759163, 0.02330126240849495, 0.031602345407009125, 0.05069557577371597, 0.02947191335260868, 0.048153724521398544, 0.007379948161542416, 8.225629426306114e-05, 0.032653648406267166, 0.028863554820418358, 0.04159433767199516, 0.0437716580927372, 0.05080052465200424, 0.032500285655260086, 0.01545642875134945, 0.04405480623245239, 0.020035305991768837, 0.03245877847075462, 0.03303660824894905, 0.023524440824985504, 0.01059116143733263, 0.023655179888010025, 0.049274373799562454, 0.035776033997535706, 0.004343794658780098, 0.03051299974322319, 0.006429243367165327, 0.053281061351299286, 0.05314341187477112, 0.03701634332537651, 0.01992143876850605, 0.02139369584619999, 0.04929206892848015, 0.013046812266111374, 0.03538058325648308, 0.025640882551670074, 0.0018618974136188626, 0.005908842198550701, 0.04770796000957489, 0.04753381758928299, 0.04876251891255379, 0.016379280015826225, 0.015900691971182823, 0.03512691333889961, 0.03171072155237198, 0.05245013162493706, 0.03280219808220863, 0.008243748918175697, 0.044303182512521744, 0.043462783098220825, 0.004904266446828842, 0.04730410501360893, 0.0008759222109802067, 0.04603278264403343, 0.04788919538259506, 0.04531008005142212, 0.03478683531284332, 0.01751706376671791, 0.02905944548547268, 0.01267789863049984, 0.046451300382614136, 0.009416903369128704, 0.019748589023947716, 0.04047293961048126, 0.016314394772052765, 0.03282974287867546, 0.011684490367770195, 0.04649067297577858, 0.03452018275856972, 0.02520301379263401, 0.012478360906243324, 0.04442852362990379, 0.005249244626611471, 0.0109244454652071, 0.012507148087024689, 0.03180855140089989, 0.033486634492874146, 0.05235859006643295, 0.00939468014985323, 0.04262519255280495, 0.008272930979728699, 0.019234731793403625, 0.0508892685174942, 0.006935227662324905, 0.014538083225488663, 0.043112222105264664, 0.05145309865474701, 0.0049245296977460384, 0.031086592003703117, 0.02160232700407505, 0.04791868478059769, 0.004517515655606985, 0.009651483036577702, 0.002699608216062188, 0.016053033992648125, 0.010133565403521061, 0.00045852080802433193, 0.006794801913201809, 0.006013770587742329, 0.038918670266866684, 0.012754619121551514, 0.04803835600614548, 0.01750420592725277, 0.04657161608338356, 0.012603000737726688, 0.02016519382596016, 0.02889486588537693, 0.027483047917485237, 0.022048616781830788, 0.020719977095723152, 0.018133845180273056, 0.021432265639305115, 0.024356184527277946, 0.02040690928697586, 0.03506499156355858, 0.046953730285167694, 0.030513711273670197, 0.022807275876402855, 0.013767150230705738, 0.04610414430499077, 0.009232786484062672, 0.030901623889803886, 0.038756851106882095, 0.03891802579164505, 0.02152610756456852, 0.006283528637140989, 0.040686607360839844, 0.028435060754418373, 0.03847217932343483, 0.0318436399102211, 0.02253156527876854, 0.04973893612623215, 0.05296175181865692, 0.02919049561023712, 0.03890908509492874, 0.001491086557507515, 0.046014729887247086, 0.05321003869175911, 0.017333481460809708, 0.045304443687200546, 0.032582130283117294, 0.023503826931118965, 0.028091037645936012, 0.04155117645859718, 0.013392691500484943, 0.024664288386702538, 0.045140642672777176, 0.03612712770700455, 0.019600804895162582, 0.007352148182690144, 0.02146289311349392, 0.049622297286987305, 0.03586812689900398, 0.022337820380926132, 0.030300261452794075, 0.0022224702406674623, 0.05305036902427673, 0.03298239782452583, 0.04153228923678398, 0.04962451010942459, 0.018202459439635277, 0.043228451162576675, 0.046500593423843384, 0.03548584505915642, 0.0313723087310791, 0.047600485384464264, 0.02390190027654171, 0.013021488673985004, 0.043381575495004654, 0.03714620694518089, 0.02182495780289173, 0.00030451681232079864, 0.05083274096250534, 0.03224967420101166, 0.00034880521707236767, 0.026561226695775986, 0.03189708665013313, 0.015992755070328712, 0.024603823199868202, 0.026407040655612946, 0.0312056727707386, 0.04633691534399986, 0.04434354230761528, 0.04148416966199875, 0.0292221587151289, 0.03268655762076378, 0.03912409022450447, 0.03017784282565117, 0.04130551964044571, 0.052566103637218475, 0.04205124080181122, 0.03273366019129753, 0.008433874696493149, 0.02538328990340233, 0.015113677829504013, 0.008195578120648861, 0.041412632912397385, 0.003141732420772314, 0.004215883556753397, 0.03539261221885681, 0.02788538858294487, 0.023785896599292755, 0.01634884439408779, 0.0009210030548274517, 0.01563998870551586, 0.014268863946199417, 0.0019568500574678183, 0.04284163936972618, 0.01778584159910679, 0.047522395849227905, 0.043178047984838486, 0.051370199769735336, 0.05102987587451935, 0.031499069184064865, 0.01659782975912094, 0.048936206847429276, 0.00269880797713995, 0.012028246186673641, 0.019326066598296165, 0.021966218948364258, 0.05033225193619728, 0.030871236696839333, 0.009951140731573105, 0.03178248926997185, 0.049753330647945404, 0.007147281430661678, 0.05233900994062424, 0.008198955096304417, 0.043730851262807846, 0.03610117360949516, 0.021531086415052414, 0.011577704921364784, 0.04121891036629677, 0.04516777768731117, 0.028223982080817223, 0.021824698895215988, 0.0009755022474564612, 0.007921029813587666, 0.04285738617181778, 0.02236703597009182, 0.018074527382850647, 0.015832820907235146, 0.0382564440369606, 0.05316615477204323, 0.02940700761973858, 0.0474163256585598, 0.008976494893431664, 0.04707895219326019, 0.03744599223136902, 0.0224912129342556, 0.046000003814697266, 0.012523806653916836, 0.030038325116038322, 0.0014152097282931209, 0.02025027945637703, 0.019279656931757927, 0.00486172828823328, 0.002411243738606572, 0.018246842548251152, 0.018937520682811737, 0.053061243146657944, 0.05031004548072815, 0.00698775053024292, 0.027619510889053345, 0.02542906254529953, 0.021372150629758835, 0.04958592355251312, 0.02745865285396576, 0.04313695430755615, 0.04698346555233002, 0.04063722491264343, 0.024745726957917213, 0.003938657697290182, 0.025069614872336388, 0.010687075555324554, 0.01111308578401804, 0.00945984199643135, 0.01887504570186138, 0.04858093708753586, 0.023099292069673538, 0.009500138461589813, 0.04007745906710625, 0.0026892228052020073, 0.004404826555401087, 0.002055841265246272, 0.02479143626987934, 0.032173801213502884, 0.00968628004193306, 0.027655456215143204], 10, map[nprobe, 16])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_169.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_170.csv</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector073, feature, array[0.57568294], 10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector_index_171</t>
+  </si>
+  <si>
+    <t>vector_index_172</t>
+  </si>
+  <si>
+    <t>vector_index_173</t>
+  </si>
+  <si>
+    <t>vector_index_174</t>
+  </si>
+  <si>
+    <t>vector_index_175</t>
+  </si>
+  <si>
+    <t>vector_index_176</t>
+  </si>
+  <si>
+    <t>vector_index_177</t>
+  </si>
+  <si>
+    <t>vector_index_179</t>
+  </si>
+  <si>
+    <t>vector_index_180</t>
+  </si>
+  <si>
+    <t>vector_index_181</t>
+  </si>
+  <si>
+    <t>vector_index_182</t>
+  </si>
+  <si>
+    <t>vector_index_183</t>
+  </si>
+  <si>
+    <t>vector_index_184</t>
+  </si>
+  <si>
+    <t>vector_index_185</t>
+  </si>
+  <si>
+    <t>vector_index_186</t>
+  </si>
+  <si>
+    <t>vector_index_187</t>
+  </si>
+  <si>
+    <t>vector_index_188</t>
+  </si>
+  <si>
+    <t>vector_index_189</t>
+  </si>
+  <si>
+    <t>vector_index_190</t>
+  </si>
+  <si>
+    <t>vector_index_191</t>
+  </si>
+  <si>
+    <t>vector_index_192</t>
+  </si>
+  <si>
+    <t>vector_index_193</t>
+  </si>
+  <si>
+    <t>IVFPQ算法 - edulidean距离 - 1维度 - 1000求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - edulidean距离 - 8维度 - 1000求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - edulidean距离 - 32维度 - 1000求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - edulidean距离 - 64维度 - 1000求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - edulidean距离 - 128维度 - 1000求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - edulidean距离 - 256维度 - 1000求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - edulidean距离 - 512维度 - 1000求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - edulidean距离 - 1024维度 - 1000求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector_index_194</t>
+  </si>
+  <si>
+    <t>vector_index_195</t>
+  </si>
+  <si>
+    <t>vector_index_ivfpq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector092</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector092, feature, array[1.1460036039352417], 10, map[nprobe, 16])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_171.csv</t>
+  </si>
+  <si>
+    <t>vector093</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_172.csv</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector093, feature, array[5.933931350708008, 0.2704865038394928, 0.20489951968193054, 0.6549103260040283, 0.9134868383407593, 0.8496164679527283, 0.044269345700740814, 0.13416512310504913], 10, map[nprobe, 6])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector093_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector094</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector094, feature, array[1.3875454664230347, 0.7626696825027466, 0.21715958416461945, 0.4816593527793884, 0.33340176939964294, 0.8789172172546387, 0.6245123147964478, 0.42354243993759155, 0.518169105052948, 0.8038954734802246, 0.7776609063148499, 0.11573372781276703, 0.7877957820892334, 0.5633759498596191, 0.5980196595191956, 0.13182960450649261, 0.663807213306427, 0.11982718855142593, 0.894885241985321, 0.8173267245292664, 0.3832005262374878, 0.3813772201538086, 0.9903861284255981, 0.8941025137901306, 0.04826643690466881, 0.9864906668663025, 0.8389081954956055, 0.7072503566741943, 0.739880383014679, 0.922918975353241, 0.03494282811880112, 0.5538699626922607], 10, map[nprobe, 4])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_173.csv</t>
+  </si>
+  <si>
+    <t>vector095</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector095, feature, array[1.8621821403503418, 0.2708185911178589, 0.09189905226230621, 0.933274507522583, 0.7153090834617615, 0.7983555793762207, 0.750082790851593, 0.6883314847946167, 0.31263604760169983, 0.4566596448421478, 0.1965976357460022, 0.6520524621009827, 0.7225580811500549, 0.6169158816337585, 0.4757600426673889, 0.8930113315582275, 0.16275887191295624, 0.8677147626876831, 0.38705652952194214, 0.3529115915298462, 0.43060439825057983, 0.03425328806042671, 0.6368623375892639, 0.07757068425416946, 0.26419928669929504, 0.8277255296707153, 0.43137165904045105, 0.08842884749174118, 0.2713584899902344, 0.9682172536849976, 0.7530999183654785, 0.9315038323402405, 0.7047898173332214, 0.724409282207489, 0.6946336627006531, 0.7282527685165405, 0.6133454442024231, 0.16090521216392517, 0.9238371253013611, 0.6565712094306946, 0.8871753215789795, 0.14609310030937195, 0.7698654532432556, 0.7012138962745667, 0.5944278836250305, 0.09350641816854477, 0.5790979266166687, 0.4277772903442383, 0.7462419867515564, 0.9512709379196167, 0.7253237366676331, 0.45405250787734985, 0.5477305054664612, 0.691687285900116, 0.8943620920181274, 0.5033979415893555, 0.486189603805542, 0.7285860180854797, 0.17546194791793823, 0.05633839592337608, 0.2782122492790222, 0.6356047987937927, 0.21174538135528564, 0.4946894347667694], 32, map[nprobe, 16])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_174.csv</t>
+  </si>
+  <si>
+    <t>vector096</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector096, feature, array[0.9942923784255981, 0.07601939141750336, 0.8223848342895508, 0.29077279567718506, 0.7544096112251282, 0.7107545733451843, 0.11972656100988388, 0.4674583673477173, 0.5878759622573853, 0.7628356218338013, 0.5963250398635864, 0.4973641335964203, 0.1391226202249527, 0.3085876405239105, 0.43839162588119507, 0.7552085518836975, 0.9042413830757141, 0.6285915970802307, 0.14940635859966278, 0.0968208760023117, 0.2549244165420532, 0.832711398601532, 0.9541964530944824, 0.5207446813583374, 0.04744589701294899, 0.07643387466669083, 0.447445273399353, 0.6366328001022339, 0.8625790476799011, 0.7592905759811401, 0.9664437770843506, 0.8875500559806824, 0.04725438728928566, 0.42646774649620056, 0.6227666139602661, 0.10289497673511505, 0.6811277270317078, 0.5723665356636047, 0.801175057888031, 0.8998327851295471, 0.4814528226852417, 0.7785786986351013, 0.6184626817703247, 0.12340367585420609, 0.6185998916625977, 0.20232152938842773, 0.022205164656043053, 0.7714211940765381, 0.4866187870502472, 0.6135231852531433, 0.788999080657959, 0.7070191502571106, 0.06620864570140839, 0.7074909806251526, 0.3387615978717804, 0.7453880310058594, 0.6473503708839417, 0.012553924694657326, 0.1371491402387619, 0.3547208309173584, 0.8730015158653259, 0.45049235224723816, 0.6056795120239258, 0.6498379707336426, 0.8631821274757385, 0.2708185911178589, 0.09189905226230621, 0.933274507522583, 0.7153090834617615, 0.7983555793762207, 0.750082790851593, 0.6883314847946167, 0.31263604760169983, 0.4566596448421478, 0.1965976357460022, 0.6520524621009827, 0.7225580811500549, 0.6169158816337585, 0.4757600426673889, 0.8930113315582275, 0.16275887191295624, 0.8677147626876831, 0.38705652952194214, 0.3529115915298462, 0.43060439825057983, 0.03425328806042671, 0.6368623375892639, 0.07757068425416946, 0.26419928669929504, 0.8277255296707153, 0.43137165904045105, 0.08842884749174118, 0.2713584899902344, 0.9682172536849976, 0.7530999183654785, 0.9315038323402405, 0.7047898173332214, 0.724409282207489, 0.6946336627006531, 0.7282527685165405, 0.6133454442024231, 0.16090521216392517, 0.9238371253013611, 0.6565712094306946, 0.8871753215789795, 0.14609310030937195, 0.7698654532432556, 0.7012138962745667, 0.5944278836250305, 0.09350641816854477, 0.5790979266166687, 0.4277772903442383, 0.7462419867515564, 0.9512709379196167, 0.7253237366676331, 0.45405250787734985, 0.5477305054664612, 0.691687285900116, 0.8943620920181274, 0.5033979415893555, 0.486189603805542, 0.7285860180854797, 0.17546194791793823, 0.05633839592337608, 0.2782122492790222, 0.6356047987937927, 0.21174538135528564, 0.4946894347667694], 10, map[nprobe, 16])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_175.csv</t>
+  </si>
+  <si>
+    <t>vector097</t>
+  </si>
+  <si>
+    <t>vector098</t>
+  </si>
+  <si>
+    <t>vector099</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector097, feature, array[1.378770112991333, 0.6224430203437805, 0.7043696641921997, 0.9191052913665771, 0.26086851954460144, 0.658689022064209, 0.03859037160873413, 0.09667620807886124, 0.08835094422101974, 0.5008041858673096, 0.018587397411465645, 0.7580321431159973, 0.7493271231651306, 0.36106300354003906, 0.704926073551178, 0.5717825889587402, 0.37350741028785706, 0.7436209321022034, 0.6090494394302368, 0.6629877090454102, 0.7141250371932983, 0.450267493724823, 0.543775200843811, 0.9666234850883484, 0.8990185856819153, 0.7119055390357971, 0.39062973856925964, 0.4343765676021576, 0.3516223430633545, 0.5473355650901794, 0.724093496799469, 0.277535080909729, 0.167818084359169, 0.3240392208099365, 0.6033129096031189, 0.8382450938224792, 0.5584244728088379, 0.2541007101535797, 0.951604425907135, 0.33220675587654114, 0.7379979491233826, 0.7967223525047302, 0.6973415017127991, 0.12068144232034683, 0.13951195776462555, 0.6880742907524109, 0.9310334324836731, 0.40059781074523926, 0.8816851377487183, 0.905667245388031, 0.5274580121040344, 0.44578680396080017, 0.7502004504203796, 0.23535023629665375, 0.2568817436695099, 0.24241557717323303, 0.8407144546508789, 0.9067634344100952, 0.6216895580291748, 0.91144859790802, 0.4027092754840851, 0.563454270362854, 0.7227501273155212, 0.5882618427276611, 0.23946058750152588, 0.4677514135837555, 0.6283088326454163, 0.8118173480033875, 0.01970723085105419, 0.7020925879478455, 0.09064045548439026, 0.43156275153160095, 0.3141074776649475, 0.35824283957481384, 0.5847647786140442, 0.3982110321521759, 0.7270205020904541, 0.4297885596752167, 0.9144589900970459, 0.6737052202224731, 0.8088598251342773, 0.26012763381004333, 0.7478787899017334, 0.2234390377998352, 0.6403365731239319, 0.6694568395614624, 0.4122609496116638, 0.35542312264442444, 0.20343448221683502, 0.9874551296234131, 0.8623238205909729, 0.5614364147186279, 0.38657912611961365, 0.9315293431282043, 0.6749474406242371, 0.3010503649711609, 0.8738755583763123, 0.7316179275512695, 0.3916900157928467, 0.14494997262954712, 0.19006171822547913, 0.5743873715400696, 0.4023633897304535, 0.17669415473937988, 0.9115904569625854, 0.9200974106788635, 0.24149015545845032, 0.44380488991737366, 0.2104913741350174, 0.36787137389183044, 0.8647742867469788, 0.8158168792724609, 0.8288285732269287, 0.9464249014854431, 0.9693216681480408, 0.2745744287967682, 0.17775459587574005, 0.9479954242706299, 0.29890531301498413, 0.41832423210144043, 0.8053778409957886, 0.48406317830085754, 0.9309419989585876, 0.3515394628047943, 0.19492487609386444, 0.05534011125564575, 0.9899139404296875, 0.4912799298763275, 0.5908764004707336, 0.2358837127685547, 0.043339941650629044, 0.4906046986579895, 0.49396997690200806, 0.7981225252151489, 0.8480699062347412, 0.7590365409851074, 0.7525428533554077, 0.8884413242340088, 0.1595989465713501, 0.19644983112812042, 0.2656191885471344, 0.3651057183742523, 0.6779343485832214, 0.8278098702430725, 0.9764223098754883, 0.3795296251773834, 0.3447924852371216, 0.36569368839263916, 0.437407523393631, 0.4742529094219208, 0.526160717010498, 0.7988599538803101, 0.028859032317996025, 0.6444850564002991, 0.03313356637954712, 0.7624076008796692, 0.5870527625083923, 0.14729389548301697, 0.9733296632766724, 0.959446132183075, 0.6102690100669861, 0.5513521432876587, 0.19067372381687164, 0.039004046469926834, 0.512133002281189, 0.18276765942573547, 0.13742727041244507, 0.01271786168217659, 0.48853039741516113, 0.359274685382843, 0.4436110258102417, 0.8102430105209351, 0.45369964838027954, 0.4024903476238251, 0.2217758446931839, 0.47787898778915405, 0.9330735802650452, 0.7278288006782532, 0.9128132462501526, 0.10163574665784836, 0.37986472249031067, 0.954140305519104, 0.5233055949211121, 0.16437236964702606, 0.7974892258644104, 0.6461623311042786, 0.22983016073703766, 0.03905296325683594, 0.9082323908805847, 0.698544979095459, 0.4329420328140259, 0.14276303350925446, 0.7512049674987793, 0.12749135494232178, 0.29352444410324097, 0.016196219250559807, 0.9938686490058899, 0.5891772508621216, 0.15184926986694336, 0.7003448605537415, 0.6145881414413452, 0.5828486084938049, 0.15822774171829224, 0.9733515381813049, 0.8800446391105652, 0.6342270374298096, 0.5378732085227966, 0.4670247733592987, 0.6080293655395508, 0.1155301183462143, 0.4022561311721802, 0.42923784255981445, 0.9000602960586548, 0.4725832939147949, 0.5480460524559021, 0.7692995667457581, 0.4510793685913086, 0.25714507699012756, 0.978748619556427, 0.7986847162246704, 0.8179019689559937, 0.6462092399597168, 0.6396266222000122, 0.36276915669441223, 0.40883371233940125, 0.4917561113834381, 0.07485639303922653, 0.2796553075313568, 0.1879693567752838, 0.7600657343864441, 0.6950889825820923, 0.05208180844783783, 0.16320586204528809, 0.44461488723754883, 0.7543023824691772, 0.1396082490682602, 0.28272515535354614, 0.04798141494393349, 0.33098506927490234, 0.04159433767199516, 0.24085299670696259, 0.8874347805976868, 0.02903219312429428, 0.6717896461486816, 0.45543089509010315, 0.13727740943431854, 0.5274479389190674, 0.22164995968341827, 0.8052409291267395, 0.31154441833496094, 0.9089944362640381, 0.45494163036346436, 0.021136855706572533, 0.7125626802444458, 0.5121524930000305, 0.6446650624275208], 10, map[nprobe, 16])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_176.csv</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector098, feature, array[0.9280381798744202, 0.44458526372909546, 0.11421280354261398, 0.7182922959327698, 0.07110431790351868, 0.24226781725883484, 0.3695947229862213, 0.8993130326271057, 0.2875322699546814, 0.7869394421577454, 0.7420486211776733, 0.6778227090835571, 0.7315680980682373, 0.2013152539730072, 0.5184952616691589, 0.9564326405525208, 0.5195212364196777, 0.7970696687698364, 0.375181645154953, 0.982855498790741, 0.6426228880882263, 0.9499534964561462, 0.03244348242878914, 0.015807781368494034, 0.42739802598953247, 0.9264262318611145, 0.6055673360824585, 0.7540596723556519, 0.13001053035259247, 0.9298628568649292, 0.5921488404273987, 0.9629314541816711, 0.6409729719161987, 0.8816754221916199, 0.7465222477912903, 0.6547877192497253, 0.8683363199234009, 0.1942540407180786, 0.20506201684474945, 0.9111261367797852, 0.748465895652771, 0.9382315874099731, 0.5464485287666321, 0.5655263662338257, 0.8342273235321045, 0.15373478829860687, 0.9814663529396057, 0.19738413393497467, 0.4043118953704834, 0.34131836891174316, 0.7158874869346619, 0.4980652332305908, 0.25321096181869507, 0.6542708873748779, 0.8695470690727234, 0.6887809634208679, 0.0867455005645752, 0.23142598569393158, 0.8705076575279236, 0.24309588968753815, 0.9834214448928833, 0.30724814534187317, 0.4510003924369812, 0.20634298026561737, 0.6395947337150574, 0.2231946885585785, 0.25346407294273376, 0.7565605044364929, 0.059569407254457474, 0.4956931173801422, 0.5055100917816162, 0.507824718952179, 0.6000626683235168, 0.4098283648490906, 0.8944247364997864, 0.9601107239723206, 0.4424718916416168, 0.3584369719028473, 0.8142503499984741, 0.33586418628692627, 0.07842046767473221, 0.47718721628189087, 0.9750044941902161, 0.9496296048164368, 0.05619080737233162, 0.04672866687178612, 0.17398904263973236, 0.8826673030853271, 0.4996427893638611, 0.2893809378147125, 0.009191651828587055, 0.650188148021698, 0.3544473648071289, 0.6689408421516418, 0.5939912796020508, 0.6020188927650452, 0.2500738501548767, 0.1370524913072586, 0.7178115248680115, 0.8675497174263, 0.9555330872535706, 0.41330352425575256, 0.8803149461746216, 0.2919802963733673, 0.07401710003614426, 0.7204731106758118, 0.6411976218223572, 0.44337114691734314, 0.7809030413627625, 0.8534911274909973, 0.12010776251554489, 0.496671199798584, 0.3609362244606018, 0.9863352179527283, 0.5116053819656372, 0.0774741992354393, 0.5313358902931213, 0.26458901166915894, 0.26790928840637207, 0.014806007035076618, 0.6896716356277466, 0.37612882256507874, 0.5570815801620483, 0.4229447543621063, 0.656370997428894, 0.3219057619571686, 0.03531838580965996, 0.1859131157398224, 0.8588796257972717, 0.674305260181427, 0.13331666588783264, 0.37703701853752136, 0.18450593948364258, 0.05264928564429283, 0.8679907321929932, 0.4433579742908478, 0.5437947511672974, 0.24423225224018097, 0.6430197954177856, 0.06946611404418945, 0.3041253983974457, 0.15912486612796783, 0.8970130085945129, 0.895421028137207, 0.5668182373046875, 0.4990484118461609, 0.05307658016681671, 0.8311125636100769, 0.7773664593696594, 0.9455102682113647, 0.6734291911125183, 0.9286069869995117, 0.8246590495109558, 0.9806768298149109, 0.516201376914978, 0.32770729064941406, 0.005871386267244816, 0.22107748687267303, 0.34921887516975403, 0.7158219814300537, 0.41915008425712585, 0.19487598538398743, 0.13835929334163666, 0.7580826878547668, 0.9694132804870605, 0.3084556758403778, 0.2792651951313019, 0.04284273833036423, 0.8693907260894775, 0.040453001856803894, 0.13330914080142975, 0.828435480594635, 0.5934156775474548, 0.3268646001815796, 0.12701047956943512, 0.5513052940368652, 0.49636709690093994, 0.3138543367385864, 0.5682827830314636, 0.778820812702179, 0.10579932481050491, 0.47008654475212097, 0.8439430594444275, 0.613008975982666, 0.14086423814296722, 0.02867121249437332, 0.1293075531721115, 0.9846811890602112, 0.1806558072566986, 0.8964135646820068, 0.15759746730327606, 0.4461385905742645, 0.6562026739120483, 0.36317700147628784, 0.6474786996841431, 0.6559386253356934, 0.9245064854621887, 0.47252708673477173, 0.7136704325675964, 0.3132008910179138, 0.26076576113700867, 0.4306317865848541, 0.09773091971874237, 0.2276291698217392, 0.051960479468107224, 0.9869140386581421, 0.9625105261802673, 0.4668925106525421, 0.47473379969596863, 0.5227413773536682, 0.5389710664749146, 0.33088019490242004, 0.7593510150909424, 0.6327823996543884, 0.4564867615699768, 0.6985312104225159, 0.28068041801452637, 0.02529607154428959, 0.6768425703048706, 0.8108940720558167, 0.6405670046806335, 0.48585349321365356, 0.09248621016740799, 0.2079823911190033, 0.4532947838306427, 0.5178763270378113, 0.08694205433130264, 0.3718554973602295, 0.165359228849411, 0.19510354101657867, 0.8010202646255493, 0.7698410749435425, 0.48936906456947327, 0.007331941742449999, 0.0008738748147152364, 0.8420559763908386, 0.7505729794502258, 0.718250572681427, 0.8218004107475281, 0.8362973928451538, 0.08034264296293259, 0.5025222897529602, 0.45972031354904175, 0.15571005642414093, 0.08945190906524658, 0.1507779210805893, 0.1297074258327484, 0.6060932278633118, 0.9851041436195374, 0.08987005054950714, 0.34991371631622314, 0.019370580092072487, 0.29004591703414917, 0.07145006954669952, 0.011683298274874687, 0.3154965043067932, 0.32931214570999146, 0.13117218017578125, 0.15277567505836487, 0.1951054036617279, 0.5124359726905823, 0.7185689806938171, 0.7177647352218628, 0.16508014500141144, 0.028500042855739594, 0.055054932832717896, 0.5517648458480835, 0.5737258791923523, 0.1893729567527771, 0.06485318392515182, 0.8916592001914978, 0.5787999033927917, 0.6566091179847717, 0.8909485340118408, 0.5663332939147949, 0.1867007166147232, 0.8026148676872253, 0.2994132936000824, 0.7449281811714172, 0.7415726780891418, 0.6891290545463562, 0.6542127728462219, 0.26438018679618835, 0.08485680818557739, 0.6796047687530518, 0.9734489917755127, 0.24252554774284363, 0.8829290270805359, 0.20056016743183136, 0.1316995918750763, 0.741577684879303, 0.8582263588905334, 0.7664816379547119, 0.5564740300178528, 0.2502431273460388, 0.06567316502332687, 0.047371622174978256, 0.8230901956558228, 0.13385890424251556, 0.5398962497711182, 0.13608448207378387, 0.8307609558105469, 0.21483361721038818, 0.06257782131433487, 0.9697452187538147, 0.4247171878814697, 0.25826528668403625, 0.4514281153678894, 0.9096243977546692, 0.19989459216594696, 0.2230977714061737, 0.4875296950340271, 0.1422831267118454, 0.9395604729652405, 0.5414695143699646, 0.40454185009002686, 0.3456386923789978, 0.4847174882888794, 0.8446424007415771, 0.7350196242332458, 0.5066976547241211, 0.9775434136390686, 0.942133367061615, 0.6589436531066895, 0.3606991469860077, 0.8261997103691101, 0.9862160086631775, 0.07491400092840195, 0.5770598649978638, 0.7885451912879944, 0.6594182252883911, 0.7617473006248474, 0.10272428393363953, 0.20818710327148438, 0.19746114313602448, 0.6396725177764893, 0.9767192006111145, 0.7475762367248535, 0.30035826563835144, 0.37847718596458435, 0.9416653513908386, 0.715986430644989, 0.05391446128487587, 0.7749239206314087, 0.7410386204719543, 0.6479222774505615, 0.05253317579627037, 0.4972829818725586, 0.029069101437926292, 0.8639436364173889, 0.39049607515335083, 0.29891565442085266, 0.3199126422405243, 0.47238075733184814, 0.5918688774108887, 0.3808765113353729, 0.22396674752235413, 0.5544300675392151, 0.8910173773765564, 0.23074765503406525, 0.5711702704429626, 0.04928134009242058, 0.5571699142456055, 0.8095689415931702, 0.007609733380377293, 0.7215369939804077, 0.15268543362617493, 0.4833413362503052, 0.5009947419166565, 0.9208973050117493, 0.359326034784317, 0.9834305644035339, 0.6922206282615662, 0.5595394968986511, 0.26777374744415283, 0.16270624101161957, 0.33169257640838623, 0.08987324684858322, 0.46450966596603394, 0.09789137542247772, 0.9382078051567078, 0.14910070598125458, 0.41668450832366943, 0.2771964371204376, 0.8064972162246704, 0.49945271015167236, 0.40134674310684204, 0.19328179955482483, 0.8709783554077148, 0.3904092013835907, 0.8782989978790283, 0.1688089221715927, 0.24859169125556946, 0.2526729106903076, 0.9409207105636597, 0.11054041981697083, 0.17023572325706482, 0.06085831671953201, 0.9530553817749023, 0.32408028841018677, 0.9897259473800659, 0.9604581594467163, 0.9626320600509644, 0.7674136161804199, 0.40337780117988586, 0.17394548654556274, 0.8381830453872681, 0.8140096664428711, 0.28524625301361084, 0.8572118878364563, 0.8798576593399048, 0.3992970585823059, 0.028776865452528, 0.7702739238739014, 0.8610913157463074, 0.3346964716911316, 0.27873021364212036, 0.1800815910100937, 0.8711404800415039, 0.13404642045497894, 0.006281466223299503, 0.19754579663276672, 0.28452515602111816, 0.9571599364280701, 0.30393731594085693, 0.19987894594669342, 0.8542295098304749, 0.08433782309293747, 0.7131807804107666, 0.9250710606575012, 0.8025881052017212, 0.944640576839447, 0.19478410482406616, 0.21415123343467712, 0.4090621769428253, 0.341785728931427, 0.6535173654556274, 0.45325616002082825, 0.8674607872962952, 0.4600127935409546, 0.10150229185819626, 0.44820284843444824, 0.5300790667533875, 0.2613048851490021, 0.6483422517776489, 0.06711512058973312, 0.09960293769836426, 0.2575109004974365, 0.32471123337745667, 0.5043879151344299, 0.34977301955223083, 0.7492573857307434, 0.9269258379936218, 0.08885488659143448, 0.011269651353359222, 0.8541161417961121, 0.16864514350891113, 0.1950804889202118, 0.6232283115386963, 0.16835589706897736, 0.4476327896118164, 0.6119879484176636, 0.2594325542449951, 0.9824452996253967, 0.6685553193092346, 0.6743354201316833, 0.9361977577209473, 0.4769512116909027, 0.9475557804107666, 0.8471337556838989, 0.8146544098854065, 0.3554985821247101, 0.44289109110832214, 0.8850129246711731, 0.934047281742096, 0.4110226333141327, 0.7709431648254395, 0.5469692349433899, 0.45847898721694946, 0.32120439410209656, 0.9341722130775452, 0.12385708093643188, 0.19255955517292023, 0.3398846685886383, 0.7695445418357849, 0.591597855091095, 0.7500520944595337, 0.28528743982315063, 0.4922447204589844, 0.3502650558948517, 0.6993582844734192, 0.6594836115837097, 0.593571662902832, 0.2431846559047699, 0.7910350561141968, 0.543161928653717, 0.40140974521636963, 0.5128881931304932, 0.199427992105484, 0.23024891316890717, 0.8619752526283264, 0.10197064280509949, 0.7673206925392151, 0.5555479526519775, 0.14225542545318604, 0.6184604167938232, 0.16881819069385529, 0.8116948008537292, 0.9693849086761475, 0.7374794483184814, 0.22605854272842407, 0.806194007396698], 10, map[nprobe, 10])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_177.csv</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector099, feature, array[1.3535224199295044, 0.31392207741737366, 0.6286861896514893, 0.5430471301078796, 0.327924519777298, 0.6388945579528809, 0.6662382483482361, 0.9540348649024963, 0.8470741510391235, 0.558837354183197, 0.9277071952819824, 0.18017378449440002, 0.20220935344696045, 0.23732851445674896, 0.8634951710700989, 0.013733146712183952, 0.6470873951911926, 0.8624395728111267, 0.0532325841486454, 0.9079377055168152, 0.32841241359710693, 0.6605964303016663, 0.10226576030254364, 0.03404153883457184, 0.34508422017097473, 0.42952463030815125, 0.42589616775512695, 0.7463461756706238, 0.13148018717765808, 0.20628729462623596, 0.6974230408668518, 0.7751299738883972, 0.42980441451072693, 0.8757259249687195, 0.8634995222091675, 0.4060722291469574, 0.11937657743692398, 0.01659681834280491, 0.9395890831947327, 0.589221179485321, 0.3559124171733856, 0.9011857509613037, 0.5132598876953125, 0.8931979537010193, 0.017754850909113884, 0.05205504968762398, 0.10376431047916412, 0.5387919545173645, 0.09737808257341385, 0.6455812454223633, 0.5163909792900085, 0.8110367059707642, 0.7585089206695557, 0.3072868287563324, 0.5092869997024536, 0.07276355475187302, 0.27697500586509705, 0.5430586934089661, 0.6564051508903503, 0.2702702283859253, 0.7595415711402893, 0.1976347416639328, 0.9247005581855774, 0.578951358795166, 0.7895205616950989, 0.8593189716339111, 0.8979884386062622, 0.7156239151954651, 0.7308275103569031, 0.06604301929473877, 0.02126903086900711, 0.912445604801178, 0.6840839982032776, 0.9050001502037048, 0.7471106052398682, 0.6554510593414307, 0.05558401718735695, 0.008919947780668736, 0.06737808883190155, 0.02276572771370411, 0.11755851656198502, 0.7885823845863342, 0.2896302342414856, 0.6111487746238708, 0.5452771782875061, 0.5070639252662659, 0.5575328469276428, 0.9821842908859253, 0.6032338738441467, 0.2464839220046997, 0.04556428641080856, 0.20409837365150452, 0.5856149792671204, 0.6793073415756226, 0.5138164162635803, 0.06337228417396545, 0.5200310349464417, 0.8398666381835938, 0.17414791882038116, 0.7912601828575134, 0.3804928958415985, 0.6220223903656006, 0.23092465102672577, 0.6921454668045044, 0.4472225308418274, 0.5277025699615479, 0.139532670378685, 0.6781741380691528, 0.8661579489707947, 0.803992748260498, 0.31101688742637634, 0.2642950415611267, 0.35684001445770264, 0.9845317006111145, 0.6832847595214844, 0.9003570079803467, 0.5688319802284241, 0.3989367187023163, 0.19944503903388977, 0.5208761096000671, 0.9899275898933411, 0.5411144495010376, 0.5617583990097046, 0.20418207347393036, 0.9012929797172546, 0.718074381351471, 0.25599873065948486, 0.8763864636421204, 0.17597444355487823, 0.7684363126754761, 0.28905537724494934, 0.7825420498847961, 0.49110525846481323, 0.46907898783683777, 0.4610026478767395, 0.7931860089302063, 0.6691699624061584, 0.8590985536575317, 0.36251100897789, 0.302160382270813, 0.6255984902381897, 0.6185368299484253, 0.3431003987789154, 0.5225530862808228, 0.17594394087791443, 0.319243848323822, 0.34648874402046204, 0.6134116053581238, 0.5962549448013306, 0.15202587842941284, 0.03358858451247215, 0.9800461530685425, 0.11197073757648468, 0.7386590242385864, 0.08929972350597382, 0.8608983755111694, 0.4285961985588074, 0.6677455306053162, 0.8629558086395264, 0.9458568692207336, 0.10144906491041183, 0.7221893668174744, 0.6134009957313538, 0.635726809501648, 0.7860614061355591, 0.04271707311272621, 0.3278331756591797, 0.2661527693271637, 0.820303738117218, 0.6541527509689331, 0.06946848332881927, 0.4497787356376648, 0.26181983947753906, 0.8207583427429199, 0.526282787322998, 0.6442065238952637, 0.4397187829017639, 0.42431023716926575, 0.863955020904541, 0.8194906711578369, 0.3692033886909485, 0.29273590445518494, 0.20331180095672607, 0.3265809416770935, 0.7198004126548767, 0.7821041941642761, 0.22568848729133606, 0.7535693049430847, 0.10962527245283127, 0.7746263146400452, 0.41499581933021545, 0.9231970906257629, 0.12129457294940948, 0.03865664079785347, 0.8412232398986816, 0.8968071937561035, 0.5044061541557312, 0.527552604675293, 0.214138463139534, 0.5709258317947388, 0.4863903224468231, 0.6553916931152344, 0.3209784924983978, 0.43311354517936707, 0.9132612943649292, 0.6129176020622253, 0.7732480764389038, 0.10157007724046707, 0.8077899813652039, 0.6300846338272095, 0.5447371006011963, 0.03293538838624954, 0.2593502700328827, 0.36692947149276733, 0.7294648289680481, 0.8853902816772461, 0.1492408663034439, 0.323038250207901, 0.8157459497451782, 0.6161888241767883, 0.2771996557712555, 0.15968436002731323, 0.7917547821998596, 0.5117677450180054, 0.9797217845916748, 0.4572522044181824, 0.633741557598114, 0.050042491406202316, 0.9816424250602722, 0.03735988214612007, 0.20834188163280487, 0.40889671444892883, 0.46471431851387024, 0.3546723425388336, 0.3371832072734833, 0.46723422408103943, 0.1978747546672821, 0.12306314706802368, 0.8566398620605469, 0.29816874861717224, 0.5706659555435181, 0.13568951189517975, 0.58491450548172, 0.058242522180080414, 0.8876081109046936, 0.4532458484172821, 0.34756678342819214, 0.019598646089434624, 0.5479026436805725, 0.5178790092468262, 0.8009217381477356, 0.05276933312416077, 0.15879449248313904, 0.5511860847473145, 0.4744284152984619, 0.31998518109321594, 0.4216269552707672, 0.772039532661438, 0.12998369336128235, 0.350511759519577, 0.26288649439811707, 0.8798844814300537, 0.16706740856170654, 0.30563458800315857, 0.4884311556816101, 0.2878722548484802, 0.24419446289539337, 0.2479081153869629, 0.8877922296524048, 0.8932329416275024, 0.6359367370605469, 0.6506319046020508, 0.38934606313705444, 0.7937962412834167, 0.14109300076961517, 0.8118140697479248, 0.9655399322509766, 0.6201736927032471, 0.5559843182563782, 0.8355616927146912, 0.8100405931472778, 0.40611961483955383, 0.8194018006324768, 0.9660396575927734, 0.7525915503501892, 0.03655319660902023, 0.8989080786705017, 0.28844553232192993, 0.709339439868927, 0.782699465751648, 0.9315032958984375, 0.6763602495193481, 0.29540425539016724, 0.8221983313560486, 0.07585986703634262, 0.8574230074882507, 0.04927975684404373, 0.27592507004737854, 0.15236325562000275, 0.17199739813804626, 0.2829899787902832, 0.06075937673449516, 0.4812662601470947, 0.20124997198581696, 0.05699349567294121, 0.21945475041866302, 0.4001869857311249, 0.8960256576538086, 0.6441617608070374, 0.1969970315694809, 0.8967918157577515, 0.20898251235485077, 0.8699110150337219, 0.8007341623306274, 0.016917230561375618, 0.6108096837997437, 0.10050247609615326, 0.36888644099235535, 0.08611364662647247, 0.45928022265434265, 0.17870646715164185, 0.40315693616867065, 0.12586042284965515, 0.06276871263980865, 0.4162765443325043, 0.5260014533996582, 0.047529708594083786, 0.26816439628601074, 0.5966269969940186, 0.6473529934883118, 0.871753990650177, 0.144949272274971, 0.822285532951355, 0.7476346492767334, 0.42069026827812195, 0.9143622517585754, 0.49050143361091614, 0.3161744177341461, 0.9122335910797119, 0.6420398354530334, 0.4559533894062042, 0.7698162794113159, 0.3468329906463623, 0.3441320061683655, 0.5831806659698486, 0.9870078563690186, 0.529897153377533, 0.8140012621879578, 0.37875986099243164, 0.2879214286804199, 0.7916374802589417, 0.034201908856630325, 0.7240689396858215, 0.309619665145874, 0.5948328375816345, 0.1482827365398407, 0.064975306391716, 0.3544246256351471, 0.24767665565013885, 0.5309166312217712, 0.8236681818962097, 0.16633279621601105, 0.6045527458190918, 0.840312659740448, 0.8818798661231995, 0.2836647629737854, 0.24866093695163727, 0.16592605412006378, 0.8696073889732361, 0.15388169884681702, 0.1234707236289978, 0.0893031656742096, 0.759905993938446, 0.14988519251346588, 0.3773735761642456, 0.305133581161499, 0.9575893878936768, 0.036850590258836746, 0.20642253756523132, 0.9915892481803894, 0.5863695740699768, 0.9472546577453613, 0.9799618721008301, 0.8103383779525757, 0.35064542293548584, 0.10905013233423233, 0.6158831119537354, 0.31979936361312866, 0.7686752676963806, 0.29659366607666016, 0.175935298204422, 0.30370092391967773, 0.07879403233528137, 0.9581267833709717, 0.5903143882751465, 0.8368186950683594, 0.4258797764778137, 0.2547442317008972, 0.3142375946044922, 0.9655606150627136, 0.9529805779457092, 0.5794531106948853, 0.8737883567810059, 0.14201901853084564, 0.5911117196083069, 0.596875011920929, 0.3460487425327301, 0.617759108543396, 0.46116796135902405, 0.7459498047828674, 0.4751615524291992, 0.07415878027677536, 0.5300676822662354, 0.20728667080402374, 0.9711235165596008, 0.9838496446609497, 0.9765100479125977, 0.5397936701774597, 0.3189065456390381, 0.1277550756931305, 0.14100432395935059, 0.9208326935768127, 0.24735726416110992, 0.0042854794301092625, 0.7794864773750305, 0.01714763231575489, 0.7499006390571594, 0.09633156657218933, 0.11551760137081146, 0.43344646692276, 0.8221164345741272, 0.916947066783905, 0.9624882936477661, 0.23329205811023712, 0.820077657699585, 0.9002286195755005, 0.18546347320079803, 0.29306188225746155, 0.4147912561893463, 0.8118062019348145, 0.9458348155021667, 0.24703262746334076, 0.48520025610923767, 0.6130959987640381, 0.9061111807823181, 0.693015456199646, 0.5204097032546997, 0.8096333146095276, 0.7873492240905762, 0.3455691635608673, 0.6505943536758423, 0.5464634299278259, 0.9939194917678833, 0.009671092964708805, 0.172136127948761, 0.8355600237846375, 0.5392587184906006, 0.3844122886657715, 0.27245110273361206, 0.08908169716596603, 0.7321572303771973, 0.3043614625930786, 0.516395628452301, 0.8712427616119385, 0.9070706963539124, 0.6003034114837646, 0.4587913155555725, 0.43092480301856995, 0.05208354815840721, 0.17264613509178162, 0.11335580796003342, 0.7337794899940491, 0.8280722498893738, 0.8515526652336121, 0.182905375957489, 0.20550097525119781, 0.5318430066108704, 0.7694017887115479, 0.3260716497898102, 0.9888104200363159, 0.3905967175960541, 0.7081881165504456, 0.08131667971611023, 0.9327805042266846, 0.09879519045352936, 0.3782595098018646, 0.1964826136827469, 0.065560482442379, 0.4647301435470581, 0.4068993330001831, 0.068758025765419, 0.37635934352874756, 0.12430961430072784, 0.15205417573451996, 0.3794234097003937, 0.7064068913459778, 0.6421923637390137, 0.1213885024189949, 0.4444319009780884, 0.787514328956604, 0.6183278560638428, 0.5016001462936401, 0.1109316274523735, 0.23703736066818237, 0.48945075273513794, 0.06614242494106293, 0.2886432707309723, 0.6472116112709045, 0.5528389811515808, 0.260344922542572, 0.45896947383880615, 0.7337946891784668, 0.9727996587753296, 0.8410258889198303, 0.16144442558288574, 0.45416712760925293, 0.40877798199653625, 0.16939617693424225, 0.6642683744430542, 0.6432697176933289, 0.3228059709072113, 0.7809991836547852, 0.4492257535457611, 0.12247347831726074, 0.8468798995018005, 0.2833680212497711, 0.754226565361023, 0.2617167532444, 0.22498548030853271, 0.6968601942062378, 0.01867150515317917, 0.45630860328674316, 0.8501220345497131, 0.8321512937545776, 0.13769303262233734, 0.8910747170448303, 0.4661495089530945, 0.6513407230377197, 0.8318792581558228, 0.28195613622665405, 0.36692488193511963, 0.7187744379043579, 0.6934444904327393, 0.1999175250530243, 0.07552443444728851, 0.44622501730918884, 0.6139288544654846, 0.2826865613460541, 0.9559957981109619, 0.24807852506637573, 0.8561092615127563, 0.9534884691238403, 0.8511945009231567, 0.9334288239479065, 0.7140789031982422, 0.388191282749176, 0.8813086152076721, 0.2990174889564514, 0.8551315665245056, 0.6261729598045349, 0.47120681405067444, 0.4749518036842346, 0.2978686988353729, 0.7673436999320984, 0.5300029516220093, 0.7782717943191528, 0.48984426259994507, 0.5372359156608582, 0.7814760208129883, 0.9203964471817017, 0.12072478979825974, 0.9859831929206848, 0.7018551826477051, 0.5309759378433228, 0.2384367287158966, 0.9594374895095825, 0.5416489839553833, 0.6988224387168884, 0.17703697085380554, 0.8895614743232727, 0.4391710162162781, 0.7611968517303467, 0.7971492409706116, 0.4065127968788147, 0.4121829569339752, 0.7725569605827332, 0.4139801859855652, 0.0163713488727808, 0.6492041349411011, 0.08953416347503662, 0.8054971694946289, 0.6981039047241211, 0.7944212555885315, 0.13323798775672913, 0.8237714171409607, 0.5783477425575256, 0.776218593120575, 0.2682107388973236, 0.3471018671989441, 0.22101500630378723, 0.0013618111843243241, 0.46306857466697693, 0.9206815958023071, 0.4903622269630432, 0.016083497554063797, 0.2783198654651642, 0.3251529037952423, 0.5013194680213928, 0.11445412039756775, 0.012079134583473206, 0.2560001611709595, 0.9028116464614868, 0.19274145364761353, 0.05333879962563515, 0.7343361377716064, 0.7589075565338135, 0.3284699320793152, 0.07905074208974838, 0.612633466720581, 0.050045695155858994, 0.4453601837158203, 0.6522535681724548, 0.7844055891036987, 0.05484423041343689, 0.5774549841880798, 0.6620239615440369, 0.33169230818748474, 0.8406599760055542, 0.5894076228141785, 0.19468770921230316, 0.4066234827041626, 0.2146763801574707, 0.8467811942100525, 0.9844373464584351, 0.4828815460205078, 0.515873908996582, 0.08487104624509811, 0.6903231739997864, 0.9226033091545105, 0.802691638469696, 0.6860600113868713, 0.4897204637527466, 0.44427889585494995, 0.9516621232032776, 0.24357430636882782, 0.2184334099292755, 0.1172204315662384, 0.30623695254325867, 0.7359335422515869, 0.35206976532936096, 0.6945627331733704, 0.14384330809116364, 0.5232542753219604, 0.858997106552124, 0.09767534583806992, 0.3239775598049164, 0.5455408692359924, 0.5925885438919067, 0.44869863986968994, 0.918238639831543, 0.8670168519020081, 0.6096367239952087, 0.5765714049339294, 0.20481634140014648, 0.013852575793862343, 0.7634700536727905, 0.5896143913269043, 0.8080111742019653, 0.7057751417160034, 0.5197216868400574, 0.7997134923934937, 0.52923983335495, 0.03232930973172188, 0.018497133627533913, 0.7039249539375305, 0.011687240563333035, 0.5172359347343445, 0.5772852301597595, 0.10513359308242798, 0.2089967429637909, 0.5673447847366333, 0.18025241792201996, 0.4207831621170044, 0.5921681523323059, 0.09777862578630447, 0.08759112656116486, 0.9734905362129211, 0.9592893123626709, 0.15649233758449554, 0.7245137691497803, 0.14614325761795044, 0.06277640908956528, 0.7213056683540344, 0.9397366046905518, 0.6714769005775452, 0.5868414640426636, 0.17096030712127686, 0.04715782031416893, 0.6168940663337708, 0.06490743905305862, 0.20420877635478973, 0.9348860383033752, 0.04705149680376053, 0.9873403310775757, 0.16766494512557983, 0.7204188108444214, 0.4140930473804474, 0.539613664150238, 0.7032927870750427, 0.7088668942451477, 0.20077580213546753, 0.5277281403541565, 0.6421862244606018, 0.8054519891738892, 0.5765840411186218, 0.3639857769012451, 0.9252842664718628, 0.5993244647979736, 0.6518167853355408, 0.8031960725784302, 0.9634014368057251, 0.8032671809196472, 0.9200478196144104, 0.6832403540611267, 0.5457735657691956, 0.8271417617797852, 0.48793771862983704, 0.4425477385520935, 0.3262253701686859, 0.913882315158844, 0.02942078560590744, 0.6699893474578857, 0.8075922131538391, 0.6672304272651672, 0.15863613784313202, 0.6991033554077148, 0.5136383175849915, 0.4518413841724396, 0.11432988196611404, 0.8337645530700684, 0.19997699558734894, 0.7787659764289856, 0.8858902454376221, 0.3331146836280823, 0.4625246226787567, 0.709303617477417, 0.8493442535400391, 0.5922209620475769, 0.05531374737620354, 0.8209349513053894, 0.41280829906463623, 0.5246221423149109, 0.2334795892238617, 0.7214219570159912, 0.1311296820640564, 0.44521600008010864, 0.6902942657470703, 0.31479501724243164, 0.4011533260345459, 0.2884719967842102, 0.6499318480491638, 0.07902435213327408, 0.587889552116394, 0.4206700623035431, 0.6996663212776184, 0.35319074988365173, 0.025650616735219955, 0.23918427526950836, 0.7409505248069763, 0.4450435936450958, 0.5256019234657288, 0.4717833697795868, 0.8258699178695679, 0.5224175453186035, 0.7758104801177979, 0.5949121117591858, 0.9227606058120728, 0.9540846347808838, 0.5391230583190918, 0.4323936998844147, 0.5126331448554993, 0.5201613306999207, 0.9423797726631165, 0.48105093836784363, 0.9516801238059998, 0.28912651538848877, 0.02632157877087593, 0.9608991146087646, 0.01087308768182993, 0.024711405858397484, 0.6115622520446777, 0.6259920001029968, 0.4615266025066376, 0.9528838992118835, 0.1402873545885086, 0.11240574717521667, 0.658463180065155, 0.31963804364204407, 0.5899862051010132, 0.9113656878471375, 0.399395614862442, 0.13844920694828033, 0.027269160374999046, 0.25427162647247314, 0.42216628789901733, 0.04987042769789696, 0.18019147217273712, 0.7941862344741821, 0.9338135719299316, 0.46885237097740173, 0.23517246544361115, 0.4200786352157593, 0.48608848452568054, 0.4442487955093384, 0.09712281078100204, 0.07257167994976044, 0.4982982277870178, 0.5579163432121277, 0.6890251636505127, 0.9634112119674683, 0.038591355085372925, 0.011482151225209236, 0.10637529194355011, 0.47698545455932617, 0.7801839709281921, 0.7333822846412659, 0.7921286821365356, 0.7396711707115173, 0.918930172920227, 0.8444852232933044, 0.35946616530418396, 0.13169533014297485, 0.8867505192756653, 0.9843819737434387, 0.45732593536376953, 0.39677712321281433, 0.7165563702583313, 0.5174497365951538, 0.28845199942588806, 0.699768602848053, 0.22804494202136993, 0.7759913206100464, 0.017792699858546257, 0.22908005118370056, 0.033014751970767975, 0.38638630509376526, 0.7582269906997681, 0.9918963313102722, 0.2277938425540924, 0.3404541611671448, 0.2818209230899811, 0.5840474963188171, 0.20378121733665466, 0.2285759150981903, 0.3664989173412323, 0.26250016689300537, 0.8654340505599976, 0.293350487947464, 0.4659748673439026, 0.8676082491874695, 0.722886323928833, 0.7667917013168335, 0.3939172327518463, 0.010212404653429985, 0.6736516356468201, 0.1699751615524292, 0.41582465171813965, 0.05516976863145828, 0.16567884385585785, 0.6887815594673157, 0.6800487041473389, 0.31047749519348145, 0.3765132427215576, 0.7969440817832947, 0.6438823342323303, 0.15393388271331787, 0.6197165846824646, 0.6464699506759644, 0.6883950233459473, 0.1250983476638794, 0.06625806540250778, 0.0498005673289299, 0.36104512214660645, 0.14150340855121613, 0.3790360689163208, 0.3583654761314392, 0.49927186965942383, 0.05921294167637825, 0.35575079917907715, 0.5574421286582947, 0.15135829150676727, 0.5173702836036682, 0.08944489806890488, 0.7415786981582642, 0.610964834690094, 0.12629124522209167, 0.6571646332740784, 0.8580804467201233, 0.8047488927841187, 0.8786532282829285, 0.45353013277053833, 0.5217942595481873, 0.059725672006607056, 0.9192184209823608, 0.7132784128189087, 0.5126069188117981, 0.22028516232967377, 0.32300373911857605, 0.8696557879447937, 0.20453821122646332, 0.15377956628799438, 0.0202034842222929, 0.4030291736125946, 0.4018510580062866, 0.7322199940681458, 0.13991300761699677, 0.4270966351032257, 0.8927143216133118, 0.06635436415672302, 0.025243913754820824, 0.6089762449264526, 0.164319708943367, 0.6504514813423157, 0.9660682082176208, 0.013212698511779308, 0.17079849541187286, 0.2274859994649887, 0.8873509764671326, 0.11539249867200851, 0.8897441029548645, 0.7119466066360474, 0.8219953775405884, 0.4518047273159027, 0.5526160597801208, 0.5156668424606323, 0.3798842430114746, 0.7591387629508972, 0.9025423526763916, 0.2689059376716614, 0.6515424847602844, 0.2789366543292999, 0.5568122267723083, 0.6634635925292969, 0.6262637376785278, 0.2085745930671692, 0.9376164078712463, 0.22791308164596558, 0.7418540120124817, 0.4057253897190094, 0.04983304813504219, 0.387042760848999, 0.45331305265426636, 0.390306293964386, 0.9865545630455017, 0.018806803971529007, 0.5152460932731628, 0.996749997138977, 0.9486609101295471, 0.39116954803466797, 0.9426976442337036, 0.8067740797996521, 0.889554500579834, 0.8979684114456177, 0.6170464754104614, 0.4870646297931671, 0.7093315720558167, 0.16865132749080658, 0.8192521929740906, 0.5919701457023621, 0.49244385957717896, 0.3616722524166107, 0.8071326017379761, 0.5368145108222961, 0.5495433807373047, 0.7324987649917603, 0.34005603194236755, 0.5569435358047485, 0.4839858114719391, 0.623735249042511, 0.3610200881958008, 0.07797244936227798, 0.1523757129907608, 0.5165678262710571, 0.28967800736427307, 0.9974238276481628, 0.6469708681106567, 0.14755597710609436, 0.10067712515592575, 0.23362165689468384, 0.16978217661380768, 0.7000492811203003, 0.334881991147995, 0.0713207945227623, 0.9313864707946777, 0.5797341465950012, 0.6120589375495911, 0.14535905420780182, 0.10906676203012466, 0.9480545520782471, 0.6738556027412415, 0.18509434163570404, 0.2789756953716278, 0.5380411744117737, 0.8931823372840881, 0.801687479019165, 0.20614159107208252, 0.8113815784454346, 0.26392629742622375, 0.7574407458305359, 0.7305825352668762, 0.37589940428733826, 0.6839823126792908, 0.5169562101364136, 0.1914183497428894, 0.10160491615533829, 0.0792914405465126, 0.5758206844329834, 0.658331573009491, 0.26919224858283997, 0.5582151412963867, 0.4865487515926361, 0.0918538048863411, 0.6479836702346802, 0.6070619225502014], 10, map[nprobe, 4])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_178.csv</t>
+  </si>
+  <si>
+    <t>vector_index_178</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - edulidean距离 - 1024维度 - 100求top1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector099, feature, array[1.596806287765503, 0.9530852437019348, 0.27465352416038513, 0.21051378548145294, 0.4916960299015045, 0.5357282161712646, 0.37085703015327454, 0.6232490539550781, 0.9905115365982056, 0.05565378814935684, 0.976271390914917, 0.22093702852725983, 0.9521338939666748, 0.9921261072158813, 0.135658860206604, 0.25788918137550354, 0.5570521354675293, 0.8184967041015625, 0.9900513291358948, 0.9636828899383545, 0.3241939842700958, 0.05959314480423927, 0.1790343075990677, 0.12839753925800323, 0.9382874965667725, 0.8684219121932983, 0.546017587184906, 0.6185161471366882, 0.14533190429210663, 0.6510460376739502, 0.370889812707901, 0.6248840093612671, 0.7841241359710693, 0.5897661447525024, 0.5858216285705566, 0.6732216477394104, 0.23575592041015625, 0.6731960773468018, 0.8987328410148621, 0.9169199466705322, 0.46832016110420227, 0.10591695457696915, 0.24832464754581451, 0.7967361211776733, 0.7818373441696167, 0.9142890572547913, 0.7776272296905518, 0.0019504133379086852, 0.34204718470573425, 0.3116171061992645, 0.8029139041900635, 0.2056700885295868, 0.3097113370895386, 0.4732672870159149, 0.18308880925178528, 0.24898722767829895, 0.4983636736869812, 0.4567992389202118, 0.8044384121894836, 0.2602790892124176, 0.36433839797973633, 0.25976458191871643, 0.7876454591751099, 0.19253508746623993, 0.9050574898719788, 0.4794468283653259, 0.23295174539089203, 0.5239722728729248, 0.5038551688194275, 0.7330762147903442, 0.8577761650085449, 0.9907607436180115, 0.38671523332595825, 0.9660098552703857, 0.9231131076812744, 0.7381659746170044, 0.07171223312616348, 0.31729015707969666, 0.4642878770828247, 0.35997530817985535, 0.2009267956018448, 0.8282569050788879, 0.9865838289260864, 0.9135036468505859, 0.13720615208148956, 0.846320390701294, 0.33996057510375977, 0.31155747175216675, 0.40192174911499023, 0.11158275604248047, 0.9066070914268494, 0.41366490721702576, 0.8453296422958374, 0.2385692149400711, 0.35722020268440247, 0.6293771862983704, 0.2987388074398041, 0.8121826648712158, 0.27254244685173035, 0.6050546765327454, 0.3509581983089447, 0.09024440497159958, 0.9605022072792053, 0.9094009399414062, 0.0047423383221030235, 0.8298129439353943, 0.06534048914909363, 0.5475450158119202, 0.13043421506881714, 0.9657529592514038, 0.9194191694259644, 0.16592352092266083, 0.4903404712677002, 0.28798067569732666, 0.2504013776779175, 0.15643854439258575, 0.602001965045929, 0.17232181131839752, 0.5064225792884827, 0.29144760966300964, 0.6578218936920166, 0.8121724128723145, 0.6869034171104431, 0.40609246492385864, 0.9206042289733887, 0.6337800025939941, 0.6358243227005005, 0.05505942925810814, 0.25437358021736145, 0.15330374240875244, 0.9374415278434753, 0.6051976680755615, 0.26239213347435, 0.09425842761993408, 0.17728225886821747, 0.7379575967788696, 0.6935216784477234, 0.2916930615901947, 0.8242577314376831, 0.15241044759750366, 0.05804507061839104, 0.4003112018108368, 0.09256019443273544, 0.6628434062004089, 0.029935741797089577, 0.4982011020183563, 0.9509184956550598, 0.25503620505332947, 0.7900165915489197, 0.8082498908042908, 0.19344812631607056, 0.6264059543609619, 0.99628746509552, 0.022587904706597328, 0.4998175799846649, 0.516963005065918, 0.12614604830741882, 0.030323002487421036, 0.6797467470169067, 0.752450168132782, 0.700892448425293, 0.091143898665905, 0.7431145310401917, 0.43021753430366516, 0.34816327691078186, 0.5840665102005005, 0.8531844615936279, 0.8413566946983337, 0.49784088134765625, 0.37117788195610046, 0.31438377499580383, 0.029036343097686768, 0.596396267414093, 0.08876316249370575, 0.9296973943710327, 0.14229507744312286, 0.5041192770004272, 0.49943453073501587, 0.49172651767730713, 0.8300368785858154, 0.18155187368392944, 0.4565810263156891, 0.33723390102386475, 0.39173629879951477, 0.4056580066680908, 0.7200303673744202, 0.8650441765785217, 0.9296712875366211, 0.514937698841095, 0.9668827056884766, 0.3386729061603546, 0.6010417938232422, 0.28672823309898376, 0.1421407163143158, 0.2167438566684723, 0.806982159614563, 0.8952023386955261, 0.015756720677018166, 0.11679846048355103, 0.9748110175132751, 0.3447931110858917, 0.6197988986968994, 0.2875216007232666, 0.12689122557640076, 0.7005501389503479, 0.3417496681213379, 0.8444570302963257, 0.7549565434455872, 0.43534427881240845, 0.5634763240814209, 0.4656939208507538, 0.9810046553611755, 0.013610693626105785, 0.5235769748687744, 0.1868165284395218, 0.3607659935951233, 0.14759671688079834, 0.7912507057189941, 0.2732934355735779, 0.821477472782135, 0.8151514530181885, 0.6672901511192322, 0.3465697169303894, 0.23925912380218506, 0.43074625730514526, 0.1204393208026886, 0.5640471577644348, 0.2935769557952881, 0.7768828868865967, 0.11930004507303238, 0.425897479057312, 0.01158488355576992, 0.6920041441917419, 0.9903997778892517, 0.8675287961959839, 0.7923703193664551, 0.7055089473724365, 0.4594559967517853, 0.1507336050271988, 0.8073820471763611, 0.6851866841316223, 0.9715391397476196, 0.37712353467941284, 0.12766169011592865, 0.4973722994327545, 0.6502329707145691, 0.4024174213409424, 0.381939560174942, 0.7121758460998535, 0.41879966855049133, 0.5058507323265076, 0.3318614959716797, 0.10576807707548141, 0.40106359124183655, 0.7714136242866516, 0.22171233594417572, 0.06601352989673615, 0.6861528158187866, 0.7346727848052979, 0.9311012029647827, 0.11515745520591736, 0.7161571979522705, 0.5047160387039185, 0.6702039837837219, 0.12730352580547333, 0.02528725191950798, 0.41937509179115295, 0.2457071989774704, 0.7077691555023193, 0.027323013171553612, 0.321931391954422, 0.9526068568229675, 0.31077778339385986, 0.8993144035339355, 0.7148497104644775, 0.6850499510765076, 0.6804989576339722, 0.14345687627792358, 0.7246773838996887, 0.6476393342018127, 0.40494272112846375, 0.035407595336437225, 0.5192702412605286, 0.08421501517295837, 0.34486937522888184, 0.16987775266170502, 0.5711086988449097, 0.4562619626522064, 0.7042873501777649, 0.8163453340530396, 0.5121675729751587, 0.5959538817405701, 0.7066412568092346, 0.5127528309822083, 0.2494923323392868, 0.46941158175468445, 0.03901291266083717, 0.8518891930580139, 0.950393795967102, 0.6298165321350098, 0.946503758430481, 0.25761541724205017, 0.5169490575790405, 0.49646010994911194, 0.21755942702293396, 0.38909968733787537, 0.4164985716342926, 0.6647462248802185, 0.5514055490493774, 0.1533018946647644, 0.7125470042228699, 0.519015371799469, 0.3669212758541107, 0.4381368160247803, 0.4678051173686981, 0.27272874116897583, 0.9394617676734924, 0.2230294793844223, 0.21894462406635284, 0.3784293830394745, 0.5581826567649841, 0.9890391230583191, 0.5159546136856079, 0.8921816945075989, 0.8646500706672668, 0.8751608729362488, 0.1360628455877304, 0.8854951858520508, 0.7165313959121704, 0.04964647814631462, 0.2798256278038025, 0.36291375756263733, 0.7168136239051819, 0.44306913018226624, 0.8963308334350586, 0.5783583521842957, 0.3869503140449524, 0.9538711905479431, 0.6784047484397888, 0.5855856537818909, 0.5327514410018921, 0.6793406009674072, 0.013094025664031506, 0.8837418556213379, 0.694688618183136, 0.6681780219078064, 0.5126833319664001, 0.5504215359687805, 0.061818499118089676, 0.793438196182251, 0.17367719113826752, 0.7902112007141113, 0.2827242612838745, 0.10736202448606491, 0.6240127086639404, 0.14374521374702454, 0.13880227506160736, 0.4212202727794647, 0.9711113572120667, 0.7165883779525757, 0.18641473352909088, 0.1312044858932495, 0.14511629939079285, 0.6108564138412476, 0.18761084973812103, 0.19505934417247772, 0.5992414355278015, 0.7604738473892212, 0.3971773684024811, 0.6575697064399719, 0.3471137285232544, 0.7388620376586914, 0.3563153147697449, 0.43509212136268616, 0.43815988302230835, 0.861045241355896, 0.3975801467895508, 0.8594518899917603, 0.4490785598754883, 0.48356032371520996, 0.024354126304388046, 0.6917322874069214, 0.572141706943512, 0.37037476897239685, 0.9890633225440979, 0.1552046239376068, 0.17766514420509338, 0.024648329243063927, 0.8514800071716309, 0.8109879493713379, 0.7113043069839478, 0.6627388596534729, 0.7526264190673828, 0.1943509429693222, 0.852518618106842, 0.32862186431884766, 0.9633485078811646, 0.5933730602264404, 0.2846603989601135, 0.31788864731788635, 0.8039383292198181, 0.5600063800811768, 0.659764289855957, 0.5165979862213135, 0.9218969941139221, 0.4647434651851654, 0.5489198565483093, 0.6853556036949158, 0.6485406756401062, 0.044623278081417084, 0.7247711420059204, 0.3027680814266205, 0.16010551154613495, 0.8080441951751709, 0.5800619125366211, 0.9683188199996948, 0.7394787073135376, 0.566362738609314, 0.11050643771886826, 0.40968918800354004, 0.9890902638435364, 0.12131485342979431, 0.3213249742984772, 0.9928126335144043, 0.16093888878822327, 0.45103156566619873, 0.04111859202384949, 0.32102668285369873, 0.5028234124183655, 0.8758991956710815, 0.3839322030544281, 0.19136467576026917, 0.2015068382024765, 0.2185981273651123, 0.8298919796943665, 0.562176525592804, 0.9653496146202087, 0.6393329501152039, 0.1407443732023239, 0.6088649034500122, 0.2082122564315796, 0.5674248337745667, 0.024625463411211967, 0.24467091262340546, 0.006522873416543007, 0.8851104378700256, 0.35266977548599243, 0.9864232540130615, 0.10111912339925766, 0.9311673641204834, 0.7987105250358582, 0.7419715523719788, 0.30922019481658936, 0.2700248956680298, 0.766757071018219, 0.5952844023704529, 0.34519562125205994, 0.12185034155845642, 0.3642492890357971, 0.7297511696815491, 0.8035641312599182, 0.476190984249115, 0.05282846465706825, 0.44114115834236145, 0.35667139291763306, 0.928841233253479, 0.12783408164978027, 0.5336344838142395, 0.3860211968421936, 0.8970383405685425, 0.2530398666858673, 0.08723969757556915, 0.1873004287481308, 0.17146091163158417, 0.5847023129463196, 0.01633966900408268, 0.07986912131309509, 0.08042974025011063, 0.8910163044929504, 0.012767563574016094, 0.4477699398994446, 0.5799049139022827, 0.00017907848814502358, 0.03248365595936775, 0.08254104107618332, 0.33599919080734253, 0.14382439851760864, 0.4857887029647827, 0.5700032114982605, 0.6516076326370239, 0.45163801312446594, 0.623045802116394, 0.172739177942276, 0.3793632686138153, 0.014265749603509903, 0.8665200471878052, 0.20062236487865448, 0.12632572650909424, 0.09440261125564575, 0.1968746930360794, 0.9220244288444519, 0.013252772390842438, 0.7999640703201294, 0.6826646327972412, 0.7118967175483704, 0.39558082818984985, 0.5503553748130798, 0.9608808159828186, 0.02497752197086811, 0.7806575894355774, 0.8998667597770691, 0.39116451144218445, 0.5500157475471497, 0.971642017364502, 0.9735432863235474, 0.20182451605796814, 0.47721296548843384, 0.9572637677192688, 0.5137233734130859, 0.3639989197254181, 0.7827183604240417, 0.16946212947368622, 0.3447047472000122, 0.006907067261636257, 0.6115983724594116, 0.4347532391548157, 0.6382417678833008, 0.7764526009559631, 0.3347403109073639, 0.6639428734779358, 0.16382983326911926, 0.8875507116317749, 0.09305152297019958, 0.6408823132514954, 0.33034712076187134, 0.06830053776502609, 0.38380196690559387, 0.9128003716468811, 0.6931731700897217, 0.25567540526390076, 0.4200512170791626, 0.640399694442749, 0.9456954598426819, 0.33706775307655334, 0.26480913162231445, 0.49433526396751404, 0.9961013197898865, 0.792833149433136, 0.3144489526748657, 0.34072887897491455, 0.605634868144989, 0.3355492949485779, 0.866000235080719, 0.8226666450500488, 0.3674819767475128, 0.005913340020924807, 0.6638931632041931, 0.2663460671901703, 0.5143115520477295, 0.7305150032043457, 0.6248257160186768, 0.35341355204582214, 0.0472293347120285, 0.42964792251586914, 0.11540526896715164, 0.09632588922977448, 0.22588658332824707, 0.2605765461921692, 0.2876918613910675, 0.10211492329835892, 0.664454996585846, 0.18490362167358398, 0.4827594459056854, 0.47264546155929565, 0.1777806580066681, 0.8691214323043823, 0.10743182897567749, 0.6893302798271179, 0.9185250997543335, 0.3888787031173706, 0.8677827715873718, 0.35098859667778015, 0.006338621024042368, 0.0039253742434084415, 0.39253681898117065, 0.6675857305526733, 0.6425376534461975, 0.33118078112602234, 0.9493565559387207, 0.9410620331764221, 0.9754370450973511, 0.6340346336364746, 0.3239191472530365, 0.5538143515586853, 0.6138201355934143, 0.28988298773765564, 0.15358543395996094, 0.4311138391494751, 0.8076610565185547, 0.6668306589126587, 0.8167520761489868, 0.6883480548858643, 0.9156597852706909, 0.6940751075744629, 0.7082298994064331, 0.6514293551445007, 0.33382418751716614, 0.44972172379493713, 0.4507167935371399, 0.23963096737861633, 0.3715897500514984, 0.9268632531166077, 0.135644793510437, 0.30302318930625916, 0.18853142857551575, 0.5903620719909668, 0.19413535296916962, 0.14715546369552612, 0.1597658395767212, 0.9166655540466309, 0.43431356549263, 0.20056910812854767, 0.8578015565872192, 0.8743382096290588, 0.28286275267601013, 0.22800038754940033, 0.0019058139296248555, 0.9685027003288269, 0.03262699767947197, 0.33330464363098145, 0.7117661237716675, 0.6934338808059692, 0.6779075860977173, 0.48093900084495544, 0.315290242433548, 0.9697685241699219, 0.5734806656837463, 0.37865614891052246, 0.41905903816223145, 0.5490906238555908, 0.13832373917102814, 0.354297935962677, 0.5372971892356873, 0.9111441969871521, 0.1782509684562683, 0.2996734380722046, 0.6199487447738647, 0.5633794069290161, 0.20694489777088165, 0.010360254906117916, 0.7553234100341797, 0.37177756428718567, 0.756881833076477, 0.18463298678398132, 0.32678401470184326, 0.7689133882522583, 0.8304637670516968, 0.29421180486679077, 0.9634458422660828, 0.8566946387290955, 0.7149925827980042, 0.26076817512512207, 0.802510142326355, 0.006658948492258787, 0.1795494556427002, 0.8712763786315918, 0.6751517653465271, 0.7314084768295288, 0.11635345965623856, 0.12758828699588776, 0.3416576683521271, 0.04491414874792099, 0.2009766846895218, 0.3551313579082489, 0.9335193037986755, 0.8997042775154114, 0.4274944067001343, 0.11475033313035965, 0.8391264081001282, 0.49883538484573364, 0.14694027602672577, 0.018790272995829582, 0.4467023015022278, 0.8110135197639465, 0.3858625292778015, 0.1359582394361496, 0.76105135679245, 0.5041544437408447, 0.03640727326273918, 0.5934978127479553, 0.18641193211078644, 0.8910730481147766, 0.9168241024017334, 0.3362073600292206, 0.8802468776702881, 0.9429932236671448, 0.5581793785095215, 0.6458896994590759, 0.46013763546943665, 0.47838252782821655, 0.18089182674884796, 0.7536806464195251, 0.6271700859069824, 0.17426277697086334, 0.7049959897994995, 0.7884112596511841, 0.10022548586130142, 0.7097893953323364, 0.20798556506633759, 0.1052551344037056, 0.8209380507469177, 0.0925396978855133, 0.10834047198295593, 0.19735215604305267, 0.3555421233177185, 0.27295196056365967, 0.4942246377468109, 0.3681899607181549, 0.08780904114246368, 0.5143633484840393, 0.3422415852546692, 0.010797719471156597, 0.41441062092781067, 0.5106329321861267, 0.4711938798427582, 0.9985347390174866, 0.7116854786872864, 0.30820944905281067, 0.6983880400657654, 0.40412968397140503, 0.9903700351715088, 0.6402249336242676, 0.79643315076828, 0.7949107885360718, 0.1309320032596588, 0.15932123363018036, 0.6292378306388855, 0.4604432284832001, 0.8787709474563599, 0.48654669523239136, 0.8684062957763672, 0.7849902510643005, 0.41592445969581604, 0.7356888651847839, 0.08902235329151154, 0.16750289499759674, 0.021026473492383957, 0.25594615936279297, 0.8190529346466064, 0.7335047721862793, 0.8704279065132141, 0.7855508327484131, 0.7879476547241211, 0.4432326555252075, 0.19924859702587128, 0.5832628607749939, 0.33078083395957947, 0.03130011260509491, 0.43552836775779724, 0.5520086884498596, 0.23266060650348663, 0.2300567924976349, 0.6775324940681458, 0.45760461688041687, 0.986105740070343, 0.9824753999710083, 0.9339448809623718, 0.6773325204849243, 0.8790497779846191, 0.007350691128522158, 0.14407901465892792, 0.49592453241348267, 0.3905007541179657, 0.7415096759796143, 0.9631860852241516, 0.22505708038806915, 0.5019029974937439, 0.2308400273323059, 0.016276098787784576, 0.44854843616485596, 0.5611958503723145, 0.602139949798584, 0.7200368046760559, 0.8339542746543884, 0.8955331444740295, 0.5390866994857788, 0.3709260821342468, 0.5345321297645569, 0.0210268497467041, 0.2245100736618042, 0.9775363802909851, 0.5520218014717102, 0.0003913170949090272, 0.3129982352256775, 0.536283552646637, 0.3178279995918274, 0.8988470435142517, 0.8584112524986267, 0.2897510528564453, 0.9101524949073792, 0.2812105715274811, 0.41043445467948914, 0.8080659508705139, 0.9355173707008362, 0.6300311088562012, 0.7384047508239746, 0.3701503276824951, 0.9823273420333862, 0.5300660133361816, 0.3147099018096924, 0.6345334649085999, 0.6955615878105164, 0.3361154794692993, 0.45193296670913696, 0.017241057008504868, 0.9704602360725403, 0.9191238880157471, 0.9790920615196228, 0.6069653630256653, 0.8812688589096069, 0.6931416392326355, 0.8056981563568115, 0.16757319867610931, 0.8462014198303223, 0.8883793950080872, 0.19573234021663666, 0.9107251167297363, 0.1605798900127411, 0.7785749435424805, 0.7456387877464294, 0.7948620915412903, 0.46974703669548035, 0.7856404781341553, 0.8276567459106445, 0.9243813753128052, 0.013878095895051956, 0.9853442311286926, 0.11505182087421417, 0.20245790481567383, 0.838047206401825, 0.24346156418323517, 0.21193675696849823, 0.9400508999824524, 0.7742969989776611, 0.7354463338851929, 0.3162704110145569, 0.0955042615532875, 0.03266829252243042, 0.7519464492797852, 0.9929614067077637, 0.45284968614578247, 0.584784984588623, 0.2745923399925232, 0.7402022480964661, 0.74982088804245, 0.9648182392120361, 0.5855893492698669, 0.1531897932291031, 0.10874906182289124, 0.40045812726020813, 0.2359602451324463, 0.41140004992485046, 0.1153879314661026, 0.8862301111221313, 0.7379536628723145, 0.429610013961792, 0.33836036920547485, 0.6763753294944763, 0.09692277014255524, 0.7297652959823608, 0.7367976903915405, 0.6830936670303345, 0.2944589853286743, 0.15385469794273376, 0.8477643132209778, 0.8202636241912842, 0.17494189739227295, 0.249573215842247, 0.2962771952152252, 0.05369146540760994, 0.14718852937221527, 0.6051258444786072, 0.3833862841129303, 0.13228249549865723, 0.5781098008155823, 0.7942613363265991, 0.2319624274969101, 0.1867154836654663, 0.32441258430480957, 0.2260856330394745, 0.6565804481506348, 0.46823471784591675, 0.6779251098632812, 0.933508038520813, 0.5198525786399841, 0.3935171067714691, 0.6167722940444946, 0.48609474301338196, 0.8452314734458923, 0.6160932779312134, 0.4649025499820709, 0.23399990797042847, 0.26778444647789, 0.8915127515792847, 0.7946352958679199, 0.7619978189468384, 0.986690878868103, 0.5977674722671509, 0.833810567855835, 0.8580195307731628, 0.7442461848258972, 0.8753593564033508, 0.322928249835968, 0.7059530019760132, 0.2523559033870697, 0.9864510297775269, 0.17907920479774475, 0.14625601470470428, 0.5661028623580933, 0.6373598575592041, 0.01984381303191185, 0.25842544436454773, 0.8357756733894348, 0.9409646987915039, 0.0867486447095871, 0.7721037268638611, 0.5765758752822876, 0.8208791017532349, 0.6028860807418823, 0.416258841753006, 0.17483997344970703, 0.9481948018074036, 0.3720783591270447, 0.7898986339569092, 0.4062842130661011, 0.41464439034461975, 0.43707600235939026, 0.8432615995407104, 0.41378527879714966, 0.585837721824646, 0.6157651543617249, 0.3199690878391266, 0.6569175720214844, 0.8318197131156921, 0.06795558333396912, 0.9352171421051025, 0.1597462296485901, 0.09771733731031418, 0.3552184998989105, 0.4082724452018738, 0.29142141342163086, 0.4140358567237854, 0.8261848092079163, 0.3232395648956299, 0.9087274670600891, 0.27958670258522034, 0.45559126138687134, 0.9478925466537476, 0.8955391049385071, 0.46299993991851807, 0.3924270272254944, 0.42887017130851746, 0.4709075391292572, 0.45306965708732605, 0.08453886955976486, 0.465684175491333, 0.1519767791032791, 0.22340251505374908, 0.5548582077026367, 0.8046561479568481, 0.6081976890563965, 0.6576899290084839, 0.1430637091398239, 0.45311662554740906, 0.055959902703762054, 0.36510464549064636, 0.6399905681610107, 0.6648254990577698, 0.39158180356025696, 0.18971514701843262, 0.8524832129478455, 0.27036064863204956, 0.5614879727363586, 0.8735694885253906, 0.391645610332489, 0.9196508526802063, 0.9502583146095276, 0.9599886536598206, 0.1392839550971985, 0.10637673735618591, 0.00842419546097517, 0.15935562551021576, 0.45861250162124634, 0.2798033058643341, 0.8080960512161255, 0.1833738535642624, 0.4602353572845459, 0.8216803669929504, 0.8272251486778259, 0.3791065216064453, 0.26143860816955566, 0.4275175929069519, 0.3803093731403351, 0.35752901434898376, 0.8357917666435242, 0.13106189668178558, 0.5563707947731018, 0.2944142818450928, 0.7682047486305237, 0.368671178817749, 0.6326341032981873, 0.1475858986377716, 0.2708606719970703, 0.3432406187057495, 0.10653529316186905, 0.8966823220252991, 0.8565285801887512, 0.6063984632492065, 0.27109161019325256, 0.07932481169700623, 0.3380233943462372, 0.11583281308412552, 0.2011593133211136, 0.6192118525505066], 1, map[nprobe, 8])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_179.csv</t>
+  </si>
+  <si>
+    <t>vector100</t>
+  </si>
+  <si>
+    <t>vector100_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_180.csv</t>
+  </si>
+  <si>
+    <t>IVFPQ算法 - dotproduct距离 - 2维度 - 10000求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector100, feature, array[0.387281, 0.815432], 20, map[nprobe, 16])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector101</t>
+  </si>
+  <si>
+    <t>vector102</t>
+  </si>
+  <si>
+    <t>vector103</t>
+  </si>
+  <si>
+    <t>vector104</t>
+  </si>
+  <si>
+    <t>vector105</t>
+  </si>
+  <si>
+    <t>vector106</t>
+  </si>
+  <si>
+    <t>vector107</t>
+  </si>
+  <si>
+    <t>vector101_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector101, feature, array[0.6020776629447937, 0.3941165506839752, 0.19068339467048645, 0.45499899983406067, 0.28198644518852234, 0.27388763427734375, 0.20737290382385254, 0.20311570167541504], 10, map[nprobe, 3])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_181.csv</t>
+  </si>
+  <si>
+    <t>IVFPQ算法 - dotproduct距离 - 8维度 - 2048求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - dotproduct距离 - 32维度 - 2048求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector102_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector102, feature, array[0.35864362120628357, 0.19712984561920166, 0.05612998083233833, 0.12449613958597183, 0.08617549389600754, 0.2271767407655716, 0.1614198386669159, 0.10947446525096893, 0.1339329481124878, 0.20778562128543854, 0.20100468397140503, 0.029914092272520065, 0.20362427830696106, 0.14561770856380463, 0.15457218885421753, 0.03407444804906845, 0.17157652974128723, 0.03097214363515377, 0.23130404949188232, 0.2112572342157364, 0.09904715418815613, 0.09857587516307831, 0.2559885084629059, 0.23110173642635345, 0.012475591152906418, 0.2549816370010376, 0.21683546900749207, 0.18280541896820068, 0.19123941659927368, 0.23855002224445343, 0.009031792171299458, 0.14316067099571228], 10, map[nprobe, 4])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>select id,feature_id,feature_index$distance from vector($vector088, feature, array[1.3535224199295044, 0.31392207741737366, 0.6286861896514893, 0.5430471301078796, 0.327924519777298, 0.6388945579528809, 0.6662382483482361, 0.9540348649024963, 0.8470741510391235, 0.558837354183197, 0.9277071952819824, 0.18017378449440002, 0.20220935344696045, 0.23732851445674896, 0.8634951710700989, 0.013733146712183952, 0.6470873951911926, 0.8624395728111267, 0.0532325841486454, 0.9079377055168152, 0.32841241359710693, 0.6605964303016663, 0.10226576030254364, 0.03404153883457184, 0.34508422017097473, 0.42952463030815125, 0.42589616775512695, 0.7463461756706238, 0.13148018717765808, 0.20628729462623596, 0.6974230408668518, 0.7751299738883972, 0.42980441451072693, 0.8757259249687195, 0.8634995222091675, 0.4060722291469574, 0.11937657743692398, 0.01659681834280491, 0.9395890831947327, 0.589221179485321, 0.3559124171733856, 0.9011857509613037, 0.5132598876953125, 0.8931979537010193, 0.017754850909113884, 0.05205504968762398, 0.10376431047916412, 0.5387919545173645, 0.09737808257341385, 0.6455812454223633, 0.5163909792900085, 0.8110367059707642, 0.7585089206695557, 0.3072868287563324, 0.5092869997024536, 0.07276355475187302, 0.27697500586509705, 0.5430586934089661, 0.6564051508903503, 0.2702702283859253, 0.7595415711402893, 0.1976347416639328, 0.9247005581855774, 0.578951358795166, 0.7895205616950989, 0.8593189716339111, 0.8979884386062622, 0.7156239151954651, 0.7308275103569031, 0.06604301929473877, 0.02126903086900711, 0.912445604801178, 0.6840839982032776, 0.9050001502037048, 0.7471106052398682, 0.6554510593414307, 0.05558401718735695, 0.008919947780668736, 0.06737808883190155, 0.02276572771370411, 0.11755851656198502, 0.7885823845863342, 0.2896302342414856, 0.6111487746238708, 0.5452771782875061, 0.5070639252662659, 0.5575328469276428, 0.9821842908859253, 0.6032338738441467, 0.2464839220046997, 0.04556428641080856, 0.20409837365150452, 0.5856149792671204, 0.6793073415756226, 0.5138164162635803, 0.06337228417396545, 0.5200310349464417, 0.8398666381835938, 0.17414791882038116, 0.7912601828575134, 0.3804928958415985, 0.6220223903656006, 0.23092465102672577, 0.6921454668045044, 0.4472225308418274, 0.5277025699615479, 0.139532670378685, 0.6781741380691528, 0.8661579489707947, 0.803992748260498, 0.31101688742637634, 0.2642950415611267, 0.35684001445770264, 0.9845317006111145, 0.6832847595214844, 0.9003570079803467, 0.5688319802284241, 0.3989367187023163, 0.19944503903388977, 0.5208761096000671, 0.9899275898933411, 0.5411144495010376, 0.5617583990097046, 0.20418207347393036, 0.9012929797172546, 0.718074381351471, 0.25599873065948486, 0.8763864636421204, 0.17597444355487823, 0.7684363126754761, 0.28905537724494934, 0.7825420498847961, 0.49110525846481323, 0.46907898783683777, 0.4610026478767395, 0.7931860089302063, 0.6691699624061584, 0.8590985536575317, 0.36251100897789, 0.302160382270813, 0.6255984902381897, 0.6185368299484253, 0.3431003987789154, 0.5225530862808228, 0.17594394087791443, 0.319243848323822, 0.34648874402046204, 0.6134116053581238, 0.5962549448013306, 0.15202587842941284, 0.03358858451247215, 0.9800461530685425, 0.11197073757648468, 0.7386590242385864, 0.08929972350597382, 0.8608983755111694, 0.4285961985588074, 0.6677455306053162, 0.8629558086395264, 0.9458568692207336, 0.10144906491041183, 0.7221893668174744, 0.6134009957313538, 0.635726809501648, 0.7860614061355591, 0.04271707311272621, 0.3278331756591797, 0.2661527693271637, 0.820303738117218, 0.6541527509689331, 0.06946848332881927, 0.4497787356376648, 0.26181983947753906, 0.8207583427429199, 0.526282787322998, 0.6442065238952637, 0.4397187829017639, 0.42431023716926575, 0.863955020904541, 0.8194906711578369, 0.3692033886909485, 0.29273590445518494, 0.20331180095672607, 0.3265809416770935, 0.7198004126548767, 0.7821041941642761, 0.22568848729133606, 0.7535693049430847, 0.10962527245283127, 0.7746263146400452, 0.41499581933021545, 0.9231970906257629, 0.12129457294940948, 0.03865664079785347, 0.8412232398986816, 0.8968071937561035, 0.5044061541557312, 0.527552604675293, 0.214138463139534, 0.5709258317947388, 0.4863903224468231, 0.6553916931152344, 0.3209784924983978, 0.43311354517936707, 0.9132612943649292, 0.6129176020622253, 0.7732480764389038, 0.10157007724046707, 0.8077899813652039, 0.6300846338272095, 0.5447371006011963, 0.03293538838624954, 0.2593502700328827, 0.36692947149276733, 0.7294648289680481, 0.8853902816772461, 0.1492408663034439, 0.323038250207901, 0.8157459497451782, 0.6161888241767883, 0.2771996557712555, 0.15968436002731323, 0.7917547821998596, 0.5117677450180054, 0.9797217845916748, 0.4572522044181824, 0.633741557598114, 0.050042491406202316, 0.9816424250602722, 0.03735988214612007, 0.20834188163280487, 0.40889671444892883, 0.46471431851387024, 0.3546723425388336, 0.3371832072734833, 0.46723422408103943, 0.1978747546672821, 0.12306314706802368, 0.8566398620605469, 0.29816874861717224, 0.5706659555435181, 0.13568951189517975, 0.58491450548172, 0.058242522180080414, 0.8876081109046936, 0.4532458484172821, 0.34756678342819214, 0.019598646089434624, 0.5479026436805725, 0.5178790092468262, 0.8009217381477356, 0.05276933312416077, 0.15879449248313904, 0.5511860847473145, 0.4744284152984619, 0.31998518109321594, 0.4216269552707672, 0.772039532661438, 0.12998369336128235, 0.350511759519577, 0.26288649439811707, 0.8798844814300537, 0.16706740856170654, 0.30563458800315857, 0.4884311556816101, 0.2878722548484802, 0.24419446289539337, 0.2479081153869629, 0.8877922296524048, 0.8932329416275024, 0.6359367370605469, 0.6506319046020508, 0.38934606313705444, 0.7937962412834167, 0.14109300076961517, 0.8118140697479248, 0.9655399322509766, 0.6201736927032471, 0.5559843182563782, 0.8355616927146912, 0.8100405931472778, 0.40611961483955383, 0.8194018006324768, 0.9660396575927734, 0.7525915503501892, 0.03655319660902023, 0.8989080786705017, 0.28844553232192993, 0.709339439868927, 0.782699465751648, 0.9315032958984375, 0.6763602495193481, 0.29540425539016724, 0.8221983313560486, 0.07585986703634262, 0.8574230074882507, 0.04927975684404373, 0.27592507004737854, 0.15236325562000275, 0.17199739813804626, 0.2829899787902832, 0.06075937673449516, 0.4812662601470947, 0.20124997198581696, 0.05699349567294121, 0.21945475041866302, 0.4001869857311249, 0.8960256576538086, 0.6441617608070374, 0.1969970315694809, 0.8967918157577515, 0.20898251235485077, 0.8699110150337219, 0.8007341623306274, 0.016917230561375618, 0.6108096837997437, 0.10050247609615326, 0.36888644099235535, 0.08611364662647247, 0.45928022265434265, 0.17870646715164185, 0.40315693616867065, 0.12586042284965515, 0.06276871263980865, 0.4162765443325043, 0.5260014533996582, 0.047529708594083786, 0.26816439628601074, 0.5966269969940186, 0.6473529934883118, 0.871753990650177, 0.144949272274971, 0.822285532951355, 0.7476346492767334, 0.42069026827812195, 0.9143622517585754, 0.49050143361091614, 0.3161744177341461, 0.9122335910797119, 0.6420398354530334, 0.4559533894062042, 0.7698162794113159, 0.3468329906463623, 0.3441320061683655, 0.5831806659698486, 0.9870078563690186, 0.529897153377533, 0.8140012621879578, 0.37875986099243164, 0.2879214286804199, 0.7916374802589417, 0.034201908856630325, 0.7240689396858215, 0.309619665145874, 0.5948328375816345, 0.1482827365398407, 0.064975306391716, 0.3544246256351471, 0.24767665565013885, 0.5309166312217712, 0.8236681818962097, 0.16633279621601105, 0.6045527458190918, 0.840312659740448, 0.8818798661231995, 0.2836647629737854, 0.24866093695163727, 0.16592605412006378, 0.8696073889732361, 0.15388169884681702, 0.1234707236289978, 0.0893031656742096, 0.759905993938446, 0.14988519251346588, 0.3773735761642456, 0.305133581161499, 0.9575893878936768, 0.036850590258836746, 0.20642253756523132, 0.9915892481803894, 0.5863695740699768, 0.9472546577453613, 0.9799618721008301, 0.8103383779525757, 0.35064542293548584, 0.10905013233423233, 0.6158831119537354, 0.31979936361312866, 0.7686752676963806, 0.29659366607666016, 0.175935298204422, 0.30370092391967773, 0.07879403233528137, 0.9581267833709717, 0.5903143882751465, 0.8368186950683594, 0.4258797764778137, 0.2547442317008972, 0.3142375946044922, 0.9655606150627136, 0.9529805779457092, 0.5794531106948853, 0.8737883567810059, 0.14201901853084564, 0.5911117196083069, 0.596875011920929, 0.3460487425327301, 0.617759108543396, 0.46116796135902405, 0.7459498047828674, 0.4751615524291992, 0.07415878027677536, 0.5300676822662354, 0.20728667080402374, 0.9711235165596008, 0.9838496446609497, 0.9765100479125977, 0.5397936701774597, 0.3189065456390381, 0.1277550756931305, 0.14100432395935059, 0.9208326935768127, 0.24735726416110992, 0.0042854794301092625, 0.7794864773750305, 0.01714763231575489, 0.7499006390571594, 0.09633156657218933, 0.11551760137081146, 0.43344646692276, 0.8221164345741272, 0.916947066783905, 0.9624882936477661, 0.23329205811023712, 0.820077657699585, 0.9002286195755005, 0.18546347320079803, 0.29306188225746155, 0.4147912561893463, 0.8118062019348145, 0.9458348155021667, 0.24703262746334076, 0.48520025610923767, 0.6130959987640381, 0.9061111807823181, 0.693015456199646, 0.5204097032546997, 0.8096333146095276, 0.7873492240905762, 0.3455691635608673, 0.6505943536758423, 0.5464634299278259, 0.9939194917678833, 0.009671092964708805, 0.172136127948761, 0.8355600237846375, 0.5392587184906006, 0.3844122886657715, 0.27245110273361206, 0.08908169716596603, 0.7321572303771973, 0.3043614625930786, 0.516395628452301, 0.8712427616119385, 0.9070706963539124, 0.6003034114837646, 0.4587913155555725, 0.43092480301856995, 0.05208354815840721, 0.17264613509178162, 0.11335580796003342, 0.7337794899940491, 0.8280722498893738, 0.8515526652336121, 0.182905375957489, 0.20550097525119781, 0.5318430066108704, 0.7694017887115479, 0.3260716497898102, 0.9888104200363159, 0.3905967175960541, 0.7081881165504456, 0.08131667971611023, 0.9327805042266846, 0.09879519045352936, 0.3782595098018646, 0.1964826136827469, 0.065560482442379, 0.4647301435470581, 0.4068993330001831, 0.068758025765419, 0.37635934352874756, 0.12430961430072784, 0.15205417573451996, 0.3794234097003937, 0.7064068913459778, 0.6421923637390137, 0.1213885024189949, 0.4444319009780884, 0.787514328956604, 0.6183278560638428, 0.5016001462936401, 0.1109316274523735, 0.23703736066818237, 0.48945075273513794, 0.06614242494106293, 0.2886432707309723, 0.6472116112709045, 0.5528389811515808, 0.260344922542572, 0.45896947383880615, 0.7337946891784668, 0.9727996587753296, 0.8410258889198303, 0.16144442558288574, 0.45416712760925293, 0.40877798199653625, 0.16939617693424225, 0.6642683744430542, 0.6432697176933289, 0.3228059709072113, 0.7809991836547852, 0.4492257535457611, 0.12247347831726074, 0.8468798995018005, 0.2833680212497711, 0.754226565361023, 0.2617167532444, 0.22498548030853271, 0.6968601942062378, 0.01867150515317917, 0.45630860328674316, 0.8501220345497131, 0.8321512937545776, 0.13769303262233734, 0.8910747170448303, 0.4661495089530945, 0.6513407230377197, 0.8318792581558228, 0.28195613622665405, 0.36692488193511963, 0.7187744379043579, 0.6934444904327393, 0.1999175250530243, 0.07552443444728851, 0.44622501730918884, 0.6139288544654846, 0.2826865613460541, 0.9559957981109619, 0.24807852506637573, 0.8561092615127563, 0.9534884691238403, 0.8511945009231567, 0.9334288239479065, 0.7140789031982422, 0.388191282749176, 0.8813086152076721, 0.2990174889564514, 0.8551315665245056, 0.6261729598045349, 0.47120681405067444, 0.4749518036842346, 0.2978686988353729, 0.7673436999320984, 0.5300029516220093, 0.7782717943191528, 0.48984426259994507, 0.5372359156608582, 0.7814760208129883, 0.9203964471817017, 0.12072478979825974, 0.9859831929206848, 0.7018551826477051, 0.5309759378433228, 0.2384367287158966, 0.9594374895095825, 0.5416489839553833, 0.6988224387168884, 0.17703697085380554, 0.8895614743232727, 0.4391710162162781, 0.7611968517303467, 0.7971492409706116, 0.4065127968788147, 0.4121829569339752, 0.7725569605827332, 0.4139801859855652, 0.0163713488727808, 0.6492041349411011, 0.08953416347503662, 0.8054971694946289, 0.6981039047241211, 0.7944212555885315, 0.13323798775672913, 0.8237714171409607, 0.5783477425575256, 0.776218593120575, 0.2682107388973236, 0.3471018671989441, 0.22101500630378723, 0.0013618111843243241, 0.46306857466697693, 0.9206815958023071, 0.4903622269630432, 0.016083497554063797, 0.2783198654651642, 0.3251529037952423, 0.5013194680213928, 0.11445412039756775, 0.012079134583473206, 0.2560001611709595, 0.9028116464614868, 0.19274145364761353, 0.05333879962563515, 0.7343361377716064, 0.7589075565338135, 0.3284699320793152, 0.07905074208974838, 0.612633466720581, 0.050045695155858994, 0.4453601837158203, 0.6522535681724548, 0.7844055891036987, 0.05484423041343689, 0.5774549841880798, 0.6620239615440369, 0.33169230818748474, 0.8406599760055542, 0.5894076228141785, 0.19468770921230316, 0.4066234827041626, 0.2146763801574707, 0.8467811942100525, 0.9844373464584351, 0.4828815460205078, 0.515873908996582, 0.08487104624509811, 0.6903231739997864, 0.9226033091545105, 0.802691638469696, 0.6860600113868713, 0.4897204637527466, 0.44427889585494995, 0.9516621232032776, 0.24357430636882782, 0.2184334099292755, 0.1172204315662384, 0.30623695254325867, 0.7359335422515869, 0.35206976532936096, 0.6945627331733704, 0.14384330809116364, 0.5232542753219604, 0.858997106552124, 0.09767534583806992, 0.3239775598049164, 0.5455408692359924, 0.5925885438919067, 0.44869863986968994, 0.918238639831543, 0.8670168519020081, 0.6096367239952087, 0.5765714049339294, 0.20481634140014648, 0.013852575793862343, 0.7634700536727905, 0.5896143913269043, 0.8080111742019653, 0.7057751417160034, 0.5197216868400574, 0.7997134923934937, 0.52923983335495, 0.03232930973172188, 0.018497133627533913, 0.7039249539375305, 0.011687240563333035, 0.5172359347343445, 0.5772852301597595, 0.10513359308242798, 0.2089967429637909, 0.5673447847366333, 0.18025241792201996, 0.4207831621170044, 0.5921681523323059, 0.09777862578630447, 0.08759112656116486, 0.9734905362129211, 0.9592893123626709, 0.15649233758449554, 0.7245137691497803, 0.14614325761795044, 0.06277640908956528, 0.7213056683540344, 0.9397366046905518, 0.6714769005775452, 0.5868414640426636, 0.17096030712127686, 0.04715782031416893, 0.6168940663337708, 0.06490743905305862, 0.20420877635478973, 0.9348860383033752, 0.04705149680376053, 0.9873403310775757, 0.16766494512557983, 0.7204188108444214, 0.4140930473804474, 0.539613664150238, 0.7032927870750427, 0.7088668942451477, 0.20077580213546753, 0.5277281403541565, 0.6421862244606018, 0.8054519891738892, 0.5765840411186218, 0.3639857769012451, 0.9252842664718628, 0.5993244647979736, 0.6518167853355408, 0.8031960725784302, 0.9634014368057251, 0.8032671809196472, 0.9200478196144104, 0.6832403540611267, 0.5457735657691956, 0.8271417617797852, 0.48793771862983704, 0.4425477385520935, 0.3262253701686859, 0.913882315158844, 0.02942078560590744, 0.6699893474578857, 0.8075922131538391, 0.6672304272651672, 0.15863613784313202, 0.6991033554077148, 0.5136383175849915, 0.4518413841724396, 0.11432988196611404, 0.8337645530700684, 0.19997699558734894, 0.7787659764289856, 0.8858902454376221, 0.3331146836280823, 0.4625246226787567, 0.709303617477417, 0.8493442535400391, 0.5922209620475769, 0.05531374737620354, 0.8209349513053894, 0.41280829906463623, 0.5246221423149109, 0.2334795892238617, 0.7214219570159912, 0.1311296820640564, 0.44521600008010864, 0.6902942657470703, 0.31479501724243164, 0.4011533260345459, 0.2884719967842102, 0.6499318480491638, 0.07902435213327408, 0.587889552116394, 0.4206700623035431, 0.6996663212776184, 0.35319074988365173, 0.025650616735219955, 0.23918427526950836, 0.7409505248069763, 0.4450435936450958, 0.5256019234657288, 0.4717833697795868, 0.8258699178695679, 0.5224175453186035, 0.7758104801177979, 0.5949121117591858, 0.9227606058120728, 0.9540846347808838, 0.5391230583190918, 0.4323936998844147, 0.5126331448554993, 0.5201613306999207, 0.9423797726631165, 0.48105093836784363, 0.9516801238059998, 0.28912651538848877, 0.02632157877087593, 0.9608991146087646, 0.01087308768182993, 0.024711405858397484, 0.6115622520446777, 0.6259920001029968, 0.4615266025066376, 0.9528838992118835, 0.1402873545885086, 0.11240574717521667, 0.658463180065155, 0.31963804364204407, 0.5899862051010132, 0.9113656878471375, 0.399395614862442, 0.13844920694828033, 0.027269160374999046, 0.25427162647247314, 0.42216628789901733, 0.04987042769789696, 0.18019147217273712, 0.7941862344741821, 0.9338135719299316, 0.46885237097740173, 0.23517246544361115, 0.4200786352157593, 0.48608848452568054, 0.4442487955093384, 0.09712281078100204, 0.07257167994976044, 0.4982982277870178, 0.5579163432121277, 0.6890251636505127, 0.9634112119674683, 0.038591355085372925, 0.011482151225209236, 0.10637529194355011, 0.47698545455932617, 0.7801839709281921, 0.7333822846412659, 0.7921286821365356, 0.7396711707115173, 0.918930172920227, 0.8444852232933044, 0.35946616530418396, 0.13169533014297485, 0.8867505192756653, 0.9843819737434387, 0.45732593536376953, 0.39677712321281433, 0.7165563702583313, 0.5174497365951538, 0.28845199942588806, 0.699768602848053, 0.22804494202136993, 0.7759913206100464, 0.017792699858546257, 0.22908005118370056, 0.033014751970767975, 0.38638630509376526, 0.7582269906997681, 0.9918963313102722, 0.2277938425540924, 0.3404541611671448, 0.2818209230899811, 0.5840474963188171, 0.20378121733665466, 0.2285759150981903, 0.3664989173412323, 0.26250016689300537, 0.8654340505599976, 0.293350487947464, 0.4659748673439026, 0.8676082491874695, 0.722886323928833, 0.7667917013168335, 0.3939172327518463, 0.010212404653429985, 0.6736516356468201, 0.1699751615524292, 0.41582465171813965, 0.05516976863145828, 0.16567884385585785, 0.6887815594673157, 0.6800487041473389, 0.31047749519348145, 0.3765132427215576, 0.7969440817832947, 0.6438823342323303, 0.15393388271331787, 0.6197165846824646, 0.6464699506759644, 0.6883950233459473, 0.1250983476638794, 0.06625806540250778, 0.0498005673289299, 0.36104512214660645, 0.14150340855121613, 0.3790360689163208, 0.3583654761314392, 0.49927186965942383, 0.05921294167637825, 0.35575079917907715, 0.5574421286582947, 0.15135829150676727, 0.5173702836036682, 0.08944489806890488, 0.7415786981582642, 0.610964834690094, 0.12629124522209167, 0.6571646332740784, 0.8580804467201233, 0.8047488927841187, 0.8786532282829285, 0.45353013277053833, 0.5217942595481873, 0.059725672006607056, 0.9192184209823608, 0.7132784128189087, 0.5126069188117981, 0.22028516232967377, 0.32300373911857605, 0.8696557879447937, 0.20453821122646332, 0.15377956628799438, 0.0202034842222929, 0.4030291736125946, 0.4018510580062866, 0.7322199940681458, 0.13991300761699677, 0.4270966351032257, 0.8927143216133118, 0.06635436415672302, 0.025243913754820824, 0.6089762449264526, 0.164319708943367, 0.6504514813423157, 0.9660682082176208, 0.013212698511779308, 0.17079849541187286, 0.2274859994649887, 0.8873509764671326, 0.11539249867200851, 0.8897441029548645, 0.7119466066360474, 0.8219953775405884, 0.4518047273159027, 0.5526160597801208, 0.5156668424606323, 0.3798842430114746, 0.7591387629508972, 0.9025423526763916, 0.2689059376716614, 0.6515424847602844, 0.2789366543292999, 0.5568122267723083, 0.6634635925292969, 0.6262637376785278, 0.2085745930671692, 0.9376164078712463, 0.22791308164596558, 0.7418540120124817, 0.4057253897190094, 0.04983304813504219, 0.387042760848999, 0.45331305265426636, 0.390306293964386, 0.9865545630455017, 0.018806803971529007, 0.5152460932731628, 0.996749997138977, 0.9486609101295471, 0.39116954803466797, 0.9426976442337036, 0.8067740797996521, 0.889554500579834, 0.8979684114456177, 0.6170464754104614, 0.4870646297931671, 0.7093315720558167, 0.16865132749080658, 0.8192521929740906, 0.5919701457023621, 0.49244385957717896, 0.3616722524166107, 0.8071326017379761, 0.5368145108222961, 0.5495433807373047, 0.7324987649917603, 0.34005603194236755, 0.5569435358047485, 0.4839858114719391, 0.623735249042511, 0.3610200881958008, 0.07797244936227798, 0.1523757129907608, 0.5165678262710571, 0.28967800736427307, 0.9974238276481628, 0.6469708681106567, 0.14755597710609436, 0.10067712515592575, 0.23362165689468384, 0.16978217661380768, 0.7000492811203003, 0.334881991147995, 0.0713207945227623, 0.9313864707946777, 0.5797341465950012, 0.6120589375495911, 0.14535905420780182, 0.10906676203012466, 0.9480545520782471, 0.6738556027412415, 0.18509434163570404, 0.2789756953716278, 0.5380411744117737, 0.8931823372840881, 0.801687479019165, 0.20614159107208252, 0.8113815784454346, 0.26392629742622375, 0.7574407458305359, 0.7305825352668762, 0.37589940428733826, 0.6839823126792908, 0.5169562101364136, 0.1914183497428894, 0.10160491615533829, 0.0792914405465126, 0.5758206844329834, 0.658331573009491, 0.26919224858283997, 0.5582151412963867, 0.4865487515926361, 0.0918538048863411, 0.6479836702346802, 0.6070619225502014], 100, map[nprobe, 16])</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>vector091</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vector091_value1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_168.csv</t>
-  </si>
-  <si>
-    <t>select id,feature_id,feature_index$distance from vector($vector091, feature, array[1.8621821403503418, 0.2708185911178589, 0.09189905226230621, 0.933274507522583, 0.7153090834617615, 0.7983555793762207, 0.750082790851593, 0.6883314847946167, 0.31263604760169983, 0.4566596448421478, 0.1965976357460022, 0.6520524621009827, 0.7225580811500549, 0.6169158816337585, 0.4757600426673889, 0.8930113315582275, 0.16275887191295624, 0.8677147626876831, 0.38705652952194214, 0.3529115915298462, 0.43060439825057983, 0.03425328806042671, 0.6368623375892639, 0.07757068425416946, 0.26419928669929504, 0.8277255296707153, 0.43137165904045105, 0.08842884749174118, 0.2713584899902344, 0.9682172536849976, 0.7530999183654785, 0.9315038323402405, 0.7047898173332214, 0.724409282207489, 0.6946336627006531, 0.7282527685165405, 0.6133454442024231, 0.16090521216392517, 0.9238371253013611, 0.6565712094306946, 0.8871753215789795, 0.14609310030937195, 0.7698654532432556, 0.7012138962745667, 0.5944278836250305, 0.09350641816854477, 0.5790979266166687, 0.4277772903442383, 0.7462419867515564, 0.9512709379196167, 0.7253237366676331, 0.45405250787734985, 0.5477305054664612, 0.691687285900116, 0.8943620920181274, 0.5033979415893555, 0.486189603805542, 0.7285860180854797, 0.17546194791793823, 0.05633839592337608, 0.2782122492790222, 0.6356047987937927, 0.21174538135528564, 0.4946894347667694], 32, map[nprobe, 2048])</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vector080_value1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select id,feature_id,feature_index$distance from vector($vector080, feature, array[0.010204729624092579, 0.033147819340229034, 0.02332344464957714, 0.04184626042842865, 0.04155944660305977, 0.014524550177156925, 0.014730843715369701, 0.04272615164518356, 0.051052533090114594, 0.046672314405441284, 0.019065575674176216, 0.026694519445300102, 0.036416951566934586, 0.037974897772073746, 0.019728070124983788, 0.02990221418440342, 0.026805777102708817, 0.0007336242124438286, 0.041178517043590546, 0.0470297671854496, 0.01944221742451191, 0.032790154218673706, 0.00401653815060854, 0.019652048125863075, 0.04972049966454506, 0.03470737859606743, 0.021164143458008766, 0.04202590510249138, 0.016881978139281273, 0.03026999905705452, 0.046309709548950195, 0.023240625858306885, 0.0427408292889595, 0.007660326547920704, 0.03752513229846954, 0.037542201578617096, 0.011657899245619774, 0.04927971586585045, 0.023558583110570908, 0.048451077193021774, 0.0031868144869804382, 0.00981936790049076, 0.0025232310872524977, 0.035959675908088684, 0.031683389097452164, 0.028416363522410393, 0.002308435970917344, 0.02991483546793461, 0.01756572164595127, 0.026799578219652176, 0.005962064489722252, 0.032353099435567856, 0.030155226588249207, 0.00036040949635207653, 0.032899145036935806, 0.04860064014792442, 0.04212149232625961, 0.05286107212305069, 0.05108783021569252, 0.042198218405246735, 0.01519902516156435, 0.03329743444919586, 0.025474268943071365, 0.01042615994811058, 0.02037101797759533, 0.002870551310479641, 0.024065179750323296, 0.05232415348291397, 0.006604038178920746, 0.006360971834510565, 0.0393507219851017, 0.031293295323848724, 0.02512999437749386, 0.005708037409931421, 0.012213451787829399, 0.047952838242053986, 0.02220587618649006, 0.028551781550049782, 0.0003308083687443286, 0.01601909101009369, 0.0232789758592844, 0.03261713311076164, 0.048924341797828674, 0.03334112465381622, 0.03761766478419304, 0.007983588613569736, 0.03975249454379082, 0.04427854344248772, 0.03376680612564087, 0.023354463279247284, 0.008129534311592579, 0.03028656728565693, 0.02814537286758423, 0.05069497600197792, 0.02559497579932213, 0.026777878403663635, 0.0286064762622118, 0.04364953935146332, 0.0030432920902967453, 0.03566879406571388, 0.04087426885962486, 0.03773050755262375, 0.04245946928858757, 0.029719168320298195, 0.05146266147494316, 0.007840960286557674, 0.0015796809457242489, 0.03164442256093025, 0.0060777622275054455, 0.05066199600696564, 0.01735466532409191, 0.010316583327949047, 0.02439357526600361, 0.049041807651519775, 0.04683943837881088, 0.013460123911499977, 0.018542950972914696, 0.009728874079883099, 0.04805039241909981, 0.037645936012268066, 0.03871854022145271, 0.047959376126527786, 0.04151618108153343, 0.031924761831760406, 0.015512024983763695, 0.008066792972385883, 0.01785910874605179, 0.035036325454711914, 0.003907910548150539, 0.0029309054370969534, 0.017220787703990936, 0.031462639570236206, 0.04549827426671982, 0.015295546501874924, 0.009221539832651615, 0.007141051348298788, 0.0529981330037117, 0.00956418365240097, 0.016919845715165138, 0.03028026968240738, 0.0004981200327165425, 0.04798925295472145, 0.05207035318017006, 0.02967301569879055, 0.004517004359513521, 0.017743369564414024, 0.03881286084651947, 0.00758938305079937, 0.029437201097607613, 0.014548561535775661, 0.05192401632666588, 0.03558168560266495, 0.013621972873806953, 0.0057711610570549965, 0.04135723412036896, 0.04169277101755142, 0.04058053717017174, 0.04872213676571846, 0.03509339690208435, 0.030284328386187553, 0.010750147514045238, 0.03720732033252716, 0.050735823810100555, 0.04741990938782692, 0.0529402419924736, 0.043622974306344986, 0.029045740142464638, 0.02404416911303997, 0.047451552003622055, 0.051858462393283844, 0.03161873295903206, 0.019505545496940613, 0.01721545308828354, 0.04643204063177109, 0.011489628814160824, 0.03916008025407791, 0.01948128081858158, 0.042711786925792694, 0.041706494987010956, 0.03737031668424606, 0.033183399587869644, 0.02630488947033882, 0.04478636756539345, 0.037942659109830856, 0.023652801290154457, 0.0016536302864551544, 0.019354501739144325, 0.038935042917728424, 0.025339610874652863, 0.018351567909121513, 0.03414802625775337, 0.0067245978862047195, 0.009136182256042957, 0.039274174720048904, 0.006768506485968828, 0.019696053117513657, 0.03220072388648987, 0.005493713542819023, 0.04275289922952652, 0.05038191005587578, 0.05216612294316292, 0.046954695135354996, 0.03344477340579033, 0.049579109996557236, 0.03861898183822632, 0.03818674385547638, 0.0021887891925871372, 0.023416904732584953, 0.015029522590339184, 0.01784958690404892, 0.004450568929314613, 0.04054031893610954, 0.027135562151670456, 0.03522258624434471, 0.033585041761398315, 0.019764091819524765, 0.023803653195500374, 0.022118208929896355, 0.025596538558602333, 0.05239442363381386, 0.019897133111953735, 0.0006610811105929315, 0.04912177100777626, 0.04653076454997063, 0.018742123618721962, 0.033575378358364105, 0.019066091626882553, 0.011339683085680008, 0.011899116449058056, 0.022355616092681885, 0.003884874749928713, 0.03467865660786629, 0.040265221148729324, 0.049665145576000214, 0.020055940374732018, 0.015821173787117004, 0.01981830596923828, 0.044102299958467484, 0.04801541566848755, 0.02276802621781826, 0.00011665943020489067, 0.002236034022644162, 0.00755485612899065, 0.031875867396593094, 0.005672535393387079, 0.015833521261811256, 0.0031113000586628914, 0.03310604766011238, 0.0012084837071597576, 0.045559875667095184, 0.016322564333677292, 0.040430255234241486, 0.030012983828783035, 0.002033502096310258, 0.03013242408633232, 0.03510675206780434, 0.009764980524778366, 0.0424884632229805, 0.03262877091765404, 0.029606876894831657, 0.03354119509458542, 0.03656172752380371, 0.012808301486074924, 0.04198315367102623, 0.045635681599378586, 0.03877915069460869, 0.03689022362232208, 0.025168271735310555, 0.045656755566596985, 0.035419512540102005, 0.01776326820254326, 0.027608344331383705, 0.021030189469456673, 0.001654415624216199, 0.03073575533926487, 0.045303959399461746, 0.0506981760263443, 0.036391157656908035, 0.004058168735355139, 0.021850179880857468, 0.002232631901279092, 0.00928119570016861, 0.030126312747597694, 0.009212159551680088, 0.03019070252776146, 0.02738768421113491, 0.04629604518413544, 0.038382258266210556, 0.04814605414867401, 0.01479215919971466, 0.013675902970135212, 0.03728228434920311, 0.048038288950920105, 0.052414074540138245, 0.03414975479245186, 0.017583781853318214, 0.03232547268271446, 0.04380713403224945, 0.0334598608314991, 0.006283293943852186, 0.015232418663799763, 0.05257684737443924, 0.023007642477750778, 0.030596930533647537, 0.028093036264181137, 0.010531546548008919, 0.008829441852867603, 0.026694271713495255, 0.05276103690266609, 0.0209930632263422, 0.0380447655916214, 0.009372706525027752, 0.0037669038865715265, 0.0083986297249794, 0.008608294650912285, 0.015113032422959805, 0.028597304597496986, 0.04120047390460968, 0.046907342970371246, 0.033962126821279526, 0.04542919993400574, 0.031860850751399994, 0.03697022795677185, 0.028622381389141083, 0.04738084226846695, 0.0027849117759615183, 0.0417303740978241, 0.007735266350209713, 0.00312762800604105, 0.0031434078700840473, 0.002769182901829481, 0.02749328315258026, 0.021579410880804062, 0.053264323621988297, 0.005784935317933559, 0.01744401641190052, 0.05316736549139023, 0.02137257717549801, 0.04706677421927452, 0.030325409024953842, 0.050791528075933456, 0.04717608541250229, 0.04152267053723335, 0.0016948288539424539, 0.051291197538375854, 0.027687732130289078, 0.011071727611124516, 0.04662783071398735, 0.011943462304770947, 0.007388184312731028, 0.038642920553684235, 0.05188639089465141, 0.028532078489661217, 0.0237001683562994, 0.0011781497159972787, 0.032288871705532074, 0.05140724778175354, 0.051556169986724854, 0.049554720520973206, 0.00984029471874237, 0.03319329023361206, 0.022003887221217155, 0.019344987347722054, 0.0019503142684698105, 0.046257562935352325, 0.03585030138492584, 0.004660749342292547, 0.04726020246744156, 0.04169205576181412, 0.01690692827105522, 0.04360220953822136, 0.027044054120779037, 0.001129242591559887, 0.02309933677315712, 0.02378089539706707, 0.012725044041872025, 0.044237978756427765, 0.0396832637488842, 0.031249357387423515, 0.026261474937200546, 0.025967780500650406, 0.014212743379175663, 0.03223680332303047, 0.040151067078113556, 0.014417537488043308, 0.027829883620142937, 0.0052392384968698025, 0.03802470117807388, 0.047104328870773315, 0.030214359983801842, 0.05298895761370659, 0.009523790329694748, 0.0006500571616925299, 0.024350246414542198, 0.0496465340256691, 0.04507872834801674, 0.025220433250069618, 0.04809083417057991, 0.012041718699038029, 0.016206221655011177, 0.038097016513347626, 0.038581762462854385, 0.0009951365645974874, 0.015228977426886559, 0.03093005158007145, 0.049595098942518234, 0.018062768504023552, 0.006398388650268316, 0.027508556842803955, 0.037255845963954926, 0.01591246947646141, 0.04590914025902748, 0.048264119774103165, 0.040952417999506, 0.013919203542172909, 0.05000372231006622, 0.05001368001103401, 0.03969820216298103, 0.048526693135499954, 0.012640043161809444, 0.02637334167957306, 0.043152742087841034, 0.05086212232708931, 0.03396701440215111, 0.04853280261158943, 0.03687911853194237, 0.0022881310433149338, 0.04441600665450096, 0.019711963832378387, 0.04990256205201149, 0.02573850378394127, 0.006678043399006128, 0.05138900503516197, 0.0009071872336789966, 0.03604971617460251, 0.007483062334358692, 0.008275534026324749, 0.034610383212566376, 0.05230547860264778, 0.037021420896053314, 0.0406002514064312, 0.02265641838312149, 0.007400658447295427, 0.0115190539509058, 0.04074552282691002, 0.0029095641802996397, 0.02611522190272808, 0.009627713821828365, 0.03361756354570389, 0.029371827840805054, 0.030215784907341003, 0.04360387101769447, 0.050032056868076324, 0.010278365574777126, 0.03798246383666992, 0.0371883250772953, 0.01376281026750803, 0.04879698529839516, 0.028365638107061386, 0.029730016365647316, 0.017198272049427032, 0.018043262884020805, 0.017706021666526794, 0.052154362201690674, 0.010827913880348206, 0.035541146993637085, 0.03062622807919979, 0.002769398968666792, 0.028924038633704185, 0.011080151423811913, 0.004853557795286179, 0.04634851589798927, 0.001458343816921115, 0.05161121487617493, 0.017450176179409027, 0.021860837936401367, 0.0072222016751766205, 0.006770473904907703, 0.022058306261897087, 0.03289925307035446, 0.007047576829791069, 0.05192327871918678, 0.009624779224395752, 0.040513720363378525, 0.025691024959087372, 0.04092554375529289, 0.016139335930347443, 0.0008085743174888194, 0.024689670652151108, 0.03747590631246567, 0.0035188565962016582, 0.03564693033695221, 0.01840815879404545, 0.031528692692518234, 0.012204653583467007, 0.014256843365728855, 0.04970381408929825, 0.04401948302984238, 0.0077496482990682125, 0.03447428718209267, 0.04709956794977188, 0.03950190916657448, 0.027478614822030067, 0.007206623442471027, 0.0021251202560961246, 0.04445516690611839, 0.006237193942070007, 0.027872459962964058, 0.04651917144656181, 0.0020624694880098104, 0.03689265623688698, 0.02537701092660427, 0.009018919430673122, 0.003365987678989768, 0.0017169961938634515, 0.012917441315948963, 0.006005357019603252, 0.021579081192612648, 0.0022417737636715174, 0.049370184540748596, 0.04983361065387726, 0.043181970715522766, 0.010035483166575432, 0.0312940739095211, 0.04814174771308899, 0.051542893052101135, 0.00359869166277349, 0.016921937465667725, 0.03713094815611839, 0.0341152586042881, 0.03370806574821472, 0.044158317148685455, 0.03799666091799736, 0.017875390127301216, 0.008935274556279182, 0.04074496403336525, 0.019145382568240166, 0.004689158406108618, 0.038873545825481415, 0.04694497957825661, 0.002198663307353854, 0.00931747816503048, 0.022384047508239746, 0.01814853772521019, 0.0023854218889027834, 0.006015187595039606, 0.02334016188979149, 0.0037869932129979134, 0.04349198192358017, 0.04614923521876335, 0.006986458320170641, 0.010295310989022255, 0.02331092394888401, 0.05173381045460701, 0.04123363271355629, 0.007021444849669933, 0.04940291866660118, 0.044107481837272644, 0.020925918594002724, 0.0074900249019265175, 0.0027779804076999426, 0.004940895829349756, 0.04726146534085274, 0.00895958673208952, 0.019335685297846794, 0.03486210107803345, 0.03222672641277313, 0.02104640193283558, 0.01996009610593319, 0.0033607061486691236, 0.022856222465634346, 0.038348883390426636, 0.04092298448085785, 0.01035651657730341, 0.04597633704543114, 0.0015303916297852993, 0.048068124800920486, 0.012603872455656528, 0.006851354613900185, 0.01693737506866455, 0.045224543660879135, 0.04434731602668762, 0.018417339771986008, 0.012786383740603924, 0.02854836732149124, 0.01446457114070654, 0.0018345799762755632, 0.03341299667954445, 0.02771783620119095, 0.0022355313412845135, 0.04036041721701622, 0.052662234753370285, 0.04270104318857193, 0.018328342586755753, 0.017870649695396423, 0.01873277686536312, 0.0236014723777771, 0.030877146869897842, 0.032905496656894684, 0.009437349624931812, 0.046088818460702896, 0.03784535080194473, 0.009091767482459545, 0.04556136205792427, 0.0010580202797427773, 0.034190833568573, 0.008649660274386406, 0.013723060488700867, 0.018255097791552544, 0.00032737827859818935, 0.02336731366813183, 0.04246889799833298, 0.036001451313495636, 0.029040461406111717, 0.030063703656196594, 0.0007451173732988536, 0.03244812414050102, 0.05267377942800522, 0.0119410939514637, 0.031288716942071915, 0.0444943904876709, 0.042226642370224, 0.01754225231707096, 0.01903282292187214, 0.051157694309949875, 0.0119244996458292, 0.011271309107542038, 0.008201060816645622, 0.026422815397381783, 0.013922568410634995, 0.02960863709449768, 0.0038851830177009106, 0.02016851119697094, 0.02456820383667946, 0.041482966393232346, 0.038387347012758255, 0.01231926679611206, 0.0013077986659482121, 0.013713174499571323, 0.02185221016407013, 0.00044752363464795053, 0.025125540792942047, 0.0454196035861969, 0.04918977990746498, 0.012331610545516014, 0.05280104652047157, 0.00031958590261638165, 0.01786315254867077, 0.042054034769535065, 0.005248988512903452, 0.023568786680698395, 0.020283201709389687, 0.04436333850026131, 0.03793547675013542, 0.018915507942438126, 0.0013126976555213332, 0.0369524210691452, 0.022443432360887527, 0.0457354299724102, 0.030641639605164528, 0.050089336931705475, 0.046902649104595184, 0.024411339312791824, 0.0009223322849720716, 0.0036581249441951513, 0.017082955688238144, 0.031559620052576065, 0.032505422830581665, 0.027303671464323997, 0.007713057100772858, 0.04671899229288101, 0.039335381239652634, 0.01989162713289261, 0.04415488988161087, 0.004808233119547367, 0.0034102832432836294, 0.026955703273415565, 0.04973577335476875, 0.00793713703751564, 0.030343536287546158, 0.003183587221428752, 0.009019634686410427, 0.0036780377849936485, 0.04827558994293213, 0.023839347064495087, 0.005668522324413061, 0.03544703498482704, 0.02676263079047203, 0.02180374227464199, 0.03878967463970184, 0.009169492870569229, 0.020485227927565575, 0.014226621016860008, 0.016422931104898453, 0.00944722443819046, 0.025712162256240845, 0.033553216606378555, 0.0031731794588267803, 0.010490743443369865, 0.014877060428261757, 0.03771480172872543, 0.017446402460336685, 0.022660940885543823, 0.0375521257519722, 0.008476108312606812, 0.023412754759192467, 0.03353258594870567, 0.04928986728191376, 0.01902138814330101, 0.04364588484168053, 0.0341087244451046, 0.03810013830661774, 0.03934536129236221, 0.051737766712903976, 0.013110239990055561, 0.0022688740864396095, 0.013203381560742855, 0.0023986210580915213, 0.03758910670876503, 0.044475678354501724, 0.049773555248975754, 0.02508527971804142, 0.027300048619508743, 0.014012387953698635, 0.005269512999802828, 0.04256492480635643, 0.007608959451317787, 0.04292828589677811, 0.04686378315091133, 0.02663724310696125, 0.04871407896280289, 0.021974576637148857, 0.010676505044102669, 0.03429139405488968, 0.021306011825799942, 0.03272809460759163, 0.02330126240849495, 0.031602345407009125, 0.05069557577371597, 0.02947191335260868, 0.048153724521398544, 0.007379948161542416, 8.225629426306114e-05, 0.032653648406267166, 0.028863554820418358, 0.04159433767199516, 0.0437716580927372, 0.05080052465200424, 0.032500285655260086, 0.01545642875134945, 0.04405480623245239, 0.020035305991768837, 0.03245877847075462, 0.03303660824894905, 0.023524440824985504, 0.01059116143733263, 0.023655179888010025, 0.049274373799562454, 0.035776033997535706, 0.004343794658780098, 0.03051299974322319, 0.006429243367165327, 0.053281061351299286, 0.05314341187477112, 0.03701634332537651, 0.01992143876850605, 0.02139369584619999, 0.04929206892848015, 0.013046812266111374, 0.03538058325648308, 0.025640882551670074, 0.0018618974136188626, 0.005908842198550701, 0.04770796000957489, 0.04753381758928299, 0.04876251891255379, 0.016379280015826225, 0.015900691971182823, 0.03512691333889961, 0.03171072155237198, 0.05245013162493706, 0.03280219808220863, 0.008243748918175697, 0.044303182512521744, 0.043462783098220825, 0.004904266446828842, 0.04730410501360893, 0.0008759222109802067, 0.04603278264403343, 0.04788919538259506, 0.04531008005142212, 0.03478683531284332, 0.01751706376671791, 0.02905944548547268, 0.01267789863049984, 0.046451300382614136, 0.009416903369128704, 0.019748589023947716, 0.04047293961048126, 0.016314394772052765, 0.03282974287867546, 0.011684490367770195, 0.04649067297577858, 0.03452018275856972, 0.02520301379263401, 0.012478360906243324, 0.04442852362990379, 0.005249244626611471, 0.0109244454652071, 0.012507148087024689, 0.03180855140089989, 0.033486634492874146, 0.05235859006643295, 0.00939468014985323, 0.04262519255280495, 0.008272930979728699, 0.019234731793403625, 0.0508892685174942, 0.006935227662324905, 0.014538083225488663, 0.043112222105264664, 0.05145309865474701, 0.0049245296977460384, 0.031086592003703117, 0.02160232700407505, 0.04791868478059769, 0.004517515655606985, 0.009651483036577702, 0.002699608216062188, 0.016053033992648125, 0.010133565403521061, 0.00045852080802433193, 0.006794801913201809, 0.006013770587742329, 0.038918670266866684, 0.012754619121551514, 0.04803835600614548, 0.01750420592725277, 0.04657161608338356, 0.012603000737726688, 0.02016519382596016, 0.02889486588537693, 0.027483047917485237, 0.022048616781830788, 0.020719977095723152, 0.018133845180273056, 0.021432265639305115, 0.024356184527277946, 0.02040690928697586, 0.03506499156355858, 0.046953730285167694, 0.030513711273670197, 0.022807275876402855, 0.013767150230705738, 0.04610414430499077, 0.009232786484062672, 0.030901623889803886, 0.038756851106882095, 0.03891802579164505, 0.02152610756456852, 0.006283528637140989, 0.040686607360839844, 0.028435060754418373, 0.03847217932343483, 0.0318436399102211, 0.02253156527876854, 0.04973893612623215, 0.05296175181865692, 0.02919049561023712, 0.03890908509492874, 0.001491086557507515, 0.046014729887247086, 0.05321003869175911, 0.017333481460809708, 0.045304443687200546, 0.032582130283117294, 0.023503826931118965, 0.028091037645936012, 0.04155117645859718, 0.013392691500484943, 0.024664288386702538, 0.045140642672777176, 0.03612712770700455, 0.019600804895162582, 0.007352148182690144, 0.02146289311349392, 0.049622297286987305, 0.03586812689900398, 0.022337820380926132, 0.030300261452794075, 0.0022224702406674623, 0.05305036902427673, 0.03298239782452583, 0.04153228923678398, 0.04962451010942459, 0.018202459439635277, 0.043228451162576675, 0.046500593423843384, 0.03548584505915642, 0.0313723087310791, 0.047600485384464264, 0.02390190027654171, 0.013021488673985004, 0.043381575495004654, 0.03714620694518089, 0.02182495780289173, 0.00030451681232079864, 0.05083274096250534, 0.03224967420101166, 0.00034880521707236767, 0.026561226695775986, 0.03189708665013313, 0.015992755070328712, 0.024603823199868202, 0.026407040655612946, 0.0312056727707386, 0.04633691534399986, 0.04434354230761528, 0.04148416966199875, 0.0292221587151289, 0.03268655762076378, 0.03912409022450447, 0.03017784282565117, 0.04130551964044571, 0.052566103637218475, 0.04205124080181122, 0.03273366019129753, 0.008433874696493149, 0.02538328990340233, 0.015113677829504013, 0.008195578120648861, 0.041412632912397385, 0.003141732420772314, 0.004215883556753397, 0.03539261221885681, 0.02788538858294487, 0.023785896599292755, 0.01634884439408779, 0.0009210030548274517, 0.01563998870551586, 0.014268863946199417, 0.0019568500574678183, 0.04284163936972618, 0.01778584159910679, 0.047522395849227905, 0.043178047984838486, 0.051370199769735336, 0.05102987587451935, 0.031499069184064865, 0.01659782975912094, 0.048936206847429276, 0.00269880797713995, 0.012028246186673641, 0.019326066598296165, 0.021966218948364258, 0.05033225193619728, 0.030871236696839333, 0.009951140731573105, 0.03178248926997185, 0.049753330647945404, 0.007147281430661678, 0.05233900994062424, 0.008198955096304417, 0.043730851262807846, 0.03610117360949516, 0.021531086415052414, 0.011577704921364784, 0.04121891036629677, 0.04516777768731117, 0.028223982080817223, 0.021824698895215988, 0.0009755022474564612, 0.007921029813587666, 0.04285738617181778, 0.02236703597009182, 0.018074527382850647, 0.015832820907235146, 0.0382564440369606, 0.05316615477204323, 0.02940700761973858, 0.0474163256585598, 0.008976494893431664, 0.04707895219326019, 0.03744599223136902, 0.0224912129342556, 0.046000003814697266, 0.012523806653916836, 0.030038325116038322, 0.0014152097282931209, 0.02025027945637703, 0.019279656931757927, 0.00486172828823328, 0.002411243738606572, 0.018246842548251152, 0.018937520682811737, 0.053061243146657944, 0.05031004548072815, 0.00698775053024292, 0.027619510889053345, 0.02542906254529953, 0.021372150629758835, 0.04958592355251312, 0.02745865285396576, 0.04313695430755615, 0.04698346555233002, 0.04063722491264343, 0.024745726957917213, 0.003938657697290182, 0.025069614872336388, 0.010687075555324554, 0.01111308578401804, 0.00945984199643135, 0.01887504570186138, 0.04858093708753586, 0.023099292069673538, 0.009500138461589813, 0.04007745906710625, 0.0026892228052020073, 0.004404826555401087, 0.002055841265246272, 0.02479143626987934, 0.032173801213502884, 0.00968628004193306, 0.027655456215143204], 1, map[nprobe, 16])</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select id,feature_id,feature_index$distance from vector($vector080, feature, array[0.010204729624092579, 0.033147819340229034, 0.02332344464957714, 0.04184626042842865, 0.04155944660305977, 0.014524550177156925, 0.014730843715369701, 0.04272615164518356, 0.051052533090114594, 0.046672314405441284, 0.019065575674176216, 0.026694519445300102, 0.036416951566934586, 0.037974897772073746, 0.019728070124983788, 0.02990221418440342, 0.026805777102708817, 0.0007336242124438286, 0.041178517043590546, 0.0470297671854496, 0.01944221742451191, 0.032790154218673706, 0.00401653815060854, 0.019652048125863075, 0.04972049966454506, 0.03470737859606743, 0.021164143458008766, 0.04202590510249138, 0.016881978139281273, 0.03026999905705452, 0.046309709548950195, 0.023240625858306885, 0.0427408292889595, 0.007660326547920704, 0.03752513229846954, 0.037542201578617096, 0.011657899245619774, 0.04927971586585045, 0.023558583110570908, 0.048451077193021774, 0.0031868144869804382, 0.00981936790049076, 0.0025232310872524977, 0.035959675908088684, 0.031683389097452164, 0.028416363522410393, 0.002308435970917344, 0.02991483546793461, 0.01756572164595127, 0.026799578219652176, 0.005962064489722252, 0.032353099435567856, 0.030155226588249207, 0.00036040949635207653, 0.032899145036935806, 0.04860064014792442, 0.04212149232625961, 0.05286107212305069, 0.05108783021569252, 0.042198218405246735, 0.01519902516156435, 0.03329743444919586, 0.025474268943071365, 0.01042615994811058, 0.02037101797759533, 0.002870551310479641, 0.024065179750323296, 0.05232415348291397, 0.006604038178920746, 0.006360971834510565, 0.0393507219851017, 0.031293295323848724, 0.02512999437749386, 0.005708037409931421, 0.012213451787829399, 0.047952838242053986, 0.02220587618649006, 0.028551781550049782, 0.0003308083687443286, 0.01601909101009369, 0.0232789758592844, 0.03261713311076164, 0.048924341797828674, 0.03334112465381622, 0.03761766478419304, 0.007983588613569736, 0.03975249454379082, 0.04427854344248772, 0.03376680612564087, 0.023354463279247284, 0.008129534311592579, 0.03028656728565693, 0.02814537286758423, 0.05069497600197792, 0.02559497579932213, 0.026777878403663635, 0.0286064762622118, 0.04364953935146332, 0.0030432920902967453, 0.03566879406571388, 0.04087426885962486, 0.03773050755262375, 0.04245946928858757, 0.029719168320298195, 0.05146266147494316, 0.007840960286557674, 0.0015796809457242489, 0.03164442256093025, 0.0060777622275054455, 0.05066199600696564, 0.01735466532409191, 0.010316583327949047, 0.02439357526600361, 0.049041807651519775, 0.04683943837881088, 0.013460123911499977, 0.018542950972914696, 0.009728874079883099, 0.04805039241909981, 0.037645936012268066, 0.03871854022145271, 0.047959376126527786, 0.04151618108153343, 0.031924761831760406, 0.015512024983763695, 0.008066792972385883, 0.01785910874605179, 0.035036325454711914, 0.003907910548150539, 0.0029309054370969534, 0.017220787703990936, 0.031462639570236206, 0.04549827426671982, 0.015295546501874924, 0.009221539832651615, 0.007141051348298788, 0.0529981330037117, 0.00956418365240097, 0.016919845715165138, 0.03028026968240738, 0.0004981200327165425, 0.04798925295472145, 0.05207035318017006, 0.02967301569879055, 0.004517004359513521, 0.017743369564414024, 0.03881286084651947, 0.00758938305079937, 0.029437201097607613, 0.014548561535775661, 0.05192401632666588, 0.03558168560266495, 0.013621972873806953, 0.0057711610570549965, 0.04135723412036896, 0.04169277101755142, 0.04058053717017174, 0.04872213676571846, 0.03509339690208435, 0.030284328386187553, 0.010750147514045238, 0.03720732033252716, 0.050735823810100555, 0.04741990938782692, 0.0529402419924736, 0.043622974306344986, 0.029045740142464638, 0.02404416911303997, 0.047451552003622055, 0.051858462393283844, 0.03161873295903206, 0.019505545496940613, 0.01721545308828354, 0.04643204063177109, 0.011489628814160824, 0.03916008025407791, 0.01948128081858158, 0.042711786925792694, 0.041706494987010956, 0.03737031668424606, 0.033183399587869644, 0.02630488947033882, 0.04478636756539345, 0.037942659109830856, 0.023652801290154457, 0.0016536302864551544, 0.019354501739144325, 0.038935042917728424, 0.025339610874652863, 0.018351567909121513, 0.03414802625775337, 0.0067245978862047195, 0.009136182256042957, 0.039274174720048904, 0.006768506485968828, 0.019696053117513657, 0.03220072388648987, 0.005493713542819023, 0.04275289922952652, 0.05038191005587578, 0.05216612294316292, 0.046954695135354996, 0.03344477340579033, 0.049579109996557236, 0.03861898183822632, 0.03818674385547638, 0.0021887891925871372, 0.023416904732584953, 0.015029522590339184, 0.01784958690404892, 0.004450568929314613, 0.04054031893610954, 0.027135562151670456, 0.03522258624434471, 0.033585041761398315, 0.019764091819524765, 0.023803653195500374, 0.022118208929896355, 0.025596538558602333, 0.05239442363381386, 0.019897133111953735, 0.0006610811105929315, 0.04912177100777626, 0.04653076454997063, 0.018742123618721962, 0.033575378358364105, 0.019066091626882553, 0.011339683085680008, 0.011899116449058056, 0.022355616092681885, 0.003884874749928713, 0.03467865660786629, 0.040265221148729324, 0.049665145576000214, 0.020055940374732018, 0.015821173787117004, 0.01981830596923828, 0.044102299958467484, 0.04801541566848755, 0.02276802621781826, 0.00011665943020489067, 0.002236034022644162, 0.00755485612899065, 0.031875867396593094, 0.005672535393387079, 0.015833521261811256, 0.0031113000586628914, 0.03310604766011238, 0.0012084837071597576, 0.045559875667095184, 0.016322564333677292, 0.040430255234241486, 0.030012983828783035, 0.002033502096310258, 0.03013242408633232, 0.03510675206780434, 0.009764980524778366, 0.0424884632229805, 0.03262877091765404, 0.029606876894831657, 0.03354119509458542, 0.03656172752380371, 0.012808301486074924, 0.04198315367102623, 0.045635681599378586, 0.03877915069460869, 0.03689022362232208, 0.025168271735310555, 0.045656755566596985, 0.035419512540102005, 0.01776326820254326, 0.027608344331383705, 0.021030189469456673, 0.001654415624216199, 0.03073575533926487, 0.045303959399461746, 0.0506981760263443, 0.036391157656908035, 0.004058168735355139, 0.021850179880857468, 0.002232631901279092, 0.00928119570016861, 0.030126312747597694, 0.009212159551680088, 0.03019070252776146, 0.02738768421113491, 0.04629604518413544, 0.038382258266210556, 0.04814605414867401, 0.01479215919971466, 0.013675902970135212, 0.03728228434920311, 0.048038288950920105, 0.052414074540138245, 0.03414975479245186, 0.017583781853318214, 0.03232547268271446, 0.04380713403224945, 0.0334598608314991, 0.006283293943852186, 0.015232418663799763, 0.05257684737443924, 0.023007642477750778, 0.030596930533647537, 0.028093036264181137, 0.010531546548008919, 0.008829441852867603, 0.026694271713495255, 0.05276103690266609, 0.0209930632263422, 0.0380447655916214, 0.009372706525027752, 0.0037669038865715265, 0.0083986297249794, 0.008608294650912285, 0.015113032422959805, 0.028597304597496986, 0.04120047390460968, 0.046907342970371246, 0.033962126821279526, 0.04542919993400574, 0.031860850751399994, 0.03697022795677185, 0.028622381389141083, 0.04738084226846695, 0.0027849117759615183, 0.0417303740978241, 0.007735266350209713, 0.00312762800604105, 0.0031434078700840473, 0.002769182901829481, 0.02749328315258026, 0.021579410880804062, 0.053264323621988297, 0.005784935317933559, 0.01744401641190052, 0.05316736549139023, 0.02137257717549801, 0.04706677421927452, 0.030325409024953842, 0.050791528075933456, 0.04717608541250229, 0.04152267053723335, 0.0016948288539424539, 0.051291197538375854, 0.027687732130289078, 0.011071727611124516, 0.04662783071398735, 0.011943462304770947, 0.007388184312731028, 0.038642920553684235, 0.05188639089465141, 0.028532078489661217, 0.0237001683562994, 0.0011781497159972787, 0.032288871705532074, 0.05140724778175354, 0.051556169986724854, 0.049554720520973206, 0.00984029471874237, 0.03319329023361206, 0.022003887221217155, 0.019344987347722054, 0.0019503142684698105, 0.046257562935352325, 0.03585030138492584, 0.004660749342292547, 0.04726020246744156, 0.04169205576181412, 0.01690692827105522, 0.04360220953822136, 0.027044054120779037, 0.001129242591559887, 0.02309933677315712, 0.02378089539706707, 0.012725044041872025, 0.044237978756427765, 0.0396832637488842, 0.031249357387423515, 0.026261474937200546, 0.025967780500650406, 0.014212743379175663, 0.03223680332303047, 0.040151067078113556, 0.014417537488043308, 0.027829883620142937, 0.0052392384968698025, 0.03802470117807388, 0.047104328870773315, 0.030214359983801842, 0.05298895761370659, 0.009523790329694748, 0.0006500571616925299, 0.024350246414542198, 0.0496465340256691, 0.04507872834801674, 0.025220433250069618, 0.04809083417057991, 0.012041718699038029, 0.016206221655011177, 0.038097016513347626, 0.038581762462854385, 0.0009951365645974874, 0.015228977426886559, 0.03093005158007145, 0.049595098942518234, 0.018062768504023552, 0.006398388650268316, 0.027508556842803955, 0.037255845963954926, 0.01591246947646141, 0.04590914025902748, 0.048264119774103165, 0.040952417999506, 0.013919203542172909, 0.05000372231006622, 0.05001368001103401, 0.03969820216298103, 0.048526693135499954, 0.012640043161809444, 0.02637334167957306, 0.043152742087841034, 0.05086212232708931, 0.03396701440215111, 0.04853280261158943, 0.03687911853194237, 0.0022881310433149338, 0.04441600665450096, 0.019711963832378387, 0.04990256205201149, 0.02573850378394127, 0.006678043399006128, 0.05138900503516197, 0.0009071872336789966, 0.03604971617460251, 0.007483062334358692, 0.008275534026324749, 0.034610383212566376, 0.05230547860264778, 0.037021420896053314, 0.0406002514064312, 0.02265641838312149, 0.007400658447295427, 0.0115190539509058, 0.04074552282691002, 0.0029095641802996397, 0.02611522190272808, 0.009627713821828365, 0.03361756354570389, 0.029371827840805054, 0.030215784907341003, 0.04360387101769447, 0.050032056868076324, 0.010278365574777126, 0.03798246383666992, 0.0371883250772953, 0.01376281026750803, 0.04879698529839516, 0.028365638107061386, 0.029730016365647316, 0.017198272049427032, 0.018043262884020805, 0.017706021666526794, 0.052154362201690674, 0.010827913880348206, 0.035541146993637085, 0.03062622807919979, 0.002769398968666792, 0.028924038633704185, 0.011080151423811913, 0.004853557795286179, 0.04634851589798927, 0.001458343816921115, 0.05161121487617493, 0.017450176179409027, 0.021860837936401367, 0.0072222016751766205, 0.006770473904907703, 0.022058306261897087, 0.03289925307035446, 0.007047576829791069, 0.05192327871918678, 0.009624779224395752, 0.040513720363378525, 0.025691024959087372, 0.04092554375529289, 0.016139335930347443, 0.0008085743174888194, 0.024689670652151108, 0.03747590631246567, 0.0035188565962016582, 0.03564693033695221, 0.01840815879404545, 0.031528692692518234, 0.012204653583467007, 0.014256843365728855, 0.04970381408929825, 0.04401948302984238, 0.0077496482990682125, 0.03447428718209267, 0.04709956794977188, 0.03950190916657448, 0.027478614822030067, 0.007206623442471027, 0.0021251202560961246, 0.04445516690611839, 0.006237193942070007, 0.027872459962964058, 0.04651917144656181, 0.0020624694880098104, 0.03689265623688698, 0.02537701092660427, 0.009018919430673122, 0.003365987678989768, 0.0017169961938634515, 0.012917441315948963, 0.006005357019603252, 0.021579081192612648, 0.0022417737636715174, 0.049370184540748596, 0.04983361065387726, 0.043181970715522766, 0.010035483166575432, 0.0312940739095211, 0.04814174771308899, 0.051542893052101135, 0.00359869166277349, 0.016921937465667725, 0.03713094815611839, 0.0341152586042881, 0.03370806574821472, 0.044158317148685455, 0.03799666091799736, 0.017875390127301216, 0.008935274556279182, 0.04074496403336525, 0.019145382568240166, 0.004689158406108618, 0.038873545825481415, 0.04694497957825661, 0.002198663307353854, 0.00931747816503048, 0.022384047508239746, 0.01814853772521019, 0.0023854218889027834, 0.006015187595039606, 0.02334016188979149, 0.0037869932129979134, 0.04349198192358017, 0.04614923521876335, 0.006986458320170641, 0.010295310989022255, 0.02331092394888401, 0.05173381045460701, 0.04123363271355629, 0.007021444849669933, 0.04940291866660118, 0.044107481837272644, 0.020925918594002724, 0.0074900249019265175, 0.0027779804076999426, 0.004940895829349756, 0.04726146534085274, 0.00895958673208952, 0.019335685297846794, 0.03486210107803345, 0.03222672641277313, 0.02104640193283558, 0.01996009610593319, 0.0033607061486691236, 0.022856222465634346, 0.038348883390426636, 0.04092298448085785, 0.01035651657730341, 0.04597633704543114, 0.0015303916297852993, 0.048068124800920486, 0.012603872455656528, 0.006851354613900185, 0.01693737506866455, 0.045224543660879135, 0.04434731602668762, 0.018417339771986008, 0.012786383740603924, 0.02854836732149124, 0.01446457114070654, 0.0018345799762755632, 0.03341299667954445, 0.02771783620119095, 0.0022355313412845135, 0.04036041721701622, 0.052662234753370285, 0.04270104318857193, 0.018328342586755753, 0.017870649695396423, 0.01873277686536312, 0.0236014723777771, 0.030877146869897842, 0.032905496656894684, 0.009437349624931812, 0.046088818460702896, 0.03784535080194473, 0.009091767482459545, 0.04556136205792427, 0.0010580202797427773, 0.034190833568573, 0.008649660274386406, 0.013723060488700867, 0.018255097791552544, 0.00032737827859818935, 0.02336731366813183, 0.04246889799833298, 0.036001451313495636, 0.029040461406111717, 0.030063703656196594, 0.0007451173732988536, 0.03244812414050102, 0.05267377942800522, 0.0119410939514637, 0.031288716942071915, 0.0444943904876709, 0.042226642370224, 0.01754225231707096, 0.01903282292187214, 0.051157694309949875, 0.0119244996458292, 0.011271309107542038, 0.008201060816645622, 0.026422815397381783, 0.013922568410634995, 0.02960863709449768, 0.0038851830177009106, 0.02016851119697094, 0.02456820383667946, 0.041482966393232346, 0.038387347012758255, 0.01231926679611206, 0.0013077986659482121, 0.013713174499571323, 0.02185221016407013, 0.00044752363464795053, 0.025125540792942047, 0.0454196035861969, 0.04918977990746498, 0.012331610545516014, 0.05280104652047157, 0.00031958590261638165, 0.01786315254867077, 0.042054034769535065, 0.005248988512903452, 0.023568786680698395, 0.020283201709389687, 0.04436333850026131, 0.03793547675013542, 0.018915507942438126, 0.0013126976555213332, 0.0369524210691452, 0.022443432360887527, 0.0457354299724102, 0.030641639605164528, 0.050089336931705475, 0.046902649104595184, 0.024411339312791824, 0.0009223322849720716, 0.0036581249441951513, 0.017082955688238144, 0.031559620052576065, 0.032505422830581665, 0.027303671464323997, 0.007713057100772858, 0.04671899229288101, 0.039335381239652634, 0.01989162713289261, 0.04415488988161087, 0.004808233119547367, 0.0034102832432836294, 0.026955703273415565, 0.04973577335476875, 0.00793713703751564, 0.030343536287546158, 0.003183587221428752, 0.009019634686410427, 0.0036780377849936485, 0.04827558994293213, 0.023839347064495087, 0.005668522324413061, 0.03544703498482704, 0.02676263079047203, 0.02180374227464199, 0.03878967463970184, 0.009169492870569229, 0.020485227927565575, 0.014226621016860008, 0.016422931104898453, 0.00944722443819046, 0.025712162256240845, 0.033553216606378555, 0.0031731794588267803, 0.010490743443369865, 0.014877060428261757, 0.03771480172872543, 0.017446402460336685, 0.022660940885543823, 0.0375521257519722, 0.008476108312606812, 0.023412754759192467, 0.03353258594870567, 0.04928986728191376, 0.01902138814330101, 0.04364588484168053, 0.0341087244451046, 0.03810013830661774, 0.03934536129236221, 0.051737766712903976, 0.013110239990055561, 0.0022688740864396095, 0.013203381560742855, 0.0023986210580915213, 0.03758910670876503, 0.044475678354501724, 0.049773555248975754, 0.02508527971804142, 0.027300048619508743, 0.014012387953698635, 0.005269512999802828, 0.04256492480635643, 0.007608959451317787, 0.04292828589677811, 0.04686378315091133, 0.02663724310696125, 0.04871407896280289, 0.021974576637148857, 0.010676505044102669, 0.03429139405488968, 0.021306011825799942, 0.03272809460759163, 0.02330126240849495, 0.031602345407009125, 0.05069557577371597, 0.02947191335260868, 0.048153724521398544, 0.007379948161542416, 8.225629426306114e-05, 0.032653648406267166, 0.028863554820418358, 0.04159433767199516, 0.0437716580927372, 0.05080052465200424, 0.032500285655260086, 0.01545642875134945, 0.04405480623245239, 0.020035305991768837, 0.03245877847075462, 0.03303660824894905, 0.023524440824985504, 0.01059116143733263, 0.023655179888010025, 0.049274373799562454, 0.035776033997535706, 0.004343794658780098, 0.03051299974322319, 0.006429243367165327, 0.053281061351299286, 0.05314341187477112, 0.03701634332537651, 0.01992143876850605, 0.02139369584619999, 0.04929206892848015, 0.013046812266111374, 0.03538058325648308, 0.025640882551670074, 0.0018618974136188626, 0.005908842198550701, 0.04770796000957489, 0.04753381758928299, 0.04876251891255379, 0.016379280015826225, 0.015900691971182823, 0.03512691333889961, 0.03171072155237198, 0.05245013162493706, 0.03280219808220863, 0.008243748918175697, 0.044303182512521744, 0.043462783098220825, 0.004904266446828842, 0.04730410501360893, 0.0008759222109802067, 0.04603278264403343, 0.04788919538259506, 0.04531008005142212, 0.03478683531284332, 0.01751706376671791, 0.02905944548547268, 0.01267789863049984, 0.046451300382614136, 0.009416903369128704, 0.019748589023947716, 0.04047293961048126, 0.016314394772052765, 0.03282974287867546, 0.011684490367770195, 0.04649067297577858, 0.03452018275856972, 0.02520301379263401, 0.012478360906243324, 0.04442852362990379, 0.005249244626611471, 0.0109244454652071, 0.012507148087024689, 0.03180855140089989, 0.033486634492874146, 0.05235859006643295, 0.00939468014985323, 0.04262519255280495, 0.008272930979728699, 0.019234731793403625, 0.0508892685174942, 0.006935227662324905, 0.014538083225488663, 0.043112222105264664, 0.05145309865474701, 0.0049245296977460384, 0.031086592003703117, 0.02160232700407505, 0.04791868478059769, 0.004517515655606985, 0.009651483036577702, 0.002699608216062188, 0.016053033992648125, 0.010133565403521061, 0.00045852080802433193, 0.006794801913201809, 0.006013770587742329, 0.038918670266866684, 0.012754619121551514, 0.04803835600614548, 0.01750420592725277, 0.04657161608338356, 0.012603000737726688, 0.02016519382596016, 0.02889486588537693, 0.027483047917485237, 0.022048616781830788, 0.020719977095723152, 0.018133845180273056, 0.021432265639305115, 0.024356184527277946, 0.02040690928697586, 0.03506499156355858, 0.046953730285167694, 0.030513711273670197, 0.022807275876402855, 0.013767150230705738, 0.04610414430499077, 0.009232786484062672, 0.030901623889803886, 0.038756851106882095, 0.03891802579164505, 0.02152610756456852, 0.006283528637140989, 0.040686607360839844, 0.028435060754418373, 0.03847217932343483, 0.0318436399102211, 0.02253156527876854, 0.04973893612623215, 0.05296175181865692, 0.02919049561023712, 0.03890908509492874, 0.001491086557507515, 0.046014729887247086, 0.05321003869175911, 0.017333481460809708, 0.045304443687200546, 0.032582130283117294, 0.023503826931118965, 0.028091037645936012, 0.04155117645859718, 0.013392691500484943, 0.024664288386702538, 0.045140642672777176, 0.03612712770700455, 0.019600804895162582, 0.007352148182690144, 0.02146289311349392, 0.049622297286987305, 0.03586812689900398, 0.022337820380926132, 0.030300261452794075, 0.0022224702406674623, 0.05305036902427673, 0.03298239782452583, 0.04153228923678398, 0.04962451010942459, 0.018202459439635277, 0.043228451162576675, 0.046500593423843384, 0.03548584505915642, 0.0313723087310791, 0.047600485384464264, 0.02390190027654171, 0.013021488673985004, 0.043381575495004654, 0.03714620694518089, 0.02182495780289173, 0.00030451681232079864, 0.05083274096250534, 0.03224967420101166, 0.00034880521707236767, 0.026561226695775986, 0.03189708665013313, 0.015992755070328712, 0.024603823199868202, 0.026407040655612946, 0.0312056727707386, 0.04633691534399986, 0.04434354230761528, 0.04148416966199875, 0.0292221587151289, 0.03268655762076378, 0.03912409022450447, 0.03017784282565117, 0.04130551964044571, 0.052566103637218475, 0.04205124080181122, 0.03273366019129753, 0.008433874696493149, 0.02538328990340233, 0.015113677829504013, 0.008195578120648861, 0.041412632912397385, 0.003141732420772314, 0.004215883556753397, 0.03539261221885681, 0.02788538858294487, 0.023785896599292755, 0.01634884439408779, 0.0009210030548274517, 0.01563998870551586, 0.014268863946199417, 0.0019568500574678183, 0.04284163936972618, 0.01778584159910679, 0.047522395849227905, 0.043178047984838486, 0.051370199769735336, 0.05102987587451935, 0.031499069184064865, 0.01659782975912094, 0.048936206847429276, 0.00269880797713995, 0.012028246186673641, 0.019326066598296165, 0.021966218948364258, 0.05033225193619728, 0.030871236696839333, 0.009951140731573105, 0.03178248926997185, 0.049753330647945404, 0.007147281430661678, 0.05233900994062424, 0.008198955096304417, 0.043730851262807846, 0.03610117360949516, 0.021531086415052414, 0.011577704921364784, 0.04121891036629677, 0.04516777768731117, 0.028223982080817223, 0.021824698895215988, 0.0009755022474564612, 0.007921029813587666, 0.04285738617181778, 0.02236703597009182, 0.018074527382850647, 0.015832820907235146, 0.0382564440369606, 0.05316615477204323, 0.02940700761973858, 0.0474163256585598, 0.008976494893431664, 0.04707895219326019, 0.03744599223136902, 0.0224912129342556, 0.046000003814697266, 0.012523806653916836, 0.030038325116038322, 0.0014152097282931209, 0.02025027945637703, 0.019279656931757927, 0.00486172828823328, 0.002411243738606572, 0.018246842548251152, 0.018937520682811737, 0.053061243146657944, 0.05031004548072815, 0.00698775053024292, 0.027619510889053345, 0.02542906254529953, 0.021372150629758835, 0.04958592355251312, 0.02745865285396576, 0.04313695430755615, 0.04698346555233002, 0.04063722491264343, 0.024745726957917213, 0.003938657697290182, 0.025069614872336388, 0.010687075555324554, 0.01111308578401804, 0.00945984199643135, 0.01887504570186138, 0.04858093708753586, 0.023099292069673538, 0.009500138461589813, 0.04007745906710625, 0.0026892228052020073, 0.004404826555401087, 0.002055841265246272, 0.02479143626987934, 0.032173801213502884, 0.00968628004193306, 0.027655456215143204], 10, map[nprobe, 16])</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_169.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_170.csv</t>
-  </si>
-  <si>
-    <t>select id,feature_id,feature_index$distance from vector($vector073, feature, array[0.57568294], 10)</t>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_182.csv</t>
+  </si>
+  <si>
+    <t>vector103_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - dotproduct距离 - 64维度 - 2048求top8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_183.csv</t>
+  </si>
+  <si>
+    <t>vector104_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - dotproduct距离 - 128维度 - 1024求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - dotproduct距离 - 256维度 - 1024求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - dotproduct距离 - 512维度 - 1024求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_184.csv</t>
+  </si>
+  <si>
+    <t>vector105_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector106_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector107_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector105, feature, array[0.14634497463703156, 0.06606714427471161, 0.0747629776597023, 0.09755537658929825, 0.027689022943377495, 0.06991435587406158, 0.004096047021448612, 0.010261375457048416, 0.009377717971801758, 0.05315619707107544, 0.0019728976767510176, 0.08045880496501923, 0.07953483611345291, 0.03832383453845978, 0.07482203841209412, 0.06068996340036392, 0.03964470326900482, 0.07892917096614838, 0.06464552879333496, 0.0703706294298172, 0.07579842954874039, 0.04779214784502983, 0.0577172115445137, 0.10259903967380524, 0.09542334079742432, 0.07556284964084625, 0.04146209731698036, 0.046105459332466125, 0.037321787327528, 0.058095116168260574, 0.07685650140047073, 0.02945804037153721, 0.017812492325901985, 0.03439406678080559, 0.06403664499521255, 0.08897273987531662, 0.05927211046218872, 0.026970675215125084, 0.10100489109754562, 0.03526098281145096, 0.0783323422074318, 0.08456544578075409, 0.0740169957280159, 0.012809330597519875, 0.014808033592998981, 0.07303336262702942, 0.09882145375013351, 0.04252012446522713, 0.09358353912830353, 0.09612904489040375, 0.05598527938127518, 0.04731655865907669, 0.07962753623723984, 0.024980468675494194, 0.02726585976779461, 0.025730395689606667, 0.0892348438501358, 0.09624539315700531, 0.06598717719316483, 0.09674268215894699, 0.042744237929582596, 0.0598059818148613, 0.0767139121890068, 0.062439098954200745, 0.025416748598217964, 0.049647919833660126, 0.06668975204229355, 0.08616765588521957, 0.0020917586516588926, 0.07452128827571869, 0.009620729833841324, 0.04580679535865784, 0.03333989530801773, 0.03802449628710747, 0.0620679147541523, 0.042266786098480225, 0.07716717571020126, 0.04561847820878029, 0.09706221520900726, 0.07150820642709732, 0.08585374057292938, 0.027610383927822113, 0.07938110828399658, 0.023716194555163383, 0.06796640157699585, 0.0710572749376297, 0.04375806823372841, 0.03772520646452904, 0.021592877805233, 0.10481014847755432, 0.0915284976363182, 0.05959180369973183, 0.041032157838344574, 0.09887409210205078, 0.07164005190134048, 0.03195399045944214, 0.09275461733341217, 0.07765515148639679, 0.0415746346116066, 0.015385233797132969, 0.020173469558358192, 0.06096643954515457, 0.042707525193691254, 0.018754614517092705, 0.09675773978233337, 0.09766068309545517, 0.02563217096030712, 0.047106195241212845, 0.022341907024383545, 0.03904648497700691, 0.09178859740495682, 0.0865921750664711, 0.08797325938940048, 0.10045512765645981, 0.10288543254137039, 0.029143791645765305, 0.018867170438170433, 0.10062182694673538, 0.03172631189227104, 0.044401638209819794, 0.08548415452241898, 0.05137927830219269, 0.09881174564361572, 0.03731298819184303, 0.020689653232693672, 0.005873892456293106, 0.10507112741470337, 0.052145276218652725, 0.06271661072969437, 0.025037093088030815, 0.004600174259394407, 0.052073605358600616, 0.05243080109357834, 0.08471406251192093, 0.09001556038856506, 0.08056541532278061, 0.07987616211175919, 0.09430065751075745, 0.016940100118517876, 0.020851515233516693, 0.028193267062306404, 0.03875293210148811, 0.07195708900690079, 0.08786512911319733, 0.10363910347223282, 0.04028391093015671, 0.03659685328602791, 0.038815341889858246, 0.0464271679520607, 0.05033800005912781, 0.05584758147597313, 0.08479233831167221, 0.0030631462577730417, 0.06840672343969345, 0.0035168523900210857, 0.08092322200536728, 0.06231076642870903, 0.015634020790457726, 0.10331084579229355, 0.10183722525835037, 0.06477497518062592, 0.058521442115306854, 0.020238429307937622, 0.0041399551555514336, 0.05435865744948387, 0.019399266690015793, 0.014586761593818665, 0.0013498951448127627, 0.05185343697667122, 0.03813401982188225, 0.04708562046289444, 0.08600055426359177, 0.04815644398331642, 0.04272099956870079, 0.02353966049849987, 0.0507228784263134, 0.09903799742460251, 0.07725296914577484, 0.09688752889633179, 0.010787788778543472, 0.04031948000192642, 0.1012740507721901, 0.05554453283548355, 0.017446760088205338, 0.08464684337377548, 0.06858475506305695, 0.024394558742642403, 0.004145147278904915, 0.09640131145715714, 0.07414473593235016, 0.04595319554209709, 0.015153108164668083, 0.07973415404558182, 0.01353214681148529, 0.03115517646074295, 0.001719093881547451, 0.10549088567495346, 0.06253626197576523, 0.016117535531520844, 0.07433577626943588, 0.06523341685533524, 0.06186452880501747, 0.016794558614492416, 0.10331316292285919, 0.09340941905975342, 0.06731792539358139, 0.05709076672792435, 0.04957079514861107, 0.06453725695610046, 0.012262560427188873, 0.042696140706539154, 0.04556002467870712, 0.09553390741348267, 0.050160784274339676, 0.05817052721977234, 0.08165474981069565, 0.04787832126021385, 0.02729381062090397, 0.10388602316379547, 0.08477373421192169, 0.08681348711252213, 0.06858973205089569, 0.06789104640483856, 0.03850492835044861, 0.0433942973613739, 0.052195820957422256, 0.007945382967591286, 0.029683083295822144, 0.019951382651925087, 0.0806746557354927, 0.07377791404724121, 0.005528050474822521, 0.017322944477200508, 0.04719217121601105, 0.08006291836500168, 0.014818253926932812, 0.030008923262357712, 0.005092828068882227, 0.0351313091814518, 0.004414892755448818, 0.025564542040228844, 0.09419381618499756, 0.0030815256759524345, 0.07130488008260727, 0.04834020137786865, 0.014570854604244232, 0.05598421022295952, 0.023526299744844437, 0.08546962589025497, 0.03306784853339195, 0.09648219496011734, 0.048288267105817795, 0.002243501367047429, 0.07563260197639465, 0.05436072498559952, 0.06842583417892456], 10, map[nprobe, 3])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_185.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_186.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_187.csv</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector103, feature, array[0.28576499223709106, 0.08687837421894073, 0.14799416065216064, 0.058550164103507996, 0.19060933589935303, 0.08999139070510864, 0.1514379382133484, 0.08630754053592682, 0.147443950176239, 0.11865786463022232, 0.08603266626596451, 0.026738379150629044, 0.04464268684387207, 0.07328195124864578, 0.1070372611284256, 0.08322914689779282, 0.034094709903001785, 0.16017472743988037, 0.03294524550437927, 0.14785508811473846, 0.18853361904621124, 0.14193195104599, 0.1404295563697815, 0.1011366918683052, 0.11323778331279755, 0.06974314898252487, 0.019739823415875435, 0.0017852566670626402, 0.19590851664543152, 0.04378505051136017, 0.13438871502876282, 0.12536169588565826, 0.037846311926841736, 0.19261693954467773, 0.15421807765960693, 0.012271392159163952, 0.08373595774173737, 0.1423385590314865, 0.13366387784481049, 0.14510740339756012, 0.02415030263364315, 0.04452469199895859, 0.0991881713271141, 0.13216648995876312, 0.10771691799163818, 0.1334938257932663, 0.10556206107139587, 0.10942403227090836, 0.10575082153081894, 0.18991316854953766, 0.1172894611954689, 0.09650064259767532, 0.16381768882274628, 0.03527522832155228, 0.09627934545278549, 0.1411363035440445, 0.09879021346569061, 0.18661963939666748, 0.036094631999731064, 0.2045263648033142, 0.18818239867687225, 0.15758785605430603, 0.02735513634979725, 0.16133542358875275], 8, map[nprobe, 2])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector104, feature, array[0.1460634469985962, 0.011167393065989017, 0.1208098977804184, 0.042715076357126236, 0.11082421243190765, 0.10441119968891144, 0.017588060349225998, 0.06867052614688873, 0.08636009693145752, 0.112062007188797, 0.08760128170251846, 0.07306373864412308, 0.02043737843632698, 0.04533211141824722, 0.0644005686044693, 0.1109415739774704, 0.1328347772359848, 0.09234130382537842, 0.021948078647255898, 0.014223171398043633, 0.037448883056640625, 0.12232688814401627, 0.1401732712984085, 0.07649838924407959, 0.006969892885535955, 0.011228282004594803, 0.06573056429624557, 0.0935225710272789, 0.12671451270580292, 0.11154123395681381, 0.14197243750095367, 0.13038279116153717, 0.006941759493201971, 0.06264892220497131, 0.09148560464382172, 0.015115467831492424, 0.10005895793437958, 0.08408173173666, 0.11769413948059082, 0.132187157869339, 0.07072633504867554, 0.11437469720840454, 0.09085334837436676, 0.018128234893083572, 0.09087350219488144, 0.029721418395638466, 0.003261981066316366, 0.11332324147224426, 0.07148522883653641, 0.09012772142887115, 0.11590547114610672, 0.1038624569773674, 0.009726176038384438, 0.10393176972866058, 0.0497647225856781, 0.10949892550706863, 0.09509700536727905, 0.0018441954161971807, 0.020147470757365227, 0.052109166979789734, 0.12824559211730957, 0.06617818772792816, 0.08897547423839569, 0.09546243399381638, 0.12680310010910034, 0.039783768355846405, 0.013500145636498928, 0.13709980249404907, 0.1050802692770958, 0.11727995425462723, 0.11018858850002289, 0.10111720860004425, 0.04592683166265488, 0.0670841708779335, 0.028880568221211433, 0.09578774869441986, 0.10614515841007233, 0.09062612056732178, 0.06989005953073502, 0.13118506968021393, 0.023909589275717735, 0.12746895849704742, 0.056859340518713, 0.05184338614344597, 0.06325660645961761, 0.005031873472034931, 0.09355629235506058, 0.011395281180739403, 0.03881137818098068, 0.12159445881843567, 0.06336931884288788, 0.012990365736186504, 0.03986307978630066, 0.1422329545021057, 0.11063181608915329, 0.13683968782424927, 0.10353496670722961, 0.10641710460186005, 0.10204301029443741, 0.10698171705007553, 0.09010161459445953, 0.023637281730771065, 0.13571342825889587, 0.09645155817270279, 0.1303277462720871, 0.021461354568600655, 0.11309470236301422, 0.1030096560716629, 0.08732258528470993, 0.013736271299421787, 0.08507058769464493, 0.06284129619598389, 0.10962437093257904, 0.13974350690841675, 0.10655143857002258, 0.06670118123292923, 0.08046265691518784, 0.10161018371582031, 0.1313834935426712, 0.07395011931657791, 0.07142218202352524, 0.10703067481517792, 0.025775695219635963, 0.008276217617094517, 0.04086991026997566, 0.09337155520915985, 0.031105799600481987, 0.0726708173751831], 10, map[nprobe, 2])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector106, feature, array[0.0712805911898613, 0.03414762392640114, 0.008772436529397964, 0.055170465260744095, 0.005461367778480053, 0.018608063459396362, 0.0283877644687891, 0.06907427310943604, 0.02208472602069378, 0.060443103313446045, 0.05699513480067253, 0.052062083035707474, 0.05619015172123909, 0.015462585724890232, 0.03982448950409889, 0.07346150279045105, 0.039903294295072556, 0.061221182346343994, 0.028816884383559227, 0.07549098879098892, 0.04935846105217934, 0.07296385616064072, 0.0024919130373746157, 0.0012141611659899354, 0.03282751142978668, 0.07115677744150162, 0.04651230573654175, 0.05791768059134483, 0.009985825046896935, 0.07142073661088943, 0.04548165947198868, 0.07396066188812256, 0.04923173785209656, 0.06771956384181976, 0.05733874440193176, 0.05029281601309776, 0.06669501960277557, 0.014920229092240334, 0.01575036719441414, 0.06998161226511002, 0.057488031685352325, 0.07206352055072784, 0.04197151958942413, 0.04343684762716293, 0.06407517939805984, 0.011808034032583237, 0.07538428902626038, 0.015160645358264446, 0.031054314225912094, 0.026215920224785805, 0.054985757917165756, 0.03825530409812927, 0.01944858208298683, 0.05025311931967735, 0.06678801774978638, 0.05290376394987106, 0.006662732921540737, 0.01777532510459423, 0.06686179339885712, 0.018671665340662003, 0.07553445547819138, 0.023599060252308846, 0.0346403568983078, 0.015848753973841667, 0.049125876277685165, 0.017143096774816513, 0.019468022510409355, 0.05810976400971413, 0.0045753964222967625, 0.0380731076002121, 0.03882712870836258, 0.03900491073727608, 0.04608950391411781, 0.031478021293878555, 0.06869881600141525, 0.07374401390552521, 0.03398530185222626, 0.027530761435627937, 0.06254079192876816, 0.02579699642956257, 0.006023305002599955, 0.03665170818567276, 0.0748879685997963, 0.07293897867202759, 0.004315893165767193, 0.003589126979932189, 0.01336371898651123, 0.0677957534790039, 0.038376472890377045, 0.022226719185709953, 0.0007059907075017691, 0.049939535558223724, 0.027224328368902206, 0.05137988552451134, 0.04562317579984665, 0.046239759773015976, 0.019207626581192017, 0.010526702739298344, 0.05513353645801544, 0.06663460284471512, 0.07339241355657578, 0.03174494206905365, 0.0676150694489479, 0.022426370531320572, 0.005685091949999332, 0.055337969213724136, 0.049248989671468735, 0.03405437245965004, 0.05997946113348007, 0.06555479019880295, 0.009225215762853622, 0.03814823180437088, 0.02772272378206253, 0.07575825601816177, 0.039295293390750885, 0.005950624123215675, 0.04081075266003609, 0.02032250538468361, 0.020577527582645416, 0.0011372171575203538, 0.05297217518091202, 0.02888963371515274, 0.042788222432136536, 0.032485462725162506, 0.050414424389600754, 0.02472488023340702, 0.0027127282228320837, 0.014279580675065517, 0.06596866995096207, 0.05179191753268242, 0.010239762254059315, 0.02895939163863659, 0.014171498827636242, 0.00404387665912509, 0.06666847318410873, 0.03405335918068886, 0.04176769033074379, 0.018758947029709816, 0.04938894882798195, 0.005335540510714054, 0.023359209299087524, 0.01222203392535448, 0.06889761239290237, 0.06877533346414566, 0.043536074459552765, 0.038330819457769394, 0.004076696466654539, 0.06383594125509262, 0.059707824140787125, 0.07262258231639862, 0.0517246276140213, 0.07132427394390106, 0.06334026157855988, 0.07532364875078201, 0.039648301899433136, 0.02517048269510269, 0.00045096836402080953, 0.016980480402708054, 0.026822740212082863, 0.054980725049972534, 0.03219400346279144, 0.014967999421060085, 0.010627076029777527, 0.058226678520441055, 0.0744585171341896, 0.023691806942224503, 0.021449750289320946, 0.0032906574197113514, 0.06677600741386414, 0.003107106778770685, 0.010239184834063053, 0.06363032013177872, 0.0455789640545845, 0.025105757638812065, 0.009755398146808147, 0.042344558984041214, 0.038124874234199524, 0.02410646714270115, 0.04364855960011482, 0.059819526970386505, 0.00812621507793665, 0.03610632196068764, 0.06482142955064774, 0.047083884477615356, 0.010819475166499615, 0.0022021732293069363, 0.009931831620633602, 0.07563121616840363, 0.013875778764486313, 0.06885156780481339, 0.012104718014597893, 0.03426693379878998, 0.05040149763226509, 0.02789483405649662, 0.04973142594099045, 0.050381217151880264, 0.0710093304514885, 0.03629377484321594, 0.054815471172332764, 0.02405627816915512, 0.020028850063681602, 0.03307588770985603, 0.007506498601287603, 0.017483700066804886, 0.003990971017628908, 0.07580271363258362, 0.0739283338189125, 0.035860996693372726, 0.03646326810121536, 0.04015062376856804, 0.04139719158411026, 0.025414185598492622, 0.058324094861745834, 0.0486026369035244, 0.035061754286289215, 0.05365265905857086, 0.021558450534939766, 0.001942936098203063, 0.051986802369356155, 0.06228300556540489, 0.04920055344700813, 0.03731734678149223, 0.007103664334863424, 0.015974674373865128, 0.03481658548116684, 0.03977695107460022, 0.006677829660475254, 0.028561409562826157, 0.0127008818089962, 0.014985477551817894, 0.06152461841702461, 0.05912981554865837, 0.03758737072348595, 0.0005631504463963211, 6.712041795253754e-05, 0.06467648595571518, 0.057649873197078705, 0.05516726151108742, 0.06312070041894913, 0.0642341822385788, 0.006170943379402161, 0.03859763965010643, 0.03531011566519737, 0.011959750205278397, 0.006870605982840061, 0.011580923572182655, 0.009962544776499271, 0.04655269905924797, 0.07566370069980621, 0.006902722641825676, 0.026876108720898628, 0.001487812027335167, 0.022277794778347015, 0.005487923976033926, 0.000897368649020791, 0.024232598021626472, 0.02529374696314335, 0.010075049474835396, 0.011734366416931152, 0.014985620975494385, 0.039359088987112045, 0.05519171804189682, 0.055129945278167725, 0.012679445557296276, 0.002189026214182377, 0.004228649195283651, 0.04237985610961914, 0.04406663402915001, 0.014545324258506298, 0.004981231410056353, 0.06848639994859695, 0.0444563589990139, 0.0504327155649662, 0.06843181699514389, 0.043498825281858444, 0.014340074732899666, 0.06164709851145744, 0.022997282445430756, 0.05721630901098251, 0.056958578526973724, 0.052930500358343124, 0.050248656421899796, 0.02030646614730358, 0.006517666392028332, 0.05219896137714386, 0.07476849108934402, 0.01862785778939724, 0.0678158551454544, 0.015404589474201202, 0.01011555828154087, 0.056958965957164764, 0.06591849774122238, 0.058871783316135406, 0.0427415557205677, 0.019220629706978798, 0.005044212564826012, 0.0036385110579431057, 0.06321976333856583, 0.010281410068273544, 0.04146825522184372, 0.010452352464199066, 0.06380894035100937, 0.01650090143084526, 0.004806465934962034, 0.07448401302099228, 0.0326215997338295, 0.0198367927223444, 0.034673210233449936, 0.06986626982688904, 0.01535346731543541, 0.017135653644800186, 0.03744609281420708, 0.010928456671535969, 0.0721655935049057, 0.04158909246325493, 0.03107197768986225, 0.026547754183411598, 0.03723009303212166, 0.06487514078617096, 0.056455254554748535, 0.03891834244132042, 0.07508298009634018, 0.07236321270465851, 0.05061202496290207, 0.02770451456308365, 0.06345859915018082, 0.07574909925460815, 0.005753980949521065, 0.04432271048426628, 0.060566436499357224, 0.05064847692847252, 0.05850815027952194, 0.007890027947723866, 0.015990396961569786, 0.01516656018793583, 0.0491318516433239, 0.07501967251300812, 0.05741969868540764, 0.02306986413896084, 0.02907000668346882, 0.07232726365327835, 0.05499335750937462, 0.004141052253544331, 0.059520214796066284, 0.05691755935549736, 0.04976549744606018, 0.004034958779811859, 0.03819522261619568, 0.0022327343467622995, 0.06635762751102448, 0.029993152245879173, 0.022959059104323387, 0.024571793153882027, 0.03628253564238548, 0.045460157096385956, 0.02925429493188858, 0.01720239780843258, 0.04258456453680992, 0.06843709945678711, 0.01772322505712509, 0.04387034475803375, 0.0037851922679692507, 0.042795006185770035, 0.062181223183870316, 0.0005844870465807617, 0.0554196834564209, 0.011727435514330864, 0.0371243953704834, 0.03848031535744667, 0.07073211669921875, 0.027599049732089043, 0.07553515583276749, 0.053167957812547684, 0.04297700896859169, 0.020567117258906364, 0.012497111223638058, 0.02547658421099186, 0.006902968045324087, 0.03567797318100929, 0.007518823258578777, 0.0720616951584816, 0.011452100239694118, 0.03200462833046913, 0.0212908536195755, 0.061945293098688126, 0.03836187347769737, 0.030826568603515625, 0.014845553785562515, 0.06689795106649399, 0.029986480250954628, 0.06746023148298264, 0.012965844944119453, 0.01909378543496132, 0.019407255575060844, 0.07227006554603577, 0.008490368723869324, 0.013075434602797031, 0.004674394614994526, 0.07320210337638855, 0.024891899898648262, 0.07601869106292725, 0.07377069443464279, 0.07393766939640045, 0.05894336476922035, 0.030982568860054016, 0.013360373675823212, 0.0643790140748024, 0.06252230703830719, 0.021909141913056374, 0.06584057211875916, 0.06757994741201401, 0.030669135972857475, 0.0022102883085608482, 0.059163060039281845, 0.06613854318857193, 0.0257073063403368, 0.02140866033732891, 0.013831674121320248, 0.06691040098667145, 0.010295812971889973, 0.00048246572259813547, 0.01517306175082922, 0.02185375615954399, 0.07351736724376678, 0.02334476262331009, 0.015352265909314156, 0.06561150401830673, 0.006477804388850927, 0.05477786064147949, 0.07105269283056259, 0.06164504215121269, 0.0725557804107666, 0.014960942789912224, 0.01644848845899105, 0.03141917288303375, 0.026251817122101784, 0.05019524320960045, 0.034813616424798965, 0.06662777066230774, 0.0353325791656971, 0.007796169724315405, 0.03442548215389252, 0.040714215487241745, 0.020070258527994156, 0.04979775473475456, 0.005154965911060572, 0.0076502845622599125, 0.01977885141968727, 0.024940362200140953, 0.038740936666727066, 0.02686530351638794, 0.057548824697732925, 0.07119515538215637, 0.0068247499875724316, 0.0008655973360873759, 0.06560280174016953, 0.012953265570104122, 0.01498370710760355, 0.04786880686879158, 0.01293104887008667, 0.034381698817014694, 0.047005459666252136, 0.01992644928395748, 0.07545948028564453, 0.05135027691721916, 0.05179423466324806, 0.07190731167793274, 0.036633580923080444, 0.07277969270944595, 0.06506649404764175, 0.06257183104753494, 0.02730507031083107, 0.034017499536275864, 0.06797591596841812, 0.07174213230609894, 0.03156975284218788, 0.05921446159482002, 0.04201151430606842, 0.03521477058529854, 0.024671008810400963, 0.07175172865390778, 0.009513191878795624, 0.014790079556405544, 0.02610580064356327, 0.059107039123773575, 0.04543934017419815, 0.05760986730456352, 0.021912306547164917, 0.037808243185281754, 0.026903094723820686, 0.05371618643403053, 0.050653498619794846, 0.04559094458818436, 0.018678482621908188, 0.060757678002119064, 0.04171908274292946, 0.030831407755613327, 0.039393823593854904, 0.015317629091441631, 0.01768491603434086, 0.0662064403295517, 0.007832142524421215, 0.0589362308382988, 0.04267042502760887, 0.010926328599452972, 0.04750259593129158, 0.012966557405889034, 0.0623445063829422, 0.0744563415646553, 0.05664418637752533, 0.017363063991069794, 0.06192200258374214], 10, map[nprobe, 1])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector107, feature, array[0.07382608950138092, 0.017122464254498482, 0.0342908576130867, 0.029619786888360977, 0.0178862102329731, 0.03484765812754631, 0.036339085549116135, 0.05203656852245331, 0.04620254039764404, 0.030481044203042984, 0.0506005622446537, 0.009827340953052044, 0.011029241606593132, 0.01294477004557848, 0.047098200768232346, 0.0007490563439205289, 0.03529452532529831, 0.04704062640666962, 0.0029035008046776056, 0.04952226206660271, 0.017912819981575012, 0.03603135794401169, 0.0055779507383704185, 0.0018567506922408938, 0.018822163343429565, 0.023427853360772133, 0.023229943588376045, 0.04070846363902092, 0.00717141292989254, 0.011251667514443398, 0.03804001584649086, 0.042278438806533813, 0.023443114012479782, 0.04776531085371971, 0.04709843918681145, 0.022148672491312027, 0.006511237472295761, 0.0009052515379153192, 0.051248643547296524, 0.032138291746377945, 0.019412772729992867, 0.04915398359298706, 0.02799508161842823, 0.048718299716711044, 0.0009684148826636374, 0.0028392737731337547, 0.005659687332808971, 0.029387693852186203, 0.005311358720064163, 0.03521237522363663, 0.02816586382687092, 0.0442369244992733, 0.041371867060661316, 0.016760554164648056, 0.027778385207057, 0.003968792036175728, 0.015107235871255398, 0.029620418325066566, 0.035802751779556274, 0.014741532504558563, 0.04142818972468376, 0.010779725387692451, 0.05043656751513481, 0.03157813474535942, 0.04306335374712944, 0.04687041789293289, 0.04897959157824516, 0.03903276100754738, 0.039862021803855896, 0.003602229058742523, 0.001160091138444841, 0.04976813867688179, 0.03731245547533035, 0.04936203733086586, 0.040750160813331604, 0.03575071319937706, 0.003031756728887558, 0.00048652675468474627, 0.00367504870519042, 0.0012417265679687262, 0.006412073969841003, 0.04301218315958977, 0.01579749770462513, 0.03333430364727974, 0.029741423204541206, 0.027657130733132362, 0.03040989115834236, 0.05357194319367409, 0.03290259465575218, 0.013444139622151852, 0.0024852438364177942, 0.011132275685667992, 0.031941596418619156, 0.03705191984772682, 0.028025437146425247, 0.0034565574023872614, 0.028364405035972595, 0.045809414237737656, 0.009498667903244495, 0.043158240616321564, 0.02075348235666752, 0.03392738848924637, 0.012595479376614094, 0.03775215893983841, 0.02439316175878048, 0.028782838955521584, 0.007610625121742487, 0.03699010983109474, 0.04724343866109848, 0.04385272040963173, 0.016964005306363106, 0.014415623620152473, 0.019463365897536278, 0.053699981421232224, 0.03726886212825775, 0.049108780920505524, 0.031026188284158707, 0.021759476512670517, 0.010878466069698334, 0.028410498052835464, 0.05399429053068161, 0.0295143723487854, 0.030640369281172752, 0.011136841028928757, 0.049159832298755646, 0.039166416972875595, 0.013963112607598305, 0.047801341861486435, 0.009598293341696262, 0.041913341730833054, 0.015766143798828125, 0.042682722210884094, 0.02678668685257435, 0.025585293769836426, 0.025144780054688454, 0.043263282626867294, 0.036498989909887314, 0.046858396381139755, 0.019772684201598167, 0.016480937600135803, 0.034122440963983536, 0.03373727202415466, 0.01871395669877529, 0.02850196696817875, 0.009596629999577999, 0.017412733286619186, 0.018898770213127136, 0.03345772624015808, 0.03252193704247475, 0.00829205010086298, 0.00183204491622746, 0.05345532298088074, 0.006107295863330364, 0.04028917849063873, 0.0048707351088523865, 0.046956565231084824, 0.02337721362709999, 0.03642129525542259, 0.04706878215074539, 0.051590513437986374, 0.005533405113965273, 0.039390865713357925, 0.03345714509487152, 0.03467487916350365, 0.04287467896938324, 0.0023299462627619505, 0.017881227657198906, 0.014516950584948063, 0.04474238306283951, 0.0356798954308033, 0.003789066569879651, 0.024532586336135864, 0.014280617237091064, 0.04476717859506607, 0.028705399483442307, 0.035137392580509186, 0.023983879014849663, 0.02314344048500061, 0.04712328314781189, 0.04469803348183632, 0.020137710496783257, 0.01596689224243164, 0.011089373379945755, 0.017812926322221756, 0.039260562509298325, 0.042658839374780655, 0.012309879995882511, 0.041102442890405655, 0.005979365669190884, 0.042250968515872955, 0.02263539843261242, 0.05035456642508507, 0.006615852005779743, 0.002108475426211953, 0.045883409678936005, 0.048915162682533264, 0.027512166649103165, 0.02877466008067131, 0.01167989894747734, 0.031140394508838654, 0.026529517024755478, 0.0357474721968174, 0.017507348209619522, 0.02362360619008541, 0.04981262981891632, 0.033430781215429306, 0.042175792157649994, 0.005540005397051573, 0.044059835374355316, 0.03436713293194771, 0.02971196547150612, 0.0017964171711355448, 0.014145917259156704, 0.020013682544231415, 0.039787694811820984, 0.04829244315624237, 0.008140145801007748, 0.017619693651795387, 0.04449378326535225, 0.03360920399427414, 0.015119488351047039, 0.008709772489964962, 0.043185219168663025, 0.027913695201277733, 0.05343762785196304, 0.024940216913819313, 0.034566596150398254, 0.002729501575231552, 0.05354238674044609, 0.0020377454347908497, 0.011363732628524303, 0.02230273000895977, 0.025347227230668068, 0.019345134496688843, 0.018391212448477745, 0.02548467367887497, 0.010792816989123821, 0.006712316535413265, 0.046724289655685425, 0.016263220459222794, 0.031126219779253006, 0.007401004899293184, 0.03190338984131813, 0.0031767613254487514, 0.048413410782814026, 0.024721695110201836, 0.01895757019519806, 0.0010689821792766452, 0.02988462522625923, 0.02824702486395836, 0.04368521645665169, 0.0028782335575670004, 0.008661235682666302, 0.03006371669471264, 0.02587706968188286, 0.01745316945016384, 0.022997085005044937, 0.04210987687110901, 0.007089788559824228, 0.01911820098757744, 0.014338796027004719, 0.04799213632941246, 0.009112470783293247, 0.016670433804392815, 0.02664083242416382, 0.01570161059498787, 0.01331926416605711, 0.013521820306777954, 0.04842345416545868, 0.048720210790634155, 0.03468632698059082, 0.03548785671591759, 0.021236365661025047, 0.04329656809568405, 0.007695731241255999, 0.044279325753450394, 0.052664097398519516, 0.0338265523314476, 0.030325429514050484, 0.0455746091902256, 0.04418259486556053, 0.02215125784277916, 0.04469318687915802, 0.05269135534763336, 0.041049111634492874, 0.0019937457982450724, 0.04902975261211395, 0.01573288068175316, 0.038689982146024704, 0.04269130900502205, 0.050807613879442215, 0.03689117729663849, 0.0161124337464571, 0.04484572261571884, 0.0041376762092113495, 0.04676700383424759, 0.002687899162992835, 0.015049967914819717, 0.008310452103614807, 0.0093813706189394, 0.015435313805937767, 0.0033140399027615786, 0.02625003270804882, 0.010976913385093212, 0.0031086348462849855, 0.011969869025051594, 0.02182766981422901, 0.048872534185647964, 0.03513495251536369, 0.010744942352175713, 0.04891432449221611, 0.011398674920201302, 0.04744814708828926, 0.04367498680949211, 0.0009227279806509614, 0.033315807580947876, 0.00548177445307374, 0.020120423287153244, 0.004696954973042011, 0.025050831958651543, 0.009747307747602463, 0.02198966220021248, 0.006864890456199646, 0.003423636546358466, 0.022705253213644028, 0.028690053150057793, 0.002592445118352771, 0.014626672491431236, 0.03254223242402077, 0.03530901297926903, 0.04754867032170296, 0.007906066253781319, 0.04485047608613968, 0.0407787449657917, 0.02294599451124668, 0.04987268149852753, 0.026753751561045647, 0.01724531501531601, 0.049756575375795364, 0.03501921519637108, 0.024869374930858612, 0.04198861122131348, 0.018917547538876534, 0.01877022534608841, 0.031808819621801376, 0.05383503809571266, 0.028902539983391762, 0.04439862072467804, 0.020658954977989197, 0.015704292804002762, 0.04317881911993027, 0.001865497906692326, 0.0394933819770813, 0.01688779518008232, 0.03244436904788017, 0.008087885566055775, 0.0035439920611679554, 0.01933162286877632, 0.013509195297956467, 0.028958145529031754, 0.04492589086294174, 0.009072402492165565, 0.03297453001141548, 0.04583374410867691, 0.048100970685482025, 0.01547211967408657, 0.01356288231909275, 0.00905021745711565, 0.0474315844476223, 0.008393273688852787, 0.006734547205269337, 0.004870923236012459, 0.041448067873716354, 0.008175289258360863, 0.020583342760801315, 0.016643106937408447, 0.05223044753074646, 0.00200996664352715, 0.011259044520556927, 0.05408492311835289, 0.03198275342583656, 0.0516667515039444, 0.053450725972652435, 0.044198837131261826, 0.01912549138069153, 0.005947995465248823, 0.033592529594898224, 0.017443032935261726, 0.04192637652158737, 0.016177309677004814, 0.009596157819032669, 0.01656496524810791, 0.004297716077417135, 0.05225975811481476, 0.032197918742895126, 0.045643169432878494, 0.023229049518704414, 0.013894687406718731, 0.017139673233032227, 0.05266522616147995, 0.05197906494140625, 0.03160550445318222, 0.047659631818532944, 0.00774623965844512, 0.03224140778183937, 0.03255575895309448, 0.018874771893024445, 0.03369485214352608, 0.02515379711985588, 0.040686845779418945, 0.025917058810591698, 0.004044892732053995, 0.028911840170621872, 0.011306177824735641, 0.052968647330999374, 0.053662776947021484, 0.05326244980096817, 0.029442332684993744, 0.017394335940480232, 0.006968231871724129, 0.007690894417464733, 0.050225600600242615, 0.013491774909198284, 0.00023374581360258162, 0.042516060173511505, 0.0009352949564345181, 0.04090233892202377, 0.0052542779594659805, 0.0063007548451423645, 0.023641765117645264, 0.04484125226736069, 0.05001366510987282, 0.05249765142798424, 0.01272460725158453, 0.0447300523519516, 0.049101781100034714, 0.010115860030055046, 0.0159846730530262, 0.022624241188168526, 0.04427889734506607, 0.05158931016921997, 0.01347406767308712, 0.02646460570394993, 0.03344051167368889, 0.04942263662815094, 0.03779961168766022, 0.028385059908032417, 0.044160377234220505, 0.04294492304325104, 0.018848612904548645, 0.03548580780625343, 0.029806125909090042, 0.05421202629804611, 0.0005274969735182822, 0.00938893761485815, 0.04557451605796814, 0.02941315434873104, 0.020967260003089905, 0.01486048474907875, 0.004858843516558409, 0.03993454948067665, 0.016600994393229485, 0.028166117146611214, 0.04752078279852867, 0.04947497323155403, 0.032742757350206375, 0.025024166330695152, 0.02350422367453575, 0.002840828150510788, 0.00941675528883934, 0.006182842887938023, 0.04002303257584572, 0.04516610503196716, 0.04644681513309479, 0.009976332075893879, 0.01120877917855978, 0.02900867350399494, 0.04196600243449211, 0.017785146832466125, 0.05393335595726967, 0.021304581314325333, 0.03862718492746353, 0.004435310605913401, 0.05087728053331375, 0.0053886529058218, 0.020631665363907814, 0.010716884396970272, 0.0035759098827838898, 0.02534809149801731, 0.0221937857568264, 0.003750315634533763, 0.020528022199869156, 0.0067803035490214825, 0.008293594233691692, 0.020695148035883904, 0.038530029356479645, 0.035027533769607544, 0.006620975211262703, 0.024240950122475624, 0.04295392706990242, 0.03372587636113167, 0.027359116822481155, 0.006050618831068277, 0.012928889133036137, 0.026696443557739258, 0.0036076512187719345, 0.015743665397167206, 0.03530130162835121, 0.030153870582580566, 0.01420016959309578, 0.02503388375043869, 0.04002385959029198, 0.05306006968021393, 0.04587264358997345, 0.008805772289633751, 0.02477194555103779, 0.022296253591775894, 0.009239490143954754, 0.036231640726327896, 0.03508629649877548, 0.01760702393949032, 0.04259856790304184, 0.024502424523234367, 0.006680153775960207, 0.04619194567203522, 0.015455934219062328, 0.041138291358947754, 0.014274993911385536, 0.012271535582840443, 0.038009319454431534, 0.001018412527628243, 0.024888750165700912, 0.046368781477212906, 0.045388590544462204, 0.007510284427553415, 0.04860249161720276, 0.025425508618354797, 0.035526517778635025, 0.04537375271320343, 0.015378925018012524, 0.020013432949781418, 0.03920460119843483, 0.037823013961315155, 0.010904236696660519, 0.004119380377233028, 0.024338753893971443, 0.03348593786358833, 0.015418765135109425, 0.05214352533221245, 0.013531114906072617, 0.046695347875356674, 0.05200676620006561, 0.04642727971076965, 0.05091264098882675, 0.03894849121570587, 0.021173380315303802, 0.04806981235742569, 0.01630951277911663, 0.04664202034473419, 0.0341537743806839, 0.025701353326439857, 0.02590561844408512, 0.0162468533962965, 0.04185374826192856, 0.02890831045806408, 0.04244980588555336, 0.026717906817793846, 0.029302822425961494, 0.0426245778799057, 0.05020180717110634, 0.006584774237126112, 0.053779151290655136, 0.03828176110982895, 0.028961380943655968, 0.013005215674638748, 0.05233125016093254, 0.029543528333306313, 0.038116347044706345, 0.009656247682869434, 0.04851995408535004, 0.023954002186655998, 0.041518475860357285, 0.043479450047016144, 0.022172702476382256, 0.022481974214315414, 0.042138099670410156, 0.02258000150322914, 0.0008929535979405046, 0.03540997952222824, 0.004883522633463144, 0.04393477737903595, 0.03807715326547623, 0.043330658227205276, 0.00726728979498148, 0.044931523501873016, 0.03154521435499191, 0.042337816208601, 0.014629200100898743, 0.01893221214413643, 0.012054971419274807, 7.427819218719378e-05, 0.02525746263563633, 0.05021736025810242, 0.02674615941941738, 0.0008772531291469932, 0.015180588699877262, 0.017735036090016365, 0.027343807741999626, 0.006242748815566301, 0.0006588404066860676, 0.013963189907371998, 0.049242667853832245, 0.010512827895581722, 0.002909294329583645, 0.04005339369177818, 0.04139360785484314, 0.017915958538651466, 0.004311718046665192, 0.033415284007787704, 0.0027296761982142925, 0.02429158240556717, 0.03557631000876427, 0.04278436675667763, 0.002991406014189124, 0.03149651736021042, 0.03610922023653984, 0.0180917177349329, 0.04585268720984459, 0.03214845806360245, 0.010618983767926693, 0.022178739309310913, 0.011709239333868027, 0.04618655890226364, 0.05369483307003975, 0.026338135823607445, 0.028137659654021263, 0.004629178903996944, 0.03765276446938515, 0.05032217875123024, 0.04378175362944603, 0.03742023557424545, 0.026711154729127884, 0.02423260547220707, 0.05190715193748474, 0.013285438530147076, 0.011914161965250969, 0.00639363331720233, 0.0167032890021801, 0.04014052078127861, 0.019203180447220802, 0.037884004414081573, 0.007845742627978325, 0.02854021266102791, 0.04685286059975624, 0.005327572580426931, 0.017670927569270134, 0.02975580468773842, 0.03232195973396301, 0.024473674595355988, 0.05008411407470703, 0.04729028791189194, 0.03325182944536209, 0.03144832327961922, 0.011171436868607998, 0.0007555704214610159, 0.04164246469736099, 0.03215973824262619, 0.044071901589632034, 0.03849557042121887, 0.028347531333565712, 0.043619316071271896, 0.028866687789559364, 0.001763359410688281, 0.0010089017450809479, 0.03839465603232384, 0.0006374650984071195, 0.02821194939315319, 0.03148726001381874, 0.0057343728840351105, 0.011399450711905956, 0.030945071950554848, 0.009831629693508148, 0.02295106090605259, 0.03229903057217598, 0.005333205685019493, 0.004777542315423489, 0.05309775471687317, 0.05232316628098488, 0.008535667322576046, 0.03951764479279518, 0.007971190847456455, 0.003424056340008974, 0.03934266418218613, 0.0512566901743412, 0.03662481904029846, 0.032008491456508636, 0.009324803948402405, 0.0025721609126776457, 0.03364767134189606, 0.003540290519595146, 0.011138297617435455, 0.050992123782634735, 0.002566361567005515, 0.053853172808885574, 0.009145062416791916, 0.0392942912876606, 0.02258615754544735, 0.029432514682412148, 0.038360174745321274, 0.038664206862449646, 0.01095105055719614, 0.028784234076738358, 0.03502719849348068, 0.043932314962148666, 0.03144901245832443, 0.019853122532367706, 0.050468407571315765, 0.03268935903906822, 0.035552483052015305, 0.04380926862359047, 0.05254745855927467, 0.04381314665079117, 0.05018279328942299, 0.03726644068956375, 0.02976849675178528, 0.045115355402231216, 0.02661391720175743, 0.024138180539011955, 0.017793530598282814, 0.049846503883600235, 0.0016047178069129586, 0.03654368221759796, 0.04404905065894127, 0.03639320284128189, 0.008652598597109318, 0.03813166916370392, 0.028015723451972008, 0.024645090103149414, 0.006235972046852112, 0.04547658562660217, 0.010907480493187904, 0.04247676208615303, 0.04831971228122711, 0.018169300630688667, 0.02522779442369938, 0.03868802636861801, 0.04632635787129402, 0.03230191022157669, 0.003017015289515257, 0.04477681219577789, 0.02251608297228813, 0.028614820912480354, 0.012734835036098957, 0.03934900835156441, 0.007152295205742121, 0.024283718317747116, 0.0376511886715889, 0.017170077189803123, 0.0218803770840168, 0.015734324231743813, 0.03544967249035835, 0.004310278687626123, 0.03206565976142883, 0.022944891825318336, 0.03816237300634384, 0.01926432177424431, 0.0013990789884701371, 0.013045989908277988, 0.04041416570544243, 0.02427431382238865, 0.02866826206445694, 0.025732800364494324, 0.04504598304629326, 0.02849457412958145, 0.04231555759906769, 0.03244869410991669, 0.0503307580947876, 0.05203928425908089, 0.029405754059553146, 0.02358434349298477, 0.027960896492004395, 0.02837151288986206, 0.05140085890889168, 0.02623828686773777, 0.051908135414123535, 0.015770023688673973, 0.0014356756582856178, 0.052410971373319626, 0.0005930581828579307, 0.0013478510081768036, 0.03335685282945633, 0.03414390608668327, 0.025173358619213104, 0.051973793655633926, 0.007651788182556629, 0.0061310227029025555, 0.03591500222682953, 0.01743423379957676, 0.03218001872301102, 0.04970923811197281, 0.021784504875540733, 0.007551528979092836, 0.0014873603358864784, 0.013868909329175949, 0.02302650175988674, 0.002720116637647152, 0.009828305803239346, 0.04331783950328827, 0.05093362554907799, 0.02557293325662613, 0.012827171012759209, 0.022912634536623955, 0.026513053104281425, 0.024230962619185448, 0.005297435447573662, 0.003958326298743486, 0.027179017663002014, 0.030430808663368225, 0.03758196532726288, 0.052547991275787354, 0.002104914514347911, 0.0006262787501327693, 0.005802099592983723, 0.026016540825366974, 0.0425541028380394, 0.040001366287469864, 0.043205611407756805, 0.04034438729286194, 0.05012183263897896, 0.046061329543590546, 0.019606607034802437, 0.007183147594332695, 0.04836663603782654, 0.0536918118596077, 0.024944238364696503, 0.02164168283343315, 0.03908361867070198, 0.028223611414432526, 0.015733232721686363, 0.03816795349121094, 0.012438409961760044, 0.042325422167778015, 0.0009704792755655944, 0.012494868598878384, 0.0018007459584623575, 0.0210749302059412, 0.041356489062309265, 0.054101672023534775, 0.012424713931977749, 0.018569622188806534, 0.015371549874544144, 0.031856097280979156, 0.011114977300167084, 0.012467371299862862, 0.01999019831418991, 0.014317724853754044, 0.04720395430922508, 0.01600041426718235, 0.02541598305106163, 0.04732254520058632, 0.03942887857556343, 0.04182364046573639, 0.021485693752765656, 0.0005570221110247076, 0.03674343600869179, 0.00927107036113739, 0.022680606693029404, 0.0030091621447354555, 0.009036733768880367, 0.03756868094205856, 0.037092357873916626, 0.016934584826231003, 0.02053641714155674, 0.04346826300024986, 0.035119712352752686, 0.008396119810640812, 0.033801622688770294, 0.035260848701000214, 0.03754759579896927, 0.006823324132710695, 0.003613958600908518, 0.0027163061313331127, 0.01969272829592228, 0.007718116510659456, 0.020674021914601326, 0.019546570256352425, 0.027232123538851738, 0.0032296916469931602, 0.019403956830501556, 0.030404943972826004, 0.008255638182163239, 0.028219278901815414, 0.004878653679043055, 0.04044843092560768, 0.03332426771521568, 0.0068883891217410564, 0.03584417700767517, 0.046802863478660583, 0.043893963098526, 0.04792497679591179, 0.024737201631069183, 0.028460577130317688, 0.003257657866925001, 0.05013755336403847, 0.0389048270881176, 0.027959465980529785, 0.012015162967145443, 0.017617812380194664, 0.04743422567844391, 0.011156266555190086, 0.008387703448534012, 0.0011019723024219275, 0.021982694044709206, 0.021918434649705887, 0.03993797302246094, 0.007631369866430759, 0.02329542115330696, 0.048691920936107635, 0.0036192110273987055, 0.0013768959324806929, 0.033215805888175964, 0.00896260142326355, 0.03547801449894905, 0.05269291251897812, 0.0007206691661849618, 0.009315977804362774, 0.012407923117280006, 0.04839938506484032, 0.006293931044638157, 0.048529915511608124, 0.03883218765258789, 0.04483465105295181, 0.02464309148490429, 0.030141713097691536, 0.028126366436481476, 0.020720284432172775, 0.04140622168779373, 0.04922797903418541, 0.014667118899524212, 0.03553752228617668, 0.015214230865240097, 0.03037058748304844, 0.03618774563074112, 0.03415872901678085, 0.011376425623893738, 0.05114104598760605, 0.012431217357516289, 0.04046344757080078, 0.022129755467176437, 0.002718077739700675, 0.021110735833644867, 0.024725360795855522, 0.021288741379976273, 0.05381031334400177, 0.0010257922112941742, 0.0281034167855978, 0.05436640977859497, 0.05174345523118973, 0.021335825324058533, 0.05141819640994072, 0.044004425406455994, 0.048519574105739594, 0.048978500068187714, 0.033655982464551926, 0.026566296815872192, 0.03868955373764038, 0.009198863990604877, 0.04468502849340439, 0.03228822723031044, 0.026859698817133904, 0.019726933911442757, 0.04402397945523262, 0.029279837384819984, 0.029974117875099182, 0.03995317593216896, 0.0185479074716568, 0.030377749353647232, 0.026398366317152977, 0.034020815044641495, 0.019691362977027893, 0.00425290409475565, 0.008311131969094276, 0.028175508603453636, 0.015800103545188904, 0.054403163492679596, 0.03528816998004913, 0.008048245683312416, 0.005491300486028194, 0.012742584571242332, 0.009260544553399086, 0.03818326070904732, 0.018265696242451668, 0.003890098538249731, 0.050801243633031845, 0.03162083402276039, 0.03338394686579704, 0.007928417064249516, 0.005948902107775211, 0.05171038210391998, 0.03675456345081329, 0.010095725767314434, 0.015216360799968243, 0.02934674359858036, 0.048717450350522995, 0.04372698441147804, 0.011243720538914204, 0.044255733489990234, 0.014395510777831078, 0.04131360352039337, 0.03984865918755531, 0.020502936094999313, 0.03730691224336624, 0.02819669246673584, 0.010440660640597343, 0.005541905760765076, 0.004324846900999546, 0.03140737861394882, 0.03590782359242439, 0.014682735316455364, 0.030447106808423996, 0.02653815783560276, 0.005010044202208519, 0.035343412309885025, 0.033111389726400375], 10, map[nprobe, 3])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector108</t>
+  </si>
+  <si>
+    <t>vector108_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector109</t>
+  </si>
+  <si>
+    <t>vector110</t>
+  </si>
+  <si>
+    <t>vector111</t>
+  </si>
+  <si>
+    <t>vector112</t>
+  </si>
+  <si>
+    <t>vector113</t>
+  </si>
+  <si>
+    <t>vector114</t>
+  </si>
+  <si>
+    <t>vector115</t>
+  </si>
+  <si>
+    <t>IVFPQ算法 - dotproduct距离 - 1024维度 - 1024求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 128维度 - 1024求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 256维度 - 1024求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 512维度 - 1024求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 1024维度 - 1024求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 2维度 - 10000求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 8维度 - 2048求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 32维度 - 2048求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 64维度 - 2048求top20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4535,25 +4950,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L230"/>
+  <dimension ref="A1:L255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C179" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J200" sqref="J200"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C242" sqref="C242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18.375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="48.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.25" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="18.875" style="1" customWidth="1"/>
     <col min="10" max="10" width="72.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="111.75" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.625" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -11069,7 +11484,7 @@
       <c r="A193" s="3" t="s">
         <v>973</v>
       </c>
-      <c r="B193" s="1" t="s">
+      <c r="B193" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C193" s="1" t="s">
@@ -11104,7 +11519,7 @@
       <c r="A194" s="3" t="s">
         <v>974</v>
       </c>
-      <c r="B194" s="1" t="s">
+      <c r="B194" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C194" s="1" t="s">
@@ -11139,7 +11554,7 @@
       <c r="A195" s="3" t="s">
         <v>975</v>
       </c>
-      <c r="B195" s="1" t="s">
+      <c r="B195" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C195" s="1" t="s">
@@ -11174,7 +11589,7 @@
       <c r="A196" s="3" t="s">
         <v>976</v>
       </c>
-      <c r="B196" s="1" t="s">
+      <c r="B196" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C196" s="1" t="s">
@@ -11209,7 +11624,7 @@
       <c r="A197" s="3" t="s">
         <v>977</v>
       </c>
-      <c r="B197" s="1" t="s">
+      <c r="B197" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C197" s="1" t="s">
@@ -11244,7 +11659,7 @@
       <c r="A198" s="3" t="s">
         <v>1136</v>
       </c>
-      <c r="B198" s="1" t="s">
+      <c r="B198" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C198" s="1" t="s">
@@ -11279,7 +11694,7 @@
       <c r="A199" s="3" t="s">
         <v>978</v>
       </c>
-      <c r="B199" s="1" t="s">
+      <c r="B199" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C199" s="1" t="s">
@@ -11314,7 +11729,7 @@
       <c r="A200" s="3" t="s">
         <v>979</v>
       </c>
-      <c r="B200" s="1" t="s">
+      <c r="B200" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C200" s="1" t="s">
@@ -11336,7 +11751,7 @@
         <v>969</v>
       </c>
       <c r="J200" s="1" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="K200" s="1" t="s">
         <v>1068</v>
@@ -11349,7 +11764,7 @@
       <c r="A201" s="3" t="s">
         <v>980</v>
       </c>
-      <c r="B201" s="1" t="s">
+      <c r="B201" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C201" s="1" t="s">
@@ -11384,7 +11799,7 @@
       <c r="A202" s="3" t="s">
         <v>981</v>
       </c>
-      <c r="B202" s="1" t="s">
+      <c r="B202" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C202" s="1" t="s">
@@ -11419,7 +11834,7 @@
       <c r="A203" s="3" t="s">
         <v>982</v>
       </c>
-      <c r="B203" s="1" t="s">
+      <c r="B203" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C203" s="1" t="s">
@@ -11454,7 +11869,7 @@
       <c r="A204" s="3" t="s">
         <v>983</v>
       </c>
-      <c r="B204" s="1" t="s">
+      <c r="B204" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C204" s="1" t="s">
@@ -11489,7 +11904,7 @@
       <c r="A205" s="3" t="s">
         <v>984</v>
       </c>
-      <c r="B205" s="1" t="s">
+      <c r="B205" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C205" s="1" t="s">
@@ -11524,7 +11939,7 @@
       <c r="A206" s="3" t="s">
         <v>985</v>
       </c>
-      <c r="B206" s="1" t="s">
+      <c r="B206" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C206" s="1" t="s">
@@ -11559,7 +11974,7 @@
       <c r="A207" s="3" t="s">
         <v>986</v>
       </c>
-      <c r="B207" s="1" t="s">
+      <c r="B207" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C207" s="1" t="s">
@@ -11594,7 +12009,7 @@
       <c r="A208" s="3" t="s">
         <v>987</v>
       </c>
-      <c r="B208" s="1" t="s">
+      <c r="B208" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C208" s="1" t="s">
@@ -11629,7 +12044,7 @@
       <c r="A209" s="3" t="s">
         <v>988</v>
       </c>
-      <c r="B209" s="1" t="s">
+      <c r="B209" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C209" s="1" t="s">
@@ -11664,7 +12079,7 @@
       <c r="A210" s="3" t="s">
         <v>989</v>
       </c>
-      <c r="B210" s="1" t="s">
+      <c r="B210" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C210" s="1" t="s">
@@ -11699,7 +12114,7 @@
       <c r="A211" s="3" t="s">
         <v>990</v>
       </c>
-      <c r="B211" s="1" t="s">
+      <c r="B211" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C211" s="1" t="s">
@@ -11734,7 +12149,7 @@
       <c r="A212" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="B212" s="1" t="s">
+      <c r="B212" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C212" s="1" t="s">
@@ -11769,7 +12184,7 @@
       <c r="A213" s="3" t="s">
         <v>992</v>
       </c>
-      <c r="B213" s="1" t="s">
+      <c r="B213" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C213" s="1" t="s">
@@ -11804,7 +12219,7 @@
       <c r="A214" s="3" t="s">
         <v>993</v>
       </c>
-      <c r="B214" s="1" t="s">
+      <c r="B214" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C214" s="1" t="s">
@@ -11839,7 +12254,7 @@
       <c r="A215" s="3" t="s">
         <v>994</v>
       </c>
-      <c r="B215" s="1" t="s">
+      <c r="B215" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C215" s="1" t="s">
@@ -11874,7 +12289,7 @@
       <c r="A216" s="3" t="s">
         <v>995</v>
       </c>
-      <c r="B216" s="1" t="s">
+      <c r="B216" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C216" s="1" t="s">
@@ -11909,7 +12324,7 @@
       <c r="A217" s="3" t="s">
         <v>1117</v>
       </c>
-      <c r="B217" s="1" t="s">
+      <c r="B217" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C217" s="1" t="s">
@@ -11941,7 +12356,7 @@
       <c r="A218" s="3" t="s">
         <v>1118</v>
       </c>
-      <c r="B218" s="1" t="s">
+      <c r="B218" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C218" s="1" t="s">
@@ -11973,7 +12388,7 @@
       <c r="A219" s="3" t="s">
         <v>1119</v>
       </c>
-      <c r="B219" s="1" t="s">
+      <c r="B219" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C219" s="1" t="s">
@@ -12008,7 +12423,7 @@
       <c r="A220" s="3" t="s">
         <v>1120</v>
       </c>
-      <c r="B220" s="1" t="s">
+      <c r="B220" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C220" s="1" t="s">
@@ -12040,7 +12455,7 @@
       <c r="A221" s="3" t="s">
         <v>1121</v>
       </c>
-      <c r="B221" s="1" t="s">
+      <c r="B221" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C221" s="1" t="s">
@@ -12057,6 +12472,9 @@
       </c>
       <c r="G221" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="I221" s="1" t="s">
+        <v>969</v>
       </c>
       <c r="J221" s="1" t="s">
         <v>1155</v>
@@ -12072,7 +12490,7 @@
       <c r="A222" s="3" t="s">
         <v>1122</v>
       </c>
-      <c r="B222" s="1" t="s">
+      <c r="B222" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C222" s="1" t="s">
@@ -12089,6 +12507,9 @@
       </c>
       <c r="G222" s="3" t="s">
         <v>1157</v>
+      </c>
+      <c r="I222" s="1" t="s">
+        <v>969</v>
       </c>
       <c r="J222" s="1" t="s">
         <v>1158</v>
@@ -12104,7 +12525,7 @@
       <c r="A223" s="3" t="s">
         <v>1123</v>
       </c>
-      <c r="B223" s="1" t="s">
+      <c r="B223" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C223" s="1" t="s">
@@ -12136,7 +12557,7 @@
       <c r="A224" s="3" t="s">
         <v>1124</v>
       </c>
-      <c r="B224" s="1" t="s">
+      <c r="B224" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C224" s="1" t="s">
@@ -12168,7 +12589,7 @@
       <c r="A225" s="3" t="s">
         <v>1128</v>
       </c>
-      <c r="B225" s="1" t="s">
+      <c r="B225" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C225" s="1" t="s">
@@ -12182,6 +12603,9 @@
       </c>
       <c r="F225" s="1" t="s">
         <v>1029</v>
+      </c>
+      <c r="I225" s="1" t="s">
+        <v>969</v>
       </c>
       <c r="J225" s="1" t="s">
         <v>1166</v>
@@ -12197,7 +12621,7 @@
       <c r="A226" s="3" t="s">
         <v>1129</v>
       </c>
-      <c r="B226" s="1" t="s">
+      <c r="B226" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C226" s="1" t="s">
@@ -12211,6 +12635,9 @@
       </c>
       <c r="F226" s="1" t="s">
         <v>1037</v>
+      </c>
+      <c r="I226" s="1" t="s">
+        <v>969</v>
       </c>
       <c r="J226" s="1" t="s">
         <v>1170</v>
@@ -12226,7 +12653,7 @@
       <c r="A227" s="3" t="s">
         <v>1130</v>
       </c>
-      <c r="B227" s="1" t="s">
+      <c r="B227" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C227" s="1" t="s">
@@ -12241,8 +12668,11 @@
       <c r="F227" s="1" t="s">
         <v>1045</v>
       </c>
+      <c r="I227" s="1" t="s">
+        <v>969</v>
+      </c>
       <c r="J227" s="1" t="s">
-        <v>1171</v>
+        <v>1262</v>
       </c>
       <c r="K227" s="1" t="s">
         <v>1169</v>
@@ -12255,7 +12685,7 @@
       <c r="A228" s="3" t="s">
         <v>1134</v>
       </c>
-      <c r="B228" s="1" t="s">
+      <c r="B228" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C228" s="1" t="s">
@@ -12268,16 +12698,19 @@
         <v>1021</v>
       </c>
       <c r="F228" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="G228" s="3" t="s">
         <v>1172</v>
       </c>
-      <c r="G228" s="3" t="s">
+      <c r="I228" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J228" s="1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="K228" s="1" t="s">
         <v>1173</v>
-      </c>
-      <c r="J228" s="1" t="s">
-        <v>1175</v>
-      </c>
-      <c r="K228" s="1" t="s">
-        <v>1174</v>
       </c>
       <c r="L228" s="1" t="s">
         <v>129</v>
@@ -12287,7 +12720,7 @@
       <c r="A229" s="3" t="s">
         <v>1152</v>
       </c>
-      <c r="B229" s="1" t="s">
+      <c r="B229" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C229" s="1" t="s">
@@ -12303,16 +12736,16 @@
         <v>1037</v>
       </c>
       <c r="G229" s="3" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="I229" s="1" t="s">
         <v>970</v>
       </c>
       <c r="J229" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="K229" s="1" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="L229" s="1" t="s">
         <v>415</v>
@@ -12322,7 +12755,7 @@
       <c r="A230" s="3" t="s">
         <v>1153</v>
       </c>
-      <c r="B230" s="1" t="s">
+      <c r="B230" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C230" s="1" t="s">
@@ -12341,13 +12774,795 @@
         <v>1152</v>
       </c>
       <c r="J230" s="1" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="K230" s="1" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="L230" s="1" t="s">
         <v>415</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A231" s="3" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B231" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F231" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="G231" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="I231" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J231" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="K231" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="L231" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A232" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B232" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F232" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G232" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="I232" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J232" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="K232" s="1" t="s">
+        <v>1218</v>
+      </c>
+      <c r="L232" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A233" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F233" s="1" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G233" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I233" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J233" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="K233" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="L233" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A234" s="3" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>1206</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F234" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G234" s="3" t="s">
+        <v>1172</v>
+      </c>
+      <c r="I234" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J234" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="K234" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="L234" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A235" s="3" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="G235" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I235" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J235" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="K235" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="L235" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A236" s="3" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F236" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G236" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I236" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J236" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="K236" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="L236" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A237" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F237" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="G237" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I237" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J237" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="K237" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="L237" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A238" s="3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F238" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="G238" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="I238" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J238" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="K238" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="L238" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A239" s="3" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D239" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="G239" s="3" t="s">
+        <v>1115</v>
+      </c>
+      <c r="I239" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J239" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="K239" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="L239" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A240" s="3" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D240" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G240" s="3" t="s">
+        <v>1244</v>
+      </c>
+      <c r="I240" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J240" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="K240" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="L240" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A241" s="3" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D241" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F241" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="G241" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="I241" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J241" s="1" t="s">
+        <v>1256</v>
+      </c>
+      <c r="K241" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="L241" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A242" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="G242" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="I242" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J242" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="K242" s="1" t="s">
+        <v>1263</v>
+      </c>
+      <c r="L242" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A243" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="G243" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="I243" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J243" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="K243" s="1" t="s">
+        <v>1266</v>
+      </c>
+      <c r="L243" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A244" s="3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="G244" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="I244" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J244" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="K244" s="1" t="s">
+        <v>1271</v>
+      </c>
+      <c r="L244" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A245" s="3" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="G245" s="3" t="s">
+        <v>1272</v>
+      </c>
+      <c r="I245" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J245" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="K245" s="1" t="s">
+        <v>1276</v>
+      </c>
+      <c r="L245" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="246" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A246" s="3" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B246" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D246" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="G246" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="I246" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J246" s="1" t="s">
+        <v>1282</v>
+      </c>
+      <c r="K246" s="1" t="s">
+        <v>1277</v>
+      </c>
+      <c r="L246" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A247" s="3" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B247" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D247" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="G247" s="3" t="s">
+        <v>1274</v>
+      </c>
+      <c r="I247" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="J247" s="1" t="s">
+        <v>1283</v>
+      </c>
+      <c r="K247" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="L247" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="248" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A248" s="3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D248" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="G248" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="I248" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A249" s="3" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D249" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>1286</v>
+      </c>
+      <c r="I249" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A250" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D250" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F250" s="1" t="s">
+        <v>1287</v>
+      </c>
+      <c r="I250" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="251" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A251" s="3" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D251" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="I251" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A252" s="3" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D252" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F252" s="1" t="s">
+        <v>1289</v>
+      </c>
+      <c r="I252" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="253" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A253" s="3" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D253" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>1290</v>
+      </c>
+      <c r="I253" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="254" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A254" s="3" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D254" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="I254" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="255" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A255" s="3" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D255" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>1292</v>
+      </c>
+      <c r="I255" s="1" t="s">
+        <v>969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add IVFPQ COSINE metricType cases
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2694" uniqueCount="1302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2724" uniqueCount="1323">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4496,9 +4496,6 @@
     <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_187.csv</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>select id,feature_id,feature_index$distance from vector($vector103, feature, array[0.28576499223709106, 0.08687837421894073, 0.14799416065216064, 0.058550164103507996, 0.19060933589935303, 0.08999139070510864, 0.1514379382133484, 0.08630754053592682, 0.147443950176239, 0.11865786463022232, 0.08603266626596451, 0.026738379150629044, 0.04464268684387207, 0.07328195124864578, 0.1070372611284256, 0.08322914689779282, 0.034094709903001785, 0.16017472743988037, 0.03294524550437927, 0.14785508811473846, 0.18853361904621124, 0.14193195104599, 0.1404295563697815, 0.1011366918683052, 0.11323778331279755, 0.06974314898252487, 0.019739823415875435, 0.0017852566670626402, 0.19590851664543152, 0.04378505051136017, 0.13438871502876282, 0.12536169588565826, 0.037846311926841736, 0.19261693954467773, 0.15421807765960693, 0.012271392159163952, 0.08373595774173737, 0.1423385590314865, 0.13366387784481049, 0.14510740339756012, 0.02415030263364315, 0.04452469199895859, 0.0991881713271141, 0.13216648995876312, 0.10771691799163818, 0.1334938257932663, 0.10556206107139587, 0.10942403227090836, 0.10575082153081894, 0.18991316854953766, 0.1172894611954689, 0.09650064259767532, 0.16381768882274628, 0.03527522832155228, 0.09627934545278549, 0.1411363035440445, 0.09879021346569061, 0.18661963939666748, 0.036094631999731064, 0.2045263648033142, 0.18818239867687225, 0.15758785605430603, 0.02735513634979725, 0.16133542358875275], 8, map[nprobe, 2])</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4547,35 +4544,115 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>IVFPQ算法 - cosine距离 - 128维度 - 1024求top20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IVFPQ算法 - cosine距离 - 256维度 - 1024求top20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IVFPQ算法 - cosine距离 - 512维度 - 1024求top20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IVFPQ算法 - cosine距离 - 1024维度 - 1024求top20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>IVFPQ算法 - cosine距离 - 2维度 - 10000求top20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>IVFPQ算法 - cosine距离 - 8维度 - 2048求top20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IVFPQ算法 - cosine距离 - 32维度 - 2048求top20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IVFPQ算法 - cosine距离 - 64维度 - 2048求top20</t>
+    <t>select id,feature_id,feature_index$distance from vector($vector108, feature, array[1.2464210987091064, 0.38489800691604614], 20, map[nprobe, 10])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_188.csv</t>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 8维度 - 4096求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector109_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_189.csv</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector109, feature, array[2.0472664833068848, 0.9864906668663025, 0.8389081954956055, 0.7072503566741943, 0.739880383014679, 0.922918975353241, 0.03494282811880112, 0.5538699626922607], 20, map[nprobe, 6])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 24维度 - 2048求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector110_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 48维度 - 2048求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 96维度 - 1024求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 384维度 - 1024求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 768维度 - 1024求top20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_190.csv</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector110, feature, array[1.564573049545288, 0.7072410583496094, 0.11729453504085541, 0.7871541380882263, 0.6492518782615662, 0.9858483076095581, 0.9944221377372742, 0.754248321056366, 0.8897051811218262, 0.2620181143283844, 0.27863410115242004, 0.25595349073410034, 0.40355879068374634, 0.40881386399269104, 0.3039799928665161, 0.06743967533111572, 0.493000864982605, 0.828986644744873, 0.3469140827655792, 0.7403325438499451, 0.8115715980529785, 0.45165303349494934, 0.5160412192344666, 0.15477801859378815], 20, map[nprobe, 4])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector111_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_191.csv</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector111, feature, array[1.3257372379302979, 0.30023276805877686, 0.04542398825287819, 0.13122403621673584, 0.03887971118092537, 0.5333496928215027, 0.7706666588783264, 0.6775711178779602, 0.5954770445823669, 0.3450349271297455, 0.7778925895690918, 0.007492134813219309, 0.21658724546432495, 0.38315293192863464, 0.5108402967453003, 0.9368900656700134, 0.6455469131469727, 0.729595959186554, 0.8933457732200623, 0.05512532219290733, 0.7491166591644287, 0.30403488874435425, 0.9714257121086121, 0.01877804473042488, 0.6930736303329468, 0.07211603224277496, 0.9768120646476746, 0.9696327447891235, 0.6193642020225525, 0.08346204459667206, 0.9946091175079346, 0.6065057516098022, 0.44910702109336853, 0.8559362292289734, 0.8261013031005859, 0.42788347601890564, 0.5626505017280579, 0.68165522813797, 0.9379053711891174, 0.7818900346755981, 0.3581961989402771, 0.5507019758224487, 0.753814160823822, 0.7240028381347656, 0.11481262743473053, 0.9589543342590332, 0.1003684252500534, 0.5384477376937866], 20, map[nprobe, 5])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector112_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_192.csv</t>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector112, feature, array[1.3880192041397095, 0.12469174712896347, 0.9666946530342102, 0.5666744709014893, 0.10549285262823105, 0.7421829104423523, 0.5228951573371887, 0.06963501870632172, 0.8357218503952026, 0.2107839733362198, 0.6844350695610046, 0.92059326171875, 0.7522045969963074, 0.6827971935272217, 0.6963796019554138, 0.2376607209444046, 0.08488169312477112, 0.5136368870735168, 0.8609928488731384, 0.3587854504585266, 0.02370700053870678, 0.5639147758483887, 0.21305610239505768, 0.06626477092504501, 0.7454515099525452, 0.24932192265987396, 0.9979525208473206, 0.16210146248340607, 0.22156071662902832, 0.9341961145401001, 0.04138911888003349, 0.829578697681427, 0.3651023209095001, 0.8069941401481628, 0.48522377014160156, 0.030845224857330322, 0.005703444126993418, 0.1486523151397705, 0.9122492671012878, 0.6314519643783569, 0.10903112590312958, 0.21460439264774323, 0.7201200723648071, 0.5305340886116028, 0.5946058034896851, 0.3007280230522156, 0.9956521987915039, 0.9989649653434753, 0.3267371952533722, 0.30023276805877686, 0.04542398825287819, 0.13122403621673584, 0.03887971118092537, 0.5333496928215027, 0.7706666588783264, 0.6775711178779602, 0.5954770445823669, 0.3450349271297455, 0.7778925895690918, 0.007492134813219309, 0.21658724546432495, 0.38315293192863464, 0.5108402967453003, 0.9368900656700134, 0.6455469131469727, 0.729595959186554, 0.8933457732200623, 0.05512532219290733, 0.7491166591644287, 0.30403488874435425, 0.9714257121086121, 0.01877804473042488, 0.6930736303329468, 0.07211603224277496, 0.9768120646476746, 0.9696327447891235, 0.6193642020225525, 0.08346204459667206, 0.9946091175079346, 0.6065057516098022, 0.44910702109336853, 0.8559362292289734, 0.8261013031005859, 0.42788347601890564, 0.5626505017280579, 0.68165522813797, 0.9379053711891174, 0.7818900346755981, 0.3581961989402771, 0.5507019758224487, 0.753814160823822, 0.7240028381347656, 0.11481262743473053, 0.9589543342590332, 0.1003684252500534, 0.5384477376937866], 20, map[nprobe, 2])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_193.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_194.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/index/expectedresult/vector/vector_index_195.csv</t>
+  </si>
+  <si>
+    <t>vector113_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector113, feature, array[0.5573107004165649, 0.5475977659225464, 0.7435486316680908, 0.3565613031387329, 0.4645957350730896, 0.8615699410438538, 0.6090434193611145, 0.8706737160682678, 0.2091873586177826, 0.3457111716270447, 0.12559424340724945, 0.9705694913864136, 0.936345100402832, 0.25495269894599915, 0.28188928961753845, 0.4460704028606415, 0.39186879992485046, 0.9247180819511414, 0.5821620225906372, 0.1643548607826233, 0.7659389972686768, 0.36264482140541077, 0.9797981381416321, 0.7769717574119568, 0.5141956210136414, 0.44024401903152466, 0.1471070647239685, 0.9306623935699463, 0.9049304723739624, 0.42996758222579956, 0.4231700003147125, 0.30604982376098633, 0.10124076902866364, 0.40273457765579224, 0.9632226824760437, 0.4629789888858795, 0.21628934144973755, 0.03723647817969322, 0.9190627336502075, 0.4960905909538269, 0.8742397427558899, 0.9957003593444824, 0.2133864313364029, 0.06709082424640656, 0.25564682483673096, 0.20974856615066528, 0.7570276856422424, 0.7581883072853088, 0.37237870693206787, 0.6456737518310547, 0.013576600700616837, 0.1961548924446106, 0.87923663854599, 0.8623427748680115, 0.7663140296936035, 0.13020335137844086, 0.9383366703987122, 0.8888826370239258, 0.38967594504356384, 0.08990185707807541, 0.5238243937492371, 0.5106544494628906, 0.8373658061027527, 0.5029324889183044, 0.8165695071220398, 0.1526104211807251, 0.5358178019523621, 0.9326645731925964, 0.08736373484134674, 0.6428569555282593, 0.3464878797531128, 0.14181573688983917, 0.5657186508178711, 0.6365295052528381, 0.7643333077430725, 0.9659092426300049, 0.25781041383743286, 0.7855146527290344, 0.29628390073776245, 0.5880396366119385, 0.03700844198465347, 0.4962700307369232, 0.2814848721027374, 0.6427823305130005, 0.6472368240356445, 0.034217555075883865, 0.5612708330154419, 0.22819916903972626, 0.709744393825531, 0.9014987349510193, 0.6699643731117249, 0.7760484218597412, 0.9885140657424927, 0.7426231503486633, 0.20101666450500488, 0.14077244699001312, 0.7799120545387268, 0.8272802233695984, 0.48410001397132874, 0.3116922974586487, 0.09117633104324341, 0.2711831033229828, 0.9587698578834534, 0.49004048109054565, 0.6198761463165283, 0.8190874457359314, 0.184182807803154, 0.35552406311035156, 0.28992581367492676, 0.4363183081150055, 0.9230287671089172, 0.33332356810569763, 0.4795174300670624, 0.7945570349693298, 0.11235758662223816, 0.15520133078098297, 0.8872007727622986, 0.03955100476741791, 0.028950747102499008, 0.8958038687705994, 0.4633913040161133, 0.010914638638496399, 0.12129586189985275, 0.41602441668510437, 0.11581309884786606, 0.7169390320777893, 0.5464498400688171, 0.2336903065443039, 0.5838220119476318, 0.8079191446304321, 0.7886563539505005, 0.43091508746147156, 0.8634766340255737, 0.8227044343948364, 0.321199893951416, 0.27349165081977844, 0.06042920798063278, 0.6126560568809509, 0.9364484548568726, 0.04338137432932854, 0.550754964351654, 0.24550166726112366, 0.22057652473449707, 0.6241461038589478, 0.7532959580421448, 0.693272590637207, 0.25671395659446716, 0.7822800874710083, 0.3241245746612549, 0.951381266117096, 0.7119452357292175, 0.2595832347869873, 0.7361104488372803, 0.8345478177070618, 0.44675183296203613, 0.84134840965271, 0.6526991724967957, 0.06595972925424576, 0.5867308378219604, 0.7806279063224792, 0.40329059958457947, 0.7884334325790405, 0.5165075063705444, 0.4947369694709778, 0.9062142968177795, 0.8425130248069763, 0.25265154242515564, 0.4547799825668335, 0.8221304416656494, 0.7222866415977478, 0.40045079588890076, 0.6540039777755737, 0.3369004726409912, 0.5101748108863831, 0.11283786594867706, 0.5844746828079224, 0.6910374760627747, 0.4220035672187805, 0.5444891452789307, 0.08900521695613861, 0.8308838605880737, 0.8352225422859192, 0.7031892538070679, 0.21150581538677216, 0.7012810111045837, 0.6396660804748535, 0.22468090057373047, 0.5154932141304016, 0.15995366871356964, 0.7491512298583984, 0.9079524278640747, 0.7840310335159302, 0.02337864600121975, 0.9019748568534851, 0.07945382595062256, 0.6005831956863403, 0.5268236398696899, 0.6142992973327637, 0.7389845848083496, 0.3301548957824707, 0.1481240689754486, 0.07424722611904144, 0.45263636112213135, 0.4751254618167877, 0.5364026427268982, 0.8152586221694946, 0.016568100079894066, 0.08270206302404404, 0.9266353249549866, 0.1279739886522293, 0.4121222496032715, 0.4771133363246918, 0.6711813807487488, 0.4530234634876251, 0.3234080374240875, 0.9267156720161438, 0.6009581685066223, 0.40514475107192993, 0.2545982301235199, 0.503394365310669, 0.7257334589958191, 0.6749785542488098, 0.5575693249702454, 0.33304736018180847, 0.05706099793314934, 0.9067155718803406, 0.41158589720726013, 0.948490560054779, 0.4701417088508606, 0.7973489761352539, 0.5507484078407288, 0.3570510447025299, 0.16167916357517242, 0.08920487016439438, 0.0670381709933281, 0.41807183623313904, 0.2163538634777069, 0.05168494954705238, 0.7865158319473267, 0.69090735912323, 0.17663712799549103, 0.816535472869873, 0.1254362016916275, 0.7719787955284119, 0.4936907887458801, 0.6336119174957275, 0.006455720867961645, 0.4414479434490204, 0.12130578607320786, 0.3864710032939911, 0.7355014681816101, 0.1267300397157669, 0.4461290240287781, 0.338182657957077, 0.22426412999629974, 0.310703843832016, 0.3852267861366272, 0.757754385471344, 0.39435502886772156, 0.536403477191925, 0.09296955913305283, 0.4815520942211151, 0.6687894463539124, 0.4690309762954712, 0.4701370298862457, 0.49064797163009644, 0.9696126580238342, 0.9595230221748352, 0.7532637715339661, 0.9239938855171204, 0.041801467537879944, 0.014459137804806232, 0.7919448018074036, 0.8390949964523315, 0.611299455165863, 0.5239371061325073, 0.17717787623405457, 0.0412648506462574, 0.7083733677864075, 0.5951250195503235, 0.47022131085395813, 0.2798783481121063, 0.18216463923454285, 0.3103827238082886, 0.8065463900566101, 0.7662434577941895, 0.9310073256492615, 0.2999851703643799, 0.6004448533058167, 0.15210449695587158, 0.3449263870716095, 0.3317602574825287, 0.3279527723789215, 0.0403720997273922, 0.0010028282413259149, 0.08736693114042282, 0.9637157917022705, 0.1693049818277359, 0.6424758434295654, 0.09569598734378815, 0.16157545149326324, 0.44887059926986694, 0.8605000376701355, 0.644922137260437, 0.6884752511978149, 0.4005511701107025, 0.47954457998275757, 0.35106131434440613, 0.5167697668075562, 0.5180469155311584, 0.7741125822067261, 0.08356183022260666, 0.8865716457366943, 0.4798181354999542, 0.4636167585849762, 0.806938648223877, 0.9411027431488037, 0.6467693448066711, 0.04733210429549217, 0.6199333071708679, 0.30885016918182373, 0.07603836804628372, 0.7394579648971558, 0.7700243592262268, 0.07663034647703171, 0.7501293420791626, 0.48464494943618774, 0.6055157780647278, 0.9349602460861206, 0.003956442233175039, 0.5077810287475586, 0.1310654878616333, 0.23291391134262085, 0.7841230034828186, 0.6712197661399841, 0.5068410038948059, 0.5105273127555847, 0.30436280369758606, 0.9073706269264221, 0.31335699558258057, 0.04734308272600174, 0.5748774409294128, 0.8396755456924438, 0.9924387335777283, 0.2584961950778961, 0.1774890273809433, 0.5963530540466309, 0.9815335869789124, 0.03408551961183548, 0.7897367477416992, 0.08567126095294952, 0.964952290058136, 0.5332897305488586, 0.8799810409545898, 0.4471714198589325, 0.9746891260147095, 0.13828907907009125, 0.817624032497406, 0.3685404360294342, 0.5755240321159363, 0.13047538697719574, 0.776817798614502, 0.5308713316917419, 0.2840717136859894, 0.8031690716743469, 0.5726034641265869, 0.7564192414283752, 0.4590134024620056, 0.16734185814857483, 0.6427420377731323, 0.2562539577484131, 0.6360147595405579, 0.8187919855117798, 0.04673970490694046, 0.8416168093681335, 0.2151395082473755, 0.24844928085803986, 0.7286049127578735, 0.3990585207939148, 0.026676755398511887, 0.41409236192703247, 0.012757880613207817, 0.31578919291496277, 0.46302610635757446], 20, map[nprobe, 2])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector114_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector114, feature, array[1.0449751615524292, 0.6438606381416321, 0.5786641240119934, 0.5287215709686279, 0.6791334748268127, 0.6974433064460754, 0.4937366247177124, 0.3432634174823761, 0.7220731377601624, 0.1801556944847107, 0.4396243095397949, 0.9073228240013123, 0.7596746683120728, 0.2695479989051819, 0.010562661103904247, 0.07539232820272446, 0.4232860207557678, 0.04567971080541611, 0.9371276497840881, 0.4668791890144348, 0.8018461465835571, 0.2909679114818573, 0.4663814604282379, 0.19185693562030792, 0.74542236328125, 0.4744141101837158, 0.8491684198379517, 0.8408550024032593, 0.4369528591632843, 0.3897745609283447, 0.606580376625061, 0.41602131724357605, 0.08610948920249939, 0.645593523979187, 0.22086763381958008, 0.14198635518550873, 0.359367698431015, 0.14821933209896088, 0.11204753071069717, 0.9274766445159912, 0.9660369753837585, 0.12130977213382721, 0.9242919087409973, 0.8051689267158508, 0.1853627860546112, 0.8377742171287537, 0.05523940548300743, 0.9158093333244324, 0.3278478682041168, 0.17365829646587372, 0.19095538556575775, 0.8475309610366821, 0.4689273238182068, 0.8106445074081421, 0.5926397442817688, 0.18490955233573914, 0.24080964922904968, 0.986060619354248, 0.0022358703427016735, 0.7458927035331726, 0.8404889106750488, 0.5208288431167603, 0.8874691724777222, 0.02594914101064205, 0.40986379981040955, 0.9452869892120361, 0.025858383625745773, 0.23968330025672913, 0.7925348281860352, 0.018865123391151428, 0.8006250262260437, 0.9691514372825623, 0.8142989873886108, 0.3108184039592743, 0.1114804744720459, 0.9611859917640686, 0.4674453139305115, 0.5850889086723328, 0.972532331943512, 0.9801634550094604, 0.05990012735128403, 0.8357988595962524, 0.989426851272583, 0.9069386124610901, 0.579948902130127, 0.03875311091542244, 0.7621203064918518, 0.6578349471092224, 0.022759804502129555, 0.4056565463542938, 0.861653208732605, 0.7786186337471008, 0.7263638377189636, 0.5693877339363098, 0.4223267734050751, 0.47807177901268005, 0.41885626316070557, 0.9240368604660034, 0.001422326429747045, 0.7285804748535156, 0.1617477536201477, 0.8162345290184021, 0.4371659457683563, 0.9878908395767212, 0.7532408833503723, 0.22208453714847565, 0.018416132777929306, 0.5741081833839417, 0.8716416954994202, 0.23808731138706207, 0.25613707304000854, 0.4247114360332489, 0.0916634202003479, 0.1078498363494873, 0.880729079246521, 0.5670473575592041, 0.888699471950531, 0.7750993967056274, 0.6656354069709778, 0.9390836358070374, 0.6386016011238098, 0.6010266542434692, 0.9038141369819641, 0.2205493301153183, 0.08724416047334671, 0.046250708401203156, 0.5160443186759949, 0.7346898317337036, 0.07731186598539352, 0.3965665102005005, 0.7175227403640747, 0.29548540711402893, 0.08592412620782852, 0.009990147314965725, 0.552700936794281, 0.2000935822725296, 0.7754365801811218, 0.38610875606536865, 0.25125589966773987, 0.8807330131530762, 0.3139873743057251, 0.9928272366523743, 0.8081032037734985, 0.9569759964942932, 0.18721060454845428, 0.3002440929412842, 0.7125759124755859, 0.5832985043525696, 0.14542290568351746, 0.012314989231526852, 0.06721560657024384, 0.6225258111953735, 0.8002826571464539, 0.498173326253891, 0.3332744836807251, 0.3356311619281769, 0.047174014151096344, 0.0881119817495346, 0.22279955446720123, 0.6182222962379456, 0.648780882358551, 0.4259796440601349, 0.7467421889305115, 0.7169514298439026, 0.2035294771194458, 0.3972628712654114, 0.5504626631736755, 0.26477891206741333, 0.48073047399520874, 0.9758182168006897, 0.9837532043457031, 0.5079091787338257, 0.953762948513031, 0.2724020779132843, 0.9008644819259644, 0.7672747373580933, 0.3656857907772064, 0.6327970623970032, 0.02971009910106659, 0.9625127911567688, 0.6240543127059937, 0.4766276180744171, 0.6795626878738403, 0.5475702285766602, 0.13602283596992493, 0.5732817053794861, 0.7514252662658691, 0.9939442873001099, 0.2833348512649536, 0.7092027068138123, 0.4178902506828308, 0.76923006772995, 0.12114061415195465, 0.2808332145214081, 0.6181038022041321, 0.5507235527038574, 0.4483649432659149, 0.8917021155357361, 0.9934014081954956, 0.1378868818283081, 0.9799187779426575, 0.2095722258090973, 0.7875756025314331, 0.7764591574668884, 0.7664162516593933, 0.5945701599121094, 0.09343475848436356, 0.7639607787132263, 0.9655550718307495, 0.06949678063392639, 0.02567734383046627, 0.8493971228599548, 0.4722873568534851, 0.3542252480983734, 0.46810176968574524, 0.6465837955474854, 0.6770493984222412, 0.29698920249938965, 0.09017357230186462, 0.5233271718025208, 0.9246906042098999, 0.4946594536304474, 0.8472185730934143, 0.7171743512153625, 0.39812222123146057, 0.9292436242103577, 0.28552454710006714, 0.41233569383621216, 0.6169673800468445, 0.6567563414573669, 0.29630351066589355, 0.18495699763298035, 0.05279312655329704, 0.9133545160293579, 0.3165737986564636, 0.6559085845947266, 0.11042081564664841, 0.8188495635986328, 0.7671093344688416, 0.827659010887146, 0.9505362510681152, 0.03132469207048416, 0.5556855797767639, 0.6006721258163452, 0.7070278525352478, 0.41409993171691895, 0.7337198853492737, 0.34161436557769775, 0.30526748299598694, 0.521228551864624, 0.24062758684158325, 0.35989147424697876, 0.005196977406740189, 0.07100411504507065, 0.970314085483551, 0.8938589096069336, 0.06807029992341995, 0.2575553059577942, 0.5915147662162781, 0.12032261490821838, 0.7962466478347778, 0.6943781971931458, 0.9921537041664124, 0.08581957221031189, 0.9351524710655212, 0.8031519055366516, 0.1318860948085785, 0.4703972041606903, 0.4472178518772125, 0.8118127584457397, 0.29355189204216003, 0.8730934858322144, 0.9799683690071106, 0.33616647124290466, 0.31396809220314026, 0.1918739229440689, 0.4669994115829468, 0.1352279931306839, 0.09313662350177765, 0.4788731336593628, 0.7697119116783142, 0.434381902217865, 0.4781843423843384, 0.2582091689109802, 0.5505799055099487, 0.6547128558158875, 0.4134124219417572, 0.8764613270759583, 0.22625266015529633, 0.4866049587726593, 0.5986716747283936, 0.06955748051404953, 0.18641895055770874, 0.6698516011238098, 0.25043049454689026, 0.8421813249588013, 0.8219397068023682, 0.37100258469581604, 0.8262695074081421, 0.9398248195648193, 0.5749589204788208, 0.8187357783317566, 0.12916991114616394, 0.7666134238243103, 0.9115617871284485, 0.692862331867218, 0.5429908037185669, 0.8731981515884399, 0.15428441762924194, 0.5700650811195374, 0.3572421371936798, 0.6732203364372253, 0.15179292857646942, 0.9866137504577637, 0.1456635743379593, 0.9707493782043457, 0.6399383544921875, 0.49514105916023254, 0.41771894693374634, 0.5297654867172241, 0.4098798632621765, 0.6600776314735413, 0.5566463470458984, 0.11286056786775589, 0.3565855920314789, 0.015208072029054165, 0.17546750605106354, 0.1362261176109314, 0.6552024483680725, 0.17709635198116302, 0.5286421179771423, 0.22644273936748505, 0.8044739365577698, 0.4013242721557617, 0.3010190427303314, 0.39689111709594727, 0.14949314296245575, 0.31387874484062195, 0.21433565020561218, 0.8950219750404358, 0.5673409104347229, 0.7191692590713501, 0.09965623915195465, 0.1627945750951767, 0.9565834403038025, 0.7182984948158264, 0.28176364302635193, 0.037181783467531204, 0.8108833432197571, 0.5802493691444397, 0.08700978010892868, 0.7916145920753479, 0.5397902727127075, 0.6012015342712402, 0.32426321506500244, 0.9425000548362732, 0.23094601929187775, 0.20790819823741913, 0.09977171570062637, 0.9648944139480591, 0.8912761211395264, 0.9964083433151245, 0.3245316743850708, 0.5365813374519348, 0.7814844250679016, 0.7811955809593201, 0.8265535235404968, 0.9620278477668762, 0.8987449407577515, 0.27844128012657166, 0.14652401208877563, 0.02323896251618862, 0.11082073301076889, 0.16992169618606567, 0.0016107039991766214, 0.21871890127658844, 0.4871930480003357, 0.24625259637832642, 0.4984169006347656, 0.21486227214336395, 0.21173439919948578, 0.29173043370246887, 0.08565999567508698, 0.5886773467063904, 0.6345279216766357, 0.4824119806289673, 0.03696056827902794, 0.726763129234314, 0.8756948113441467, 0.3511827290058136, 0.6555613875389099, 0.436270534992218, 0.09676741808652878, 0.8130906224250793, 0.011573629453778267, 0.12047906965017319, 0.4739246964454651, 0.15434345602989197, 0.9875195026397705, 0.9345647692680359, 0.4109625518321991, 0.41080236434936523, 0.6679548621177673, 0.10405734926462173, 0.07058192789554596, 0.24848397076129913, 0.35256996750831604, 0.6640636920928955, 0.052339378744363785, 0.716637134552002, 0.4655773937702179, 0.3227013051509857, 0.2541847229003906, 0.26686564087867737, 0.591152012348175, 0.5846475958824158, 0.1693047136068344, 0.5493166446685791, 0.5403175354003906, 0.22481870651245117, 0.008304706774652004, 0.20862248539924622, 0.5537424683570862, 0.45669451355934143, 0.7966304421424866, 0.45194944739341736, 0.013733670115470886, 0.19584766030311584, 0.6489018201828003, 0.42340731620788574, 0.8251070976257324, 0.5958651900291443, 0.8008478879928589, 0.13535967469215393, 0.6079177856445312, 0.5777745246887207, 0.6988573670387268, 0.1991470456123352, 0.8022451996803284, 0.5252223014831543, 0.9244032502174377, 0.9803556799888611, 0.8092208504676819, 0.9832926988601685, 0.89023357629776, 0.17671582102775574, 0.17749956250190735, 0.18731893599033356, 0.24934975802898407, 0.5372945666313171, 0.17311705648899078, 0.9481943249702454, 0.28688111901283264, 0.6077295541763306, 0.6036965250968933, 0.1860133558511734, 0.714789628982544, 0.7110152244567871, 0.21389447152614594, 0.2658546566963196, 0.3709697723388672, 0.9712091684341431, 0.1784229278564453, 0.5211862921714783, 0.35579922795295715, 0.8018534183502197, 0.3654511868953705, 0.9140967130661011, 0.07715299725532532, 0.23687028884887695, 0.06142176687717438, 0.03382579982280731, 0.5617294311523438, 0.48650237917900085, 0.8110563158988953, 0.7171922326087952, 0.22330601513385773, 0.4305540919303894, 0.1827339380979538, 0.9354550242424011, 0.6644001007080078, 0.8482269048690796, 0.933756947517395, 0.6246568560600281, 0.9649973511695862, 0.9741939902305603, 0.2185945063829422, 0.02331354282796383, 0.7172597050666809, 0.9490103125572205, 0.7089510560035706, 0.4935244917869568, 0.10538972169160843, 0.6565831899642944, 0.7097471952438354, 0.9868389368057251, 0.7619495391845703, 0.6746072769165039, 0.6860854029655457, 0.9931010007858276, 0.6194504499435425, 0.39565950632095337, 0.9230505228042603, 0.9053921699523926, 0.8412156701087952, 0.07399551570415497, 0.9781930446624756, 0.23119322955608368, 0.09070639312267303, 0.725421667098999, 0.4425022304058075, 0.6515668034553528, 0.06385461986064911, 0.9149104356765747, 0.9418982863426208, 0.06481432169675827, 0.21126538515090942, 0.3786473870277405, 0.4528483748435974, 0.314597487449646, 0.5504764914512634, 0.1734945923089981, 0.4001966416835785, 0.346720814704895, 0.32737207412719727, 0.6484793424606323, 0.03623906522989273, 0.9724771976470947, 0.053302109241485596, 0.6831585764884949, 0.5849616527557373, 0.4628060758113861, 0.41511887311935425, 0.4009139835834503, 0.033058006316423416, 0.8419308066368103, 0.24198362231254578, 0.38903170824050903, 0.6128711700439453, 0.8019378185272217, 0.6195152401924133, 0.7502688765525818, 0.16205833852291107, 0.48737621307373047, 0.8338391184806824, 0.820027232170105, 0.8271459937095642, 0.13839314877986908, 0.5982616543769836, 0.9063892364501953, 0.8532602190971375, 0.8648112416267395, 0.963438093662262, 0.9551274180412292, 0.9573898315429688, 0.6479527354240417, 0.17927388846874237, 0.933710515499115, 0.40480777621269226, 0.005202859174460173, 0.010705084539949894, 0.23611335456371307, 0.7043103575706482, 0.12269102036952972, 0.3687782883644104, 0.8314900994300842, 0.987348735332489, 0.16771696507930756, 0.08087381720542908, 0.37183907628059387, 0.5774405598640442, 0.35026249289512634, 0.9580845236778259, 0.5263229608535767, 0.15821415185928345, 0.6917675137519836, 0.5384197235107422, 0.4530535042285919, 0.2735464870929718, 0.6869832873344421, 0.5884127616882324, 0.1470378041267395, 0.03902622312307358, 0.8493537902832031, 0.9549892544746399, 0.4440450966358185, 0.18894773721694946, 0.3229064345359802, 0.29552870988845825, 0.5923060178756714, 0.9304932355880737, 0.6321811676025391, 0.34879598021507263, 0.4553232789039612, 0.5835397243499756, 0.9640840291976929, 0.7123296856880188, 0.9584895968437195, 0.06722105294466019, 0.10524654388427734, 0.384044885635376, 0.7480373382568359, 0.0015745179262012243, 0.9919617772102356, 0.8900533318519592, 0.3375338315963745, 0.12749430537223816, 0.1778029203414917, 0.3933278024196625, 0.004998977296054363, 0.967164158821106, 0.18252262473106384, 0.4246516823768616, 0.9466995000839233, 0.6618911623954773, 0.5756800770759583, 0.8770455121994019, 0.08556395024061203, 0.2355605959892273, 0.8815645575523376, 0.12941919267177582, 0.1733749508857727, 0.5371890068054199, 0.5147970914840698, 0.5896971821784973, 0.8938300609588623, 0.7695490121841431, 0.05197066813707352, 0.00800657831132412, 0.7868567109107971, 0.27977070212364197, 0.7381390929222107, 0.45987415313720703, 0.32768768072128296, 0.678010106086731, 0.13425227999687195, 0.02424146793782711, 0.19710186123847961, 0.9239782094955444, 0.4522116780281067, 0.9520038962364197, 0.9115758538246155, 0.19578678905963898, 0.5331628322601318, 0.7805359959602356, 0.6302956938743591, 0.8419826626777649, 0.7766551375389099, 0.14337708055973053, 0.17434526979923248, 0.4596658945083618, 0.28707122802734375, 0.5171709656715393, 0.29147663712501526, 0.7001183032989502, 0.7757300138473511, 0.2110271006822586, 0.49688273668289185, 0.3242947459220886, 0.8788022994995117, 0.6961814761161804, 0.8788007497787476, 0.5459599494934082, 0.5740014314651489, 0.049843527376651764, 0.9727349281311035, 0.7073594331741333, 0.3456420302391052, 0.4508548974990845, 0.641571581363678, 0.7891095876693726, 0.74407559633255, 0.019806085154414177, 0.3949742615222931, 0.2961771786212921, 0.21972808241844177, 0.047016311436891556, 0.7904474139213562, 0.20079998672008514, 0.06383122503757477, 0.34375500679016113, 0.12595444917678833, 0.6216675639152527, 0.6235424280166626, 0.5859535336494446, 0.8561268448829651, 0.009821767918765545, 0.27908724546432495, 0.6350058913230896, 0.9335972666740417, 0.39599505066871643, 0.417370080947876, 0.40554019808769226, 0.8605796098709106, 0.726032018661499, 0.3859851360321045, 0.251936137676239, 0.5074277520179749, 0.4724961221218109, 0.4547683000564575, 0.9887772798538208, 0.700387179851532, 0.9577260613441467, 0.8210719227790833, 0.36226150393486023, 0.08448237180709839, 0.8746665120124817, 0.7254707217216492, 0.4853966534137726, 0.4762662947177887, 0.2468544840812683, 0.19896796345710754, 0.5713694095611572, 0.9782240390777588, 0.39332592487335205, 0.00355304847471416, 0.3692082166671753, 0.13343580067157745, 0.8580567836761475, 0.9201350808143616, 0.12545821070671082, 0.9490429162979126, 0.055997759103775024, 0.9220232963562012, 0.40480437874794006, 0.0020276112481951714, 0.09205994755029678, 0.3576927185058594, 0.3525591492652893, 0.06537027657032013, 0.5350173711776733, 0.40607669949531555, 0.15910427272319794, 0.16664764285087585, 0.8849092721939087, 0.4102189838886261, 0.3766339123249054, 0.3556791841983795, 0.9710025191307068, 0.28549090027809143, 0.5054121613502502, 0.7048563361167908, 0.740104615688324, 0.3418636620044708, 0.18338769674301147, 0.561529278755188, 0.23851150274276733, 0.4170273542404175, 0.027689296752214432, 0.8754422664642334, 0.4420372247695923, 0.5807412266731262, 0.4825296103954315, 0.6244035959243774, 0.9306355118751526, 0.10463228076696396, 0.18627820909023285, 0.7923347353935242, 0.8809717893600464, 0.4899749159812927, 0.031418830156326294, 0.923637866973877, 0.4399312138557434, 0.8818597793579102, 0.9028787016868591, 0.22564777731895447, 0.94058758020401, 0.8865091800689697], 20, map[nprobe, 2])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IVFPQ算法 - cosine距离 - 1536维度 - 128求top10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,feature_id,feature_index$distance from vector($vector115, feature, array[0.9902235269546509, 0.10431499034166336, 0.4925372302532196, 0.8681201934814453, 0.8722683191299438, 0.830732524394989, 0.1524062156677246, 0.9349273443222046, 0.9830064177513123, 0.20973382890224457, 0.9838352203369141, 0.5014108419418335, 0.2647353410720825, 0.6980723738670349, 0.8327855467796326, 0.5319531559944153, 0.15155324339866638, 0.017415184527635574, 0.4389483630657196, 0.257061243057251, 0.15360957384109497, 0.3058664798736572, 0.9838027954101562, 0.360340416431427, 0.746213972568512, 0.07666397839784622, 0.4372844099998474, 0.014756870456039906, 0.5788666605949402, 0.5449406504631042, 0.9139546155929565, 0.8067901730537415, 0.6736865043640137, 0.07143417000770569, 0.8128687739372253, 0.08907461166381836, 0.28962501883506775, 0.012927844189107418, 0.9696642160415649, 0.6620621085166931, 0.3114590048789978, 0.03006383776664734, 0.5796226859092712, 0.2140612006187439, 0.6916781067848206, 0.967767059803009, 0.5517066121101379, 0.16160210967063904, 0.49476298689842224, 0.446463942527771, 0.6734089255332947, 0.19210585951805115, 0.5712792277336121, 0.2841925621032715, 0.5058475136756897, 0.14268431067466736, 0.12685224413871765, 0.7860594391822815, 0.3492421507835388, 0.893543541431427, 0.7209875583648682, 0.6450263857841492, 0.5675541758537292, 0.23288927972316742, 0.7606458067893982, 0.07128461450338364, 0.6964651346206665, 0.24048973619937897, 0.6247967481613159, 0.8964740037918091, 0.45580175518989563, 0.7296887040138245, 0.22816988825798035, 0.029268542304635048, 0.8915632367134094, 0.40926042199134827, 0.2030932605266571, 0.6919152736663818, 0.8419082760810852, 0.2563587427139282, 0.12631629407405853, 0.7140357494354248, 0.15265466272830963, 0.7328639030456543, 0.4638957381248474, 0.7255092263221741, 0.21460771560668945, 0.21966920793056488, 0.9287545680999756, 0.03616950288414955, 0.18558597564697266, 0.4677453935146332, 0.9435461759567261, 0.4441729784011841, 0.2739681303501129, 0.6308834552764893, 0.8681932687759399, 0.11704379320144653, 0.589827835559845, 0.6223616600036621, 0.22368013858795166, 0.9446212649345398, 0.6212049722671509, 0.31601354479789734, 0.4408273994922638, 0.3333006501197815, 0.03972972184419632, 0.056194256991147995, 0.8861505389213562, 0.9818869829177856, 0.6056957244873047, 0.9775523543357849, 0.6636890172958374, 0.40653443336486816, 0.8600038886070251, 0.8776096105575562, 0.9745752215385437, 0.972199022769928, 0.8638783693313599, 0.6721484065055847, 0.5186344981193542, 0.791917085647583, 0.9451949596405029, 0.888151228427887, 0.97093665599823, 0.5097098350524902, 0.2753954529762268, 0.49438029527664185, 0.7956991195678711, 0.9898937344551086, 0.4951379597187042, 0.3869473934173584, 0.19586464762687683, 0.8953040242195129, 0.0009835307719185948, 0.9355499148368835, 0.9517822265625, 0.7543898820877075, 0.7343156337738037, 0.4359067678451538, 0.7509841322898865, 0.30458179116249084, 0.1464567333459854, 0.6193007230758667, 0.8668887615203857, 0.5020105838775635, 0.6219688653945923, 0.09826795756816864, 0.788691520690918, 0.2709279954433441, 0.9040477275848389, 0.1951267421245575, 0.018649810925126076, 0.1581597775220871, 0.32359930872917175, 0.6054627895355225, 0.682092547416687, 0.2932957410812378, 0.39800047874450684, 0.15062150359153748, 0.3486483693122864, 0.17219838500022888, 0.9427631497383118, 0.24497780203819275, 0.369671106338501, 0.8383969664573669, 0.9376201033592224, 0.3204548954963684, 0.8091537952423096, 0.18348929286003113, 0.7939112186431885, 0.8889263868331909, 0.6047505140304565, 0.6250599026679993, 0.29245203733444214, 0.899971067905426, 0.22505472600460052, 0.9743149280548096, 0.6746429204940796, 0.37511003017425537, 0.8312550783157349, 0.455399751663208, 0.5906211137771606, 0.12419106066226959, 0.3229463994503021, 0.30098292231559753, 0.15001018345355988, 0.7588010430335999, 0.7687546014785767, 0.6517909169197083, 0.0766993910074234, 0.8894836902618408, 0.7034062147140503, 0.7792702913284302, 0.7765412330627441, 0.31707504391670227, 0.6997724771499634, 0.6622527837753296, 0.47220128774642944, 0.32911673188209534, 0.9556384682655334, 0.3046383559703827, 0.14930294454097748, 0.7901278138160706, 0.5603054165840149, 0.49803611636161804, 0.45862188935279846, 0.7027131915092468, 0.3309139311313629, 0.3433569669723511, 0.24075841903686523, 0.47841811180114746, 0.09821527451276779, 0.8468405604362488, 0.7989208102226257, 0.6315018534660339, 0.7078220844268799, 0.032576873898506165, 0.11913882941007614, 0.808164119720459, 0.35538816452026367, 0.393353670835495, 0.2193855345249176, 0.89907306432724, 0.11825469881296158, 0.9549816846847534, 0.0005904135177843273, 0.638552188873291, 0.20891346037387848, 0.0793919786810875, 0.8178072571754456, 0.5769234299659729, 0.8885272145271301, 0.45078858733177185, 0.09329517930746078, 0.7293152213096619, 0.0677352249622345, 0.0134489880874753, 0.020049866288900375, 0.4047183394432068, 0.6793797016143799, 0.6672581434249878, 0.600193440914154, 0.3501960337162018, 0.9053044319152832, 0.43740057945251465, 0.6974921822547913, 0.22054646909236908, 0.2693362236022949, 0.890095591545105, 0.15740422904491425, 0.7033600807189941, 0.13587848842144012, 0.8914653062820435, 0.30210092663764954, 0.9178286194801331, 0.18185602128505707, 0.15479016304016113, 0.8494400978088379, 0.7593747973442078, 0.7473207116127014, 0.48755943775177, 0.4769561290740967, 0.4950885474681854, 0.4827111065387726, 0.9361315965652466, 0.4797084629535675, 0.5216492414474487, 0.47123172879219055, 0.6359973549842834, 0.5099602341651917, 0.03890925273299217, 0.26113447546958923, 0.9460735321044922, 0.3888813555240631, 0.5715094804763794, 0.5333307385444641, 0.9247259497642517, 0.6850947737693787, 0.8652344346046448, 0.0874122902750969, 0.04754435643553734, 0.31448766589164734, 0.5250023603439331, 0.2405785173177719, 0.6725209355354309, 0.5341150760650635, 0.38017794489860535, 0.7739356756210327, 0.4966346025466919, 0.995715856552124, 0.6718922257423401, 0.5896984338760376, 0.2216217964887619, 0.15965242683887482, 0.6196257472038269, 0.531399130821228, 0.26334846019744873, 0.4372881054878235, 0.5249695777893066, 0.7433487176895142, 0.9068548083305359, 0.2210480123758316, 0.2822028696537018, 0.4108716547489166, 0.7857139110565186, 0.27395138144493103, 0.20482881367206573, 0.9258070588111877, 0.6310699582099915, 0.5921266078948975, 0.5859371423721313, 0.0067001995630562305, 0.49284690618515015, 0.9688669443130493, 0.5649298429489136, 0.09057779610157013, 0.19492579996585846, 0.9782233834266663, 0.6728528141975403, 0.26003211736679077, 0.1505855768918991, 0.1489274948835373, 0.05706246197223663, 0.9388375282287598, 0.18222551047801971, 0.1313900351524353, 0.9627377986907959, 0.3706483244895935, 0.5246455073356628, 0.7725783586502075, 0.7702359557151794, 0.5866581201553345, 0.17769668996334076, 0.9544842839241028, 0.5680734515190125, 0.8845875263214111, 0.5783229470252991, 0.2774977385997772, 0.8771805763244629, 0.45748788118362427, 0.11635572463274002, 0.528388500213623, 0.4006480872631073, 0.606464147567749, 0.755187451839447, 0.34578827023506165, 0.5682968497276306, 0.7122334837913513, 0.5424001216888428, 0.917868971824646, 0.8127769231796265, 0.02478407695889473, 0.5514575839042664, 0.0049731191247701645, 0.9176387786865234, 0.002859156345948577, 0.5905631184577942, 0.16881851851940155, 0.016540611162781715, 0.5920075178146362, 0.2915170192718506, 0.2122717797756195, 0.49616947770118713, 0.2694140672683716, 0.7864028215408325, 0.2011972814798355, 0.22466951608657837, 0.0072517795488238335, 0.7205490469932556, 0.7928007245063782, 0.4883838891983032, 0.06322711706161499, 0.7535420060157776, 0.5698924660682678, 0.17615631222724915, 0.9928708076477051, 0.17343948781490326, 0.1237945482134819, 0.8786767721176147, 0.8966941833496094, 0.3080652356147766, 0.04352223500609398, 0.546010434627533, 0.8659591674804688, 0.1526016891002655, 0.09960544109344482, 0.02918417938053608, 0.07468264549970627, 0.3006387948989868, 0.7012244462966919, 0.8984241485595703, 0.650434672832489, 0.8699777722358704, 0.7138668894767761, 0.5873762369155884, 0.618304967880249, 0.11495287716388702, 0.30427223443984985, 0.3498757779598236, 0.3505840301513672, 0.10299947112798691, 0.72786545753479, 0.27773043513298035, 0.5042670369148254, 0.3558466136455536, 0.8995752334594727, 0.02561158873140812, 0.0841745063662529, 0.46816393733024597, 0.7122877836227417, 0.9924346804618835, 0.7917988896369934, 0.1384432315826416, 0.8408766984939575, 0.33010903000831604, 0.505934476852417, 0.878890335559845, 0.32835277915000916, 0.7709540724754333, 0.9224629998207092, 0.04817458614706993, 0.6690673828125, 0.48130860924720764, 0.8828980922698975, 0.7406775951385498, 0.0045904736034572124, 0.46130016446113586, 0.49253806471824646, 0.5105828046798706, 0.3459140658378601, 0.5170886516571045, 0.9654001593589783, 0.9951261281967163, 0.7578433156013489, 0.9665701389312744, 0.26521801948547363, 0.7781181335449219, 0.5220229625701904, 0.8422088623046875, 0.891946017742157, 0.25643181800842285, 0.12808963656425476, 0.14494113624095917, 0.4559922218322754, 0.9382727146148682, 0.7970611453056335, 0.5102805495262146, 0.2452685385942459, 0.9435397982597351, 0.1397826075553894, 0.8129761219024658, 0.4322268068790436, 0.11890196055173874, 0.2577558755874634, 0.6904773712158203, 0.16196441650390625, 0.8507242202758789, 0.022312331944704056, 0.4390030801296234, 0.6317897439002991, 0.267055869102478, 0.9840227961540222, 0.2265866994857788, 0.4850917160511017, 0.8768416047096252, 0.9088805913925171, 0.20929481089115143, 0.1866832822561264, 0.13339482247829437, 0.8052598237991333, 0.4309256374835968, 0.3309306800365448, 0.6407923698425293, 0.28302469849586487, 0.8368085622787476, 0.0835670605301857, 0.13155408203601837, 0.9648972749710083, 0.4055004119873047, 0.5493667721748352, 0.46748796105384827, 0.24159188568592072, 0.6395735740661621, 0.5471751689910889, 0.7100662589073181, 0.400621622800827, 0.9984897971153259, 0.9803318381309509, 0.39545440673828125, 0.1151449903845787, 0.9904844760894775, 0.2478373646736145, 0.2618675231933594, 0.1895902007818222, 0.3733517825603485, 0.1559653878211975, 0.4321887493133545, 0.7668293714523315, 0.582956075668335, 0.030917683616280556, 0.5985668897628784, 0.35136914253234863, 0.5254815220832825, 0.16164334118366241, 0.5031083822250366, 0.8812853097915649, 0.45757395029067993, 0.9772512912750244, 0.9559372663497925, 0.8792067766189575, 0.8774374723434448, 0.1446678340435028, 0.10850758850574493, 0.3240841329097748, 0.13229094445705414, 0.9260293245315552, 0.03915002942085266, 0.5516790747642517, 0.9809667468070984, 0.05196494981646538, 0.11876443028450012, 0.7931789755821228, 0.23084916174411774, 0.7028468251228333, 0.25613224506378174, 0.5647616982460022, 0.22060178220272064, 0.9715662002563477, 0.09961102157831192, 0.49895238876342773, 0.40517812967300415, 0.9969459772109985, 0.7935271263122559, 0.4981478452682495, 0.29133665561676025, 0.44439953565597534, 0.425699383020401, 0.4763699173927307, 0.9215809106826782, 0.24236030876636505, 0.7956124544143677, 0.014775332994759083, 0.32487258315086365, 0.7371284365653992, 0.5908387899398804, 0.30247777700424194, 0.43907877802848816, 0.9903702139854431, 0.1989789456129074, 0.5918221473693848, 0.7085360884666443, 0.5898317694664001, 0.4510810673236847, 0.6613816618919373, 0.2952318489551544, 0.02493247762322426, 0.12391345947980881, 0.6733596324920654, 0.05711675062775612, 0.47925394773483276, 0.8671201467514038, 0.8791252970695496, 0.860435962677002, 0.7794710993766785, 0.23672603070735931, 0.9939964413642883, 0.2947549819946289, 0.03671910986304283, 0.937823474407196, 0.8802260160446167, 0.31307414174079895, 0.3523872196674347, 0.04728609696030617, 0.9888927340507507, 0.7850785255432129, 0.4869828224182129, 0.31264635920524597, 0.06642528623342514, 0.9304323792457581, 0.21197645366191864, 0.7239446640014648, 0.872456431388855, 0.8789159059524536, 0.6340766549110413, 0.449869841337204, 0.44816216826438904, 0.534173309803009, 0.9126707911491394, 0.4711556136608124, 0.5168650150299072, 0.6492165923118591, 0.8386184573173523, 0.6387537717819214, 0.8471029996871948, 0.31365832686424255, 0.16466949880123138, 0.3805263042449951, 0.777142345905304, 0.8887110948562622, 0.5459561944007874, 0.9729193449020386, 0.8573066592216492, 0.3737916648387909, 0.517247200012207, 0.6410920023918152, 0.20879340171813965, 0.9273661375045776, 0.48032259941101074, 0.18216298520565033, 0.43896523118019104, 0.8830050230026245, 0.30291175842285156, 0.7757983803749084, 0.8128688931465149, 0.024925503879785538, 0.5879754424095154, 0.7618100643157959, 0.5647273063659668, 0.05252961069345474, 0.2591903805732727, 0.14655964076519012, 0.42745181918144226, 0.15190084278583527, 0.4318661093711853, 0.8434489965438843, 0.03704701364040375, 0.5753170847892761, 0.8302214741706848, 0.9486076831817627, 0.5900678038597107, 0.9620041847229004, 0.34370487928390503, 0.0218867938965559, 0.7149175405502319, 0.7317449450492859, 0.2506178319454193, 0.23113417625427246, 0.45467403531074524, 0.9072763919830322, 0.23693597316741943, 0.7983786463737488, 0.4105972647666931, 0.0062048714607954025, 0.37672513723373413, 0.7877068519592285, 0.6916950345039368, 0.616522490978241, 0.8136075735092163, 0.19002509117126465, 0.27153536677360535, 0.6925373673439026, 0.06465853005647659, 0.07165776938199997, 0.5824829936027527, 0.3678259551525116, 0.45163843035697937, 0.36982086300849915, 0.7873246669769287, 0.21836048364639282, 0.4204391539096832, 0.8240039348602295, 0.07276085764169693, 0.38298696279525757, 0.7950550317764282, 0.2184973657131195, 0.8491131663322449, 0.567008912563324, 0.6902289986610413, 0.6796565651893616, 0.10449163615703583, 0.40591517090797424, 0.5448713302612305, 0.37248215079307556, 0.955883264541626, 0.9698770642280579, 0.7933648824691772, 0.5064224004745483, 0.5269209146499634, 0.6102035641670227, 0.36456477642059326, 0.5992593169212341, 0.7629435658454895, 0.3763626217842102, 0.1819257140159607, 0.016094574704766273, 0.21366019546985626, 0.4362291097640991, 0.6657033562660217, 0.7677537798881531, 0.09514069557189941, 0.8201241493225098, 0.6003590226173401, 0.34790557622909546, 0.6916331648826599, 0.13445493578910828, 0.09603383392095566, 0.2183833122253418, 0.8688173890113831, 0.2770954966545105, 0.29056283831596375, 0.48777198791503906, 0.6394345164299011, 0.16867268085479736, 0.16801856458187103, 0.37362125515937805, 0.49325835704803467, 0.7062516808509827, 0.5450416803359985, 0.872252881526947, 0.04811717942357063, 0.8077472448348999, 0.5270453095436096, 0.5785672068595886, 0.31484946608543396, 0.06011920049786568, 0.7946820259094238, 0.7681082487106323, 0.5854048132896423, 0.7023257613182068, 0.07396937906742096, 0.32049256563186646, 0.5329755544662476, 0.1350337415933609, 0.341896653175354, 0.6244831085205078, 0.1056995615363121, 0.05128299072384834, 0.6489439606666565, 0.8833436369895935, 0.06266388297080994, 0.6422408819198608, 0.5717710256576538, 0.7413339614868164, 0.20014527440071106, 0.7578933835029602, 0.40550288558006287, 0.03538919985294342, 0.9284769892692566, 0.6607732176780701, 0.8208974599838257, 0.450675368309021, 0.14262966811656952, 0.4532223641872406, 0.8754578828811646, 0.20653071999549866, 0.9700903296470642, 0.01905982755124569, 0.3742181956768036, 0.11592420190572739, 0.42438939213752747, 0.292267382144928, 0.9955736994743347, 0.5782875418663025, 0.6286752820014954, 0.5036677122116089, 0.967823326587677, 0.4833261966705322, 0.766798734664917, 0.19579093158245087, 0.7847087979316711, 0.14064885675907135, 0.3163905441761017, 0.3534391522407532, 0.5600557327270508, 0.579900324344635, 0.23404008150100708, 0.005727048963308334, 0.5813160538673401, 0.01717018522322178, 0.5092810988426208, 0.9841327667236328, 0.6338550448417664, 0.19782783091068268, 0.16464705765247345, 0.5760481953620911, 0.520610511302948, 0.28165581822395325, 0.46545112133026123, 0.6136520504951477, 0.8143494725227356, 0.09393561631441116, 0.5538557171821594, 0.44886714220046997, 0.2512478232383728, 0.8680607676506042, 0.399354487657547, 0.5526840686798096, 0.5933082699775696, 0.13844867050647736, 0.1981501430273056, 0.8916971683502197, 0.5876959562301636, 0.5719329714775085, 0.3537253439426422, 0.04788757860660553, 0.02979571372270584, 0.09272931516170502, 0.27187415957450867, 0.852651834487915, 0.19329948723316193, 0.46743708848953247, 0.939703106880188, 0.47911715507507324, 0.9209043383598328, 0.5309937000274658, 0.7260075807571411, 0.9828304052352905, 0.7219918966293335, 0.659299373626709, 0.5417682528495789, 0.8763168454170227, 0.5106425285339355, 0.9952358603477478, 0.6798291206359863, 0.5453009605407715, 0.09697271138429642, 0.1733456254005432, 0.8664087653160095, 0.44362762570381165, 0.2626873254776001, 0.7167802453041077, 0.1244666650891304, 0.6653802990913391, 0.6156637072563171, 0.4706658720970154, 0.9674145579338074, 0.6807290315628052, 0.7481148838996887, 0.6719505786895752, 0.46235352754592896, 0.6014818549156189, 0.9597489833831787, 0.48914626240730286, 0.01173090748488903, 0.1175665482878685, 0.3604207932949066, 0.18631888926029205, 0.4665635824203491, 0.4978933334350586, 0.040717560797929764, 0.9495974183082581, 0.6180967688560486, 0.24315766990184784, 0.11525940895080566, 0.7962961792945862, 0.08771093934774399, 0.08928979933261871, 0.5935438275337219, 0.7828124761581421, 0.4482303261756897, 0.2758917510509491, 0.5934372544288635, 0.09283921867609024, 0.22732587158679962, 0.29399821162223816, 0.9434512257575989, 0.26096436381340027, 0.8421211242675781, 0.974748969078064, 0.9371832609176636, 0.12602777779102325, 0.9594656825065613, 0.07364021241664886, 0.5264202356338501, 0.7890608310699463, 0.18414585292339325, 0.49163490533828735, 0.8185514211654663, 0.10454992204904556, 0.6770040392875671, 0.22754012048244476, 0.7239787578582764, 0.5678955912590027, 0.3811268210411072, 0.3339203894138336, 0.8703245520591736, 0.03550371155142784, 0.36733147501945496, 0.058192674070596695, 0.7903568744659424, 0.12307365238666534, 0.10755634307861328, 0.5055915117263794, 0.508309543132782, 0.5379215478897095, 0.5199129581451416, 0.2715112566947937, 0.8450196981430054, 0.18779662251472473, 0.9275662302970886, 0.19050894677639008, 0.6769587397575378, 0.12378307431936264, 0.31935378909111023, 0.7833172678947449, 0.6862653493881226, 0.9170185923576355, 0.0231446772813797, 0.17521077394485474, 0.35699254274368286, 0.2215559035539627, 0.37011924386024475, 0.5294469594955444, 6.717982614645734e-05, 0.9129687547683716, 0.7356518507003784, 0.13426870107650757, 0.7087186574935913, 0.3463948369026184, 0.4057849645614624, 0.7860741019248962, 0.10635919868946075, 0.15712665021419525, 0.12894678115844727, 0.3107292056083679, 0.8087502717971802, 0.4636392295360565, 0.8801515698432922, 0.6633811593055725, 0.86961829662323, 0.2541981041431427, 0.7937475442886353, 0.5168886780738831, 0.31621718406677246, 0.054082371294498444, 0.08715332299470901, 0.09082730859518051, 0.6406719088554382, 0.025813834741711617, 0.5210179686546326, 0.7468615770339966, 0.735705554485321, 0.7209197282791138, 0.16627326607704163, 0.6818466186523438, 0.07570032775402069, 0.6452698707580566, 0.9032213687896729, 0.09087177366018295, 0.6876680254936218, 0.8248136043548584, 0.1988743245601654, 0.1987718641757965, 0.09440569579601288, 0.3404725193977356, 0.6257284879684448, 0.1982394903898239, 0.7607031464576721, 0.06344626843929291, 0.4921787679195404, 0.7729811668395996, 0.3456858992576599, 0.5470910668373108, 0.633741021156311, 0.016785666346549988, 0.6021753549575806, 0.2552485466003418, 0.6180494427680969, 0.5762574076652527, 0.20972971618175507, 0.9751070141792297, 0.6453699469566345, 0.7886140942573547, 0.46664610505104065, 0.39756059646606445, 0.23134426772594452, 0.3185988664627075, 0.9185174703598022, 0.03797558322548866, 0.5000339150428772, 0.3471233546733856, 0.7015897631645203, 0.716751217842102, 0.9473224878311157, 0.562950074672699, 0.22759200632572174, 0.5228664875030518, 0.6346879005432129, 0.01928076148033142, 0.4793979525566101, 0.366658091545105, 0.1526632010936737, 0.166905015707016, 0.3889158368110657, 0.5573446750640869, 0.28172141313552856, 0.2902773916721344, 0.05255081504583359, 0.9439998865127563, 0.9997389912605286, 0.7220163941383362, 0.8085923790931702, 0.7423213720321655, 0.15351726114749908, 0.587762713432312, 0.7473716139793396, 0.4295557141304016, 0.018429404124617577, 0.6862674951553345, 0.09170002490282059, 0.05863531678915024, 0.4788166582584381, 0.21656790375709534, 0.6931068897247314, 0.13190516829490662, 0.1157134547829628, 0.5468841791152954, 0.3306739926338196, 0.9127704501152039, 0.3808678388595581, 0.8459193706512451, 0.32666724920272827, 0.9610130786895752, 0.4825980067253113, 0.45404165983200073, 0.5204469561576843, 0.19685064256191254, 0.6858335733413696, 0.8462364077568054, 0.3045005202293396, 0.39347872138023376, 0.044037505984306335, 0.2996792793273926, 0.7998414635658264, 0.06761251389980316, 0.9685580134391785, 0.5936104655265808, 0.4198245108127594, 0.41583484411239624, 0.5145580768585205, 0.6971230506896973, 0.21945533156394958, 0.39292266964912415, 0.8407564163208008, 0.15536290407180786, 0.9024173617362976, 0.00247236923314631, 0.29345983266830444, 0.5096447467803955, 0.0034719877876341343, 0.7949544191360474, 0.931050181388855, 0.9282593727111816, 0.25616368651390076, 0.7313158512115479, 0.9769437909126282, 0.35913974046707153, 0.5074560046195984, 0.22851108014583588, 0.9156183004379272, 0.9055492281913757, 0.6943511962890625, 0.46594855189323425, 0.09837134927511215, 0.06936425715684891, 0.009466690011322498, 0.6253657937049866, 0.8391492366790771, 0.9122130274772644, 0.3704187273979187, 0.8572385907173157, 0.5044439435005188, 0.7268729209899902, 0.8660553693771362, 0.13155615329742432, 0.8488684296607971, 0.8632239699363708, 0.4802361726760864, 0.6805127263069153, 0.386896550655365, 0.585968017578125, 0.37017130851745605, 0.08078940957784653, 0.14147186279296875, 0.60914546251297, 0.36866000294685364, 0.13373130559921265, 0.059651073068380356, 0.1937275230884552, 0.6160009503364563, 0.042797837406396866, 0.9807227253913879, 0.184631809592247, 0.48665565252304077, 0.27797529101371765, 0.3090546131134033, 0.5570073127746582, 0.08491866290569305, 0.8760199546813965, 0.23532593250274658, 0.5632840991020203, 0.08473226428031921, 0.8284323811531067, 0.8508289456367493, 0.6349027156829834, 0.7027525305747986, 0.2421765774488449, 0.3333284854888916, 0.5980463624000549, 0.4671682119369507, 0.666409432888031, 0.0005141752189956605, 0.033727847039699554, 0.2065356969833374, 0.630534827709198, 0.008353018201887608, 0.9305593371391296, 0.6358621716499329, 0.9827827215194702, 0.3788571059703827, 0.0977051705121994, 0.24773113429546356, 0.09445073455572128, 0.2571496367454529, 0.4321674406528473, 0.34575697779655457, 0.5095869898796082, 0.7434729933738708, 0.8296504020690918, 0.4839027523994446, 0.7105902433395386, 0.4466587007045746, 0.6153427362442017, 0.002875693142414093, 0.46688929200172424, 0.6457183361053467, 0.5869255065917969, 0.4247977137565613, 0.8592257499694824, 0.17829230427742004, 0.7157182097434998, 0.06392519921064377, 0.7079163789749146, 0.11764603108167648, 0.7123359441757202, 0.627219557762146, 0.33176979422569275, 0.45311209559440613, 0.8139302134513855, 0.8223478198051453, 0.43897387385368347, 0.8864006996154785, 0.960909366607666, 0.052766717970371246, 0.5082341432571411, 0.36199989914894104, 0.6047079563140869, 0.9416998624801636, 0.30298563838005066, 0.11604651808738708, 0.5360314249992371, 0.7739596962928772, 0.49034741520881653, 0.1231665089726448, 0.2907046973705292, 0.5804620385169983, 0.2557554244995117, 0.9237532615661621, 0.6670106649398804, 0.3446386754512787, 0.7404107451438904, 0.9482900500297546, 0.31070035696029663, 0.5474882125854492, 0.6283774375915527, 0.4318910539150238, 0.0639648288488388, 0.7692599296569824, 0.5423433780670166, 0.2561149597167969, 0.5230444073677063, 0.14105580747127533, 0.14943192899227142, 0.11810968816280365, 0.4393440783023834, 0.5630103945732117, 0.7929814457893372, 0.6630560755729675, 0.8917015194892883, 0.4747299551963806, 0.036505404859781265, 0.21109193563461304, 0.5875652432441711, 0.45002779364585876, 0.43828272819519043, 0.21201376616954803, 0.38454151153564453, 0.44878706336021423, 0.5782598853111267, 0.2619844973087311, 0.009038439020514488, 0.5415060520172119, 0.45001932978630066, 0.01530265249311924, 0.5731189846992493, 0.024035373702645302, 0.6066468358039856, 0.3898581564426422, 0.2473974972963333, 0.5242909789085388, 0.11061633378267288, 0.19682657718658447, 0.8347025513648987, 0.01720421388745308, 0.03111749142408371, 0.6841902732849121, 0.3329467475414276, 0.19958436489105225, 0.6310383081436157, 0.5089201331138611, 0.5387365818023682, 0.7201129794120789, 0.3405286967754364, 0.04960660636425018, 0.5655655264854431, 0.36494195461273193, 0.7684902548789978, 0.42518776655197144, 0.8779001832008362, 0.03508290648460388, 0.30599987506866455, 0.6106510758399963, 0.6684430837631226, 0.8076345920562744, 0.26441749930381775, 0.9292536973953247, 0.8187693357467651, 0.3178878724575043, 0.18841876089572906, 0.23955197632312775, 0.2733471691608429, 0.8531033396720886, 0.39104071259498596, 0.5649981498718262, 0.06740880012512207, 0.2897658348083496, 0.7194886803627014, 0.19315999746322632, 0.9832680821418762, 0.26382723450660706, 0.4986177980899811, 0.7895559668540955, 0.7448020577430725, 0.9712573289871216, 0.5988581776618958, 0.07977522909641266, 0.007080813404172659, 0.8211133480072021, 0.5567675828933716, 0.9537816047668457, 0.9336162209510803, 0.8342453837394714, 0.46236658096313477, 0.46453168988227844, 0.17018693685531616, 0.8445934057235718, 0.49934864044189453, 0.654381513595581, 0.5808459520339966, 0.7013759613037109, 0.7584179043769836, 0.08299725502729416, 0.24084189534187317, 0.5675965547561646, 0.06994365900754929, 0.020431555807590485, 0.6405585408210754, 0.06533528119325638, 0.13273325562477112, 0.3106120526790619, 0.30822446942329407, 0.7650657296180725, 0.6063564419746399, 0.838714063167572, 0.6945788860321045, 0.12809361517429352, 0.347777783870697, 0.27233177423477173, 0.8397007584571838, 0.8174160122871399, 0.646308183670044, 0.9672423005104065, 0.23640835285186768, 0.968144953250885, 0.1399688720703125, 0.045676879584789276, 0.2696036100387573, 0.05715697631239891, 0.9280192852020264, 0.9468095898628235, 0.2615559995174408, 0.6287650465965271, 0.47174689173698425, 0.6059722304344177, 0.7091386318206787, 0.4409760534763336, 0.08488119393587112, 0.8894966244697571, 0.5357226729393005, 0.45271894335746765, 0.4052424728870392, 0.7691981792449951, 0.9568786025047302, 0.10862185060977936, 0.7089368104934692, 0.8359880447387695, 0.5120929479598999, 0.42965301871299744, 0.6743569374084473, 0.6707550883293152, 0.8416394591331482, 0.8370009660720825, 0.009814570657908916, 0.9164296388626099, 0.4565296769142151, 0.48369884490966797, 0.5746312737464905, 0.5153519511222839, 0.3172641396522522, 0.8007677793502808, 0.12933330237865448, 0.29192593693733215, 0.610188901424408, 0.519863486289978, 0.11111748218536377, 0.255191445350647, 0.5477582812309265, 0.606847882270813, 0.6999751925468445, 0.9626180529594421, 0.4698432981967926, 0.7564738392829895, 0.1280393898487091, 0.3040427565574646, 0.45134568214416504, 0.0934700071811676, 0.139090433716774, 0.05378109589219093, 0.9277908205986023, 0.6391209363937378, 0.027721915394067764, 0.08225604891777039, 0.026309454813599586, 0.3507021367549896, 0.6619359254837036, 0.2175619900226593, 0.4157404601573944, 0.18545623123645782, 0.09934478998184204, 0.2810831069946289, 0.7510949373245239, 0.4693436026573181, 0.17964975535869598, 0.20145252346992493, 0.7700541019439697, 0.6085237264633179, 0.9989972710609436, 0.8452189564704895, 0.6333275437355042, 0.46379053592681885, 0.3697148859500885, 0.6963803768157959, 0.6128230690956116, 0.9614061713218689, 0.907155454158783, 0.7865278720855713, 0.09122147411108017, 0.21625956892967224, 0.5652353167533875, 0.3149380385875702, 0.3779014050960541, 0.934637188911438, 0.3907920718193054, 0.6841690540313721, 0.7081262469291687, 0.1339622586965561, 0.4651813507080078, 0.824341893196106, 0.807670533657074, 0.7774966359138489, 0.1051517203450203, 0.10685788840055466, 0.9956139326095581, 0.7164419889450073, 0.2343447059392929, 0.3706846833229065, 0.7692639231681824, 0.6972052454948425, 0.6042316555976868, 0.8667473196983337, 0.8110538125038147, 0.50572669506073, 0.49257585406303406, 0.24587547779083252, 0.11286971718072891, 0.8328279852867126, 0.20043061673641205, 0.1039147600531578, 0.7267220616340637, 0.7081754207611084, 0.8249654769897461, 0.4123005270957947, 0.7710753679275513, 0.5381021499633789, 0.5463727712631226, 0.8270867466926575, 0.01593414694070816, 0.19534611701965332, 0.401783287525177, 0.7744907736778259, 0.48401397466659546, 0.8049760460853577, 0.909207820892334, 0.8808935284614563, 0.5254150032997131, 0.7754223346710205, 0.7936505079269409, 0.8643978834152222, 0.4903126060962677, 0.5160192251205444, 0.7755321264266968, 0.38127943873405457, 0.4602121412754059, 0.7903076410293579, 0.5362173914909363, 0.7737277150154114, 0.7356213927268982, 0.9877470135688782, 0.7999483346939087, 0.8856385350227356, 0.8227282166481018, 0.47895029187202454, 0.11099491268396378, 0.3312976658344269, 0.699544370174408, 0.6535815000534058, 0.6789493560791016, 0.7733816504478455, 0.35773003101348877, 0.061042334884405136, 0.9580310583114624, 0.5968562960624695, 0.7581431865692139, 0.020538950338959694, 0.3414766490459442, 0.5249534249305725, 0.8918085694313049, 0.9821330904960632, 0.6482757925987244, 0.30821436643600464, 0.11024878174066544, 0.5639818906784058, 0.35285237431526184, 0.4563414454460144, 0.942164421081543, 0.9474254846572876, 0.028075125068426132, 0.2743256688117981, 0.08473861962556839, 0.6840551495552063, 0.5567184686660767, 0.810767650604248, 0.6355850100517273, 0.7172819375991821, 0.5425448417663574, 0.19951596856117249, 0.5432964563369751, 0.17484483122825623, 0.4648190438747406, 0.7156330943107605, 0.835309624671936, 0.11984552443027496, 0.10014937072992325, 0.34979158639907837, 0.5436074733734131, 0.5514843463897705, 0.11967451125383377, 0.3954598009586334, 0.21164147555828094, 0.9456548690795898, 0.546157717704773, 0.37832701206207275, 0.6458828449249268, 0.9365729689598083, 0.277798593044281, 0.39090943336486816, 0.5618823766708374, 0.8573434948921204, 0.9585562348365784, 0.9310038685798645, 0.8510586619377136, 0.7534677386283875, 0.7573729157447815, 0.5645626187324524, 0.47448647022247314, 0.5411547422409058, 0.02151353284716606, 0.9607899785041809, 0.40741363167762756, 0.2519567310810089, 0.09171804785728455, 0.5359310507774353, 0.475903183221817, 0.0474948026239872, 0.7082989811897278, 0.9888678193092346, 0.12648242712020874, 0.32068783044815063, 0.7392951250076294, 0.30736541748046875, 0.3329375088214874, 0.9997708797454834, 0.20799744129180908, 0.28629162907600403, 0.0791289210319519, 0.08272352069616318, 0.36255156993865967, 0.9535930156707764, 0.8446369171142578, 0.959002673625946, 0.9685333371162415, 0.1986090987920761, 0.10240170359611511, 0.1988026648759842, 0.9589047431945801, 0.6871894001960754, 0.7604759931564331, 0.7184842824935913, 0.39039474725723267, 0.4590420722961426, 0.150106281042099, 0.7402786016464233, 0.8850541114807129, 0.7388550639152527, 0.5613917112350464], 10, map[nprobe, 5])</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4952,8 +5029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L255"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C242" sqref="C242"/>
+    <sheetView tabSelected="1" topLeftCell="A221" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E258" sqref="E258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -13229,7 +13306,7 @@
         <v>969</v>
       </c>
       <c r="J243" s="1" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="K243" s="1" t="s">
         <v>1266</v>
@@ -13264,7 +13341,7 @@
         <v>969</v>
       </c>
       <c r="J244" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="K244" s="1" t="s">
         <v>1271</v>
@@ -13334,7 +13411,7 @@
         <v>969</v>
       </c>
       <c r="J246" s="1" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="K246" s="1" t="s">
         <v>1277</v>
@@ -13351,7 +13428,7 @@
         <v>8</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="D247" s="3" t="s">
         <v>13</v>
@@ -13369,7 +13446,7 @@
         <v>969</v>
       </c>
       <c r="J247" s="1" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="K247" s="1" t="s">
         <v>1278</v>
@@ -13382,11 +13459,11 @@
       <c r="A248" s="3" t="s">
         <v>1197</v>
       </c>
-      <c r="B248" s="1" t="s">
-        <v>1279</v>
+      <c r="B248" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>1298</v>
+        <v>1293</v>
       </c>
       <c r="D248" s="3" t="s">
         <v>13</v>
@@ -13395,24 +13472,33 @@
         <v>1213</v>
       </c>
       <c r="F248" s="1" t="s">
+        <v>1283</v>
+      </c>
+      <c r="G248" s="3" t="s">
         <v>1284</v>
       </c>
-      <c r="G248" s="3" t="s">
-        <v>1285</v>
-      </c>
       <c r="I248" s="1" t="s">
         <v>969</v>
+      </c>
+      <c r="J248" s="1" t="s">
+        <v>1294</v>
+      </c>
+      <c r="K248" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="L248" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A249" s="3" t="s">
         <v>1198</v>
       </c>
-      <c r="B249" s="1" t="s">
-        <v>1279</v>
+      <c r="B249" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>1299</v>
+        <v>1296</v>
       </c>
       <c r="D249" s="3" t="s">
         <v>13</v>
@@ -13421,18 +13507,30 @@
         <v>1213</v>
       </c>
       <c r="F249" s="1" t="s">
-        <v>1286</v>
+        <v>1285</v>
+      </c>
+      <c r="G249" s="3" t="s">
+        <v>1297</v>
       </c>
       <c r="I249" s="1" t="s">
         <v>969</v>
+      </c>
+      <c r="J249" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="K249" s="1" t="s">
+        <v>1298</v>
+      </c>
+      <c r="L249" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A250" s="3" t="s">
         <v>1199</v>
       </c>
-      <c r="B250" s="1" t="s">
-        <v>1279</v>
+      <c r="B250" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>1300</v>
@@ -13444,21 +13542,33 @@
         <v>1213</v>
       </c>
       <c r="F250" s="1" t="s">
-        <v>1287</v>
+        <v>1286</v>
+      </c>
+      <c r="G250" s="3" t="s">
+        <v>1301</v>
       </c>
       <c r="I250" s="1" t="s">
         <v>969</v>
+      </c>
+      <c r="J250" s="1" t="s">
+        <v>1307</v>
+      </c>
+      <c r="K250" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="L250" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A251" s="3" t="s">
         <v>1200</v>
       </c>
-      <c r="B251" s="1" t="s">
-        <v>1279</v>
+      <c r="B251" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="D251" s="3" t="s">
         <v>13</v>
@@ -13467,21 +13577,33 @@
         <v>1213</v>
       </c>
       <c r="F251" s="1" t="s">
-        <v>1288</v>
+        <v>1287</v>
+      </c>
+      <c r="G251" s="3" t="s">
+        <v>1308</v>
       </c>
       <c r="I251" s="1" t="s">
         <v>969</v>
+      </c>
+      <c r="J251" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="K251" s="1" t="s">
+        <v>1309</v>
+      </c>
+      <c r="L251" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A252" s="3" t="s">
         <v>1201</v>
       </c>
-      <c r="B252" s="1" t="s">
-        <v>1279</v>
+      <c r="B252" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>1294</v>
+        <v>1303</v>
       </c>
       <c r="D252" s="3" t="s">
         <v>13</v>
@@ -13490,21 +13612,33 @@
         <v>1213</v>
       </c>
       <c r="F252" s="1" t="s">
-        <v>1289</v>
+        <v>1288</v>
+      </c>
+      <c r="G252" s="3" t="s">
+        <v>1311</v>
       </c>
       <c r="I252" s="1" t="s">
         <v>969</v>
+      </c>
+      <c r="J252" s="1" t="s">
+        <v>1313</v>
+      </c>
+      <c r="K252" s="1" t="s">
+        <v>1312</v>
+      </c>
+      <c r="L252" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A253" s="3" t="s">
         <v>1202</v>
       </c>
-      <c r="B253" s="1" t="s">
-        <v>1279</v>
+      <c r="B253" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>1295</v>
+        <v>1304</v>
       </c>
       <c r="D253" s="3" t="s">
         <v>13</v>
@@ -13513,21 +13647,33 @@
         <v>1213</v>
       </c>
       <c r="F253" s="1" t="s">
-        <v>1290</v>
+        <v>1289</v>
+      </c>
+      <c r="G253" s="3" t="s">
+        <v>1317</v>
       </c>
       <c r="I253" s="1" t="s">
         <v>969</v>
+      </c>
+      <c r="J253" s="1" t="s">
+        <v>1318</v>
+      </c>
+      <c r="K253" s="1" t="s">
+        <v>1314</v>
+      </c>
+      <c r="L253" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A254" s="3" t="s">
         <v>1211</v>
       </c>
-      <c r="B254" s="1" t="s">
-        <v>1279</v>
+      <c r="B254" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>1296</v>
+        <v>1305</v>
       </c>
       <c r="D254" s="3" t="s">
         <v>13</v>
@@ -13536,21 +13682,33 @@
         <v>1213</v>
       </c>
       <c r="F254" s="1" t="s">
-        <v>1291</v>
+        <v>1290</v>
+      </c>
+      <c r="G254" s="3" t="s">
+        <v>1319</v>
       </c>
       <c r="I254" s="1" t="s">
         <v>969</v>
+      </c>
+      <c r="J254" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="K254" s="1" t="s">
+        <v>1315</v>
+      </c>
+      <c r="L254" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A255" s="3" t="s">
         <v>1212</v>
       </c>
-      <c r="B255" s="1" t="s">
-        <v>1279</v>
+      <c r="B255" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>1297</v>
+        <v>1321</v>
       </c>
       <c r="D255" s="3" t="s">
         <v>13</v>
@@ -13559,10 +13717,19 @@
         <v>1213</v>
       </c>
       <c r="F255" s="1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="I255" s="1" t="s">
         <v>969</v>
+      </c>
+      <c r="J255" s="1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="K255" s="1" t="s">
+        <v>1316</v>
+      </c>
+      <c r="L255" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
string function case update
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2724" uniqueCount="1323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2725" uniqueCount="1324">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4653,6 +4653,10 @@
   </si>
   <si>
     <t>select id,feature_id,feature_index$distance from vector($vector115, feature, array[0.9902235269546509, 0.10431499034166336, 0.4925372302532196, 0.8681201934814453, 0.8722683191299438, 0.830732524394989, 0.1524062156677246, 0.9349273443222046, 0.9830064177513123, 0.20973382890224457, 0.9838352203369141, 0.5014108419418335, 0.2647353410720825, 0.6980723738670349, 0.8327855467796326, 0.5319531559944153, 0.15155324339866638, 0.017415184527635574, 0.4389483630657196, 0.257061243057251, 0.15360957384109497, 0.3058664798736572, 0.9838027954101562, 0.360340416431427, 0.746213972568512, 0.07666397839784622, 0.4372844099998474, 0.014756870456039906, 0.5788666605949402, 0.5449406504631042, 0.9139546155929565, 0.8067901730537415, 0.6736865043640137, 0.07143417000770569, 0.8128687739372253, 0.08907461166381836, 0.28962501883506775, 0.012927844189107418, 0.9696642160415649, 0.6620621085166931, 0.3114590048789978, 0.03006383776664734, 0.5796226859092712, 0.2140612006187439, 0.6916781067848206, 0.967767059803009, 0.5517066121101379, 0.16160210967063904, 0.49476298689842224, 0.446463942527771, 0.6734089255332947, 0.19210585951805115, 0.5712792277336121, 0.2841925621032715, 0.5058475136756897, 0.14268431067466736, 0.12685224413871765, 0.7860594391822815, 0.3492421507835388, 0.893543541431427, 0.7209875583648682, 0.6450263857841492, 0.5675541758537292, 0.23288927972316742, 0.7606458067893982, 0.07128461450338364, 0.6964651346206665, 0.24048973619937897, 0.6247967481613159, 0.8964740037918091, 0.45580175518989563, 0.7296887040138245, 0.22816988825798035, 0.029268542304635048, 0.8915632367134094, 0.40926042199134827, 0.2030932605266571, 0.6919152736663818, 0.8419082760810852, 0.2563587427139282, 0.12631629407405853, 0.7140357494354248, 0.15265466272830963, 0.7328639030456543, 0.4638957381248474, 0.7255092263221741, 0.21460771560668945, 0.21966920793056488, 0.9287545680999756, 0.03616950288414955, 0.18558597564697266, 0.4677453935146332, 0.9435461759567261, 0.4441729784011841, 0.2739681303501129, 0.6308834552764893, 0.8681932687759399, 0.11704379320144653, 0.589827835559845, 0.6223616600036621, 0.22368013858795166, 0.9446212649345398, 0.6212049722671509, 0.31601354479789734, 0.4408273994922638, 0.3333006501197815, 0.03972972184419632, 0.056194256991147995, 0.8861505389213562, 0.9818869829177856, 0.6056957244873047, 0.9775523543357849, 0.6636890172958374, 0.40653443336486816, 0.8600038886070251, 0.8776096105575562, 0.9745752215385437, 0.972199022769928, 0.8638783693313599, 0.6721484065055847, 0.5186344981193542, 0.791917085647583, 0.9451949596405029, 0.888151228427887, 0.97093665599823, 0.5097098350524902, 0.2753954529762268, 0.49438029527664185, 0.7956991195678711, 0.9898937344551086, 0.4951379597187042, 0.3869473934173584, 0.19586464762687683, 0.8953040242195129, 0.0009835307719185948, 0.9355499148368835, 0.9517822265625, 0.7543898820877075, 0.7343156337738037, 0.4359067678451538, 0.7509841322898865, 0.30458179116249084, 0.1464567333459854, 0.6193007230758667, 0.8668887615203857, 0.5020105838775635, 0.6219688653945923, 0.09826795756816864, 0.788691520690918, 0.2709279954433441, 0.9040477275848389, 0.1951267421245575, 0.018649810925126076, 0.1581597775220871, 0.32359930872917175, 0.6054627895355225, 0.682092547416687, 0.2932957410812378, 0.39800047874450684, 0.15062150359153748, 0.3486483693122864, 0.17219838500022888, 0.9427631497383118, 0.24497780203819275, 0.369671106338501, 0.8383969664573669, 0.9376201033592224, 0.3204548954963684, 0.8091537952423096, 0.18348929286003113, 0.7939112186431885, 0.8889263868331909, 0.6047505140304565, 0.6250599026679993, 0.29245203733444214, 0.899971067905426, 0.22505472600460052, 0.9743149280548096, 0.6746429204940796, 0.37511003017425537, 0.8312550783157349, 0.455399751663208, 0.5906211137771606, 0.12419106066226959, 0.3229463994503021, 0.30098292231559753, 0.15001018345355988, 0.7588010430335999, 0.7687546014785767, 0.6517909169197083, 0.0766993910074234, 0.8894836902618408, 0.7034062147140503, 0.7792702913284302, 0.7765412330627441, 0.31707504391670227, 0.6997724771499634, 0.6622527837753296, 0.47220128774642944, 0.32911673188209534, 0.9556384682655334, 0.3046383559703827, 0.14930294454097748, 0.7901278138160706, 0.5603054165840149, 0.49803611636161804, 0.45862188935279846, 0.7027131915092468, 0.3309139311313629, 0.3433569669723511, 0.24075841903686523, 0.47841811180114746, 0.09821527451276779, 0.8468405604362488, 0.7989208102226257, 0.6315018534660339, 0.7078220844268799, 0.032576873898506165, 0.11913882941007614, 0.808164119720459, 0.35538816452026367, 0.393353670835495, 0.2193855345249176, 0.89907306432724, 0.11825469881296158, 0.9549816846847534, 0.0005904135177843273, 0.638552188873291, 0.20891346037387848, 0.0793919786810875, 0.8178072571754456, 0.5769234299659729, 0.8885272145271301, 0.45078858733177185, 0.09329517930746078, 0.7293152213096619, 0.0677352249622345, 0.0134489880874753, 0.020049866288900375, 0.4047183394432068, 0.6793797016143799, 0.6672581434249878, 0.600193440914154, 0.3501960337162018, 0.9053044319152832, 0.43740057945251465, 0.6974921822547913, 0.22054646909236908, 0.2693362236022949, 0.890095591545105, 0.15740422904491425, 0.7033600807189941, 0.13587848842144012, 0.8914653062820435, 0.30210092663764954, 0.9178286194801331, 0.18185602128505707, 0.15479016304016113, 0.8494400978088379, 0.7593747973442078, 0.7473207116127014, 0.48755943775177, 0.4769561290740967, 0.4950885474681854, 0.4827111065387726, 0.9361315965652466, 0.4797084629535675, 0.5216492414474487, 0.47123172879219055, 0.6359973549842834, 0.5099602341651917, 0.03890925273299217, 0.26113447546958923, 0.9460735321044922, 0.3888813555240631, 0.5715094804763794, 0.5333307385444641, 0.9247259497642517, 0.6850947737693787, 0.8652344346046448, 0.0874122902750969, 0.04754435643553734, 0.31448766589164734, 0.5250023603439331, 0.2405785173177719, 0.6725209355354309, 0.5341150760650635, 0.38017794489860535, 0.7739356756210327, 0.4966346025466919, 0.995715856552124, 0.6718922257423401, 0.5896984338760376, 0.2216217964887619, 0.15965242683887482, 0.6196257472038269, 0.531399130821228, 0.26334846019744873, 0.4372881054878235, 0.5249695777893066, 0.7433487176895142, 0.9068548083305359, 0.2210480123758316, 0.2822028696537018, 0.4108716547489166, 0.7857139110565186, 0.27395138144493103, 0.20482881367206573, 0.9258070588111877, 0.6310699582099915, 0.5921266078948975, 0.5859371423721313, 0.0067001995630562305, 0.49284690618515015, 0.9688669443130493, 0.5649298429489136, 0.09057779610157013, 0.19492579996585846, 0.9782233834266663, 0.6728528141975403, 0.26003211736679077, 0.1505855768918991, 0.1489274948835373, 0.05706246197223663, 0.9388375282287598, 0.18222551047801971, 0.1313900351524353, 0.9627377986907959, 0.3706483244895935, 0.5246455073356628, 0.7725783586502075, 0.7702359557151794, 0.5866581201553345, 0.17769668996334076, 0.9544842839241028, 0.5680734515190125, 0.8845875263214111, 0.5783229470252991, 0.2774977385997772, 0.8771805763244629, 0.45748788118362427, 0.11635572463274002, 0.528388500213623, 0.4006480872631073, 0.606464147567749, 0.755187451839447, 0.34578827023506165, 0.5682968497276306, 0.7122334837913513, 0.5424001216888428, 0.917868971824646, 0.8127769231796265, 0.02478407695889473, 0.5514575839042664, 0.0049731191247701645, 0.9176387786865234, 0.002859156345948577, 0.5905631184577942, 0.16881851851940155, 0.016540611162781715, 0.5920075178146362, 0.2915170192718506, 0.2122717797756195, 0.49616947770118713, 0.2694140672683716, 0.7864028215408325, 0.2011972814798355, 0.22466951608657837, 0.0072517795488238335, 0.7205490469932556, 0.7928007245063782, 0.4883838891983032, 0.06322711706161499, 0.7535420060157776, 0.5698924660682678, 0.17615631222724915, 0.9928708076477051, 0.17343948781490326, 0.1237945482134819, 0.8786767721176147, 0.8966941833496094, 0.3080652356147766, 0.04352223500609398, 0.546010434627533, 0.8659591674804688, 0.1526016891002655, 0.09960544109344482, 0.02918417938053608, 0.07468264549970627, 0.3006387948989868, 0.7012244462966919, 0.8984241485595703, 0.650434672832489, 0.8699777722358704, 0.7138668894767761, 0.5873762369155884, 0.618304967880249, 0.11495287716388702, 0.30427223443984985, 0.3498757779598236, 0.3505840301513672, 0.10299947112798691, 0.72786545753479, 0.27773043513298035, 0.5042670369148254, 0.3558466136455536, 0.8995752334594727, 0.02561158873140812, 0.0841745063662529, 0.46816393733024597, 0.7122877836227417, 0.9924346804618835, 0.7917988896369934, 0.1384432315826416, 0.8408766984939575, 0.33010903000831604, 0.505934476852417, 0.878890335559845, 0.32835277915000916, 0.7709540724754333, 0.9224629998207092, 0.04817458614706993, 0.6690673828125, 0.48130860924720764, 0.8828980922698975, 0.7406775951385498, 0.0045904736034572124, 0.46130016446113586, 0.49253806471824646, 0.5105828046798706, 0.3459140658378601, 0.5170886516571045, 0.9654001593589783, 0.9951261281967163, 0.7578433156013489, 0.9665701389312744, 0.26521801948547363, 0.7781181335449219, 0.5220229625701904, 0.8422088623046875, 0.891946017742157, 0.25643181800842285, 0.12808963656425476, 0.14494113624095917, 0.4559922218322754, 0.9382727146148682, 0.7970611453056335, 0.5102805495262146, 0.2452685385942459, 0.9435397982597351, 0.1397826075553894, 0.8129761219024658, 0.4322268068790436, 0.11890196055173874, 0.2577558755874634, 0.6904773712158203, 0.16196441650390625, 0.8507242202758789, 0.022312331944704056, 0.4390030801296234, 0.6317897439002991, 0.267055869102478, 0.9840227961540222, 0.2265866994857788, 0.4850917160511017, 0.8768416047096252, 0.9088805913925171, 0.20929481089115143, 0.1866832822561264, 0.13339482247829437, 0.8052598237991333, 0.4309256374835968, 0.3309306800365448, 0.6407923698425293, 0.28302469849586487, 0.8368085622787476, 0.0835670605301857, 0.13155408203601837, 0.9648972749710083, 0.4055004119873047, 0.5493667721748352, 0.46748796105384827, 0.24159188568592072, 0.6395735740661621, 0.5471751689910889, 0.7100662589073181, 0.400621622800827, 0.9984897971153259, 0.9803318381309509, 0.39545440673828125, 0.1151449903845787, 0.9904844760894775, 0.2478373646736145, 0.2618675231933594, 0.1895902007818222, 0.3733517825603485, 0.1559653878211975, 0.4321887493133545, 0.7668293714523315, 0.582956075668335, 0.030917683616280556, 0.5985668897628784, 0.35136914253234863, 0.5254815220832825, 0.16164334118366241, 0.5031083822250366, 0.8812853097915649, 0.45757395029067993, 0.9772512912750244, 0.9559372663497925, 0.8792067766189575, 0.8774374723434448, 0.1446678340435028, 0.10850758850574493, 0.3240841329097748, 0.13229094445705414, 0.9260293245315552, 0.03915002942085266, 0.5516790747642517, 0.9809667468070984, 0.05196494981646538, 0.11876443028450012, 0.7931789755821228, 0.23084916174411774, 0.7028468251228333, 0.25613224506378174, 0.5647616982460022, 0.22060178220272064, 0.9715662002563477, 0.09961102157831192, 0.49895238876342773, 0.40517812967300415, 0.9969459772109985, 0.7935271263122559, 0.4981478452682495, 0.29133665561676025, 0.44439953565597534, 0.425699383020401, 0.4763699173927307, 0.9215809106826782, 0.24236030876636505, 0.7956124544143677, 0.014775332994759083, 0.32487258315086365, 0.7371284365653992, 0.5908387899398804, 0.30247777700424194, 0.43907877802848816, 0.9903702139854431, 0.1989789456129074, 0.5918221473693848, 0.7085360884666443, 0.5898317694664001, 0.4510810673236847, 0.6613816618919373, 0.2952318489551544, 0.02493247762322426, 0.12391345947980881, 0.6733596324920654, 0.05711675062775612, 0.47925394773483276, 0.8671201467514038, 0.8791252970695496, 0.860435962677002, 0.7794710993766785, 0.23672603070735931, 0.9939964413642883, 0.2947549819946289, 0.03671910986304283, 0.937823474407196, 0.8802260160446167, 0.31307414174079895, 0.3523872196674347, 0.04728609696030617, 0.9888927340507507, 0.7850785255432129, 0.4869828224182129, 0.31264635920524597, 0.06642528623342514, 0.9304323792457581, 0.21197645366191864, 0.7239446640014648, 0.872456431388855, 0.8789159059524536, 0.6340766549110413, 0.449869841337204, 0.44816216826438904, 0.534173309803009, 0.9126707911491394, 0.4711556136608124, 0.5168650150299072, 0.6492165923118591, 0.8386184573173523, 0.6387537717819214, 0.8471029996871948, 0.31365832686424255, 0.16466949880123138, 0.3805263042449951, 0.777142345905304, 0.8887110948562622, 0.5459561944007874, 0.9729193449020386, 0.8573066592216492, 0.3737916648387909, 0.517247200012207, 0.6410920023918152, 0.20879340171813965, 0.9273661375045776, 0.48032259941101074, 0.18216298520565033, 0.43896523118019104, 0.8830050230026245, 0.30291175842285156, 0.7757983803749084, 0.8128688931465149, 0.024925503879785538, 0.5879754424095154, 0.7618100643157959, 0.5647273063659668, 0.05252961069345474, 0.2591903805732727, 0.14655964076519012, 0.42745181918144226, 0.15190084278583527, 0.4318661093711853, 0.8434489965438843, 0.03704701364040375, 0.5753170847892761, 0.8302214741706848, 0.9486076831817627, 0.5900678038597107, 0.9620041847229004, 0.34370487928390503, 0.0218867938965559, 0.7149175405502319, 0.7317449450492859, 0.2506178319454193, 0.23113417625427246, 0.45467403531074524, 0.9072763919830322, 0.23693597316741943, 0.7983786463737488, 0.4105972647666931, 0.0062048714607954025, 0.37672513723373413, 0.7877068519592285, 0.6916950345039368, 0.616522490978241, 0.8136075735092163, 0.19002509117126465, 0.27153536677360535, 0.6925373673439026, 0.06465853005647659, 0.07165776938199997, 0.5824829936027527, 0.3678259551525116, 0.45163843035697937, 0.36982086300849915, 0.7873246669769287, 0.21836048364639282, 0.4204391539096832, 0.8240039348602295, 0.07276085764169693, 0.38298696279525757, 0.7950550317764282, 0.2184973657131195, 0.8491131663322449, 0.567008912563324, 0.6902289986610413, 0.6796565651893616, 0.10449163615703583, 0.40591517090797424, 0.5448713302612305, 0.37248215079307556, 0.955883264541626, 0.9698770642280579, 0.7933648824691772, 0.5064224004745483, 0.5269209146499634, 0.6102035641670227, 0.36456477642059326, 0.5992593169212341, 0.7629435658454895, 0.3763626217842102, 0.1819257140159607, 0.016094574704766273, 0.21366019546985626, 0.4362291097640991, 0.6657033562660217, 0.7677537798881531, 0.09514069557189941, 0.8201241493225098, 0.6003590226173401, 0.34790557622909546, 0.6916331648826599, 0.13445493578910828, 0.09603383392095566, 0.2183833122253418, 0.8688173890113831, 0.2770954966545105, 0.29056283831596375, 0.48777198791503906, 0.6394345164299011, 0.16867268085479736, 0.16801856458187103, 0.37362125515937805, 0.49325835704803467, 0.7062516808509827, 0.5450416803359985, 0.872252881526947, 0.04811717942357063, 0.8077472448348999, 0.5270453095436096, 0.5785672068595886, 0.31484946608543396, 0.06011920049786568, 0.7946820259094238, 0.7681082487106323, 0.5854048132896423, 0.7023257613182068, 0.07396937906742096, 0.32049256563186646, 0.5329755544662476, 0.1350337415933609, 0.341896653175354, 0.6244831085205078, 0.1056995615363121, 0.05128299072384834, 0.6489439606666565, 0.8833436369895935, 0.06266388297080994, 0.6422408819198608, 0.5717710256576538, 0.7413339614868164, 0.20014527440071106, 0.7578933835029602, 0.40550288558006287, 0.03538919985294342, 0.9284769892692566, 0.6607732176780701, 0.8208974599838257, 0.450675368309021, 0.14262966811656952, 0.4532223641872406, 0.8754578828811646, 0.20653071999549866, 0.9700903296470642, 0.01905982755124569, 0.3742181956768036, 0.11592420190572739, 0.42438939213752747, 0.292267382144928, 0.9955736994743347, 0.5782875418663025, 0.6286752820014954, 0.5036677122116089, 0.967823326587677, 0.4833261966705322, 0.766798734664917, 0.19579093158245087, 0.7847087979316711, 0.14064885675907135, 0.3163905441761017, 0.3534391522407532, 0.5600557327270508, 0.579900324344635, 0.23404008150100708, 0.005727048963308334, 0.5813160538673401, 0.01717018522322178, 0.5092810988426208, 0.9841327667236328, 0.6338550448417664, 0.19782783091068268, 0.16464705765247345, 0.5760481953620911, 0.520610511302948, 0.28165581822395325, 0.46545112133026123, 0.6136520504951477, 0.8143494725227356, 0.09393561631441116, 0.5538557171821594, 0.44886714220046997, 0.2512478232383728, 0.8680607676506042, 0.399354487657547, 0.5526840686798096, 0.5933082699775696, 0.13844867050647736, 0.1981501430273056, 0.8916971683502197, 0.5876959562301636, 0.5719329714775085, 0.3537253439426422, 0.04788757860660553, 0.02979571372270584, 0.09272931516170502, 0.27187415957450867, 0.852651834487915, 0.19329948723316193, 0.46743708848953247, 0.939703106880188, 0.47911715507507324, 0.9209043383598328, 0.5309937000274658, 0.7260075807571411, 0.9828304052352905, 0.7219918966293335, 0.659299373626709, 0.5417682528495789, 0.8763168454170227, 0.5106425285339355, 0.9952358603477478, 0.6798291206359863, 0.5453009605407715, 0.09697271138429642, 0.1733456254005432, 0.8664087653160095, 0.44362762570381165, 0.2626873254776001, 0.7167802453041077, 0.1244666650891304, 0.6653802990913391, 0.6156637072563171, 0.4706658720970154, 0.9674145579338074, 0.6807290315628052, 0.7481148838996887, 0.6719505786895752, 0.46235352754592896, 0.6014818549156189, 0.9597489833831787, 0.48914626240730286, 0.01173090748488903, 0.1175665482878685, 0.3604207932949066, 0.18631888926029205, 0.4665635824203491, 0.4978933334350586, 0.040717560797929764, 0.9495974183082581, 0.6180967688560486, 0.24315766990184784, 0.11525940895080566, 0.7962961792945862, 0.08771093934774399, 0.08928979933261871, 0.5935438275337219, 0.7828124761581421, 0.4482303261756897, 0.2758917510509491, 0.5934372544288635, 0.09283921867609024, 0.22732587158679962, 0.29399821162223816, 0.9434512257575989, 0.26096436381340027, 0.8421211242675781, 0.974748969078064, 0.9371832609176636, 0.12602777779102325, 0.9594656825065613, 0.07364021241664886, 0.5264202356338501, 0.7890608310699463, 0.18414585292339325, 0.49163490533828735, 0.8185514211654663, 0.10454992204904556, 0.6770040392875671, 0.22754012048244476, 0.7239787578582764, 0.5678955912590027, 0.3811268210411072, 0.3339203894138336, 0.8703245520591736, 0.03550371155142784, 0.36733147501945496, 0.058192674070596695, 0.7903568744659424, 0.12307365238666534, 0.10755634307861328, 0.5055915117263794, 0.508309543132782, 0.5379215478897095, 0.5199129581451416, 0.2715112566947937, 0.8450196981430054, 0.18779662251472473, 0.9275662302970886, 0.19050894677639008, 0.6769587397575378, 0.12378307431936264, 0.31935378909111023, 0.7833172678947449, 0.6862653493881226, 0.9170185923576355, 0.0231446772813797, 0.17521077394485474, 0.35699254274368286, 0.2215559035539627, 0.37011924386024475, 0.5294469594955444, 6.717982614645734e-05, 0.9129687547683716, 0.7356518507003784, 0.13426870107650757, 0.7087186574935913, 0.3463948369026184, 0.4057849645614624, 0.7860741019248962, 0.10635919868946075, 0.15712665021419525, 0.12894678115844727, 0.3107292056083679, 0.8087502717971802, 0.4636392295360565, 0.8801515698432922, 0.6633811593055725, 0.86961829662323, 0.2541981041431427, 0.7937475442886353, 0.5168886780738831, 0.31621718406677246, 0.054082371294498444, 0.08715332299470901, 0.09082730859518051, 0.6406719088554382, 0.025813834741711617, 0.5210179686546326, 0.7468615770339966, 0.735705554485321, 0.7209197282791138, 0.16627326607704163, 0.6818466186523438, 0.07570032775402069, 0.6452698707580566, 0.9032213687896729, 0.09087177366018295, 0.6876680254936218, 0.8248136043548584, 0.1988743245601654, 0.1987718641757965, 0.09440569579601288, 0.3404725193977356, 0.6257284879684448, 0.1982394903898239, 0.7607031464576721, 0.06344626843929291, 0.4921787679195404, 0.7729811668395996, 0.3456858992576599, 0.5470910668373108, 0.633741021156311, 0.016785666346549988, 0.6021753549575806, 0.2552485466003418, 0.6180494427680969, 0.5762574076652527, 0.20972971618175507, 0.9751070141792297, 0.6453699469566345, 0.7886140942573547, 0.46664610505104065, 0.39756059646606445, 0.23134426772594452, 0.3185988664627075, 0.9185174703598022, 0.03797558322548866, 0.5000339150428772, 0.3471233546733856, 0.7015897631645203, 0.716751217842102, 0.9473224878311157, 0.562950074672699, 0.22759200632572174, 0.5228664875030518, 0.6346879005432129, 0.01928076148033142, 0.4793979525566101, 0.366658091545105, 0.1526632010936737, 0.166905015707016, 0.3889158368110657, 0.5573446750640869, 0.28172141313552856, 0.2902773916721344, 0.05255081504583359, 0.9439998865127563, 0.9997389912605286, 0.7220163941383362, 0.8085923790931702, 0.7423213720321655, 0.15351726114749908, 0.587762713432312, 0.7473716139793396, 0.4295557141304016, 0.018429404124617577, 0.6862674951553345, 0.09170002490282059, 0.05863531678915024, 0.4788166582584381, 0.21656790375709534, 0.6931068897247314, 0.13190516829490662, 0.1157134547829628, 0.5468841791152954, 0.3306739926338196, 0.9127704501152039, 0.3808678388595581, 0.8459193706512451, 0.32666724920272827, 0.9610130786895752, 0.4825980067253113, 0.45404165983200073, 0.5204469561576843, 0.19685064256191254, 0.6858335733413696, 0.8462364077568054, 0.3045005202293396, 0.39347872138023376, 0.044037505984306335, 0.2996792793273926, 0.7998414635658264, 0.06761251389980316, 0.9685580134391785, 0.5936104655265808, 0.4198245108127594, 0.41583484411239624, 0.5145580768585205, 0.6971230506896973, 0.21945533156394958, 0.39292266964912415, 0.8407564163208008, 0.15536290407180786, 0.9024173617362976, 0.00247236923314631, 0.29345983266830444, 0.5096447467803955, 0.0034719877876341343, 0.7949544191360474, 0.931050181388855, 0.9282593727111816, 0.25616368651390076, 0.7313158512115479, 0.9769437909126282, 0.35913974046707153, 0.5074560046195984, 0.22851108014583588, 0.9156183004379272, 0.9055492281913757, 0.6943511962890625, 0.46594855189323425, 0.09837134927511215, 0.06936425715684891, 0.009466690011322498, 0.6253657937049866, 0.8391492366790771, 0.9122130274772644, 0.3704187273979187, 0.8572385907173157, 0.5044439435005188, 0.7268729209899902, 0.8660553693771362, 0.13155615329742432, 0.8488684296607971, 0.8632239699363708, 0.4802361726760864, 0.6805127263069153, 0.386896550655365, 0.585968017578125, 0.37017130851745605, 0.08078940957784653, 0.14147186279296875, 0.60914546251297, 0.36866000294685364, 0.13373130559921265, 0.059651073068380356, 0.1937275230884552, 0.6160009503364563, 0.042797837406396866, 0.9807227253913879, 0.184631809592247, 0.48665565252304077, 0.27797529101371765, 0.3090546131134033, 0.5570073127746582, 0.08491866290569305, 0.8760199546813965, 0.23532593250274658, 0.5632840991020203, 0.08473226428031921, 0.8284323811531067, 0.8508289456367493, 0.6349027156829834, 0.7027525305747986, 0.2421765774488449, 0.3333284854888916, 0.5980463624000549, 0.4671682119369507, 0.666409432888031, 0.0005141752189956605, 0.033727847039699554, 0.2065356969833374, 0.630534827709198, 0.008353018201887608, 0.9305593371391296, 0.6358621716499329, 0.9827827215194702, 0.3788571059703827, 0.0977051705121994, 0.24773113429546356, 0.09445073455572128, 0.2571496367454529, 0.4321674406528473, 0.34575697779655457, 0.5095869898796082, 0.7434729933738708, 0.8296504020690918, 0.4839027523994446, 0.7105902433395386, 0.4466587007045746, 0.6153427362442017, 0.002875693142414093, 0.46688929200172424, 0.6457183361053467, 0.5869255065917969, 0.4247977137565613, 0.8592257499694824, 0.17829230427742004, 0.7157182097434998, 0.06392519921064377, 0.7079163789749146, 0.11764603108167648, 0.7123359441757202, 0.627219557762146, 0.33176979422569275, 0.45311209559440613, 0.8139302134513855, 0.8223478198051453, 0.43897387385368347, 0.8864006996154785, 0.960909366607666, 0.052766717970371246, 0.5082341432571411, 0.36199989914894104, 0.6047079563140869, 0.9416998624801636, 0.30298563838005066, 0.11604651808738708, 0.5360314249992371, 0.7739596962928772, 0.49034741520881653, 0.1231665089726448, 0.2907046973705292, 0.5804620385169983, 0.2557554244995117, 0.9237532615661621, 0.6670106649398804, 0.3446386754512787, 0.7404107451438904, 0.9482900500297546, 0.31070035696029663, 0.5474882125854492, 0.6283774375915527, 0.4318910539150238, 0.0639648288488388, 0.7692599296569824, 0.5423433780670166, 0.2561149597167969, 0.5230444073677063, 0.14105580747127533, 0.14943192899227142, 0.11810968816280365, 0.4393440783023834, 0.5630103945732117, 0.7929814457893372, 0.6630560755729675, 0.8917015194892883, 0.4747299551963806, 0.036505404859781265, 0.21109193563461304, 0.5875652432441711, 0.45002779364585876, 0.43828272819519043, 0.21201376616954803, 0.38454151153564453, 0.44878706336021423, 0.5782598853111267, 0.2619844973087311, 0.009038439020514488, 0.5415060520172119, 0.45001932978630066, 0.01530265249311924, 0.5731189846992493, 0.024035373702645302, 0.6066468358039856, 0.3898581564426422, 0.2473974972963333, 0.5242909789085388, 0.11061633378267288, 0.19682657718658447, 0.8347025513648987, 0.01720421388745308, 0.03111749142408371, 0.6841902732849121, 0.3329467475414276, 0.19958436489105225, 0.6310383081436157, 0.5089201331138611, 0.5387365818023682, 0.7201129794120789, 0.3405286967754364, 0.04960660636425018, 0.5655655264854431, 0.36494195461273193, 0.7684902548789978, 0.42518776655197144, 0.8779001832008362, 0.03508290648460388, 0.30599987506866455, 0.6106510758399963, 0.6684430837631226, 0.8076345920562744, 0.26441749930381775, 0.9292536973953247, 0.8187693357467651, 0.3178878724575043, 0.18841876089572906, 0.23955197632312775, 0.2733471691608429, 0.8531033396720886, 0.39104071259498596, 0.5649981498718262, 0.06740880012512207, 0.2897658348083496, 0.7194886803627014, 0.19315999746322632, 0.9832680821418762, 0.26382723450660706, 0.4986177980899811, 0.7895559668540955, 0.7448020577430725, 0.9712573289871216, 0.5988581776618958, 0.07977522909641266, 0.007080813404172659, 0.8211133480072021, 0.5567675828933716, 0.9537816047668457, 0.9336162209510803, 0.8342453837394714, 0.46236658096313477, 0.46453168988227844, 0.17018693685531616, 0.8445934057235718, 0.49934864044189453, 0.654381513595581, 0.5808459520339966, 0.7013759613037109, 0.7584179043769836, 0.08299725502729416, 0.24084189534187317, 0.5675965547561646, 0.06994365900754929, 0.020431555807590485, 0.6405585408210754, 0.06533528119325638, 0.13273325562477112, 0.3106120526790619, 0.30822446942329407, 0.7650657296180725, 0.6063564419746399, 0.838714063167572, 0.6945788860321045, 0.12809361517429352, 0.347777783870697, 0.27233177423477173, 0.8397007584571838, 0.8174160122871399, 0.646308183670044, 0.9672423005104065, 0.23640835285186768, 0.968144953250885, 0.1399688720703125, 0.045676879584789276, 0.2696036100387573, 0.05715697631239891, 0.9280192852020264, 0.9468095898628235, 0.2615559995174408, 0.6287650465965271, 0.47174689173698425, 0.6059722304344177, 0.7091386318206787, 0.4409760534763336, 0.08488119393587112, 0.8894966244697571, 0.5357226729393005, 0.45271894335746765, 0.4052424728870392, 0.7691981792449951, 0.9568786025047302, 0.10862185060977936, 0.7089368104934692, 0.8359880447387695, 0.5120929479598999, 0.42965301871299744, 0.6743569374084473, 0.6707550883293152, 0.8416394591331482, 0.8370009660720825, 0.009814570657908916, 0.9164296388626099, 0.4565296769142151, 0.48369884490966797, 0.5746312737464905, 0.5153519511222839, 0.3172641396522522, 0.8007677793502808, 0.12933330237865448, 0.29192593693733215, 0.610188901424408, 0.519863486289978, 0.11111748218536377, 0.255191445350647, 0.5477582812309265, 0.606847882270813, 0.6999751925468445, 0.9626180529594421, 0.4698432981967926, 0.7564738392829895, 0.1280393898487091, 0.3040427565574646, 0.45134568214416504, 0.0934700071811676, 0.139090433716774, 0.05378109589219093, 0.9277908205986023, 0.6391209363937378, 0.027721915394067764, 0.08225604891777039, 0.026309454813599586, 0.3507021367549896, 0.6619359254837036, 0.2175619900226593, 0.4157404601573944, 0.18545623123645782, 0.09934478998184204, 0.2810831069946289, 0.7510949373245239, 0.4693436026573181, 0.17964975535869598, 0.20145252346992493, 0.7700541019439697, 0.6085237264633179, 0.9989972710609436, 0.8452189564704895, 0.6333275437355042, 0.46379053592681885, 0.3697148859500885, 0.6963803768157959, 0.6128230690956116, 0.9614061713218689, 0.907155454158783, 0.7865278720855713, 0.09122147411108017, 0.21625956892967224, 0.5652353167533875, 0.3149380385875702, 0.3779014050960541, 0.934637188911438, 0.3907920718193054, 0.6841690540313721, 0.7081262469291687, 0.1339622586965561, 0.4651813507080078, 0.824341893196106, 0.807670533657074, 0.7774966359138489, 0.1051517203450203, 0.10685788840055466, 0.9956139326095581, 0.7164419889450073, 0.2343447059392929, 0.3706846833229065, 0.7692639231681824, 0.6972052454948425, 0.6042316555976868, 0.8667473196983337, 0.8110538125038147, 0.50572669506073, 0.49257585406303406, 0.24587547779083252, 0.11286971718072891, 0.8328279852867126, 0.20043061673641205, 0.1039147600531578, 0.7267220616340637, 0.7081754207611084, 0.8249654769897461, 0.4123005270957947, 0.7710753679275513, 0.5381021499633789, 0.5463727712631226, 0.8270867466926575, 0.01593414694070816, 0.19534611701965332, 0.401783287525177, 0.7744907736778259, 0.48401397466659546, 0.8049760460853577, 0.909207820892334, 0.8808935284614563, 0.5254150032997131, 0.7754223346710205, 0.7936505079269409, 0.8643978834152222, 0.4903126060962677, 0.5160192251205444, 0.7755321264266968, 0.38127943873405457, 0.4602121412754059, 0.7903076410293579, 0.5362173914909363, 0.7737277150154114, 0.7356213927268982, 0.9877470135688782, 0.7999483346939087, 0.8856385350227356, 0.8227282166481018, 0.47895029187202454, 0.11099491268396378, 0.3312976658344269, 0.699544370174408, 0.6535815000534058, 0.6789493560791016, 0.7733816504478455, 0.35773003101348877, 0.061042334884405136, 0.9580310583114624, 0.5968562960624695, 0.7581431865692139, 0.020538950338959694, 0.3414766490459442, 0.5249534249305725, 0.8918085694313049, 0.9821330904960632, 0.6482757925987244, 0.30821436643600464, 0.11024878174066544, 0.5639818906784058, 0.35285237431526184, 0.4563414454460144, 0.942164421081543, 0.9474254846572876, 0.028075125068426132, 0.2743256688117981, 0.08473861962556839, 0.6840551495552063, 0.5567184686660767, 0.810767650604248, 0.6355850100517273, 0.7172819375991821, 0.5425448417663574, 0.19951596856117249, 0.5432964563369751, 0.17484483122825623, 0.4648190438747406, 0.7156330943107605, 0.835309624671936, 0.11984552443027496, 0.10014937072992325, 0.34979158639907837, 0.5436074733734131, 0.5514843463897705, 0.11967451125383377, 0.3954598009586334, 0.21164147555828094, 0.9456548690795898, 0.546157717704773, 0.37832701206207275, 0.6458828449249268, 0.9365729689598083, 0.277798593044281, 0.39090943336486816, 0.5618823766708374, 0.8573434948921204, 0.9585562348365784, 0.9310038685798645, 0.8510586619377136, 0.7534677386283875, 0.7573729157447815, 0.5645626187324524, 0.47448647022247314, 0.5411547422409058, 0.02151353284716606, 0.9607899785041809, 0.40741363167762756, 0.2519567310810089, 0.09171804785728455, 0.5359310507774353, 0.475903183221817, 0.0474948026239872, 0.7082989811897278, 0.9888678193092346, 0.12648242712020874, 0.32068783044815063, 0.7392951250076294, 0.30736541748046875, 0.3329375088214874, 0.9997708797454834, 0.20799744129180908, 0.28629162907600403, 0.0791289210319519, 0.08272352069616318, 0.36255156993865967, 0.9535930156707764, 0.8446369171142578, 0.959002673625946, 0.9685333371162415, 0.1986090987920761, 0.10240170359611511, 0.1988026648759842, 0.9589047431945801, 0.6871894001960754, 0.7604759931564331, 0.7184842824935913, 0.39039474725723267, 0.4590420722961426, 0.150106281042099, 0.7402786016464233, 0.8850541114807129, 0.7388550639152527, 0.5613917112350464], 10, map[nprobe, 5])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vector115_value1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5030,7 +5034,7 @@
   <dimension ref="A1:L255"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A221" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E258" sqref="E258"/>
+      <selection activeCell="H252" sqref="H252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -13718,6 +13722,9 @@
       </c>
       <c r="F255" s="1" t="s">
         <v>1291</v>
+      </c>
+      <c r="G255" s="3" t="s">
+        <v>1323</v>
       </c>
       <c r="I255" s="1" t="s">
         <v>969</v>

</xml_diff>

<commit_message>
update some cases expected result for pow function
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/index/index_cases1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2747" uniqueCount="1334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2747" uniqueCount="1335">
   <si>
     <t>TestID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4694,6 +4694,9 @@
   <si>
     <t>select price from $scalar005 where price=2.5</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -5069,8 +5072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C228" sqref="C228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -12803,7 +12806,7 @@
         <v>1133</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>8</v>
+        <v>1334</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>1134</v>

</xml_diff>